<commit_message>
hoant2 : fix bug 003 013
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/ローマ字氏名届_帳票テンプレート.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/ローマ字氏名届_帳票テンプレート.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ACBC893-CF62-4A59-A474-EFF4265221CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{643680F2-0959-4932-9298-495B5B29373B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14,10 +14,6 @@
     <definedName name="A1_0">'2号'!$C$4</definedName>
     <definedName name="A1_1">'2号'!$B$12:$E$12</definedName>
     <definedName name="A1_9">'2号'!$C$4</definedName>
-    <definedName name="A2_1">'2号'!$F$15</definedName>
-    <definedName name="A2_2">'2号'!$T$15</definedName>
-    <definedName name="A2_3">'2号'!$F$14</definedName>
-    <definedName name="A2_4">'2号'!$T$14</definedName>
     <definedName name="A3_1">'2号'!$F$25</definedName>
     <definedName name="A3_3">'2号'!$F$27:$Q$29</definedName>
     <definedName name="A3_4">'2号'!$F$30:$Q$32</definedName>
@@ -1544,6 +1540,63 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1565,9 +1618,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1598,74 +1648,20 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="6"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="6"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3531,8 +3527,8 @@
   </sheetPr>
   <dimension ref="A1:AL43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="T15" sqref="T15:AJ15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="T17" sqref="T17:T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.140625" defaultRowHeight="15"/>
@@ -3575,11 +3571,11 @@
       <c r="AC1" s="27"/>
       <c r="AD1" s="27"/>
       <c r="AE1" s="27"/>
-      <c r="AI1" s="111">
+      <c r="AI1" s="130">
         <v>72073</v>
       </c>
-      <c r="AJ1" s="111"/>
-      <c r="AK1" s="111"/>
+      <c r="AJ1" s="130"/>
+      <c r="AK1" s="130"/>
       <c r="AL1" s="27"/>
     </row>
     <row r="2" spans="1:38" ht="26.25" customHeight="1">
@@ -3614,16 +3610,16 @@
       <c r="AC2" s="27"/>
       <c r="AD2" s="27"/>
       <c r="AE2" s="27"/>
-      <c r="AF2" s="123" t="s">
+      <c r="AF2" s="141" t="s">
         <v>23</v>
       </c>
-      <c r="AG2" s="124"/>
-      <c r="AH2" s="125"/>
-      <c r="AI2" s="126" t="s">
+      <c r="AG2" s="142"/>
+      <c r="AH2" s="143"/>
+      <c r="AI2" s="144" t="s">
         <v>24</v>
       </c>
-      <c r="AJ2" s="124"/>
-      <c r="AK2" s="125"/>
+      <c r="AJ2" s="142"/>
+      <c r="AK2" s="143"/>
       <c r="AL2" s="27"/>
     </row>
     <row r="3" spans="1:38" ht="26.25" customHeight="1">
@@ -3747,122 +3743,122 @@
     </row>
     <row r="6" spans="1:38" ht="13.5" customHeight="1">
       <c r="A6" s="82"/>
-      <c r="B6" s="132" t="s">
+      <c r="B6" s="124" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="132"/>
-      <c r="D6" s="132"/>
-      <c r="E6" s="132"/>
-      <c r="F6" s="132"/>
-      <c r="G6" s="132"/>
-      <c r="H6" s="132"/>
-      <c r="I6" s="132"/>
-      <c r="J6" s="132"/>
-      <c r="K6" s="132"/>
-      <c r="L6" s="132"/>
-      <c r="M6" s="132"/>
-      <c r="N6" s="132"/>
-      <c r="O6" s="132"/>
-      <c r="P6" s="132"/>
-      <c r="Q6" s="132"/>
-      <c r="R6" s="132"/>
-      <c r="S6" s="132"/>
-      <c r="T6" s="132"/>
-      <c r="U6" s="132"/>
-      <c r="V6" s="132"/>
-      <c r="W6" s="132"/>
-      <c r="X6" s="132"/>
-      <c r="Y6" s="132"/>
-      <c r="Z6" s="132"/>
-      <c r="AA6" s="132"/>
-      <c r="AB6" s="132"/>
-      <c r="AC6" s="132"/>
-      <c r="AD6" s="132"/>
-      <c r="AE6" s="132"/>
-      <c r="AF6" s="132"/>
-      <c r="AG6" s="132"/>
-      <c r="AH6" s="132"/>
-      <c r="AI6" s="132"/>
-      <c r="AJ6" s="132"/>
-      <c r="AK6" s="133"/>
+      <c r="C6" s="124"/>
+      <c r="D6" s="124"/>
+      <c r="E6" s="124"/>
+      <c r="F6" s="124"/>
+      <c r="G6" s="124"/>
+      <c r="H6" s="124"/>
+      <c r="I6" s="124"/>
+      <c r="J6" s="124"/>
+      <c r="K6" s="124"/>
+      <c r="L6" s="124"/>
+      <c r="M6" s="124"/>
+      <c r="N6" s="124"/>
+      <c r="O6" s="124"/>
+      <c r="P6" s="124"/>
+      <c r="Q6" s="124"/>
+      <c r="R6" s="124"/>
+      <c r="S6" s="124"/>
+      <c r="T6" s="124"/>
+      <c r="U6" s="124"/>
+      <c r="V6" s="124"/>
+      <c r="W6" s="124"/>
+      <c r="X6" s="124"/>
+      <c r="Y6" s="124"/>
+      <c r="Z6" s="124"/>
+      <c r="AA6" s="124"/>
+      <c r="AB6" s="124"/>
+      <c r="AC6" s="124"/>
+      <c r="AD6" s="124"/>
+      <c r="AE6" s="124"/>
+      <c r="AF6" s="124"/>
+      <c r="AG6" s="124"/>
+      <c r="AH6" s="124"/>
+      <c r="AI6" s="124"/>
+      <c r="AJ6" s="124"/>
+      <c r="AK6" s="125"/>
     </row>
     <row r="7" spans="1:38" ht="13.5" customHeight="1">
       <c r="A7" s="83"/>
-      <c r="B7" s="134"/>
-      <c r="C7" s="134"/>
-      <c r="D7" s="134"/>
-      <c r="E7" s="134"/>
-      <c r="F7" s="134"/>
-      <c r="G7" s="134"/>
-      <c r="H7" s="134"/>
-      <c r="I7" s="134"/>
-      <c r="J7" s="134"/>
-      <c r="K7" s="134"/>
-      <c r="L7" s="134"/>
-      <c r="M7" s="134"/>
-      <c r="N7" s="134"/>
-      <c r="O7" s="134"/>
-      <c r="P7" s="134"/>
-      <c r="Q7" s="134"/>
-      <c r="R7" s="134"/>
-      <c r="S7" s="134"/>
-      <c r="T7" s="134"/>
-      <c r="U7" s="134"/>
-      <c r="V7" s="134"/>
-      <c r="W7" s="134"/>
-      <c r="X7" s="134"/>
-      <c r="Y7" s="134"/>
-      <c r="Z7" s="134"/>
-      <c r="AA7" s="134"/>
-      <c r="AB7" s="134"/>
-      <c r="AC7" s="134"/>
-      <c r="AD7" s="134"/>
-      <c r="AE7" s="134"/>
-      <c r="AF7" s="134"/>
-      <c r="AG7" s="134"/>
-      <c r="AH7" s="134"/>
-      <c r="AI7" s="134"/>
-      <c r="AJ7" s="134"/>
-      <c r="AK7" s="135"/>
+      <c r="B7" s="126"/>
+      <c r="C7" s="126"/>
+      <c r="D7" s="126"/>
+      <c r="E7" s="126"/>
+      <c r="F7" s="126"/>
+      <c r="G7" s="126"/>
+      <c r="H7" s="126"/>
+      <c r="I7" s="126"/>
+      <c r="J7" s="126"/>
+      <c r="K7" s="126"/>
+      <c r="L7" s="126"/>
+      <c r="M7" s="126"/>
+      <c r="N7" s="126"/>
+      <c r="O7" s="126"/>
+      <c r="P7" s="126"/>
+      <c r="Q7" s="126"/>
+      <c r="R7" s="126"/>
+      <c r="S7" s="126"/>
+      <c r="T7" s="126"/>
+      <c r="U7" s="126"/>
+      <c r="V7" s="126"/>
+      <c r="W7" s="126"/>
+      <c r="X7" s="126"/>
+      <c r="Y7" s="126"/>
+      <c r="Z7" s="126"/>
+      <c r="AA7" s="126"/>
+      <c r="AB7" s="126"/>
+      <c r="AC7" s="126"/>
+      <c r="AD7" s="126"/>
+      <c r="AE7" s="126"/>
+      <c r="AF7" s="126"/>
+      <c r="AG7" s="126"/>
+      <c r="AH7" s="126"/>
+      <c r="AI7" s="126"/>
+      <c r="AJ7" s="126"/>
+      <c r="AK7" s="127"/>
     </row>
     <row r="8" spans="1:38" ht="13.5" customHeight="1">
       <c r="A8" s="83"/>
-      <c r="B8" s="134"/>
-      <c r="C8" s="134"/>
-      <c r="D8" s="134"/>
-      <c r="E8" s="134"/>
-      <c r="F8" s="134"/>
-      <c r="G8" s="134"/>
-      <c r="H8" s="134"/>
-      <c r="I8" s="134"/>
-      <c r="J8" s="134"/>
-      <c r="K8" s="134"/>
-      <c r="L8" s="134"/>
-      <c r="M8" s="134"/>
-      <c r="N8" s="134"/>
-      <c r="O8" s="134"/>
-      <c r="P8" s="134"/>
-      <c r="Q8" s="134"/>
-      <c r="R8" s="134"/>
-      <c r="S8" s="134"/>
-      <c r="T8" s="134"/>
-      <c r="U8" s="134"/>
-      <c r="V8" s="134"/>
-      <c r="W8" s="134"/>
-      <c r="X8" s="134"/>
-      <c r="Y8" s="134"/>
-      <c r="Z8" s="134"/>
-      <c r="AA8" s="134"/>
-      <c r="AB8" s="134"/>
-      <c r="AC8" s="134"/>
-      <c r="AD8" s="134"/>
-      <c r="AE8" s="134"/>
-      <c r="AF8" s="134"/>
-      <c r="AG8" s="134"/>
-      <c r="AH8" s="134"/>
-      <c r="AI8" s="134"/>
-      <c r="AJ8" s="134"/>
-      <c r="AK8" s="135"/>
+      <c r="B8" s="126"/>
+      <c r="C8" s="126"/>
+      <c r="D8" s="126"/>
+      <c r="E8" s="126"/>
+      <c r="F8" s="126"/>
+      <c r="G8" s="126"/>
+      <c r="H8" s="126"/>
+      <c r="I8" s="126"/>
+      <c r="J8" s="126"/>
+      <c r="K8" s="126"/>
+      <c r="L8" s="126"/>
+      <c r="M8" s="126"/>
+      <c r="N8" s="126"/>
+      <c r="O8" s="126"/>
+      <c r="P8" s="126"/>
+      <c r="Q8" s="126"/>
+      <c r="R8" s="126"/>
+      <c r="S8" s="126"/>
+      <c r="T8" s="126"/>
+      <c r="U8" s="126"/>
+      <c r="V8" s="126"/>
+      <c r="W8" s="126"/>
+      <c r="X8" s="126"/>
+      <c r="Y8" s="126"/>
+      <c r="Z8" s="126"/>
+      <c r="AA8" s="126"/>
+      <c r="AB8" s="126"/>
+      <c r="AC8" s="126"/>
+      <c r="AD8" s="126"/>
+      <c r="AE8" s="126"/>
+      <c r="AF8" s="126"/>
+      <c r="AG8" s="126"/>
+      <c r="AH8" s="126"/>
+      <c r="AI8" s="126"/>
+      <c r="AJ8" s="126"/>
+      <c r="AK8" s="127"/>
     </row>
     <row r="9" spans="1:38" ht="18.75" customHeight="1">
       <c r="A9" s="83"/>
@@ -3978,27 +3974,27 @@
       <c r="S11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="T11" s="112" t="s">
+      <c r="T11" s="131" t="s">
         <v>27</v>
       </c>
-      <c r="U11" s="113"/>
-      <c r="V11" s="112" t="s">
+      <c r="U11" s="132"/>
+      <c r="V11" s="131" t="s">
         <v>18</v>
       </c>
-      <c r="W11" s="116"/>
-      <c r="X11" s="116"/>
-      <c r="Y11" s="116"/>
-      <c r="Z11" s="113"/>
-      <c r="AA11" s="118"/>
-      <c r="AB11" s="119"/>
-      <c r="AC11" s="119"/>
-      <c r="AD11" s="119"/>
-      <c r="AE11" s="119"/>
-      <c r="AF11" s="122"/>
-      <c r="AG11" s="119"/>
-      <c r="AH11" s="119"/>
-      <c r="AI11" s="119"/>
-      <c r="AJ11" s="119"/>
+      <c r="W11" s="135"/>
+      <c r="X11" s="135"/>
+      <c r="Y11" s="135"/>
+      <c r="Z11" s="132"/>
+      <c r="AA11" s="136"/>
+      <c r="AB11" s="137"/>
+      <c r="AC11" s="137"/>
+      <c r="AD11" s="137"/>
+      <c r="AE11" s="137"/>
+      <c r="AF11" s="140"/>
+      <c r="AG11" s="137"/>
+      <c r="AH11" s="137"/>
+      <c r="AI11" s="137"/>
+      <c r="AJ11" s="137"/>
       <c r="AK11" s="84"/>
     </row>
     <row r="12" spans="1:38" ht="40.5" customHeight="1" thickBot="1">
@@ -4021,23 +4017,23 @@
       <c r="Q12" s="57"/>
       <c r="R12" s="58"/>
       <c r="S12" s="50"/>
-      <c r="T12" s="114"/>
-      <c r="U12" s="115"/>
-      <c r="V12" s="114"/>
-      <c r="W12" s="117"/>
-      <c r="X12" s="117"/>
-      <c r="Y12" s="117"/>
-      <c r="Z12" s="115"/>
-      <c r="AA12" s="120"/>
-      <c r="AB12" s="121"/>
-      <c r="AC12" s="121"/>
-      <c r="AD12" s="121"/>
-      <c r="AE12" s="121"/>
-      <c r="AF12" s="121"/>
-      <c r="AG12" s="121"/>
-      <c r="AH12" s="121"/>
-      <c r="AI12" s="121"/>
-      <c r="AJ12" s="121"/>
+      <c r="T12" s="133"/>
+      <c r="U12" s="134"/>
+      <c r="V12" s="133"/>
+      <c r="W12" s="128"/>
+      <c r="X12" s="128"/>
+      <c r="Y12" s="128"/>
+      <c r="Z12" s="134"/>
+      <c r="AA12" s="138"/>
+      <c r="AB12" s="139"/>
+      <c r="AC12" s="139"/>
+      <c r="AD12" s="139"/>
+      <c r="AE12" s="139"/>
+      <c r="AF12" s="139"/>
+      <c r="AG12" s="139"/>
+      <c r="AH12" s="139"/>
+      <c r="AI12" s="139"/>
+      <c r="AJ12" s="139"/>
       <c r="AK12" s="84"/>
     </row>
     <row r="13" spans="1:38" ht="23.25" customHeight="1" thickBot="1">
@@ -4083,7 +4079,7 @@
     </row>
     <row r="14" spans="1:38" ht="25.5" customHeight="1">
       <c r="A14" s="83"/>
-      <c r="B14" s="128" t="s">
+      <c r="B14" s="120" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -4091,78 +4087,78 @@
       </c>
       <c r="D14" s="26"/>
       <c r="E14" s="96"/>
-      <c r="F14" s="139"/>
-      <c r="G14" s="139"/>
-      <c r="H14" s="139"/>
-      <c r="I14" s="139"/>
-      <c r="J14" s="139"/>
-      <c r="K14" s="139"/>
-      <c r="L14" s="139"/>
-      <c r="M14" s="139"/>
-      <c r="N14" s="139"/>
-      <c r="O14" s="139"/>
-      <c r="P14" s="139"/>
-      <c r="Q14" s="139"/>
-      <c r="R14" s="139"/>
-      <c r="S14" s="139"/>
-      <c r="T14" s="139"/>
-      <c r="U14" s="139"/>
-      <c r="V14" s="139"/>
-      <c r="W14" s="139"/>
-      <c r="X14" s="139"/>
-      <c r="Y14" s="139"/>
-      <c r="Z14" s="139"/>
-      <c r="AA14" s="139"/>
-      <c r="AB14" s="139"/>
-      <c r="AC14" s="139"/>
-      <c r="AD14" s="139"/>
-      <c r="AE14" s="139"/>
-      <c r="AF14" s="139"/>
-      <c r="AG14" s="139"/>
-      <c r="AH14" s="139"/>
-      <c r="AI14" s="139"/>
-      <c r="AJ14" s="140"/>
+      <c r="F14" s="149"/>
+      <c r="G14" s="149"/>
+      <c r="H14" s="149"/>
+      <c r="I14" s="149"/>
+      <c r="J14" s="149"/>
+      <c r="K14" s="149"/>
+      <c r="L14" s="149"/>
+      <c r="M14" s="149"/>
+      <c r="N14" s="149"/>
+      <c r="O14" s="149"/>
+      <c r="P14" s="149"/>
+      <c r="Q14" s="149"/>
+      <c r="R14" s="149"/>
+      <c r="S14" s="149"/>
+      <c r="T14" s="149"/>
+      <c r="U14" s="149"/>
+      <c r="V14" s="149"/>
+      <c r="W14" s="149"/>
+      <c r="X14" s="149"/>
+      <c r="Y14" s="149"/>
+      <c r="Z14" s="149"/>
+      <c r="AA14" s="149"/>
+      <c r="AB14" s="149"/>
+      <c r="AC14" s="149"/>
+      <c r="AD14" s="149"/>
+      <c r="AE14" s="149"/>
+      <c r="AF14" s="149"/>
+      <c r="AG14" s="149"/>
+      <c r="AH14" s="149"/>
+      <c r="AI14" s="149"/>
+      <c r="AJ14" s="150"/>
       <c r="AK14" s="84"/>
     </row>
     <row r="15" spans="1:38" ht="60.75" customHeight="1" thickBot="1">
       <c r="A15" s="83"/>
-      <c r="B15" s="129"/>
+      <c r="B15" s="121"/>
       <c r="C15" s="6" t="s">
         <v>30</v>
       </c>
       <c r="D15" s="35"/>
       <c r="E15" s="95"/>
-      <c r="F15" s="136"/>
-      <c r="G15" s="136"/>
-      <c r="H15" s="136"/>
-      <c r="I15" s="136"/>
-      <c r="J15" s="136"/>
-      <c r="K15" s="136"/>
-      <c r="L15" s="136"/>
-      <c r="M15" s="136"/>
-      <c r="N15" s="136"/>
-      <c r="O15" s="136"/>
-      <c r="P15" s="136"/>
-      <c r="Q15" s="136"/>
-      <c r="R15" s="136"/>
-      <c r="S15" s="136"/>
-      <c r="T15" s="137"/>
-      <c r="U15" s="137"/>
-      <c r="V15" s="137"/>
-      <c r="W15" s="137"/>
-      <c r="X15" s="137"/>
-      <c r="Y15" s="137"/>
-      <c r="Z15" s="137"/>
-      <c r="AA15" s="137"/>
-      <c r="AB15" s="137"/>
-      <c r="AC15" s="137"/>
-      <c r="AD15" s="137"/>
-      <c r="AE15" s="137"/>
-      <c r="AF15" s="137"/>
-      <c r="AG15" s="137"/>
-      <c r="AH15" s="137"/>
-      <c r="AI15" s="137"/>
-      <c r="AJ15" s="138"/>
+      <c r="F15" s="146"/>
+      <c r="G15" s="146"/>
+      <c r="H15" s="146"/>
+      <c r="I15" s="146"/>
+      <c r="J15" s="146"/>
+      <c r="K15" s="146"/>
+      <c r="L15" s="146"/>
+      <c r="M15" s="146"/>
+      <c r="N15" s="146"/>
+      <c r="O15" s="146"/>
+      <c r="P15" s="146"/>
+      <c r="Q15" s="146"/>
+      <c r="R15" s="146"/>
+      <c r="S15" s="146"/>
+      <c r="T15" s="147"/>
+      <c r="U15" s="147"/>
+      <c r="V15" s="147"/>
+      <c r="W15" s="147"/>
+      <c r="X15" s="147"/>
+      <c r="Y15" s="147"/>
+      <c r="Z15" s="147"/>
+      <c r="AA15" s="147"/>
+      <c r="AB15" s="147"/>
+      <c r="AC15" s="147"/>
+      <c r="AD15" s="147"/>
+      <c r="AE15" s="147"/>
+      <c r="AF15" s="147"/>
+      <c r="AG15" s="147"/>
+      <c r="AH15" s="147"/>
+      <c r="AI15" s="147"/>
+      <c r="AJ15" s="148"/>
       <c r="AK15" s="84"/>
     </row>
     <row r="16" spans="1:38" ht="23.25" customHeight="1" thickBot="1">
@@ -4187,30 +4183,30 @@
       <c r="Q16" s="64"/>
       <c r="R16" s="64"/>
       <c r="S16" s="64"/>
-      <c r="T16" s="130" t="s">
+      <c r="T16" s="122" t="s">
         <v>29</v>
       </c>
-      <c r="U16" s="130"/>
-      <c r="V16" s="130"/>
-      <c r="W16" s="130"/>
-      <c r="X16" s="130"/>
-      <c r="Y16" s="130"/>
-      <c r="Z16" s="130"/>
-      <c r="AA16" s="130"/>
-      <c r="AB16" s="130"/>
-      <c r="AC16" s="130"/>
-      <c r="AD16" s="130"/>
-      <c r="AE16" s="130"/>
-      <c r="AF16" s="130"/>
-      <c r="AG16" s="130"/>
-      <c r="AH16" s="130"/>
-      <c r="AI16" s="130"/>
-      <c r="AJ16" s="130"/>
+      <c r="U16" s="122"/>
+      <c r="V16" s="122"/>
+      <c r="W16" s="122"/>
+      <c r="X16" s="122"/>
+      <c r="Y16" s="122"/>
+      <c r="Z16" s="122"/>
+      <c r="AA16" s="122"/>
+      <c r="AB16" s="122"/>
+      <c r="AC16" s="122"/>
+      <c r="AD16" s="122"/>
+      <c r="AE16" s="122"/>
+      <c r="AF16" s="122"/>
+      <c r="AG16" s="122"/>
+      <c r="AH16" s="122"/>
+      <c r="AI16" s="122"/>
+      <c r="AJ16" s="122"/>
       <c r="AK16" s="84"/>
     </row>
     <row r="17" spans="1:37" ht="25.5" customHeight="1">
       <c r="A17" s="83"/>
-      <c r="B17" s="128" t="s">
+      <c r="B17" s="120" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -4232,7 +4228,7 @@
       <c r="Q17" s="101"/>
       <c r="R17" s="104"/>
       <c r="S17" s="27"/>
-      <c r="T17" s="128" t="s">
+      <c r="T17" s="120" t="s">
         <v>19</v>
       </c>
       <c r="U17" s="65"/>
@@ -4255,7 +4251,7 @@
     </row>
     <row r="18" spans="1:37" ht="37.5" customHeight="1" thickBot="1">
       <c r="A18" s="83"/>
-      <c r="B18" s="129"/>
+      <c r="B18" s="121"/>
       <c r="C18" s="6" t="s">
         <v>4</v>
       </c>
@@ -4277,7 +4273,7 @@
       <c r="Q18" s="100"/>
       <c r="R18" s="106"/>
       <c r="S18" s="27"/>
-      <c r="T18" s="131"/>
+      <c r="T18" s="123"/>
       <c r="U18" s="70"/>
       <c r="V18" s="27"/>
       <c r="W18" s="71"/>
@@ -4298,7 +4294,7 @@
     </row>
     <row r="19" spans="1:37" ht="25.5" customHeight="1" thickBot="1">
       <c r="A19" s="83"/>
-      <c r="B19" s="128" t="s">
+      <c r="B19" s="120" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="5" t="s">
@@ -4320,28 +4316,28 @@
       <c r="Q19" s="101"/>
       <c r="R19" s="104"/>
       <c r="S19" s="27"/>
-      <c r="T19" s="129"/>
+      <c r="T19" s="121"/>
       <c r="U19" s="43"/>
       <c r="V19" s="25"/>
       <c r="W19" s="25"/>
       <c r="X19" s="25"/>
-      <c r="Y19" s="117"/>
-      <c r="Z19" s="117"/>
-      <c r="AA19" s="117"/>
-      <c r="AB19" s="117"/>
-      <c r="AC19" s="117"/>
-      <c r="AD19" s="117"/>
-      <c r="AE19" s="117"/>
-      <c r="AF19" s="117"/>
-      <c r="AG19" s="117"/>
-      <c r="AH19" s="117"/>
-      <c r="AI19" s="117"/>
+      <c r="Y19" s="128"/>
+      <c r="Z19" s="128"/>
+      <c r="AA19" s="128"/>
+      <c r="AB19" s="128"/>
+      <c r="AC19" s="128"/>
+      <c r="AD19" s="128"/>
+      <c r="AE19" s="128"/>
+      <c r="AF19" s="128"/>
+      <c r="AG19" s="128"/>
+      <c r="AH19" s="128"/>
+      <c r="AI19" s="128"/>
       <c r="AJ19" s="24"/>
       <c r="AK19" s="84"/>
     </row>
     <row r="20" spans="1:37" ht="37.5" customHeight="1" thickBot="1">
       <c r="A20" s="83"/>
-      <c r="B20" s="129"/>
+      <c r="B20" s="121"/>
       <c r="C20" s="6" t="s">
         <v>4</v>
       </c>
@@ -4511,13 +4507,13 @@
       <c r="I24" s="28"/>
       <c r="J24" s="28"/>
       <c r="K24" s="28"/>
-      <c r="L24" s="127" t="s">
+      <c r="L24" s="145" t="s">
         <v>25</v>
       </c>
-      <c r="M24" s="127"/>
-      <c r="N24" s="127"/>
-      <c r="O24" s="127"/>
-      <c r="P24" s="127"/>
+      <c r="M24" s="145"/>
+      <c r="N24" s="145"/>
+      <c r="O24" s="145"/>
+      <c r="P24" s="145"/>
       <c r="Q24" s="29" t="s">
         <v>31</v>
       </c>
@@ -4548,13 +4544,13 @@
       <c r="C25" s="27"/>
       <c r="D25" s="27"/>
       <c r="E25" s="59"/>
-      <c r="F25" s="110" t="s">
+      <c r="F25" s="129" t="s">
         <v>28</v>
       </c>
-      <c r="G25" s="110"/>
-      <c r="H25" s="110"/>
-      <c r="I25" s="110"/>
-      <c r="J25" s="110"/>
+      <c r="G25" s="129"/>
+      <c r="H25" s="129"/>
+      <c r="I25" s="129"/>
+      <c r="J25" s="129"/>
       <c r="K25" s="28"/>
       <c r="L25" s="28"/>
       <c r="M25" s="28"/>
@@ -4589,11 +4585,11 @@
       <c r="C26" s="27"/>
       <c r="D26" s="27"/>
       <c r="E26" s="59"/>
-      <c r="F26" s="110"/>
-      <c r="G26" s="110"/>
-      <c r="H26" s="110"/>
-      <c r="I26" s="110"/>
-      <c r="J26" s="110"/>
+      <c r="F26" s="129"/>
+      <c r="G26" s="129"/>
+      <c r="H26" s="129"/>
+      <c r="I26" s="129"/>
+      <c r="J26" s="129"/>
       <c r="K26" s="28"/>
       <c r="L26" s="28"/>
       <c r="M26" s="28"/>
@@ -4628,18 +4624,18 @@
       <c r="C27" s="27"/>
       <c r="D27" s="27"/>
       <c r="E27" s="59"/>
-      <c r="F27" s="146"/>
-      <c r="G27" s="146"/>
-      <c r="H27" s="146"/>
-      <c r="I27" s="146"/>
-      <c r="J27" s="146"/>
-      <c r="K27" s="146"/>
-      <c r="L27" s="146"/>
-      <c r="M27" s="146"/>
-      <c r="N27" s="146"/>
-      <c r="O27" s="146"/>
-      <c r="P27" s="146"/>
-      <c r="Q27" s="146"/>
+      <c r="F27" s="115"/>
+      <c r="G27" s="115"/>
+      <c r="H27" s="115"/>
+      <c r="I27" s="115"/>
+      <c r="J27" s="115"/>
+      <c r="K27" s="115"/>
+      <c r="L27" s="115"/>
+      <c r="M27" s="115"/>
+      <c r="N27" s="115"/>
+      <c r="O27" s="115"/>
+      <c r="P27" s="115"/>
+      <c r="Q27" s="115"/>
       <c r="R27" s="40"/>
       <c r="S27" s="27"/>
       <c r="T27" s="27"/>
@@ -4663,24 +4659,24 @@
     </row>
     <row r="28" spans="1:37" ht="11.25" customHeight="1">
       <c r="A28" s="83"/>
-      <c r="B28" s="143" t="s">
+      <c r="B28" s="112" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="144"/>
-      <c r="D28" s="144"/>
-      <c r="E28" s="145"/>
-      <c r="F28" s="146"/>
-      <c r="G28" s="146"/>
-      <c r="H28" s="146"/>
-      <c r="I28" s="146"/>
-      <c r="J28" s="146"/>
-      <c r="K28" s="146"/>
-      <c r="L28" s="146"/>
-      <c r="M28" s="146"/>
-      <c r="N28" s="146"/>
-      <c r="O28" s="146"/>
-      <c r="P28" s="146"/>
-      <c r="Q28" s="146"/>
+      <c r="C28" s="113"/>
+      <c r="D28" s="113"/>
+      <c r="E28" s="114"/>
+      <c r="F28" s="115"/>
+      <c r="G28" s="115"/>
+      <c r="H28" s="115"/>
+      <c r="I28" s="115"/>
+      <c r="J28" s="115"/>
+      <c r="K28" s="115"/>
+      <c r="L28" s="115"/>
+      <c r="M28" s="115"/>
+      <c r="N28" s="115"/>
+      <c r="O28" s="115"/>
+      <c r="P28" s="115"/>
+      <c r="Q28" s="115"/>
       <c r="R28" s="40"/>
       <c r="S28" s="27"/>
       <c r="T28" s="27"/>
@@ -4708,18 +4704,18 @@
       <c r="C29" s="27"/>
       <c r="D29" s="27"/>
       <c r="E29" s="59"/>
-      <c r="F29" s="146"/>
-      <c r="G29" s="146"/>
-      <c r="H29" s="146"/>
-      <c r="I29" s="146"/>
-      <c r="J29" s="146"/>
-      <c r="K29" s="146"/>
-      <c r="L29" s="146"/>
-      <c r="M29" s="146"/>
-      <c r="N29" s="146"/>
-      <c r="O29" s="146"/>
-      <c r="P29" s="146"/>
-      <c r="Q29" s="146"/>
+      <c r="F29" s="115"/>
+      <c r="G29" s="115"/>
+      <c r="H29" s="115"/>
+      <c r="I29" s="115"/>
+      <c r="J29" s="115"/>
+      <c r="K29" s="115"/>
+      <c r="L29" s="115"/>
+      <c r="M29" s="115"/>
+      <c r="N29" s="115"/>
+      <c r="O29" s="115"/>
+      <c r="P29" s="115"/>
+      <c r="Q29" s="115"/>
       <c r="R29" s="40"/>
       <c r="S29" s="27"/>
       <c r="T29" s="27"/>
@@ -4747,18 +4743,18 @@
       <c r="C30" s="27"/>
       <c r="D30" s="27"/>
       <c r="E30" s="27"/>
-      <c r="F30" s="147"/>
-      <c r="G30" s="146"/>
-      <c r="H30" s="146"/>
-      <c r="I30" s="146"/>
-      <c r="J30" s="146"/>
-      <c r="K30" s="146"/>
-      <c r="L30" s="146"/>
-      <c r="M30" s="146"/>
-      <c r="N30" s="146"/>
-      <c r="O30" s="146"/>
-      <c r="P30" s="146"/>
-      <c r="Q30" s="146"/>
+      <c r="F30" s="116"/>
+      <c r="G30" s="115"/>
+      <c r="H30" s="115"/>
+      <c r="I30" s="115"/>
+      <c r="J30" s="115"/>
+      <c r="K30" s="115"/>
+      <c r="L30" s="115"/>
+      <c r="M30" s="115"/>
+      <c r="N30" s="115"/>
+      <c r="O30" s="115"/>
+      <c r="P30" s="115"/>
+      <c r="Q30" s="115"/>
       <c r="R30" s="40"/>
       <c r="S30" s="27"/>
       <c r="T30" s="27"/>
@@ -4782,24 +4778,24 @@
     </row>
     <row r="31" spans="1:37" ht="11.25" customHeight="1">
       <c r="A31" s="83"/>
-      <c r="B31" s="143" t="s">
+      <c r="B31" s="112" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="144"/>
-      <c r="D31" s="144"/>
-      <c r="E31" s="144"/>
-      <c r="F31" s="147"/>
-      <c r="G31" s="146"/>
-      <c r="H31" s="146"/>
-      <c r="I31" s="146"/>
-      <c r="J31" s="146"/>
-      <c r="K31" s="146"/>
-      <c r="L31" s="146"/>
-      <c r="M31" s="146"/>
-      <c r="N31" s="146"/>
-      <c r="O31" s="146"/>
-      <c r="P31" s="146"/>
-      <c r="Q31" s="146"/>
+      <c r="C31" s="113"/>
+      <c r="D31" s="113"/>
+      <c r="E31" s="113"/>
+      <c r="F31" s="116"/>
+      <c r="G31" s="115"/>
+      <c r="H31" s="115"/>
+      <c r="I31" s="115"/>
+      <c r="J31" s="115"/>
+      <c r="K31" s="115"/>
+      <c r="L31" s="115"/>
+      <c r="M31" s="115"/>
+      <c r="N31" s="115"/>
+      <c r="O31" s="115"/>
+      <c r="P31" s="115"/>
+      <c r="Q31" s="115"/>
       <c r="R31" s="40"/>
       <c r="S31" s="27"/>
       <c r="T31" s="27"/>
@@ -4827,18 +4823,18 @@
       <c r="C32" s="11"/>
       <c r="D32" s="11"/>
       <c r="E32" s="11"/>
-      <c r="F32" s="147"/>
-      <c r="G32" s="146"/>
-      <c r="H32" s="146"/>
-      <c r="I32" s="146"/>
-      <c r="J32" s="146"/>
-      <c r="K32" s="146"/>
-      <c r="L32" s="146"/>
-      <c r="M32" s="146"/>
-      <c r="N32" s="146"/>
-      <c r="O32" s="146"/>
-      <c r="P32" s="146"/>
-      <c r="Q32" s="146"/>
+      <c r="F32" s="116"/>
+      <c r="G32" s="115"/>
+      <c r="H32" s="115"/>
+      <c r="I32" s="115"/>
+      <c r="J32" s="115"/>
+      <c r="K32" s="115"/>
+      <c r="L32" s="115"/>
+      <c r="M32" s="115"/>
+      <c r="N32" s="115"/>
+      <c r="O32" s="115"/>
+      <c r="P32" s="115"/>
+      <c r="Q32" s="115"/>
       <c r="R32" s="40"/>
       <c r="S32" s="27"/>
       <c r="T32" s="27"/>
@@ -4866,17 +4862,17 @@
       <c r="C33" s="11"/>
       <c r="D33" s="11"/>
       <c r="E33" s="11"/>
-      <c r="F33" s="148"/>
-      <c r="G33" s="149"/>
-      <c r="H33" s="149"/>
-      <c r="I33" s="149"/>
-      <c r="J33" s="149"/>
-      <c r="K33" s="149"/>
-      <c r="L33" s="149"/>
-      <c r="M33" s="149"/>
-      <c r="N33" s="149"/>
-      <c r="O33" s="149"/>
-      <c r="P33" s="149"/>
+      <c r="F33" s="117"/>
+      <c r="G33" s="118"/>
+      <c r="H33" s="118"/>
+      <c r="I33" s="118"/>
+      <c r="J33" s="118"/>
+      <c r="K33" s="118"/>
+      <c r="L33" s="118"/>
+      <c r="M33" s="118"/>
+      <c r="N33" s="118"/>
+      <c r="O33" s="118"/>
+      <c r="P33" s="118"/>
       <c r="Q33" s="9"/>
       <c r="R33" s="40"/>
       <c r="S33" s="27"/>
@@ -4901,24 +4897,24 @@
     </row>
     <row r="34" spans="1:37" ht="11.25" customHeight="1">
       <c r="A34" s="83"/>
-      <c r="B34" s="143" t="s">
+      <c r="B34" s="112" t="s">
         <v>11</v>
       </c>
-      <c r="C34" s="144"/>
-      <c r="D34" s="144"/>
-      <c r="E34" s="144"/>
-      <c r="F34" s="148"/>
-      <c r="G34" s="149"/>
-      <c r="H34" s="149"/>
-      <c r="I34" s="149"/>
-      <c r="J34" s="149"/>
-      <c r="K34" s="149"/>
-      <c r="L34" s="149"/>
-      <c r="M34" s="149"/>
-      <c r="N34" s="149"/>
-      <c r="O34" s="149"/>
-      <c r="P34" s="149"/>
-      <c r="Q34" s="150" t="s">
+      <c r="C34" s="113"/>
+      <c r="D34" s="113"/>
+      <c r="E34" s="113"/>
+      <c r="F34" s="117"/>
+      <c r="G34" s="118"/>
+      <c r="H34" s="118"/>
+      <c r="I34" s="118"/>
+      <c r="J34" s="118"/>
+      <c r="K34" s="118"/>
+      <c r="L34" s="118"/>
+      <c r="M34" s="118"/>
+      <c r="N34" s="118"/>
+      <c r="O34" s="118"/>
+      <c r="P34" s="118"/>
+      <c r="Q34" s="119" t="s">
         <v>6</v>
       </c>
       <c r="R34" s="40"/>
@@ -4948,18 +4944,18 @@
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
       <c r="E35" s="10"/>
-      <c r="F35" s="148"/>
-      <c r="G35" s="149"/>
-      <c r="H35" s="149"/>
-      <c r="I35" s="149"/>
-      <c r="J35" s="149"/>
-      <c r="K35" s="149"/>
-      <c r="L35" s="149"/>
-      <c r="M35" s="149"/>
-      <c r="N35" s="149"/>
-      <c r="O35" s="149"/>
-      <c r="P35" s="149"/>
-      <c r="Q35" s="150"/>
+      <c r="F35" s="117"/>
+      <c r="G35" s="118"/>
+      <c r="H35" s="118"/>
+      <c r="I35" s="118"/>
+      <c r="J35" s="118"/>
+      <c r="K35" s="118"/>
+      <c r="L35" s="118"/>
+      <c r="M35" s="118"/>
+      <c r="N35" s="118"/>
+      <c r="O35" s="118"/>
+      <c r="P35" s="118"/>
+      <c r="Q35" s="119"/>
       <c r="R35" s="40"/>
       <c r="S35" s="27"/>
       <c r="T35" s="27"/>
@@ -4987,20 +4983,20 @@
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
       <c r="E36" s="61"/>
-      <c r="F36" s="141" t="s">
+      <c r="F36" s="110" t="s">
         <v>32</v>
       </c>
-      <c r="G36" s="142"/>
-      <c r="H36" s="142"/>
-      <c r="I36" s="142"/>
-      <c r="J36" s="142"/>
-      <c r="K36" s="142"/>
-      <c r="L36" s="142"/>
-      <c r="M36" s="142"/>
-      <c r="N36" s="142"/>
-      <c r="O36" s="142"/>
-      <c r="P36" s="142"/>
-      <c r="Q36" s="142"/>
+      <c r="G36" s="111"/>
+      <c r="H36" s="111"/>
+      <c r="I36" s="111"/>
+      <c r="J36" s="111"/>
+      <c r="K36" s="111"/>
+      <c r="L36" s="111"/>
+      <c r="M36" s="111"/>
+      <c r="N36" s="111"/>
+      <c r="O36" s="111"/>
+      <c r="P36" s="111"/>
+      <c r="Q36" s="111"/>
       <c r="R36" s="40"/>
       <c r="S36" s="27"/>
       <c r="T36" s="27"/>
@@ -5024,24 +5020,24 @@
     </row>
     <row r="37" spans="1:37" ht="11.25" customHeight="1">
       <c r="A37" s="83"/>
-      <c r="B37" s="143" t="s">
+      <c r="B37" s="112" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="144"/>
-      <c r="D37" s="144"/>
-      <c r="E37" s="145"/>
-      <c r="F37" s="141"/>
-      <c r="G37" s="142"/>
-      <c r="H37" s="142"/>
-      <c r="I37" s="142"/>
-      <c r="J37" s="142"/>
-      <c r="K37" s="142"/>
-      <c r="L37" s="142"/>
-      <c r="M37" s="142"/>
-      <c r="N37" s="142"/>
-      <c r="O37" s="142"/>
-      <c r="P37" s="142"/>
-      <c r="Q37" s="142"/>
+      <c r="C37" s="113"/>
+      <c r="D37" s="113"/>
+      <c r="E37" s="114"/>
+      <c r="F37" s="110"/>
+      <c r="G37" s="111"/>
+      <c r="H37" s="111"/>
+      <c r="I37" s="111"/>
+      <c r="J37" s="111"/>
+      <c r="K37" s="111"/>
+      <c r="L37" s="111"/>
+      <c r="M37" s="111"/>
+      <c r="N37" s="111"/>
+      <c r="O37" s="111"/>
+      <c r="P37" s="111"/>
+      <c r="Q37" s="111"/>
       <c r="R37" s="40"/>
       <c r="S37" s="27"/>
       <c r="T37" s="27"/>
@@ -5069,18 +5065,18 @@
       <c r="C38" s="27"/>
       <c r="D38" s="27"/>
       <c r="E38" s="59"/>
-      <c r="F38" s="141"/>
-      <c r="G38" s="142"/>
-      <c r="H38" s="142"/>
-      <c r="I38" s="142"/>
-      <c r="J38" s="142"/>
-      <c r="K38" s="142"/>
-      <c r="L38" s="142"/>
-      <c r="M38" s="142"/>
-      <c r="N38" s="142"/>
-      <c r="O38" s="142"/>
-      <c r="P38" s="142"/>
-      <c r="Q38" s="142"/>
+      <c r="F38" s="110"/>
+      <c r="G38" s="111"/>
+      <c r="H38" s="111"/>
+      <c r="I38" s="111"/>
+      <c r="J38" s="111"/>
+      <c r="K38" s="111"/>
+      <c r="L38" s="111"/>
+      <c r="M38" s="111"/>
+      <c r="N38" s="111"/>
+      <c r="O38" s="111"/>
+      <c r="P38" s="111"/>
+      <c r="Q38" s="111"/>
       <c r="R38" s="40"/>
       <c r="S38" s="27"/>
       <c r="T38" s="27"/>
@@ -5302,7 +5298,23 @@
       <c r="AK43" s="85"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
+  <mergeCells count="25">
+    <mergeCell ref="F25:J26"/>
+    <mergeCell ref="AI1:AK1"/>
+    <mergeCell ref="T11:U12"/>
+    <mergeCell ref="V11:Z12"/>
+    <mergeCell ref="AA11:AE12"/>
+    <mergeCell ref="AF11:AJ12"/>
+    <mergeCell ref="AF2:AH2"/>
+    <mergeCell ref="AI2:AK2"/>
+    <mergeCell ref="L24:P24"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="T16:AJ16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="T17:T19"/>
+    <mergeCell ref="B6:AK8"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="Y19:AI19"/>
     <mergeCell ref="F36:Q38"/>
     <mergeCell ref="B37:E37"/>
     <mergeCell ref="F27:Q29"/>
@@ -5312,26 +5324,6 @@
     <mergeCell ref="B34:E34"/>
     <mergeCell ref="Q34:Q35"/>
     <mergeCell ref="B31:E31"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="T16:AJ16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="T17:T19"/>
-    <mergeCell ref="B6:AK8"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="F15:S15"/>
-    <mergeCell ref="T15:AJ15"/>
-    <mergeCell ref="F14:S14"/>
-    <mergeCell ref="T14:AJ14"/>
-    <mergeCell ref="Y19:AI19"/>
-    <mergeCell ref="F25:J26"/>
-    <mergeCell ref="AI1:AK1"/>
-    <mergeCell ref="T11:U12"/>
-    <mergeCell ref="V11:Z12"/>
-    <mergeCell ref="AA11:AE12"/>
-    <mergeCell ref="AF11:AJ12"/>
-    <mergeCell ref="AF2:AH2"/>
-    <mergeCell ref="AI2:AK2"/>
-    <mergeCell ref="L24:P24"/>
   </mergeCells>
   <phoneticPr fontId="16"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
hoant2 : code comit
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/ローマ字氏名届_帳票テンプレート.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/ローマ字氏名届_帳票テンプレート.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49698D44-88B6-4B51-B8F5-45B438D66464}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B8C14C2-4B05-4940-84FB-D4581094C4AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1534,6 +1534,81 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="center" indent="1"/>
     </xf>
@@ -1544,81 +1619,6 @@
       <alignment horizontal="distributed" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3486,7 +3486,7 @@
   <dimension ref="A1:AL43"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="U45" sqref="U45"/>
+      <selection activeCell="V36" sqref="V36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.140625" defaultRowHeight="15"/>
@@ -3529,11 +3529,11 @@
       <c r="AC1" s="27"/>
       <c r="AD1" s="27"/>
       <c r="AE1" s="27"/>
-      <c r="AI1" s="129">
+      <c r="AI1" s="116">
         <v>72073</v>
       </c>
-      <c r="AJ1" s="129"/>
-      <c r="AK1" s="129"/>
+      <c r="AJ1" s="116"/>
+      <c r="AK1" s="116"/>
       <c r="AL1" s="27"/>
     </row>
     <row r="2" spans="1:38" ht="26.25" customHeight="1">
@@ -3568,16 +3568,16 @@
       <c r="AC2" s="27"/>
       <c r="AD2" s="27"/>
       <c r="AE2" s="27"/>
-      <c r="AF2" s="140" t="s">
+      <c r="AF2" s="128" t="s">
         <v>23</v>
       </c>
-      <c r="AG2" s="141"/>
-      <c r="AH2" s="142"/>
-      <c r="AI2" s="143" t="s">
+      <c r="AG2" s="129"/>
+      <c r="AH2" s="130"/>
+      <c r="AI2" s="131" t="s">
         <v>24</v>
       </c>
-      <c r="AJ2" s="141"/>
-      <c r="AK2" s="142"/>
+      <c r="AJ2" s="129"/>
+      <c r="AK2" s="130"/>
       <c r="AL2" s="27"/>
     </row>
     <row r="3" spans="1:38" ht="26.25" customHeight="1">
@@ -3701,122 +3701,122 @@
     </row>
     <row r="6" spans="1:38" ht="13.5" customHeight="1">
       <c r="A6" s="82"/>
-      <c r="B6" s="124" t="s">
+      <c r="B6" s="137" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="124"/>
-      <c r="D6" s="124"/>
-      <c r="E6" s="124"/>
-      <c r="F6" s="124"/>
-      <c r="G6" s="124"/>
-      <c r="H6" s="124"/>
-      <c r="I6" s="124"/>
-      <c r="J6" s="124"/>
-      <c r="K6" s="124"/>
-      <c r="L6" s="124"/>
-      <c r="M6" s="124"/>
-      <c r="N6" s="124"/>
-      <c r="O6" s="124"/>
-      <c r="P6" s="124"/>
-      <c r="Q6" s="124"/>
-      <c r="R6" s="124"/>
-      <c r="S6" s="124"/>
-      <c r="T6" s="124"/>
-      <c r="U6" s="124"/>
-      <c r="V6" s="124"/>
-      <c r="W6" s="124"/>
-      <c r="X6" s="124"/>
-      <c r="Y6" s="124"/>
-      <c r="Z6" s="124"/>
-      <c r="AA6" s="124"/>
-      <c r="AB6" s="124"/>
-      <c r="AC6" s="124"/>
-      <c r="AD6" s="124"/>
-      <c r="AE6" s="124"/>
-      <c r="AF6" s="124"/>
-      <c r="AG6" s="124"/>
-      <c r="AH6" s="124"/>
-      <c r="AI6" s="124"/>
-      <c r="AJ6" s="124"/>
-      <c r="AK6" s="125"/>
+      <c r="C6" s="137"/>
+      <c r="D6" s="137"/>
+      <c r="E6" s="137"/>
+      <c r="F6" s="137"/>
+      <c r="G6" s="137"/>
+      <c r="H6" s="137"/>
+      <c r="I6" s="137"/>
+      <c r="J6" s="137"/>
+      <c r="K6" s="137"/>
+      <c r="L6" s="137"/>
+      <c r="M6" s="137"/>
+      <c r="N6" s="137"/>
+      <c r="O6" s="137"/>
+      <c r="P6" s="137"/>
+      <c r="Q6" s="137"/>
+      <c r="R6" s="137"/>
+      <c r="S6" s="137"/>
+      <c r="T6" s="137"/>
+      <c r="U6" s="137"/>
+      <c r="V6" s="137"/>
+      <c r="W6" s="137"/>
+      <c r="X6" s="137"/>
+      <c r="Y6" s="137"/>
+      <c r="Z6" s="137"/>
+      <c r="AA6" s="137"/>
+      <c r="AB6" s="137"/>
+      <c r="AC6" s="137"/>
+      <c r="AD6" s="137"/>
+      <c r="AE6" s="137"/>
+      <c r="AF6" s="137"/>
+      <c r="AG6" s="137"/>
+      <c r="AH6" s="137"/>
+      <c r="AI6" s="137"/>
+      <c r="AJ6" s="137"/>
+      <c r="AK6" s="138"/>
     </row>
     <row r="7" spans="1:38" ht="13.5" customHeight="1">
       <c r="A7" s="83"/>
-      <c r="B7" s="126"/>
-      <c r="C7" s="126"/>
-      <c r="D7" s="126"/>
-      <c r="E7" s="126"/>
-      <c r="F7" s="126"/>
-      <c r="G7" s="126"/>
-      <c r="H7" s="126"/>
-      <c r="I7" s="126"/>
-      <c r="J7" s="126"/>
-      <c r="K7" s="126"/>
-      <c r="L7" s="126"/>
-      <c r="M7" s="126"/>
-      <c r="N7" s="126"/>
-      <c r="O7" s="126"/>
-      <c r="P7" s="126"/>
-      <c r="Q7" s="126"/>
-      <c r="R7" s="126"/>
-      <c r="S7" s="126"/>
-      <c r="T7" s="126"/>
-      <c r="U7" s="126"/>
-      <c r="V7" s="126"/>
-      <c r="W7" s="126"/>
-      <c r="X7" s="126"/>
-      <c r="Y7" s="126"/>
-      <c r="Z7" s="126"/>
-      <c r="AA7" s="126"/>
-      <c r="AB7" s="126"/>
-      <c r="AC7" s="126"/>
-      <c r="AD7" s="126"/>
-      <c r="AE7" s="126"/>
-      <c r="AF7" s="126"/>
-      <c r="AG7" s="126"/>
-      <c r="AH7" s="126"/>
-      <c r="AI7" s="126"/>
-      <c r="AJ7" s="126"/>
-      <c r="AK7" s="127"/>
+      <c r="B7" s="139"/>
+      <c r="C7" s="139"/>
+      <c r="D7" s="139"/>
+      <c r="E7" s="139"/>
+      <c r="F7" s="139"/>
+      <c r="G7" s="139"/>
+      <c r="H7" s="139"/>
+      <c r="I7" s="139"/>
+      <c r="J7" s="139"/>
+      <c r="K7" s="139"/>
+      <c r="L7" s="139"/>
+      <c r="M7" s="139"/>
+      <c r="N7" s="139"/>
+      <c r="O7" s="139"/>
+      <c r="P7" s="139"/>
+      <c r="Q7" s="139"/>
+      <c r="R7" s="139"/>
+      <c r="S7" s="139"/>
+      <c r="T7" s="139"/>
+      <c r="U7" s="139"/>
+      <c r="V7" s="139"/>
+      <c r="W7" s="139"/>
+      <c r="X7" s="139"/>
+      <c r="Y7" s="139"/>
+      <c r="Z7" s="139"/>
+      <c r="AA7" s="139"/>
+      <c r="AB7" s="139"/>
+      <c r="AC7" s="139"/>
+      <c r="AD7" s="139"/>
+      <c r="AE7" s="139"/>
+      <c r="AF7" s="139"/>
+      <c r="AG7" s="139"/>
+      <c r="AH7" s="139"/>
+      <c r="AI7" s="139"/>
+      <c r="AJ7" s="139"/>
+      <c r="AK7" s="140"/>
     </row>
     <row r="8" spans="1:38" ht="13.5" customHeight="1">
       <c r="A8" s="83"/>
-      <c r="B8" s="126"/>
-      <c r="C8" s="126"/>
-      <c r="D8" s="126"/>
-      <c r="E8" s="126"/>
-      <c r="F8" s="126"/>
-      <c r="G8" s="126"/>
-      <c r="H8" s="126"/>
-      <c r="I8" s="126"/>
-      <c r="J8" s="126"/>
-      <c r="K8" s="126"/>
-      <c r="L8" s="126"/>
-      <c r="M8" s="126"/>
-      <c r="N8" s="126"/>
-      <c r="O8" s="126"/>
-      <c r="P8" s="126"/>
-      <c r="Q8" s="126"/>
-      <c r="R8" s="126"/>
-      <c r="S8" s="126"/>
-      <c r="T8" s="126"/>
-      <c r="U8" s="126"/>
-      <c r="V8" s="126"/>
-      <c r="W8" s="126"/>
-      <c r="X8" s="126"/>
-      <c r="Y8" s="126"/>
-      <c r="Z8" s="126"/>
-      <c r="AA8" s="126"/>
-      <c r="AB8" s="126"/>
-      <c r="AC8" s="126"/>
-      <c r="AD8" s="126"/>
-      <c r="AE8" s="126"/>
-      <c r="AF8" s="126"/>
-      <c r="AG8" s="126"/>
-      <c r="AH8" s="126"/>
-      <c r="AI8" s="126"/>
-      <c r="AJ8" s="126"/>
-      <c r="AK8" s="127"/>
+      <c r="B8" s="139"/>
+      <c r="C8" s="139"/>
+      <c r="D8" s="139"/>
+      <c r="E8" s="139"/>
+      <c r="F8" s="139"/>
+      <c r="G8" s="139"/>
+      <c r="H8" s="139"/>
+      <c r="I8" s="139"/>
+      <c r="J8" s="139"/>
+      <c r="K8" s="139"/>
+      <c r="L8" s="139"/>
+      <c r="M8" s="139"/>
+      <c r="N8" s="139"/>
+      <c r="O8" s="139"/>
+      <c r="P8" s="139"/>
+      <c r="Q8" s="139"/>
+      <c r="R8" s="139"/>
+      <c r="S8" s="139"/>
+      <c r="T8" s="139"/>
+      <c r="U8" s="139"/>
+      <c r="V8" s="139"/>
+      <c r="W8" s="139"/>
+      <c r="X8" s="139"/>
+      <c r="Y8" s="139"/>
+      <c r="Z8" s="139"/>
+      <c r="AA8" s="139"/>
+      <c r="AB8" s="139"/>
+      <c r="AC8" s="139"/>
+      <c r="AD8" s="139"/>
+      <c r="AE8" s="139"/>
+      <c r="AF8" s="139"/>
+      <c r="AG8" s="139"/>
+      <c r="AH8" s="139"/>
+      <c r="AI8" s="139"/>
+      <c r="AJ8" s="139"/>
+      <c r="AK8" s="140"/>
     </row>
     <row r="9" spans="1:38" ht="18.75" customHeight="1">
       <c r="A9" s="83"/>
@@ -3932,27 +3932,27 @@
       <c r="S11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="T11" s="130" t="s">
+      <c r="T11" s="117" t="s">
         <v>27</v>
       </c>
-      <c r="U11" s="131"/>
-      <c r="V11" s="130" t="s">
+      <c r="U11" s="118"/>
+      <c r="V11" s="117" t="s">
         <v>18</v>
       </c>
-      <c r="W11" s="134"/>
-      <c r="X11" s="134"/>
-      <c r="Y11" s="134"/>
-      <c r="Z11" s="131"/>
-      <c r="AA11" s="135"/>
-      <c r="AB11" s="136"/>
-      <c r="AC11" s="136"/>
-      <c r="AD11" s="136"/>
-      <c r="AE11" s="136"/>
-      <c r="AF11" s="139"/>
-      <c r="AG11" s="136"/>
-      <c r="AH11" s="136"/>
-      <c r="AI11" s="136"/>
-      <c r="AJ11" s="136"/>
+      <c r="W11" s="121"/>
+      <c r="X11" s="121"/>
+      <c r="Y11" s="121"/>
+      <c r="Z11" s="118"/>
+      <c r="AA11" s="123"/>
+      <c r="AB11" s="124"/>
+      <c r="AC11" s="124"/>
+      <c r="AD11" s="124"/>
+      <c r="AE11" s="124"/>
+      <c r="AF11" s="127"/>
+      <c r="AG11" s="124"/>
+      <c r="AH11" s="124"/>
+      <c r="AI11" s="124"/>
+      <c r="AJ11" s="124"/>
       <c r="AK11" s="84"/>
     </row>
     <row r="12" spans="1:38" ht="40.5" customHeight="1" thickBot="1">
@@ -3975,23 +3975,23 @@
       <c r="Q12" s="57"/>
       <c r="R12" s="58"/>
       <c r="S12" s="50"/>
-      <c r="T12" s="132"/>
-      <c r="U12" s="133"/>
-      <c r="V12" s="132"/>
-      <c r="W12" s="128"/>
-      <c r="X12" s="128"/>
-      <c r="Y12" s="128"/>
-      <c r="Z12" s="133"/>
-      <c r="AA12" s="137"/>
-      <c r="AB12" s="138"/>
-      <c r="AC12" s="138"/>
-      <c r="AD12" s="138"/>
-      <c r="AE12" s="138"/>
-      <c r="AF12" s="138"/>
-      <c r="AG12" s="138"/>
-      <c r="AH12" s="138"/>
-      <c r="AI12" s="138"/>
-      <c r="AJ12" s="138"/>
+      <c r="T12" s="119"/>
+      <c r="U12" s="120"/>
+      <c r="V12" s="119"/>
+      <c r="W12" s="122"/>
+      <c r="X12" s="122"/>
+      <c r="Y12" s="122"/>
+      <c r="Z12" s="120"/>
+      <c r="AA12" s="125"/>
+      <c r="AB12" s="126"/>
+      <c r="AC12" s="126"/>
+      <c r="AD12" s="126"/>
+      <c r="AE12" s="126"/>
+      <c r="AF12" s="126"/>
+      <c r="AG12" s="126"/>
+      <c r="AH12" s="126"/>
+      <c r="AI12" s="126"/>
+      <c r="AJ12" s="126"/>
       <c r="AK12" s="84"/>
     </row>
     <row r="13" spans="1:38" ht="23.25" customHeight="1" thickBot="1">
@@ -4037,7 +4037,7 @@
     </row>
     <row r="14" spans="1:38" ht="25.5" customHeight="1">
       <c r="A14" s="83"/>
-      <c r="B14" s="120" t="s">
+      <c r="B14" s="133" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -4080,7 +4080,7 @@
     </row>
     <row r="15" spans="1:38" ht="60.75" customHeight="1" thickBot="1">
       <c r="A15" s="83"/>
-      <c r="B15" s="121"/>
+      <c r="B15" s="134"/>
       <c r="C15" s="6" t="s">
         <v>30</v>
       </c>
@@ -4141,30 +4141,30 @@
       <c r="Q16" s="64"/>
       <c r="R16" s="64"/>
       <c r="S16" s="64"/>
-      <c r="T16" s="122" t="s">
+      <c r="T16" s="135" t="s">
         <v>29</v>
       </c>
-      <c r="U16" s="122"/>
-      <c r="V16" s="122"/>
-      <c r="W16" s="122"/>
-      <c r="X16" s="122"/>
-      <c r="Y16" s="122"/>
-      <c r="Z16" s="122"/>
-      <c r="AA16" s="122"/>
-      <c r="AB16" s="122"/>
-      <c r="AC16" s="122"/>
-      <c r="AD16" s="122"/>
-      <c r="AE16" s="122"/>
-      <c r="AF16" s="122"/>
-      <c r="AG16" s="122"/>
-      <c r="AH16" s="122"/>
-      <c r="AI16" s="122"/>
-      <c r="AJ16" s="122"/>
+      <c r="U16" s="135"/>
+      <c r="V16" s="135"/>
+      <c r="W16" s="135"/>
+      <c r="X16" s="135"/>
+      <c r="Y16" s="135"/>
+      <c r="Z16" s="135"/>
+      <c r="AA16" s="135"/>
+      <c r="AB16" s="135"/>
+      <c r="AC16" s="135"/>
+      <c r="AD16" s="135"/>
+      <c r="AE16" s="135"/>
+      <c r="AF16" s="135"/>
+      <c r="AG16" s="135"/>
+      <c r="AH16" s="135"/>
+      <c r="AI16" s="135"/>
+      <c r="AJ16" s="135"/>
       <c r="AK16" s="84"/>
     </row>
     <row r="17" spans="1:37" ht="25.5" customHeight="1">
       <c r="A17" s="83"/>
-      <c r="B17" s="120" t="s">
+      <c r="B17" s="133" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -4186,7 +4186,7 @@
       <c r="Q17" s="101"/>
       <c r="R17" s="104"/>
       <c r="S17" s="27"/>
-      <c r="T17" s="120" t="s">
+      <c r="T17" s="133" t="s">
         <v>19</v>
       </c>
       <c r="U17" s="65"/>
@@ -4209,7 +4209,7 @@
     </row>
     <row r="18" spans="1:37" ht="37.5" customHeight="1" thickBot="1">
       <c r="A18" s="83"/>
-      <c r="B18" s="121"/>
+      <c r="B18" s="134"/>
       <c r="C18" s="6" t="s">
         <v>4</v>
       </c>
@@ -4231,7 +4231,7 @@
       <c r="Q18" s="100"/>
       <c r="R18" s="106"/>
       <c r="S18" s="27"/>
-      <c r="T18" s="123"/>
+      <c r="T18" s="136"/>
       <c r="U18" s="70"/>
       <c r="V18" s="27"/>
       <c r="W18" s="71"/>
@@ -4252,7 +4252,7 @@
     </row>
     <row r="19" spans="1:37" ht="25.5" customHeight="1" thickBot="1">
       <c r="A19" s="83"/>
-      <c r="B19" s="120" t="s">
+      <c r="B19" s="133" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="5" t="s">
@@ -4274,28 +4274,28 @@
       <c r="Q19" s="101"/>
       <c r="R19" s="104"/>
       <c r="S19" s="27"/>
-      <c r="T19" s="121"/>
+      <c r="T19" s="134"/>
       <c r="U19" s="43"/>
       <c r="V19" s="25"/>
       <c r="W19" s="25"/>
       <c r="X19" s="25"/>
-      <c r="Y19" s="128"/>
-      <c r="Z19" s="128"/>
-      <c r="AA19" s="128"/>
-      <c r="AB19" s="128"/>
-      <c r="AC19" s="128"/>
-      <c r="AD19" s="128"/>
-      <c r="AE19" s="128"/>
-      <c r="AF19" s="128"/>
-      <c r="AG19" s="128"/>
-      <c r="AH19" s="128"/>
-      <c r="AI19" s="128"/>
+      <c r="Y19" s="122"/>
+      <c r="Z19" s="122"/>
+      <c r="AA19" s="122"/>
+      <c r="AB19" s="122"/>
+      <c r="AC19" s="122"/>
+      <c r="AD19" s="122"/>
+      <c r="AE19" s="122"/>
+      <c r="AF19" s="122"/>
+      <c r="AG19" s="122"/>
+      <c r="AH19" s="122"/>
+      <c r="AI19" s="122"/>
       <c r="AJ19" s="24"/>
       <c r="AK19" s="84"/>
     </row>
     <row r="20" spans="1:37" ht="37.5" customHeight="1" thickBot="1">
       <c r="A20" s="83"/>
-      <c r="B20" s="121"/>
+      <c r="B20" s="134"/>
       <c r="C20" s="6" t="s">
         <v>4</v>
       </c>
@@ -4465,13 +4465,13 @@
       <c r="I24" s="28"/>
       <c r="J24" s="28"/>
       <c r="K24" s="28"/>
-      <c r="L24" s="144" t="s">
+      <c r="L24" s="132" t="s">
         <v>25</v>
       </c>
-      <c r="M24" s="144"/>
-      <c r="N24" s="144"/>
-      <c r="O24" s="144"/>
-      <c r="P24" s="144"/>
+      <c r="M24" s="132"/>
+      <c r="N24" s="132"/>
+      <c r="O24" s="132"/>
+      <c r="P24" s="132"/>
       <c r="Q24" s="29" t="s">
         <v>31</v>
       </c>
@@ -4617,12 +4617,12 @@
     </row>
     <row r="28" spans="1:37" ht="11.25" customHeight="1">
       <c r="A28" s="83"/>
-      <c r="B28" s="116" t="s">
+      <c r="B28" s="141" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="117"/>
-      <c r="D28" s="117"/>
-      <c r="E28" s="118"/>
+      <c r="C28" s="142"/>
+      <c r="D28" s="142"/>
+      <c r="E28" s="143"/>
       <c r="F28" s="115"/>
       <c r="G28" s="115"/>
       <c r="H28" s="115"/>
@@ -4736,12 +4736,12 @@
     </row>
     <row r="31" spans="1:37" ht="11.25" customHeight="1">
       <c r="A31" s="83"/>
-      <c r="B31" s="116" t="s">
+      <c r="B31" s="141" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="117"/>
-      <c r="D31" s="117"/>
-      <c r="E31" s="117"/>
+      <c r="C31" s="142"/>
+      <c r="D31" s="142"/>
+      <c r="E31" s="142"/>
       <c r="F31" s="115"/>
       <c r="G31" s="115"/>
       <c r="H31" s="115"/>
@@ -4855,12 +4855,12 @@
     </row>
     <row r="34" spans="1:37" ht="11.25" customHeight="1">
       <c r="A34" s="83"/>
-      <c r="B34" s="116" t="s">
+      <c r="B34" s="141" t="s">
         <v>11</v>
       </c>
-      <c r="C34" s="117"/>
-      <c r="D34" s="117"/>
-      <c r="E34" s="117"/>
+      <c r="C34" s="142"/>
+      <c r="D34" s="142"/>
+      <c r="E34" s="142"/>
       <c r="F34" s="115"/>
       <c r="G34" s="115"/>
       <c r="H34" s="115"/>
@@ -4872,7 +4872,7 @@
       <c r="N34" s="115"/>
       <c r="O34" s="115"/>
       <c r="P34" s="115"/>
-      <c r="Q34" s="119" t="s">
+      <c r="Q34" s="144" t="s">
         <v>6</v>
       </c>
       <c r="R34" s="40"/>
@@ -4913,7 +4913,7 @@
       <c r="N35" s="115"/>
       <c r="O35" s="115"/>
       <c r="P35" s="115"/>
-      <c r="Q35" s="119"/>
+      <c r="Q35" s="144"/>
       <c r="R35" s="40"/>
       <c r="S35" s="27"/>
       <c r="T35" s="27"/>
@@ -4978,12 +4978,12 @@
     </row>
     <row r="37" spans="1:37" ht="11.25" customHeight="1">
       <c r="A37" s="83"/>
-      <c r="B37" s="116" t="s">
+      <c r="B37" s="141" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="117"/>
-      <c r="D37" s="117"/>
-      <c r="E37" s="118"/>
+      <c r="C37" s="142"/>
+      <c r="D37" s="142"/>
+      <c r="E37" s="143"/>
       <c r="F37" s="115"/>
       <c r="G37" s="115"/>
       <c r="H37" s="115"/>
@@ -5257,6 +5257,22 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="F36:Q38"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="F27:Q29"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="F30:Q32"/>
+    <mergeCell ref="F33:P35"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="Q34:Q35"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="T16:AJ16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="T17:T19"/>
+    <mergeCell ref="B6:AK8"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="Y19:AI19"/>
     <mergeCell ref="F25:J26"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="T11:U12"/>
@@ -5266,22 +5282,6 @@
     <mergeCell ref="AF2:AH2"/>
     <mergeCell ref="AI2:AK2"/>
     <mergeCell ref="L24:P24"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="T16:AJ16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="T17:T19"/>
-    <mergeCell ref="B6:AK8"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="Y19:AI19"/>
-    <mergeCell ref="F36:Q38"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="F27:Q29"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="F30:Q32"/>
-    <mergeCell ref="F33:P35"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="Q34:Q35"/>
-    <mergeCell ref="B31:E31"/>
   </mergeCells>
   <phoneticPr fontId="15"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
hoant2 : commit code A, B 003
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/ローマ字氏名届_帳票テンプレート.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/ローマ字氏名届_帳票テンプレート.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B8C14C2-4B05-4940-84FB-D4581094C4AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA290CD-D86D-46B9-9F94-76A5E2BF06BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="A3_6">'2号'!$F$36:$Q$38</definedName>
     <definedName name="A3_7">'2号'!$L$24:$P$24</definedName>
     <definedName name="A4_5">'2号'!$Y$19:$AI$19</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'2号'!$A$1:$AK$43</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'2号'!$A$1:$AK$48</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -1189,7 +1189,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1516,24 +1516,48 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1552,9 +1576,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1585,40 +1606,16 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3485,8 +3482,8 @@
   </sheetPr>
   <dimension ref="A1:AL43"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="V36" sqref="V36"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="55" workbookViewId="0">
+      <selection activeCell="W45" sqref="W45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.140625" defaultRowHeight="15"/>
@@ -3529,11 +3526,11 @@
       <c r="AC1" s="27"/>
       <c r="AD1" s="27"/>
       <c r="AE1" s="27"/>
-      <c r="AI1" s="116">
+      <c r="AI1" s="124">
         <v>72073</v>
       </c>
-      <c r="AJ1" s="116"/>
-      <c r="AK1" s="116"/>
+      <c r="AJ1" s="124"/>
+      <c r="AK1" s="124"/>
       <c r="AL1" s="27"/>
     </row>
     <row r="2" spans="1:38" ht="26.25" customHeight="1">
@@ -3568,16 +3565,16 @@
       <c r="AC2" s="27"/>
       <c r="AD2" s="27"/>
       <c r="AE2" s="27"/>
-      <c r="AF2" s="128" t="s">
+      <c r="AF2" s="135" t="s">
         <v>23</v>
       </c>
-      <c r="AG2" s="129"/>
-      <c r="AH2" s="130"/>
-      <c r="AI2" s="131" t="s">
+      <c r="AG2" s="136"/>
+      <c r="AH2" s="137"/>
+      <c r="AI2" s="138" t="s">
         <v>24</v>
       </c>
-      <c r="AJ2" s="129"/>
-      <c r="AK2" s="130"/>
+      <c r="AJ2" s="136"/>
+      <c r="AK2" s="137"/>
       <c r="AL2" s="27"/>
     </row>
     <row r="3" spans="1:38" ht="26.25" customHeight="1">
@@ -3701,122 +3698,122 @@
     </row>
     <row r="6" spans="1:38" ht="13.5" customHeight="1">
       <c r="A6" s="82"/>
-      <c r="B6" s="137" t="s">
+      <c r="B6" s="119" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="137"/>
-      <c r="D6" s="137"/>
-      <c r="E6" s="137"/>
-      <c r="F6" s="137"/>
-      <c r="G6" s="137"/>
-      <c r="H6" s="137"/>
-      <c r="I6" s="137"/>
-      <c r="J6" s="137"/>
-      <c r="K6" s="137"/>
-      <c r="L6" s="137"/>
-      <c r="M6" s="137"/>
-      <c r="N6" s="137"/>
-      <c r="O6" s="137"/>
-      <c r="P6" s="137"/>
-      <c r="Q6" s="137"/>
-      <c r="R6" s="137"/>
-      <c r="S6" s="137"/>
-      <c r="T6" s="137"/>
-      <c r="U6" s="137"/>
-      <c r="V6" s="137"/>
-      <c r="W6" s="137"/>
-      <c r="X6" s="137"/>
-      <c r="Y6" s="137"/>
-      <c r="Z6" s="137"/>
-      <c r="AA6" s="137"/>
-      <c r="AB6" s="137"/>
-      <c r="AC6" s="137"/>
-      <c r="AD6" s="137"/>
-      <c r="AE6" s="137"/>
-      <c r="AF6" s="137"/>
-      <c r="AG6" s="137"/>
-      <c r="AH6" s="137"/>
-      <c r="AI6" s="137"/>
-      <c r="AJ6" s="137"/>
-      <c r="AK6" s="138"/>
+      <c r="C6" s="119"/>
+      <c r="D6" s="119"/>
+      <c r="E6" s="119"/>
+      <c r="F6" s="119"/>
+      <c r="G6" s="119"/>
+      <c r="H6" s="119"/>
+      <c r="I6" s="119"/>
+      <c r="J6" s="119"/>
+      <c r="K6" s="119"/>
+      <c r="L6" s="119"/>
+      <c r="M6" s="119"/>
+      <c r="N6" s="119"/>
+      <c r="O6" s="119"/>
+      <c r="P6" s="119"/>
+      <c r="Q6" s="119"/>
+      <c r="R6" s="119"/>
+      <c r="S6" s="119"/>
+      <c r="T6" s="119"/>
+      <c r="U6" s="119"/>
+      <c r="V6" s="119"/>
+      <c r="W6" s="119"/>
+      <c r="X6" s="119"/>
+      <c r="Y6" s="119"/>
+      <c r="Z6" s="119"/>
+      <c r="AA6" s="119"/>
+      <c r="AB6" s="119"/>
+      <c r="AC6" s="119"/>
+      <c r="AD6" s="119"/>
+      <c r="AE6" s="119"/>
+      <c r="AF6" s="119"/>
+      <c r="AG6" s="119"/>
+      <c r="AH6" s="119"/>
+      <c r="AI6" s="119"/>
+      <c r="AJ6" s="119"/>
+      <c r="AK6" s="120"/>
     </row>
     <row r="7" spans="1:38" ht="13.5" customHeight="1">
       <c r="A7" s="83"/>
-      <c r="B7" s="139"/>
-      <c r="C7" s="139"/>
-      <c r="D7" s="139"/>
-      <c r="E7" s="139"/>
-      <c r="F7" s="139"/>
-      <c r="G7" s="139"/>
-      <c r="H7" s="139"/>
-      <c r="I7" s="139"/>
-      <c r="J7" s="139"/>
-      <c r="K7" s="139"/>
-      <c r="L7" s="139"/>
-      <c r="M7" s="139"/>
-      <c r="N7" s="139"/>
-      <c r="O7" s="139"/>
-      <c r="P7" s="139"/>
-      <c r="Q7" s="139"/>
-      <c r="R7" s="139"/>
-      <c r="S7" s="139"/>
-      <c r="T7" s="139"/>
-      <c r="U7" s="139"/>
-      <c r="V7" s="139"/>
-      <c r="W7" s="139"/>
-      <c r="X7" s="139"/>
-      <c r="Y7" s="139"/>
-      <c r="Z7" s="139"/>
-      <c r="AA7" s="139"/>
-      <c r="AB7" s="139"/>
-      <c r="AC7" s="139"/>
-      <c r="AD7" s="139"/>
-      <c r="AE7" s="139"/>
-      <c r="AF7" s="139"/>
-      <c r="AG7" s="139"/>
-      <c r="AH7" s="139"/>
-      <c r="AI7" s="139"/>
-      <c r="AJ7" s="139"/>
-      <c r="AK7" s="140"/>
+      <c r="B7" s="121"/>
+      <c r="C7" s="121"/>
+      <c r="D7" s="121"/>
+      <c r="E7" s="121"/>
+      <c r="F7" s="121"/>
+      <c r="G7" s="121"/>
+      <c r="H7" s="121"/>
+      <c r="I7" s="121"/>
+      <c r="J7" s="121"/>
+      <c r="K7" s="121"/>
+      <c r="L7" s="121"/>
+      <c r="M7" s="121"/>
+      <c r="N7" s="121"/>
+      <c r="O7" s="121"/>
+      <c r="P7" s="121"/>
+      <c r="Q7" s="121"/>
+      <c r="R7" s="121"/>
+      <c r="S7" s="121"/>
+      <c r="T7" s="121"/>
+      <c r="U7" s="121"/>
+      <c r="V7" s="121"/>
+      <c r="W7" s="121"/>
+      <c r="X7" s="121"/>
+      <c r="Y7" s="121"/>
+      <c r="Z7" s="121"/>
+      <c r="AA7" s="121"/>
+      <c r="AB7" s="121"/>
+      <c r="AC7" s="121"/>
+      <c r="AD7" s="121"/>
+      <c r="AE7" s="121"/>
+      <c r="AF7" s="121"/>
+      <c r="AG7" s="121"/>
+      <c r="AH7" s="121"/>
+      <c r="AI7" s="121"/>
+      <c r="AJ7" s="121"/>
+      <c r="AK7" s="122"/>
     </row>
     <row r="8" spans="1:38" ht="13.5" customHeight="1">
       <c r="A8" s="83"/>
-      <c r="B8" s="139"/>
-      <c r="C8" s="139"/>
-      <c r="D8" s="139"/>
-      <c r="E8" s="139"/>
-      <c r="F8" s="139"/>
-      <c r="G8" s="139"/>
-      <c r="H8" s="139"/>
-      <c r="I8" s="139"/>
-      <c r="J8" s="139"/>
-      <c r="K8" s="139"/>
-      <c r="L8" s="139"/>
-      <c r="M8" s="139"/>
-      <c r="N8" s="139"/>
-      <c r="O8" s="139"/>
-      <c r="P8" s="139"/>
-      <c r="Q8" s="139"/>
-      <c r="R8" s="139"/>
-      <c r="S8" s="139"/>
-      <c r="T8" s="139"/>
-      <c r="U8" s="139"/>
-      <c r="V8" s="139"/>
-      <c r="W8" s="139"/>
-      <c r="X8" s="139"/>
-      <c r="Y8" s="139"/>
-      <c r="Z8" s="139"/>
-      <c r="AA8" s="139"/>
-      <c r="AB8" s="139"/>
-      <c r="AC8" s="139"/>
-      <c r="AD8" s="139"/>
-      <c r="AE8" s="139"/>
-      <c r="AF8" s="139"/>
-      <c r="AG8" s="139"/>
-      <c r="AH8" s="139"/>
-      <c r="AI8" s="139"/>
-      <c r="AJ8" s="139"/>
-      <c r="AK8" s="140"/>
+      <c r="B8" s="121"/>
+      <c r="C8" s="121"/>
+      <c r="D8" s="121"/>
+      <c r="E8" s="121"/>
+      <c r="F8" s="121"/>
+      <c r="G8" s="121"/>
+      <c r="H8" s="121"/>
+      <c r="I8" s="121"/>
+      <c r="J8" s="121"/>
+      <c r="K8" s="121"/>
+      <c r="L8" s="121"/>
+      <c r="M8" s="121"/>
+      <c r="N8" s="121"/>
+      <c r="O8" s="121"/>
+      <c r="P8" s="121"/>
+      <c r="Q8" s="121"/>
+      <c r="R8" s="121"/>
+      <c r="S8" s="121"/>
+      <c r="T8" s="121"/>
+      <c r="U8" s="121"/>
+      <c r="V8" s="121"/>
+      <c r="W8" s="121"/>
+      <c r="X8" s="121"/>
+      <c r="Y8" s="121"/>
+      <c r="Z8" s="121"/>
+      <c r="AA8" s="121"/>
+      <c r="AB8" s="121"/>
+      <c r="AC8" s="121"/>
+      <c r="AD8" s="121"/>
+      <c r="AE8" s="121"/>
+      <c r="AF8" s="121"/>
+      <c r="AG8" s="121"/>
+      <c r="AH8" s="121"/>
+      <c r="AI8" s="121"/>
+      <c r="AJ8" s="121"/>
+      <c r="AK8" s="122"/>
     </row>
     <row r="9" spans="1:38" ht="18.75" customHeight="1">
       <c r="A9" s="83"/>
@@ -3932,27 +3929,27 @@
       <c r="S11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="T11" s="117" t="s">
+      <c r="T11" s="125" t="s">
         <v>27</v>
       </c>
-      <c r="U11" s="118"/>
-      <c r="V11" s="117" t="s">
+      <c r="U11" s="126"/>
+      <c r="V11" s="125" t="s">
         <v>18</v>
       </c>
-      <c r="W11" s="121"/>
-      <c r="X11" s="121"/>
-      <c r="Y11" s="121"/>
-      <c r="Z11" s="118"/>
-      <c r="AA11" s="123"/>
-      <c r="AB11" s="124"/>
-      <c r="AC11" s="124"/>
-      <c r="AD11" s="124"/>
-      <c r="AE11" s="124"/>
-      <c r="AF11" s="127"/>
-      <c r="AG11" s="124"/>
-      <c r="AH11" s="124"/>
-      <c r="AI11" s="124"/>
-      <c r="AJ11" s="124"/>
+      <c r="W11" s="129"/>
+      <c r="X11" s="129"/>
+      <c r="Y11" s="129"/>
+      <c r="Z11" s="126"/>
+      <c r="AA11" s="130"/>
+      <c r="AB11" s="131"/>
+      <c r="AC11" s="131"/>
+      <c r="AD11" s="131"/>
+      <c r="AE11" s="131"/>
+      <c r="AF11" s="134"/>
+      <c r="AG11" s="131"/>
+      <c r="AH11" s="131"/>
+      <c r="AI11" s="131"/>
+      <c r="AJ11" s="131"/>
       <c r="AK11" s="84"/>
     </row>
     <row r="12" spans="1:38" ht="40.5" customHeight="1" thickBot="1">
@@ -3975,23 +3972,23 @@
       <c r="Q12" s="57"/>
       <c r="R12" s="58"/>
       <c r="S12" s="50"/>
-      <c r="T12" s="119"/>
-      <c r="U12" s="120"/>
-      <c r="V12" s="119"/>
-      <c r="W12" s="122"/>
-      <c r="X12" s="122"/>
-      <c r="Y12" s="122"/>
-      <c r="Z12" s="120"/>
-      <c r="AA12" s="125"/>
-      <c r="AB12" s="126"/>
-      <c r="AC12" s="126"/>
-      <c r="AD12" s="126"/>
-      <c r="AE12" s="126"/>
-      <c r="AF12" s="126"/>
-      <c r="AG12" s="126"/>
-      <c r="AH12" s="126"/>
-      <c r="AI12" s="126"/>
-      <c r="AJ12" s="126"/>
+      <c r="T12" s="127"/>
+      <c r="U12" s="128"/>
+      <c r="V12" s="127"/>
+      <c r="W12" s="123"/>
+      <c r="X12" s="123"/>
+      <c r="Y12" s="123"/>
+      <c r="Z12" s="128"/>
+      <c r="AA12" s="132"/>
+      <c r="AB12" s="133"/>
+      <c r="AC12" s="133"/>
+      <c r="AD12" s="133"/>
+      <c r="AE12" s="133"/>
+      <c r="AF12" s="133"/>
+      <c r="AG12" s="133"/>
+      <c r="AH12" s="133"/>
+      <c r="AI12" s="133"/>
+      <c r="AJ12" s="133"/>
       <c r="AK12" s="84"/>
     </row>
     <row r="13" spans="1:38" ht="23.25" customHeight="1" thickBot="1">
@@ -4037,7 +4034,7 @@
     </row>
     <row r="14" spans="1:38" ht="25.5" customHeight="1">
       <c r="A14" s="83"/>
-      <c r="B14" s="133" t="s">
+      <c r="B14" s="115" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -4045,78 +4042,78 @@
       </c>
       <c r="D14" s="26"/>
       <c r="E14" s="96"/>
-      <c r="F14" s="113"/>
-      <c r="G14" s="113"/>
-      <c r="H14" s="113"/>
-      <c r="I14" s="113"/>
-      <c r="J14" s="113"/>
-      <c r="K14" s="113"/>
-      <c r="L14" s="113"/>
-      <c r="M14" s="113"/>
-      <c r="N14" s="113"/>
-      <c r="O14" s="113"/>
-      <c r="P14" s="113"/>
-      <c r="Q14" s="113"/>
-      <c r="R14" s="113"/>
-      <c r="S14" s="113"/>
-      <c r="T14" s="113"/>
-      <c r="U14" s="113"/>
-      <c r="V14" s="113"/>
-      <c r="W14" s="113"/>
-      <c r="X14" s="113"/>
-      <c r="Y14" s="113"/>
-      <c r="Z14" s="113"/>
-      <c r="AA14" s="113"/>
-      <c r="AB14" s="113"/>
-      <c r="AC14" s="113"/>
-      <c r="AD14" s="113"/>
-      <c r="AE14" s="113"/>
-      <c r="AF14" s="113"/>
-      <c r="AG14" s="113"/>
-      <c r="AH14" s="113"/>
-      <c r="AI14" s="113"/>
-      <c r="AJ14" s="114"/>
+      <c r="F14" s="140"/>
+      <c r="G14" s="140"/>
+      <c r="H14" s="140"/>
+      <c r="I14" s="140"/>
+      <c r="J14" s="140"/>
+      <c r="K14" s="140"/>
+      <c r="L14" s="140"/>
+      <c r="M14" s="140"/>
+      <c r="N14" s="140"/>
+      <c r="O14" s="140"/>
+      <c r="P14" s="140"/>
+      <c r="Q14" s="140"/>
+      <c r="R14" s="140"/>
+      <c r="S14" s="140"/>
+      <c r="T14" s="140"/>
+      <c r="U14" s="140"/>
+      <c r="V14" s="140"/>
+      <c r="W14" s="140"/>
+      <c r="X14" s="140"/>
+      <c r="Y14" s="140"/>
+      <c r="Z14" s="140"/>
+      <c r="AA14" s="140"/>
+      <c r="AB14" s="140"/>
+      <c r="AC14" s="140"/>
+      <c r="AD14" s="140"/>
+      <c r="AE14" s="140"/>
+      <c r="AF14" s="140"/>
+      <c r="AG14" s="140"/>
+      <c r="AH14" s="140"/>
+      <c r="AI14" s="140"/>
+      <c r="AJ14" s="141"/>
       <c r="AK14" s="84"/>
     </row>
     <row r="15" spans="1:38" ht="60.75" customHeight="1" thickBot="1">
       <c r="A15" s="83"/>
-      <c r="B15" s="134"/>
+      <c r="B15" s="116"/>
       <c r="C15" s="6" t="s">
         <v>30</v>
       </c>
       <c r="D15" s="35"/>
       <c r="E15" s="95"/>
-      <c r="F15" s="110"/>
-      <c r="G15" s="110"/>
-      <c r="H15" s="110"/>
-      <c r="I15" s="110"/>
-      <c r="J15" s="110"/>
-      <c r="K15" s="110"/>
-      <c r="L15" s="110"/>
-      <c r="M15" s="110"/>
-      <c r="N15" s="110"/>
-      <c r="O15" s="110"/>
-      <c r="P15" s="110"/>
-      <c r="Q15" s="110"/>
-      <c r="R15" s="110"/>
-      <c r="S15" s="110"/>
-      <c r="T15" s="111"/>
-      <c r="U15" s="111"/>
-      <c r="V15" s="111"/>
-      <c r="W15" s="111"/>
-      <c r="X15" s="111"/>
-      <c r="Y15" s="111"/>
-      <c r="Z15" s="111"/>
-      <c r="AA15" s="111"/>
-      <c r="AB15" s="111"/>
-      <c r="AC15" s="111"/>
-      <c r="AD15" s="111"/>
-      <c r="AE15" s="111"/>
-      <c r="AF15" s="111"/>
-      <c r="AG15" s="111"/>
-      <c r="AH15" s="111"/>
-      <c r="AI15" s="111"/>
-      <c r="AJ15" s="112"/>
+      <c r="F15" s="142"/>
+      <c r="G15" s="142"/>
+      <c r="H15" s="142"/>
+      <c r="I15" s="142"/>
+      <c r="J15" s="142"/>
+      <c r="K15" s="142"/>
+      <c r="L15" s="142"/>
+      <c r="M15" s="142"/>
+      <c r="N15" s="142"/>
+      <c r="O15" s="142"/>
+      <c r="P15" s="142"/>
+      <c r="Q15" s="142"/>
+      <c r="R15" s="142"/>
+      <c r="S15" s="142"/>
+      <c r="T15" s="142"/>
+      <c r="U15" s="142"/>
+      <c r="V15" s="142"/>
+      <c r="W15" s="142"/>
+      <c r="X15" s="142"/>
+      <c r="Y15" s="142"/>
+      <c r="Z15" s="142"/>
+      <c r="AA15" s="142"/>
+      <c r="AB15" s="142"/>
+      <c r="AC15" s="142"/>
+      <c r="AD15" s="142"/>
+      <c r="AE15" s="142"/>
+      <c r="AF15" s="142"/>
+      <c r="AG15" s="142"/>
+      <c r="AH15" s="142"/>
+      <c r="AI15" s="142"/>
+      <c r="AJ15" s="143"/>
       <c r="AK15" s="84"/>
     </row>
     <row r="16" spans="1:38" ht="23.25" customHeight="1" thickBot="1">
@@ -4141,30 +4138,30 @@
       <c r="Q16" s="64"/>
       <c r="R16" s="64"/>
       <c r="S16" s="64"/>
-      <c r="T16" s="135" t="s">
+      <c r="T16" s="117" t="s">
         <v>29</v>
       </c>
-      <c r="U16" s="135"/>
-      <c r="V16" s="135"/>
-      <c r="W16" s="135"/>
-      <c r="X16" s="135"/>
-      <c r="Y16" s="135"/>
-      <c r="Z16" s="135"/>
-      <c r="AA16" s="135"/>
-      <c r="AB16" s="135"/>
-      <c r="AC16" s="135"/>
-      <c r="AD16" s="135"/>
-      <c r="AE16" s="135"/>
-      <c r="AF16" s="135"/>
-      <c r="AG16" s="135"/>
-      <c r="AH16" s="135"/>
-      <c r="AI16" s="135"/>
-      <c r="AJ16" s="135"/>
+      <c r="U16" s="117"/>
+      <c r="V16" s="117"/>
+      <c r="W16" s="117"/>
+      <c r="X16" s="117"/>
+      <c r="Y16" s="117"/>
+      <c r="Z16" s="117"/>
+      <c r="AA16" s="117"/>
+      <c r="AB16" s="117"/>
+      <c r="AC16" s="117"/>
+      <c r="AD16" s="117"/>
+      <c r="AE16" s="117"/>
+      <c r="AF16" s="117"/>
+      <c r="AG16" s="117"/>
+      <c r="AH16" s="117"/>
+      <c r="AI16" s="117"/>
+      <c r="AJ16" s="117"/>
       <c r="AK16" s="84"/>
     </row>
     <row r="17" spans="1:37" ht="25.5" customHeight="1">
       <c r="A17" s="83"/>
-      <c r="B17" s="133" t="s">
+      <c r="B17" s="115" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -4186,7 +4183,7 @@
       <c r="Q17" s="101"/>
       <c r="R17" s="104"/>
       <c r="S17" s="27"/>
-      <c r="T17" s="133" t="s">
+      <c r="T17" s="115" t="s">
         <v>19</v>
       </c>
       <c r="U17" s="65"/>
@@ -4209,7 +4206,7 @@
     </row>
     <row r="18" spans="1:37" ht="37.5" customHeight="1" thickBot="1">
       <c r="A18" s="83"/>
-      <c r="B18" s="134"/>
+      <c r="B18" s="116"/>
       <c r="C18" s="6" t="s">
         <v>4</v>
       </c>
@@ -4231,7 +4228,7 @@
       <c r="Q18" s="100"/>
       <c r="R18" s="106"/>
       <c r="S18" s="27"/>
-      <c r="T18" s="136"/>
+      <c r="T18" s="118"/>
       <c r="U18" s="70"/>
       <c r="V18" s="27"/>
       <c r="W18" s="71"/>
@@ -4252,7 +4249,7 @@
     </row>
     <row r="19" spans="1:37" ht="25.5" customHeight="1" thickBot="1">
       <c r="A19" s="83"/>
-      <c r="B19" s="133" t="s">
+      <c r="B19" s="115" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="5" t="s">
@@ -4274,28 +4271,28 @@
       <c r="Q19" s="101"/>
       <c r="R19" s="104"/>
       <c r="S19" s="27"/>
-      <c r="T19" s="134"/>
+      <c r="T19" s="116"/>
       <c r="U19" s="43"/>
       <c r="V19" s="25"/>
       <c r="W19" s="25"/>
       <c r="X19" s="25"/>
-      <c r="Y19" s="122"/>
-      <c r="Z19" s="122"/>
-      <c r="AA19" s="122"/>
-      <c r="AB19" s="122"/>
-      <c r="AC19" s="122"/>
-      <c r="AD19" s="122"/>
-      <c r="AE19" s="122"/>
-      <c r="AF19" s="122"/>
-      <c r="AG19" s="122"/>
-      <c r="AH19" s="122"/>
-      <c r="AI19" s="122"/>
+      <c r="Y19" s="123"/>
+      <c r="Z19" s="123"/>
+      <c r="AA19" s="123"/>
+      <c r="AB19" s="123"/>
+      <c r="AC19" s="123"/>
+      <c r="AD19" s="123"/>
+      <c r="AE19" s="123"/>
+      <c r="AF19" s="123"/>
+      <c r="AG19" s="123"/>
+      <c r="AH19" s="123"/>
+      <c r="AI19" s="123"/>
       <c r="AJ19" s="24"/>
       <c r="AK19" s="84"/>
     </row>
     <row r="20" spans="1:37" ht="37.5" customHeight="1" thickBot="1">
       <c r="A20" s="83"/>
-      <c r="B20" s="134"/>
+      <c r="B20" s="116"/>
       <c r="C20" s="6" t="s">
         <v>4</v>
       </c>
@@ -4465,13 +4462,13 @@
       <c r="I24" s="28"/>
       <c r="J24" s="28"/>
       <c r="K24" s="28"/>
-      <c r="L24" s="132" t="s">
+      <c r="L24" s="139" t="s">
         <v>25</v>
       </c>
-      <c r="M24" s="132"/>
-      <c r="N24" s="132"/>
-      <c r="O24" s="132"/>
-      <c r="P24" s="132"/>
+      <c r="M24" s="139"/>
+      <c r="N24" s="139"/>
+      <c r="O24" s="139"/>
+      <c r="P24" s="139"/>
       <c r="Q24" s="29" t="s">
         <v>31</v>
       </c>
@@ -4502,13 +4499,13 @@
       <c r="C25" s="27"/>
       <c r="D25" s="27"/>
       <c r="E25" s="59"/>
-      <c r="F25" s="115" t="s">
+      <c r="F25" s="110" t="s">
         <v>28</v>
       </c>
-      <c r="G25" s="115"/>
-      <c r="H25" s="115"/>
-      <c r="I25" s="115"/>
-      <c r="J25" s="115"/>
+      <c r="G25" s="110"/>
+      <c r="H25" s="110"/>
+      <c r="I25" s="110"/>
+      <c r="J25" s="110"/>
       <c r="K25" s="28"/>
       <c r="L25" s="28"/>
       <c r="M25" s="28"/>
@@ -4543,11 +4540,11 @@
       <c r="C26" s="27"/>
       <c r="D26" s="27"/>
       <c r="E26" s="59"/>
-      <c r="F26" s="115"/>
-      <c r="G26" s="115"/>
-      <c r="H26" s="115"/>
-      <c r="I26" s="115"/>
-      <c r="J26" s="115"/>
+      <c r="F26" s="110"/>
+      <c r="G26" s="110"/>
+      <c r="H26" s="110"/>
+      <c r="I26" s="110"/>
+      <c r="J26" s="110"/>
       <c r="K26" s="28"/>
       <c r="L26" s="28"/>
       <c r="M26" s="28"/>
@@ -4582,18 +4579,18 @@
       <c r="C27" s="27"/>
       <c r="D27" s="27"/>
       <c r="E27" s="59"/>
-      <c r="F27" s="115"/>
-      <c r="G27" s="115"/>
-      <c r="H27" s="115"/>
-      <c r="I27" s="115"/>
-      <c r="J27" s="115"/>
-      <c r="K27" s="115"/>
-      <c r="L27" s="115"/>
-      <c r="M27" s="115"/>
-      <c r="N27" s="115"/>
-      <c r="O27" s="115"/>
-      <c r="P27" s="115"/>
-      <c r="Q27" s="115"/>
+      <c r="F27" s="110"/>
+      <c r="G27" s="110"/>
+      <c r="H27" s="110"/>
+      <c r="I27" s="110"/>
+      <c r="J27" s="110"/>
+      <c r="K27" s="110"/>
+      <c r="L27" s="110"/>
+      <c r="M27" s="110"/>
+      <c r="N27" s="110"/>
+      <c r="O27" s="110"/>
+      <c r="P27" s="110"/>
+      <c r="Q27" s="110"/>
       <c r="R27" s="40"/>
       <c r="S27" s="27"/>
       <c r="T27" s="27"/>
@@ -4617,24 +4614,24 @@
     </row>
     <row r="28" spans="1:37" ht="11.25" customHeight="1">
       <c r="A28" s="83"/>
-      <c r="B28" s="141" t="s">
+      <c r="B28" s="111" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="142"/>
-      <c r="D28" s="142"/>
-      <c r="E28" s="143"/>
-      <c r="F28" s="115"/>
-      <c r="G28" s="115"/>
-      <c r="H28" s="115"/>
-      <c r="I28" s="115"/>
-      <c r="J28" s="115"/>
-      <c r="K28" s="115"/>
-      <c r="L28" s="115"/>
-      <c r="M28" s="115"/>
-      <c r="N28" s="115"/>
-      <c r="O28" s="115"/>
-      <c r="P28" s="115"/>
-      <c r="Q28" s="115"/>
+      <c r="C28" s="112"/>
+      <c r="D28" s="112"/>
+      <c r="E28" s="113"/>
+      <c r="F28" s="110"/>
+      <c r="G28" s="110"/>
+      <c r="H28" s="110"/>
+      <c r="I28" s="110"/>
+      <c r="J28" s="110"/>
+      <c r="K28" s="110"/>
+      <c r="L28" s="110"/>
+      <c r="M28" s="110"/>
+      <c r="N28" s="110"/>
+      <c r="O28" s="110"/>
+      <c r="P28" s="110"/>
+      <c r="Q28" s="110"/>
       <c r="R28" s="40"/>
       <c r="S28" s="27"/>
       <c r="T28" s="27"/>
@@ -4662,18 +4659,18 @@
       <c r="C29" s="27"/>
       <c r="D29" s="27"/>
       <c r="E29" s="59"/>
-      <c r="F29" s="115"/>
-      <c r="G29" s="115"/>
-      <c r="H29" s="115"/>
-      <c r="I29" s="115"/>
-      <c r="J29" s="115"/>
-      <c r="K29" s="115"/>
-      <c r="L29" s="115"/>
-      <c r="M29" s="115"/>
-      <c r="N29" s="115"/>
-      <c r="O29" s="115"/>
-      <c r="P29" s="115"/>
-      <c r="Q29" s="115"/>
+      <c r="F29" s="110"/>
+      <c r="G29" s="110"/>
+      <c r="H29" s="110"/>
+      <c r="I29" s="110"/>
+      <c r="J29" s="110"/>
+      <c r="K29" s="110"/>
+      <c r="L29" s="110"/>
+      <c r="M29" s="110"/>
+      <c r="N29" s="110"/>
+      <c r="O29" s="110"/>
+      <c r="P29" s="110"/>
+      <c r="Q29" s="110"/>
       <c r="R29" s="40"/>
       <c r="S29" s="27"/>
       <c r="T29" s="27"/>
@@ -4701,18 +4698,18 @@
       <c r="C30" s="27"/>
       <c r="D30" s="27"/>
       <c r="E30" s="27"/>
-      <c r="F30" s="115"/>
-      <c r="G30" s="115"/>
-      <c r="H30" s="115"/>
-      <c r="I30" s="115"/>
-      <c r="J30" s="115"/>
-      <c r="K30" s="115"/>
-      <c r="L30" s="115"/>
-      <c r="M30" s="115"/>
-      <c r="N30" s="115"/>
-      <c r="O30" s="115"/>
-      <c r="P30" s="115"/>
-      <c r="Q30" s="115"/>
+      <c r="F30" s="110"/>
+      <c r="G30" s="110"/>
+      <c r="H30" s="110"/>
+      <c r="I30" s="110"/>
+      <c r="J30" s="110"/>
+      <c r="K30" s="110"/>
+      <c r="L30" s="110"/>
+      <c r="M30" s="110"/>
+      <c r="N30" s="110"/>
+      <c r="O30" s="110"/>
+      <c r="P30" s="110"/>
+      <c r="Q30" s="110"/>
       <c r="R30" s="40"/>
       <c r="S30" s="27"/>
       <c r="T30" s="27"/>
@@ -4736,24 +4733,24 @@
     </row>
     <row r="31" spans="1:37" ht="11.25" customHeight="1">
       <c r="A31" s="83"/>
-      <c r="B31" s="141" t="s">
+      <c r="B31" s="111" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="142"/>
-      <c r="D31" s="142"/>
-      <c r="E31" s="142"/>
-      <c r="F31" s="115"/>
-      <c r="G31" s="115"/>
-      <c r="H31" s="115"/>
-      <c r="I31" s="115"/>
-      <c r="J31" s="115"/>
-      <c r="K31" s="115"/>
-      <c r="L31" s="115"/>
-      <c r="M31" s="115"/>
-      <c r="N31" s="115"/>
-      <c r="O31" s="115"/>
-      <c r="P31" s="115"/>
-      <c r="Q31" s="115"/>
+      <c r="C31" s="112"/>
+      <c r="D31" s="112"/>
+      <c r="E31" s="112"/>
+      <c r="F31" s="110"/>
+      <c r="G31" s="110"/>
+      <c r="H31" s="110"/>
+      <c r="I31" s="110"/>
+      <c r="J31" s="110"/>
+      <c r="K31" s="110"/>
+      <c r="L31" s="110"/>
+      <c r="M31" s="110"/>
+      <c r="N31" s="110"/>
+      <c r="O31" s="110"/>
+      <c r="P31" s="110"/>
+      <c r="Q31" s="110"/>
       <c r="R31" s="40"/>
       <c r="S31" s="27"/>
       <c r="T31" s="27"/>
@@ -4781,18 +4778,18 @@
       <c r="C32" s="11"/>
       <c r="D32" s="11"/>
       <c r="E32" s="11"/>
-      <c r="F32" s="115"/>
-      <c r="G32" s="115"/>
-      <c r="H32" s="115"/>
-      <c r="I32" s="115"/>
-      <c r="J32" s="115"/>
-      <c r="K32" s="115"/>
-      <c r="L32" s="115"/>
-      <c r="M32" s="115"/>
-      <c r="N32" s="115"/>
-      <c r="O32" s="115"/>
-      <c r="P32" s="115"/>
-      <c r="Q32" s="115"/>
+      <c r="F32" s="110"/>
+      <c r="G32" s="110"/>
+      <c r="H32" s="110"/>
+      <c r="I32" s="110"/>
+      <c r="J32" s="110"/>
+      <c r="K32" s="110"/>
+      <c r="L32" s="110"/>
+      <c r="M32" s="110"/>
+      <c r="N32" s="110"/>
+      <c r="O32" s="110"/>
+      <c r="P32" s="110"/>
+      <c r="Q32" s="110"/>
       <c r="R32" s="40"/>
       <c r="S32" s="27"/>
       <c r="T32" s="27"/>
@@ -4820,17 +4817,17 @@
       <c r="C33" s="11"/>
       <c r="D33" s="11"/>
       <c r="E33" s="11"/>
-      <c r="F33" s="115"/>
-      <c r="G33" s="115"/>
-      <c r="H33" s="115"/>
-      <c r="I33" s="115"/>
-      <c r="J33" s="115"/>
-      <c r="K33" s="115"/>
-      <c r="L33" s="115"/>
-      <c r="M33" s="115"/>
-      <c r="N33" s="115"/>
-      <c r="O33" s="115"/>
-      <c r="P33" s="115"/>
+      <c r="F33" s="110"/>
+      <c r="G33" s="110"/>
+      <c r="H33" s="110"/>
+      <c r="I33" s="110"/>
+      <c r="J33" s="110"/>
+      <c r="K33" s="110"/>
+      <c r="L33" s="110"/>
+      <c r="M33" s="110"/>
+      <c r="N33" s="110"/>
+      <c r="O33" s="110"/>
+      <c r="P33" s="110"/>
       <c r="Q33" s="9"/>
       <c r="R33" s="40"/>
       <c r="S33" s="27"/>
@@ -4855,24 +4852,24 @@
     </row>
     <row r="34" spans="1:37" ht="11.25" customHeight="1">
       <c r="A34" s="83"/>
-      <c r="B34" s="141" t="s">
+      <c r="B34" s="111" t="s">
         <v>11</v>
       </c>
-      <c r="C34" s="142"/>
-      <c r="D34" s="142"/>
-      <c r="E34" s="142"/>
-      <c r="F34" s="115"/>
-      <c r="G34" s="115"/>
-      <c r="H34" s="115"/>
-      <c r="I34" s="115"/>
-      <c r="J34" s="115"/>
-      <c r="K34" s="115"/>
-      <c r="L34" s="115"/>
-      <c r="M34" s="115"/>
-      <c r="N34" s="115"/>
-      <c r="O34" s="115"/>
-      <c r="P34" s="115"/>
-      <c r="Q34" s="144" t="s">
+      <c r="C34" s="112"/>
+      <c r="D34" s="112"/>
+      <c r="E34" s="112"/>
+      <c r="F34" s="110"/>
+      <c r="G34" s="110"/>
+      <c r="H34" s="110"/>
+      <c r="I34" s="110"/>
+      <c r="J34" s="110"/>
+      <c r="K34" s="110"/>
+      <c r="L34" s="110"/>
+      <c r="M34" s="110"/>
+      <c r="N34" s="110"/>
+      <c r="O34" s="110"/>
+      <c r="P34" s="110"/>
+      <c r="Q34" s="114" t="s">
         <v>6</v>
       </c>
       <c r="R34" s="40"/>
@@ -4902,18 +4899,18 @@
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
       <c r="E35" s="10"/>
-      <c r="F35" s="115"/>
-      <c r="G35" s="115"/>
-      <c r="H35" s="115"/>
-      <c r="I35" s="115"/>
-      <c r="J35" s="115"/>
-      <c r="K35" s="115"/>
-      <c r="L35" s="115"/>
-      <c r="M35" s="115"/>
-      <c r="N35" s="115"/>
-      <c r="O35" s="115"/>
-      <c r="P35" s="115"/>
-      <c r="Q35" s="144"/>
+      <c r="F35" s="110"/>
+      <c r="G35" s="110"/>
+      <c r="H35" s="110"/>
+      <c r="I35" s="110"/>
+      <c r="J35" s="110"/>
+      <c r="K35" s="110"/>
+      <c r="L35" s="110"/>
+      <c r="M35" s="110"/>
+      <c r="N35" s="110"/>
+      <c r="O35" s="110"/>
+      <c r="P35" s="110"/>
+      <c r="Q35" s="114"/>
       <c r="R35" s="40"/>
       <c r="S35" s="27"/>
       <c r="T35" s="27"/>
@@ -4941,20 +4938,20 @@
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
       <c r="E36" s="61"/>
-      <c r="F36" s="115" t="s">
+      <c r="F36" s="110" t="s">
         <v>32</v>
       </c>
-      <c r="G36" s="115"/>
-      <c r="H36" s="115"/>
-      <c r="I36" s="115"/>
-      <c r="J36" s="115"/>
-      <c r="K36" s="115"/>
-      <c r="L36" s="115"/>
-      <c r="M36" s="115"/>
-      <c r="N36" s="115"/>
-      <c r="O36" s="115"/>
-      <c r="P36" s="115"/>
-      <c r="Q36" s="115"/>
+      <c r="G36" s="110"/>
+      <c r="H36" s="110"/>
+      <c r="I36" s="110"/>
+      <c r="J36" s="110"/>
+      <c r="K36" s="110"/>
+      <c r="L36" s="110"/>
+      <c r="M36" s="110"/>
+      <c r="N36" s="110"/>
+      <c r="O36" s="110"/>
+      <c r="P36" s="110"/>
+      <c r="Q36" s="110"/>
       <c r="R36" s="40"/>
       <c r="S36" s="27"/>
       <c r="T36" s="27"/>
@@ -4978,24 +4975,24 @@
     </row>
     <row r="37" spans="1:37" ht="11.25" customHeight="1">
       <c r="A37" s="83"/>
-      <c r="B37" s="141" t="s">
+      <c r="B37" s="111" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="142"/>
-      <c r="D37" s="142"/>
-      <c r="E37" s="143"/>
-      <c r="F37" s="115"/>
-      <c r="G37" s="115"/>
-      <c r="H37" s="115"/>
-      <c r="I37" s="115"/>
-      <c r="J37" s="115"/>
-      <c r="K37" s="115"/>
-      <c r="L37" s="115"/>
-      <c r="M37" s="115"/>
-      <c r="N37" s="115"/>
-      <c r="O37" s="115"/>
-      <c r="P37" s="115"/>
-      <c r="Q37" s="115"/>
+      <c r="C37" s="112"/>
+      <c r="D37" s="112"/>
+      <c r="E37" s="113"/>
+      <c r="F37" s="110"/>
+      <c r="G37" s="110"/>
+      <c r="H37" s="110"/>
+      <c r="I37" s="110"/>
+      <c r="J37" s="110"/>
+      <c r="K37" s="110"/>
+      <c r="L37" s="110"/>
+      <c r="M37" s="110"/>
+      <c r="N37" s="110"/>
+      <c r="O37" s="110"/>
+      <c r="P37" s="110"/>
+      <c r="Q37" s="110"/>
       <c r="R37" s="40"/>
       <c r="S37" s="27"/>
       <c r="T37" s="27"/>
@@ -5023,18 +5020,18 @@
       <c r="C38" s="27"/>
       <c r="D38" s="27"/>
       <c r="E38" s="59"/>
-      <c r="F38" s="115"/>
-      <c r="G38" s="115"/>
-      <c r="H38" s="115"/>
-      <c r="I38" s="115"/>
-      <c r="J38" s="115"/>
-      <c r="K38" s="115"/>
-      <c r="L38" s="115"/>
-      <c r="M38" s="115"/>
-      <c r="N38" s="115"/>
-      <c r="O38" s="115"/>
-      <c r="P38" s="115"/>
-      <c r="Q38" s="115"/>
+      <c r="F38" s="110"/>
+      <c r="G38" s="110"/>
+      <c r="H38" s="110"/>
+      <c r="I38" s="110"/>
+      <c r="J38" s="110"/>
+      <c r="K38" s="110"/>
+      <c r="L38" s="110"/>
+      <c r="M38" s="110"/>
+      <c r="N38" s="110"/>
+      <c r="O38" s="110"/>
+      <c r="P38" s="110"/>
+      <c r="Q38" s="110"/>
       <c r="R38" s="40"/>
       <c r="S38" s="27"/>
       <c r="T38" s="27"/>
@@ -5257,6 +5254,22 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="F25:J26"/>
+    <mergeCell ref="AI1:AK1"/>
+    <mergeCell ref="T11:U12"/>
+    <mergeCell ref="V11:Z12"/>
+    <mergeCell ref="AA11:AE12"/>
+    <mergeCell ref="AF11:AJ12"/>
+    <mergeCell ref="AF2:AH2"/>
+    <mergeCell ref="AI2:AK2"/>
+    <mergeCell ref="L24:P24"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="T16:AJ16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="T17:T19"/>
+    <mergeCell ref="B6:AK8"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="Y19:AI19"/>
     <mergeCell ref="F36:Q38"/>
     <mergeCell ref="B37:E37"/>
     <mergeCell ref="F27:Q29"/>
@@ -5266,27 +5279,11 @@
     <mergeCell ref="B34:E34"/>
     <mergeCell ref="Q34:Q35"/>
     <mergeCell ref="B31:E31"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="T16:AJ16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="T17:T19"/>
-    <mergeCell ref="B6:AK8"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="Y19:AI19"/>
-    <mergeCell ref="F25:J26"/>
-    <mergeCell ref="AI1:AK1"/>
-    <mergeCell ref="T11:U12"/>
-    <mergeCell ref="V11:Z12"/>
-    <mergeCell ref="AA11:AE12"/>
-    <mergeCell ref="AF11:AJ12"/>
-    <mergeCell ref="AF2:AH2"/>
-    <mergeCell ref="AI2:AK2"/>
-    <mergeCell ref="L24:P24"/>
   </mergeCells>
   <phoneticPr fontId="15"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.19685039370078741" header="0.19685039370078741" footer="0.19685039370078741"/>
-  <pageSetup paperSize="9" scale="71" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="65" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
hoant2 : fix bug
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/ローマ字氏名届_帳票テンプレート.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/ローマ字氏名届_帳票テンプレート.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F5A14E-3298-42A7-A935-98113CEBA7F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F589028E-CF44-4771-8AB0-0C9BE660F004}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="A3_6">'2号'!$F$36:$Q$38</definedName>
     <definedName name="A3_7">'2号'!$L$24:$P$24</definedName>
     <definedName name="A4_5">'2号'!$Y$19:$AI$19</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'2号'!$A$1:$AK$43</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'2号'!$A$1:$AL$43</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -1531,6 +1531,81 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="center" indent="1"/>
     </xf>
@@ -1541,81 +1616,6 @@
       <alignment horizontal="distributed" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1640,15 +1640,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>315402</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>295272</xdr:rowOff>
+      <xdr:colOff>147313</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>15125</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>107576</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>124385</xdr:rowOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>286869</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>34739</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1663,7 +1663,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6400196" y="6335243"/>
+          <a:off x="6232107" y="6536949"/>
           <a:ext cx="6045056" cy="2215966"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1700,7 +1700,7 @@
             </a:lnSpc>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -1710,7 +1710,7 @@
             <a:t>【</a:t>
           </a:r>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1050">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -1720,7 +1720,7 @@
             <a:t>記入上の注意</a:t>
           </a:r>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -1749,7 +1749,7 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1050">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -1778,7 +1778,7 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1050">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -1807,7 +1807,7 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1050">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -1836,7 +1836,7 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1050">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -1865,7 +1865,7 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1050">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -1874,7 +1874,7 @@
             </a:rPr>
             <a:t>　　　氏名欄」に被保険者資格取得届等に記載したカナ氏名を記入のうえ、「理由記入欄」に その理由</a:t>
           </a:r>
-          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050">
             <a:solidFill>
               <a:sysClr val="windowText" lastClr="000000"/>
             </a:solidFill>
@@ -1901,7 +1901,7 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1050">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -1930,7 +1930,7 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1050">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -2000,7 +2000,7 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" baseline="0">
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1050" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -2012,7 +2012,7 @@
             <a:t>　</a:t>
           </a:r>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="1100" baseline="0">
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="1050" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -2023,7 +2023,7 @@
             </a:rPr>
             <a:t>□短期在留者であるため</a:t>
           </a:r>
-          <a:endParaRPr lang="ja-JP" altLang="ja-JP">
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP" sz="1050">
             <a:solidFill>
               <a:sysClr val="windowText" lastClr="000000"/>
             </a:solidFill>
@@ -2032,7 +2032,7 @@
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" baseline="0">
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1050" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -2043,7 +2043,7 @@
             </a:rPr>
             <a:t>　□海外に住所を有している者であるため</a:t>
           </a:r>
-          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
             <a:solidFill>
               <a:sysClr val="windowText" lastClr="000000"/>
             </a:solidFill>
@@ -2055,7 +2055,7 @@
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" baseline="0">
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1050" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -2067,7 +2067,7 @@
             <a:t>　</a:t>
           </a:r>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="1100" baseline="0">
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="1050" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -2079,7 +2079,7 @@
             <a:t>□在留カード</a:t>
           </a:r>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" baseline="0">
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1050" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -2091,7 +2091,7 @@
             <a:t>（または特別永住者証明書）</a:t>
           </a:r>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="1100" baseline="0">
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="1050" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -2102,7 +2102,7 @@
             </a:rPr>
             <a:t>にローマ字氏名が記載されていないため</a:t>
           </a:r>
-          <a:endParaRPr lang="ja-JP" altLang="ja-JP">
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP" sz="1050">
             <a:solidFill>
               <a:sysClr val="windowText" lastClr="000000"/>
             </a:solidFill>
@@ -2111,7 +2111,7 @@
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1050">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -2123,7 +2123,7 @@
             <a:t>　</a:t>
           </a:r>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="1100">
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="1050">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -2134,7 +2134,7 @@
             </a:rPr>
             <a:t>□その他　理由（　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　          　）</a:t>
           </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1050">
             <a:solidFill>
               <a:sysClr val="windowText" lastClr="000000"/>
             </a:solidFill>
@@ -3482,8 +3482,8 @@
   </sheetPr>
   <dimension ref="A1:AL43"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="V36" sqref="V36"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="55" workbookViewId="0">
+      <selection activeCell="Y37" sqref="Y37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.140625" defaultRowHeight="15"/>
@@ -3526,11 +3526,11 @@
       <c r="AC1" s="27"/>
       <c r="AD1" s="27"/>
       <c r="AE1" s="27"/>
-      <c r="AI1" s="128">
+      <c r="AI1" s="115">
         <v>72073</v>
       </c>
-      <c r="AJ1" s="128"/>
-      <c r="AK1" s="128"/>
+      <c r="AJ1" s="115"/>
+      <c r="AK1" s="115"/>
       <c r="AL1" s="27"/>
     </row>
     <row r="2" spans="1:38" ht="26.25" customHeight="1">
@@ -3565,16 +3565,16 @@
       <c r="AC2" s="27"/>
       <c r="AD2" s="27"/>
       <c r="AE2" s="27"/>
-      <c r="AF2" s="139" t="s">
+      <c r="AF2" s="127" t="s">
         <v>23</v>
       </c>
-      <c r="AG2" s="140"/>
-      <c r="AH2" s="141"/>
-      <c r="AI2" s="142" t="s">
+      <c r="AG2" s="128"/>
+      <c r="AH2" s="129"/>
+      <c r="AI2" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="AJ2" s="140"/>
-      <c r="AK2" s="141"/>
+      <c r="AJ2" s="128"/>
+      <c r="AK2" s="129"/>
       <c r="AL2" s="27"/>
     </row>
     <row r="3" spans="1:38" ht="26.25" customHeight="1">
@@ -3698,122 +3698,122 @@
     </row>
     <row r="6" spans="1:38" ht="13.5" customHeight="1">
       <c r="A6" s="82"/>
-      <c r="B6" s="123" t="s">
+      <c r="B6" s="136" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="123"/>
-      <c r="D6" s="123"/>
-      <c r="E6" s="123"/>
-      <c r="F6" s="123"/>
-      <c r="G6" s="123"/>
-      <c r="H6" s="123"/>
-      <c r="I6" s="123"/>
-      <c r="J6" s="123"/>
-      <c r="K6" s="123"/>
-      <c r="L6" s="123"/>
-      <c r="M6" s="123"/>
-      <c r="N6" s="123"/>
-      <c r="O6" s="123"/>
-      <c r="P6" s="123"/>
-      <c r="Q6" s="123"/>
-      <c r="R6" s="123"/>
-      <c r="S6" s="123"/>
-      <c r="T6" s="123"/>
-      <c r="U6" s="123"/>
-      <c r="V6" s="123"/>
-      <c r="W6" s="123"/>
-      <c r="X6" s="123"/>
-      <c r="Y6" s="123"/>
-      <c r="Z6" s="123"/>
-      <c r="AA6" s="123"/>
-      <c r="AB6" s="123"/>
-      <c r="AC6" s="123"/>
-      <c r="AD6" s="123"/>
-      <c r="AE6" s="123"/>
-      <c r="AF6" s="123"/>
-      <c r="AG6" s="123"/>
-      <c r="AH6" s="123"/>
-      <c r="AI6" s="123"/>
-      <c r="AJ6" s="123"/>
-      <c r="AK6" s="124"/>
+      <c r="C6" s="136"/>
+      <c r="D6" s="136"/>
+      <c r="E6" s="136"/>
+      <c r="F6" s="136"/>
+      <c r="G6" s="136"/>
+      <c r="H6" s="136"/>
+      <c r="I6" s="136"/>
+      <c r="J6" s="136"/>
+      <c r="K6" s="136"/>
+      <c r="L6" s="136"/>
+      <c r="M6" s="136"/>
+      <c r="N6" s="136"/>
+      <c r="O6" s="136"/>
+      <c r="P6" s="136"/>
+      <c r="Q6" s="136"/>
+      <c r="R6" s="136"/>
+      <c r="S6" s="136"/>
+      <c r="T6" s="136"/>
+      <c r="U6" s="136"/>
+      <c r="V6" s="136"/>
+      <c r="W6" s="136"/>
+      <c r="X6" s="136"/>
+      <c r="Y6" s="136"/>
+      <c r="Z6" s="136"/>
+      <c r="AA6" s="136"/>
+      <c r="AB6" s="136"/>
+      <c r="AC6" s="136"/>
+      <c r="AD6" s="136"/>
+      <c r="AE6" s="136"/>
+      <c r="AF6" s="136"/>
+      <c r="AG6" s="136"/>
+      <c r="AH6" s="136"/>
+      <c r="AI6" s="136"/>
+      <c r="AJ6" s="136"/>
+      <c r="AK6" s="137"/>
     </row>
     <row r="7" spans="1:38" ht="13.5" customHeight="1">
       <c r="A7" s="83"/>
-      <c r="B7" s="125"/>
-      <c r="C7" s="125"/>
-      <c r="D7" s="125"/>
-      <c r="E7" s="125"/>
-      <c r="F7" s="125"/>
-      <c r="G7" s="125"/>
-      <c r="H7" s="125"/>
-      <c r="I7" s="125"/>
-      <c r="J7" s="125"/>
-      <c r="K7" s="125"/>
-      <c r="L7" s="125"/>
-      <c r="M7" s="125"/>
-      <c r="N7" s="125"/>
-      <c r="O7" s="125"/>
-      <c r="P7" s="125"/>
-      <c r="Q7" s="125"/>
-      <c r="R7" s="125"/>
-      <c r="S7" s="125"/>
-      <c r="T7" s="125"/>
-      <c r="U7" s="125"/>
-      <c r="V7" s="125"/>
-      <c r="W7" s="125"/>
-      <c r="X7" s="125"/>
-      <c r="Y7" s="125"/>
-      <c r="Z7" s="125"/>
-      <c r="AA7" s="125"/>
-      <c r="AB7" s="125"/>
-      <c r="AC7" s="125"/>
-      <c r="AD7" s="125"/>
-      <c r="AE7" s="125"/>
-      <c r="AF7" s="125"/>
-      <c r="AG7" s="125"/>
-      <c r="AH7" s="125"/>
-      <c r="AI7" s="125"/>
-      <c r="AJ7" s="125"/>
-      <c r="AK7" s="126"/>
+      <c r="B7" s="138"/>
+      <c r="C7" s="138"/>
+      <c r="D7" s="138"/>
+      <c r="E7" s="138"/>
+      <c r="F7" s="138"/>
+      <c r="G7" s="138"/>
+      <c r="H7" s="138"/>
+      <c r="I7" s="138"/>
+      <c r="J7" s="138"/>
+      <c r="K7" s="138"/>
+      <c r="L7" s="138"/>
+      <c r="M7" s="138"/>
+      <c r="N7" s="138"/>
+      <c r="O7" s="138"/>
+      <c r="P7" s="138"/>
+      <c r="Q7" s="138"/>
+      <c r="R7" s="138"/>
+      <c r="S7" s="138"/>
+      <c r="T7" s="138"/>
+      <c r="U7" s="138"/>
+      <c r="V7" s="138"/>
+      <c r="W7" s="138"/>
+      <c r="X7" s="138"/>
+      <c r="Y7" s="138"/>
+      <c r="Z7" s="138"/>
+      <c r="AA7" s="138"/>
+      <c r="AB7" s="138"/>
+      <c r="AC7" s="138"/>
+      <c r="AD7" s="138"/>
+      <c r="AE7" s="138"/>
+      <c r="AF7" s="138"/>
+      <c r="AG7" s="138"/>
+      <c r="AH7" s="138"/>
+      <c r="AI7" s="138"/>
+      <c r="AJ7" s="138"/>
+      <c r="AK7" s="139"/>
     </row>
     <row r="8" spans="1:38" ht="13.5" customHeight="1">
       <c r="A8" s="83"/>
-      <c r="B8" s="125"/>
-      <c r="C8" s="125"/>
-      <c r="D8" s="125"/>
-      <c r="E8" s="125"/>
-      <c r="F8" s="125"/>
-      <c r="G8" s="125"/>
-      <c r="H8" s="125"/>
-      <c r="I8" s="125"/>
-      <c r="J8" s="125"/>
-      <c r="K8" s="125"/>
-      <c r="L8" s="125"/>
-      <c r="M8" s="125"/>
-      <c r="N8" s="125"/>
-      <c r="O8" s="125"/>
-      <c r="P8" s="125"/>
-      <c r="Q8" s="125"/>
-      <c r="R8" s="125"/>
-      <c r="S8" s="125"/>
-      <c r="T8" s="125"/>
-      <c r="U8" s="125"/>
-      <c r="V8" s="125"/>
-      <c r="W8" s="125"/>
-      <c r="X8" s="125"/>
-      <c r="Y8" s="125"/>
-      <c r="Z8" s="125"/>
-      <c r="AA8" s="125"/>
-      <c r="AB8" s="125"/>
-      <c r="AC8" s="125"/>
-      <c r="AD8" s="125"/>
-      <c r="AE8" s="125"/>
-      <c r="AF8" s="125"/>
-      <c r="AG8" s="125"/>
-      <c r="AH8" s="125"/>
-      <c r="AI8" s="125"/>
-      <c r="AJ8" s="125"/>
-      <c r="AK8" s="126"/>
+      <c r="B8" s="138"/>
+      <c r="C8" s="138"/>
+      <c r="D8" s="138"/>
+      <c r="E8" s="138"/>
+      <c r="F8" s="138"/>
+      <c r="G8" s="138"/>
+      <c r="H8" s="138"/>
+      <c r="I8" s="138"/>
+      <c r="J8" s="138"/>
+      <c r="K8" s="138"/>
+      <c r="L8" s="138"/>
+      <c r="M8" s="138"/>
+      <c r="N8" s="138"/>
+      <c r="O8" s="138"/>
+      <c r="P8" s="138"/>
+      <c r="Q8" s="138"/>
+      <c r="R8" s="138"/>
+      <c r="S8" s="138"/>
+      <c r="T8" s="138"/>
+      <c r="U8" s="138"/>
+      <c r="V8" s="138"/>
+      <c r="W8" s="138"/>
+      <c r="X8" s="138"/>
+      <c r="Y8" s="138"/>
+      <c r="Z8" s="138"/>
+      <c r="AA8" s="138"/>
+      <c r="AB8" s="138"/>
+      <c r="AC8" s="138"/>
+      <c r="AD8" s="138"/>
+      <c r="AE8" s="138"/>
+      <c r="AF8" s="138"/>
+      <c r="AG8" s="138"/>
+      <c r="AH8" s="138"/>
+      <c r="AI8" s="138"/>
+      <c r="AJ8" s="138"/>
+      <c r="AK8" s="139"/>
     </row>
     <row r="9" spans="1:38" ht="18.75" customHeight="1">
       <c r="A9" s="83"/>
@@ -3929,27 +3929,27 @@
       <c r="S11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="T11" s="129" t="s">
+      <c r="T11" s="116" t="s">
         <v>27</v>
       </c>
-      <c r="U11" s="130"/>
-      <c r="V11" s="129" t="s">
+      <c r="U11" s="117"/>
+      <c r="V11" s="116" t="s">
         <v>18</v>
       </c>
-      <c r="W11" s="133"/>
-      <c r="X11" s="133"/>
-      <c r="Y11" s="133"/>
-      <c r="Z11" s="130"/>
-      <c r="AA11" s="134"/>
-      <c r="AB11" s="135"/>
-      <c r="AC11" s="135"/>
-      <c r="AD11" s="135"/>
-      <c r="AE11" s="135"/>
-      <c r="AF11" s="138"/>
-      <c r="AG11" s="135"/>
-      <c r="AH11" s="135"/>
-      <c r="AI11" s="135"/>
-      <c r="AJ11" s="135"/>
+      <c r="W11" s="120"/>
+      <c r="X11" s="120"/>
+      <c r="Y11" s="120"/>
+      <c r="Z11" s="117"/>
+      <c r="AA11" s="122"/>
+      <c r="AB11" s="123"/>
+      <c r="AC11" s="123"/>
+      <c r="AD11" s="123"/>
+      <c r="AE11" s="123"/>
+      <c r="AF11" s="126"/>
+      <c r="AG11" s="123"/>
+      <c r="AH11" s="123"/>
+      <c r="AI11" s="123"/>
+      <c r="AJ11" s="123"/>
       <c r="AK11" s="84"/>
     </row>
     <row r="12" spans="1:38" ht="40.5" customHeight="1" thickBot="1">
@@ -3972,23 +3972,23 @@
       <c r="Q12" s="57"/>
       <c r="R12" s="58"/>
       <c r="S12" s="50"/>
-      <c r="T12" s="131"/>
-      <c r="U12" s="132"/>
-      <c r="V12" s="131"/>
-      <c r="W12" s="127"/>
-      <c r="X12" s="127"/>
-      <c r="Y12" s="127"/>
-      <c r="Z12" s="132"/>
-      <c r="AA12" s="136"/>
-      <c r="AB12" s="137"/>
-      <c r="AC12" s="137"/>
-      <c r="AD12" s="137"/>
-      <c r="AE12" s="137"/>
-      <c r="AF12" s="137"/>
-      <c r="AG12" s="137"/>
-      <c r="AH12" s="137"/>
-      <c r="AI12" s="137"/>
-      <c r="AJ12" s="137"/>
+      <c r="T12" s="118"/>
+      <c r="U12" s="119"/>
+      <c r="V12" s="118"/>
+      <c r="W12" s="121"/>
+      <c r="X12" s="121"/>
+      <c r="Y12" s="121"/>
+      <c r="Z12" s="119"/>
+      <c r="AA12" s="124"/>
+      <c r="AB12" s="125"/>
+      <c r="AC12" s="125"/>
+      <c r="AD12" s="125"/>
+      <c r="AE12" s="125"/>
+      <c r="AF12" s="125"/>
+      <c r="AG12" s="125"/>
+      <c r="AH12" s="125"/>
+      <c r="AI12" s="125"/>
+      <c r="AJ12" s="125"/>
       <c r="AK12" s="84"/>
     </row>
     <row r="13" spans="1:38" ht="23.25" customHeight="1" thickBot="1">
@@ -4034,7 +4034,7 @@
     </row>
     <row r="14" spans="1:38" ht="25.5" customHeight="1">
       <c r="A14" s="83"/>
-      <c r="B14" s="119" t="s">
+      <c r="B14" s="132" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -4077,7 +4077,7 @@
     </row>
     <row r="15" spans="1:38" ht="60.75" customHeight="1" thickBot="1">
       <c r="A15" s="83"/>
-      <c r="B15" s="120"/>
+      <c r="B15" s="133"/>
       <c r="C15" s="6" t="s">
         <v>30</v>
       </c>
@@ -4138,30 +4138,30 @@
       <c r="Q16" s="64"/>
       <c r="R16" s="64"/>
       <c r="S16" s="64"/>
-      <c r="T16" s="121" t="s">
+      <c r="T16" s="134" t="s">
         <v>29</v>
       </c>
-      <c r="U16" s="121"/>
-      <c r="V16" s="121"/>
-      <c r="W16" s="121"/>
-      <c r="X16" s="121"/>
-      <c r="Y16" s="121"/>
-      <c r="Z16" s="121"/>
-      <c r="AA16" s="121"/>
-      <c r="AB16" s="121"/>
-      <c r="AC16" s="121"/>
-      <c r="AD16" s="121"/>
-      <c r="AE16" s="121"/>
-      <c r="AF16" s="121"/>
-      <c r="AG16" s="121"/>
-      <c r="AH16" s="121"/>
-      <c r="AI16" s="121"/>
-      <c r="AJ16" s="121"/>
+      <c r="U16" s="134"/>
+      <c r="V16" s="134"/>
+      <c r="W16" s="134"/>
+      <c r="X16" s="134"/>
+      <c r="Y16" s="134"/>
+      <c r="Z16" s="134"/>
+      <c r="AA16" s="134"/>
+      <c r="AB16" s="134"/>
+      <c r="AC16" s="134"/>
+      <c r="AD16" s="134"/>
+      <c r="AE16" s="134"/>
+      <c r="AF16" s="134"/>
+      <c r="AG16" s="134"/>
+      <c r="AH16" s="134"/>
+      <c r="AI16" s="134"/>
+      <c r="AJ16" s="134"/>
       <c r="AK16" s="84"/>
     </row>
     <row r="17" spans="1:37" ht="25.5" customHeight="1">
       <c r="A17" s="83"/>
-      <c r="B17" s="119" t="s">
+      <c r="B17" s="132" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -4183,7 +4183,7 @@
       <c r="Q17" s="101"/>
       <c r="R17" s="104"/>
       <c r="S17" s="27"/>
-      <c r="T17" s="119" t="s">
+      <c r="T17" s="132" t="s">
         <v>19</v>
       </c>
       <c r="U17" s="65"/>
@@ -4206,7 +4206,7 @@
     </row>
     <row r="18" spans="1:37" ht="37.5" customHeight="1" thickBot="1">
       <c r="A18" s="83"/>
-      <c r="B18" s="120"/>
+      <c r="B18" s="133"/>
       <c r="C18" s="6" t="s">
         <v>4</v>
       </c>
@@ -4228,7 +4228,7 @@
       <c r="Q18" s="100"/>
       <c r="R18" s="106"/>
       <c r="S18" s="27"/>
-      <c r="T18" s="122"/>
+      <c r="T18" s="135"/>
       <c r="U18" s="70"/>
       <c r="V18" s="27"/>
       <c r="W18" s="71"/>
@@ -4249,7 +4249,7 @@
     </row>
     <row r="19" spans="1:37" ht="25.5" customHeight="1" thickBot="1">
       <c r="A19" s="83"/>
-      <c r="B19" s="119" t="s">
+      <c r="B19" s="132" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="5" t="s">
@@ -4271,28 +4271,28 @@
       <c r="Q19" s="101"/>
       <c r="R19" s="104"/>
       <c r="S19" s="27"/>
-      <c r="T19" s="120"/>
+      <c r="T19" s="133"/>
       <c r="U19" s="43"/>
       <c r="V19" s="25"/>
       <c r="W19" s="25"/>
       <c r="X19" s="25"/>
-      <c r="Y19" s="127"/>
-      <c r="Z19" s="127"/>
-      <c r="AA19" s="127"/>
-      <c r="AB19" s="127"/>
-      <c r="AC19" s="127"/>
-      <c r="AD19" s="127"/>
-      <c r="AE19" s="127"/>
-      <c r="AF19" s="127"/>
-      <c r="AG19" s="127"/>
-      <c r="AH19" s="127"/>
-      <c r="AI19" s="127"/>
+      <c r="Y19" s="121"/>
+      <c r="Z19" s="121"/>
+      <c r="AA19" s="121"/>
+      <c r="AB19" s="121"/>
+      <c r="AC19" s="121"/>
+      <c r="AD19" s="121"/>
+      <c r="AE19" s="121"/>
+      <c r="AF19" s="121"/>
+      <c r="AG19" s="121"/>
+      <c r="AH19" s="121"/>
+      <c r="AI19" s="121"/>
       <c r="AJ19" s="24"/>
       <c r="AK19" s="84"/>
     </row>
     <row r="20" spans="1:37" ht="37.5" customHeight="1" thickBot="1">
       <c r="A20" s="83"/>
-      <c r="B20" s="120"/>
+      <c r="B20" s="133"/>
       <c r="C20" s="6" t="s">
         <v>4</v>
       </c>
@@ -4462,13 +4462,13 @@
       <c r="I24" s="28"/>
       <c r="J24" s="28"/>
       <c r="K24" s="28"/>
-      <c r="L24" s="143" t="s">
+      <c r="L24" s="131" t="s">
         <v>25</v>
       </c>
-      <c r="M24" s="143"/>
-      <c r="N24" s="143"/>
-      <c r="O24" s="143"/>
-      <c r="P24" s="143"/>
+      <c r="M24" s="131"/>
+      <c r="N24" s="131"/>
+      <c r="O24" s="131"/>
+      <c r="P24" s="131"/>
       <c r="Q24" s="29" t="s">
         <v>31</v>
       </c>
@@ -4614,12 +4614,12 @@
     </row>
     <row r="28" spans="1:37" ht="11.25" customHeight="1">
       <c r="A28" s="83"/>
-      <c r="B28" s="115" t="s">
+      <c r="B28" s="140" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="116"/>
-      <c r="D28" s="116"/>
-      <c r="E28" s="117"/>
+      <c r="C28" s="141"/>
+      <c r="D28" s="141"/>
+      <c r="E28" s="142"/>
       <c r="F28" s="114"/>
       <c r="G28" s="114"/>
       <c r="H28" s="114"/>
@@ -4733,12 +4733,12 @@
     </row>
     <row r="31" spans="1:37" ht="11.25" customHeight="1">
       <c r="A31" s="83"/>
-      <c r="B31" s="115" t="s">
+      <c r="B31" s="140" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="116"/>
-      <c r="D31" s="116"/>
-      <c r="E31" s="116"/>
+      <c r="C31" s="141"/>
+      <c r="D31" s="141"/>
+      <c r="E31" s="141"/>
       <c r="F31" s="114"/>
       <c r="G31" s="114"/>
       <c r="H31" s="114"/>
@@ -4852,12 +4852,12 @@
     </row>
     <row r="34" spans="1:37" ht="11.25" customHeight="1">
       <c r="A34" s="83"/>
-      <c r="B34" s="115" t="s">
+      <c r="B34" s="140" t="s">
         <v>11</v>
       </c>
-      <c r="C34" s="116"/>
-      <c r="D34" s="116"/>
-      <c r="E34" s="116"/>
+      <c r="C34" s="141"/>
+      <c r="D34" s="141"/>
+      <c r="E34" s="141"/>
       <c r="F34" s="114"/>
       <c r="G34" s="114"/>
       <c r="H34" s="114"/>
@@ -4869,7 +4869,7 @@
       <c r="N34" s="114"/>
       <c r="O34" s="114"/>
       <c r="P34" s="114"/>
-      <c r="Q34" s="118" t="s">
+      <c r="Q34" s="143" t="s">
         <v>6</v>
       </c>
       <c r="R34" s="40"/>
@@ -4910,7 +4910,7 @@
       <c r="N35" s="114"/>
       <c r="O35" s="114"/>
       <c r="P35" s="114"/>
-      <c r="Q35" s="118"/>
+      <c r="Q35" s="143"/>
       <c r="R35" s="40"/>
       <c r="S35" s="27"/>
       <c r="T35" s="27"/>
@@ -4975,12 +4975,12 @@
     </row>
     <row r="37" spans="1:37" ht="11.25" customHeight="1">
       <c r="A37" s="83"/>
-      <c r="B37" s="115" t="s">
+      <c r="B37" s="140" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="116"/>
-      <c r="D37" s="116"/>
-      <c r="E37" s="117"/>
+      <c r="C37" s="141"/>
+      <c r="D37" s="141"/>
+      <c r="E37" s="142"/>
       <c r="F37" s="114"/>
       <c r="G37" s="114"/>
       <c r="H37" s="114"/>
@@ -5254,6 +5254,22 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="F36:Q38"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="F27:Q29"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="F30:Q32"/>
+    <mergeCell ref="F33:P35"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="Q34:Q35"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="T16:AJ16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="T17:T19"/>
+    <mergeCell ref="B6:AK8"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="Y19:AI19"/>
     <mergeCell ref="F25:J26"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="T11:U12"/>
@@ -5263,22 +5279,6 @@
     <mergeCell ref="AF2:AH2"/>
     <mergeCell ref="AI2:AK2"/>
     <mergeCell ref="L24:P24"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="T16:AJ16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="T17:T19"/>
-    <mergeCell ref="B6:AK8"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="Y19:AI19"/>
-    <mergeCell ref="F36:Q38"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="F27:Q29"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="F30:Q32"/>
-    <mergeCell ref="F33:P35"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="Q34:Q35"/>
-    <mergeCell ref="B31:E31"/>
   </mergeCells>
   <phoneticPr fontId="15"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
hoant2 : fix bug 003 20190929
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/ローマ字氏名届_帳票テンプレート.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/ローマ字氏名届_帳票テンプレート.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F589028E-CF44-4771-8AB0-0C9BE660F004}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE43FAE3-320C-4635-9FDA-D0A80CFBD005}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1531,6 +1531,45 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1549,9 +1588,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1580,42 +1616,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1640,15 +1640,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>147313</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>15125</xdr:rowOff>
+      <xdr:colOff>292988</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>463360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>286869</xdr:colOff>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>235323</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>34739</xdr:rowOff>
+      <xdr:rowOff>1121</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1663,8 +1663,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6232107" y="6536949"/>
-          <a:ext cx="6045056" cy="2215966"/>
+          <a:off x="6377782" y="6503331"/>
+          <a:ext cx="6195217" cy="2215966"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3482,7 +3482,7 @@
   </sheetPr>
   <dimension ref="A1:AL43"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="55" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="55" workbookViewId="0">
       <selection activeCell="Y37" sqref="Y37"/>
     </sheetView>
   </sheetViews>
@@ -3526,11 +3526,11 @@
       <c r="AC1" s="27"/>
       <c r="AD1" s="27"/>
       <c r="AE1" s="27"/>
-      <c r="AI1" s="115">
+      <c r="AI1" s="128">
         <v>72073</v>
       </c>
-      <c r="AJ1" s="115"/>
-      <c r="AK1" s="115"/>
+      <c r="AJ1" s="128"/>
+      <c r="AK1" s="128"/>
       <c r="AL1" s="27"/>
     </row>
     <row r="2" spans="1:38" ht="26.25" customHeight="1">
@@ -3565,16 +3565,16 @@
       <c r="AC2" s="27"/>
       <c r="AD2" s="27"/>
       <c r="AE2" s="27"/>
-      <c r="AF2" s="127" t="s">
+      <c r="AF2" s="139" t="s">
         <v>23</v>
       </c>
-      <c r="AG2" s="128"/>
-      <c r="AH2" s="129"/>
-      <c r="AI2" s="130" t="s">
+      <c r="AG2" s="140"/>
+      <c r="AH2" s="141"/>
+      <c r="AI2" s="142" t="s">
         <v>24</v>
       </c>
-      <c r="AJ2" s="128"/>
-      <c r="AK2" s="129"/>
+      <c r="AJ2" s="140"/>
+      <c r="AK2" s="141"/>
       <c r="AL2" s="27"/>
     </row>
     <row r="3" spans="1:38" ht="26.25" customHeight="1">
@@ -3698,122 +3698,122 @@
     </row>
     <row r="6" spans="1:38" ht="13.5" customHeight="1">
       <c r="A6" s="82"/>
-      <c r="B6" s="136" t="s">
+      <c r="B6" s="123" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="136"/>
-      <c r="D6" s="136"/>
-      <c r="E6" s="136"/>
-      <c r="F6" s="136"/>
-      <c r="G6" s="136"/>
-      <c r="H6" s="136"/>
-      <c r="I6" s="136"/>
-      <c r="J6" s="136"/>
-      <c r="K6" s="136"/>
-      <c r="L6" s="136"/>
-      <c r="M6" s="136"/>
-      <c r="N6" s="136"/>
-      <c r="O6" s="136"/>
-      <c r="P6" s="136"/>
-      <c r="Q6" s="136"/>
-      <c r="R6" s="136"/>
-      <c r="S6" s="136"/>
-      <c r="T6" s="136"/>
-      <c r="U6" s="136"/>
-      <c r="V6" s="136"/>
-      <c r="W6" s="136"/>
-      <c r="X6" s="136"/>
-      <c r="Y6" s="136"/>
-      <c r="Z6" s="136"/>
-      <c r="AA6" s="136"/>
-      <c r="AB6" s="136"/>
-      <c r="AC6" s="136"/>
-      <c r="AD6" s="136"/>
-      <c r="AE6" s="136"/>
-      <c r="AF6" s="136"/>
-      <c r="AG6" s="136"/>
-      <c r="AH6" s="136"/>
-      <c r="AI6" s="136"/>
-      <c r="AJ6" s="136"/>
-      <c r="AK6" s="137"/>
+      <c r="C6" s="123"/>
+      <c r="D6" s="123"/>
+      <c r="E6" s="123"/>
+      <c r="F6" s="123"/>
+      <c r="G6" s="123"/>
+      <c r="H6" s="123"/>
+      <c r="I6" s="123"/>
+      <c r="J6" s="123"/>
+      <c r="K6" s="123"/>
+      <c r="L6" s="123"/>
+      <c r="M6" s="123"/>
+      <c r="N6" s="123"/>
+      <c r="O6" s="123"/>
+      <c r="P6" s="123"/>
+      <c r="Q6" s="123"/>
+      <c r="R6" s="123"/>
+      <c r="S6" s="123"/>
+      <c r="T6" s="123"/>
+      <c r="U6" s="123"/>
+      <c r="V6" s="123"/>
+      <c r="W6" s="123"/>
+      <c r="X6" s="123"/>
+      <c r="Y6" s="123"/>
+      <c r="Z6" s="123"/>
+      <c r="AA6" s="123"/>
+      <c r="AB6" s="123"/>
+      <c r="AC6" s="123"/>
+      <c r="AD6" s="123"/>
+      <c r="AE6" s="123"/>
+      <c r="AF6" s="123"/>
+      <c r="AG6" s="123"/>
+      <c r="AH6" s="123"/>
+      <c r="AI6" s="123"/>
+      <c r="AJ6" s="123"/>
+      <c r="AK6" s="124"/>
     </row>
     <row r="7" spans="1:38" ht="13.5" customHeight="1">
       <c r="A7" s="83"/>
-      <c r="B7" s="138"/>
-      <c r="C7" s="138"/>
-      <c r="D7" s="138"/>
-      <c r="E7" s="138"/>
-      <c r="F7" s="138"/>
-      <c r="G7" s="138"/>
-      <c r="H7" s="138"/>
-      <c r="I7" s="138"/>
-      <c r="J7" s="138"/>
-      <c r="K7" s="138"/>
-      <c r="L7" s="138"/>
-      <c r="M7" s="138"/>
-      <c r="N7" s="138"/>
-      <c r="O7" s="138"/>
-      <c r="P7" s="138"/>
-      <c r="Q7" s="138"/>
-      <c r="R7" s="138"/>
-      <c r="S7" s="138"/>
-      <c r="T7" s="138"/>
-      <c r="U7" s="138"/>
-      <c r="V7" s="138"/>
-      <c r="W7" s="138"/>
-      <c r="X7" s="138"/>
-      <c r="Y7" s="138"/>
-      <c r="Z7" s="138"/>
-      <c r="AA7" s="138"/>
-      <c r="AB7" s="138"/>
-      <c r="AC7" s="138"/>
-      <c r="AD7" s="138"/>
-      <c r="AE7" s="138"/>
-      <c r="AF7" s="138"/>
-      <c r="AG7" s="138"/>
-      <c r="AH7" s="138"/>
-      <c r="AI7" s="138"/>
-      <c r="AJ7" s="138"/>
-      <c r="AK7" s="139"/>
+      <c r="B7" s="125"/>
+      <c r="C7" s="125"/>
+      <c r="D7" s="125"/>
+      <c r="E7" s="125"/>
+      <c r="F7" s="125"/>
+      <c r="G7" s="125"/>
+      <c r="H7" s="125"/>
+      <c r="I7" s="125"/>
+      <c r="J7" s="125"/>
+      <c r="K7" s="125"/>
+      <c r="L7" s="125"/>
+      <c r="M7" s="125"/>
+      <c r="N7" s="125"/>
+      <c r="O7" s="125"/>
+      <c r="P7" s="125"/>
+      <c r="Q7" s="125"/>
+      <c r="R7" s="125"/>
+      <c r="S7" s="125"/>
+      <c r="T7" s="125"/>
+      <c r="U7" s="125"/>
+      <c r="V7" s="125"/>
+      <c r="W7" s="125"/>
+      <c r="X7" s="125"/>
+      <c r="Y7" s="125"/>
+      <c r="Z7" s="125"/>
+      <c r="AA7" s="125"/>
+      <c r="AB7" s="125"/>
+      <c r="AC7" s="125"/>
+      <c r="AD7" s="125"/>
+      <c r="AE7" s="125"/>
+      <c r="AF7" s="125"/>
+      <c r="AG7" s="125"/>
+      <c r="AH7" s="125"/>
+      <c r="AI7" s="125"/>
+      <c r="AJ7" s="125"/>
+      <c r="AK7" s="126"/>
     </row>
     <row r="8" spans="1:38" ht="13.5" customHeight="1">
       <c r="A8" s="83"/>
-      <c r="B8" s="138"/>
-      <c r="C8" s="138"/>
-      <c r="D8" s="138"/>
-      <c r="E8" s="138"/>
-      <c r="F8" s="138"/>
-      <c r="G8" s="138"/>
-      <c r="H8" s="138"/>
-      <c r="I8" s="138"/>
-      <c r="J8" s="138"/>
-      <c r="K8" s="138"/>
-      <c r="L8" s="138"/>
-      <c r="M8" s="138"/>
-      <c r="N8" s="138"/>
-      <c r="O8" s="138"/>
-      <c r="P8" s="138"/>
-      <c r="Q8" s="138"/>
-      <c r="R8" s="138"/>
-      <c r="S8" s="138"/>
-      <c r="T8" s="138"/>
-      <c r="U8" s="138"/>
-      <c r="V8" s="138"/>
-      <c r="W8" s="138"/>
-      <c r="X8" s="138"/>
-      <c r="Y8" s="138"/>
-      <c r="Z8" s="138"/>
-      <c r="AA8" s="138"/>
-      <c r="AB8" s="138"/>
-      <c r="AC8" s="138"/>
-      <c r="AD8" s="138"/>
-      <c r="AE8" s="138"/>
-      <c r="AF8" s="138"/>
-      <c r="AG8" s="138"/>
-      <c r="AH8" s="138"/>
-      <c r="AI8" s="138"/>
-      <c r="AJ8" s="138"/>
-      <c r="AK8" s="139"/>
+      <c r="B8" s="125"/>
+      <c r="C8" s="125"/>
+      <c r="D8" s="125"/>
+      <c r="E8" s="125"/>
+      <c r="F8" s="125"/>
+      <c r="G8" s="125"/>
+      <c r="H8" s="125"/>
+      <c r="I8" s="125"/>
+      <c r="J8" s="125"/>
+      <c r="K8" s="125"/>
+      <c r="L8" s="125"/>
+      <c r="M8" s="125"/>
+      <c r="N8" s="125"/>
+      <c r="O8" s="125"/>
+      <c r="P8" s="125"/>
+      <c r="Q8" s="125"/>
+      <c r="R8" s="125"/>
+      <c r="S8" s="125"/>
+      <c r="T8" s="125"/>
+      <c r="U8" s="125"/>
+      <c r="V8" s="125"/>
+      <c r="W8" s="125"/>
+      <c r="X8" s="125"/>
+      <c r="Y8" s="125"/>
+      <c r="Z8" s="125"/>
+      <c r="AA8" s="125"/>
+      <c r="AB8" s="125"/>
+      <c r="AC8" s="125"/>
+      <c r="AD8" s="125"/>
+      <c r="AE8" s="125"/>
+      <c r="AF8" s="125"/>
+      <c r="AG8" s="125"/>
+      <c r="AH8" s="125"/>
+      <c r="AI8" s="125"/>
+      <c r="AJ8" s="125"/>
+      <c r="AK8" s="126"/>
     </row>
     <row r="9" spans="1:38" ht="18.75" customHeight="1">
       <c r="A9" s="83"/>
@@ -3929,27 +3929,27 @@
       <c r="S11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="T11" s="116" t="s">
+      <c r="T11" s="129" t="s">
         <v>27</v>
       </c>
-      <c r="U11" s="117"/>
-      <c r="V11" s="116" t="s">
+      <c r="U11" s="130"/>
+      <c r="V11" s="129" t="s">
         <v>18</v>
       </c>
-      <c r="W11" s="120"/>
-      <c r="X11" s="120"/>
-      <c r="Y11" s="120"/>
-      <c r="Z11" s="117"/>
-      <c r="AA11" s="122"/>
-      <c r="AB11" s="123"/>
-      <c r="AC11" s="123"/>
-      <c r="AD11" s="123"/>
-      <c r="AE11" s="123"/>
-      <c r="AF11" s="126"/>
-      <c r="AG11" s="123"/>
-      <c r="AH11" s="123"/>
-      <c r="AI11" s="123"/>
-      <c r="AJ11" s="123"/>
+      <c r="W11" s="133"/>
+      <c r="X11" s="133"/>
+      <c r="Y11" s="133"/>
+      <c r="Z11" s="130"/>
+      <c r="AA11" s="134"/>
+      <c r="AB11" s="135"/>
+      <c r="AC11" s="135"/>
+      <c r="AD11" s="135"/>
+      <c r="AE11" s="135"/>
+      <c r="AF11" s="138"/>
+      <c r="AG11" s="135"/>
+      <c r="AH11" s="135"/>
+      <c r="AI11" s="135"/>
+      <c r="AJ11" s="135"/>
       <c r="AK11" s="84"/>
     </row>
     <row r="12" spans="1:38" ht="40.5" customHeight="1" thickBot="1">
@@ -3972,23 +3972,23 @@
       <c r="Q12" s="57"/>
       <c r="R12" s="58"/>
       <c r="S12" s="50"/>
-      <c r="T12" s="118"/>
-      <c r="U12" s="119"/>
-      <c r="V12" s="118"/>
-      <c r="W12" s="121"/>
-      <c r="X12" s="121"/>
-      <c r="Y12" s="121"/>
-      <c r="Z12" s="119"/>
-      <c r="AA12" s="124"/>
-      <c r="AB12" s="125"/>
-      <c r="AC12" s="125"/>
-      <c r="AD12" s="125"/>
-      <c r="AE12" s="125"/>
-      <c r="AF12" s="125"/>
-      <c r="AG12" s="125"/>
-      <c r="AH12" s="125"/>
-      <c r="AI12" s="125"/>
-      <c r="AJ12" s="125"/>
+      <c r="T12" s="131"/>
+      <c r="U12" s="132"/>
+      <c r="V12" s="131"/>
+      <c r="W12" s="127"/>
+      <c r="X12" s="127"/>
+      <c r="Y12" s="127"/>
+      <c r="Z12" s="132"/>
+      <c r="AA12" s="136"/>
+      <c r="AB12" s="137"/>
+      <c r="AC12" s="137"/>
+      <c r="AD12" s="137"/>
+      <c r="AE12" s="137"/>
+      <c r="AF12" s="137"/>
+      <c r="AG12" s="137"/>
+      <c r="AH12" s="137"/>
+      <c r="AI12" s="137"/>
+      <c r="AJ12" s="137"/>
       <c r="AK12" s="84"/>
     </row>
     <row r="13" spans="1:38" ht="23.25" customHeight="1" thickBot="1">
@@ -4034,7 +4034,7 @@
     </row>
     <row r="14" spans="1:38" ht="25.5" customHeight="1">
       <c r="A14" s="83"/>
-      <c r="B14" s="132" t="s">
+      <c r="B14" s="119" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -4077,7 +4077,7 @@
     </row>
     <row r="15" spans="1:38" ht="60.75" customHeight="1" thickBot="1">
       <c r="A15" s="83"/>
-      <c r="B15" s="133"/>
+      <c r="B15" s="120"/>
       <c r="C15" s="6" t="s">
         <v>30</v>
       </c>
@@ -4138,30 +4138,30 @@
       <c r="Q16" s="64"/>
       <c r="R16" s="64"/>
       <c r="S16" s="64"/>
-      <c r="T16" s="134" t="s">
+      <c r="T16" s="121" t="s">
         <v>29</v>
       </c>
-      <c r="U16" s="134"/>
-      <c r="V16" s="134"/>
-      <c r="W16" s="134"/>
-      <c r="X16" s="134"/>
-      <c r="Y16" s="134"/>
-      <c r="Z16" s="134"/>
-      <c r="AA16" s="134"/>
-      <c r="AB16" s="134"/>
-      <c r="AC16" s="134"/>
-      <c r="AD16" s="134"/>
-      <c r="AE16" s="134"/>
-      <c r="AF16" s="134"/>
-      <c r="AG16" s="134"/>
-      <c r="AH16" s="134"/>
-      <c r="AI16" s="134"/>
-      <c r="AJ16" s="134"/>
+      <c r="U16" s="121"/>
+      <c r="V16" s="121"/>
+      <c r="W16" s="121"/>
+      <c r="X16" s="121"/>
+      <c r="Y16" s="121"/>
+      <c r="Z16" s="121"/>
+      <c r="AA16" s="121"/>
+      <c r="AB16" s="121"/>
+      <c r="AC16" s="121"/>
+      <c r="AD16" s="121"/>
+      <c r="AE16" s="121"/>
+      <c r="AF16" s="121"/>
+      <c r="AG16" s="121"/>
+      <c r="AH16" s="121"/>
+      <c r="AI16" s="121"/>
+      <c r="AJ16" s="121"/>
       <c r="AK16" s="84"/>
     </row>
     <row r="17" spans="1:37" ht="25.5" customHeight="1">
       <c r="A17" s="83"/>
-      <c r="B17" s="132" t="s">
+      <c r="B17" s="119" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -4183,7 +4183,7 @@
       <c r="Q17" s="101"/>
       <c r="R17" s="104"/>
       <c r="S17" s="27"/>
-      <c r="T17" s="132" t="s">
+      <c r="T17" s="119" t="s">
         <v>19</v>
       </c>
       <c r="U17" s="65"/>
@@ -4206,7 +4206,7 @@
     </row>
     <row r="18" spans="1:37" ht="37.5" customHeight="1" thickBot="1">
       <c r="A18" s="83"/>
-      <c r="B18" s="133"/>
+      <c r="B18" s="120"/>
       <c r="C18" s="6" t="s">
         <v>4</v>
       </c>
@@ -4228,7 +4228,7 @@
       <c r="Q18" s="100"/>
       <c r="R18" s="106"/>
       <c r="S18" s="27"/>
-      <c r="T18" s="135"/>
+      <c r="T18" s="122"/>
       <c r="U18" s="70"/>
       <c r="V18" s="27"/>
       <c r="W18" s="71"/>
@@ -4249,7 +4249,7 @@
     </row>
     <row r="19" spans="1:37" ht="25.5" customHeight="1" thickBot="1">
       <c r="A19" s="83"/>
-      <c r="B19" s="132" t="s">
+      <c r="B19" s="119" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="5" t="s">
@@ -4271,28 +4271,28 @@
       <c r="Q19" s="101"/>
       <c r="R19" s="104"/>
       <c r="S19" s="27"/>
-      <c r="T19" s="133"/>
+      <c r="T19" s="120"/>
       <c r="U19" s="43"/>
       <c r="V19" s="25"/>
       <c r="W19" s="25"/>
       <c r="X19" s="25"/>
-      <c r="Y19" s="121"/>
-      <c r="Z19" s="121"/>
-      <c r="AA19" s="121"/>
-      <c r="AB19" s="121"/>
-      <c r="AC19" s="121"/>
-      <c r="AD19" s="121"/>
-      <c r="AE19" s="121"/>
-      <c r="AF19" s="121"/>
-      <c r="AG19" s="121"/>
-      <c r="AH19" s="121"/>
-      <c r="AI19" s="121"/>
+      <c r="Y19" s="127"/>
+      <c r="Z19" s="127"/>
+      <c r="AA19" s="127"/>
+      <c r="AB19" s="127"/>
+      <c r="AC19" s="127"/>
+      <c r="AD19" s="127"/>
+      <c r="AE19" s="127"/>
+      <c r="AF19" s="127"/>
+      <c r="AG19" s="127"/>
+      <c r="AH19" s="127"/>
+      <c r="AI19" s="127"/>
       <c r="AJ19" s="24"/>
       <c r="AK19" s="84"/>
     </row>
     <row r="20" spans="1:37" ht="37.5" customHeight="1" thickBot="1">
       <c r="A20" s="83"/>
-      <c r="B20" s="133"/>
+      <c r="B20" s="120"/>
       <c r="C20" s="6" t="s">
         <v>4</v>
       </c>
@@ -4462,13 +4462,13 @@
       <c r="I24" s="28"/>
       <c r="J24" s="28"/>
       <c r="K24" s="28"/>
-      <c r="L24" s="131" t="s">
+      <c r="L24" s="143" t="s">
         <v>25</v>
       </c>
-      <c r="M24" s="131"/>
-      <c r="N24" s="131"/>
-      <c r="O24" s="131"/>
-      <c r="P24" s="131"/>
+      <c r="M24" s="143"/>
+      <c r="N24" s="143"/>
+      <c r="O24" s="143"/>
+      <c r="P24" s="143"/>
       <c r="Q24" s="29" t="s">
         <v>31</v>
       </c>
@@ -4614,12 +4614,12 @@
     </row>
     <row r="28" spans="1:37" ht="11.25" customHeight="1">
       <c r="A28" s="83"/>
-      <c r="B28" s="140" t="s">
+      <c r="B28" s="115" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="141"/>
-      <c r="D28" s="141"/>
-      <c r="E28" s="142"/>
+      <c r="C28" s="116"/>
+      <c r="D28" s="116"/>
+      <c r="E28" s="117"/>
       <c r="F28" s="114"/>
       <c r="G28" s="114"/>
       <c r="H28" s="114"/>
@@ -4733,12 +4733,12 @@
     </row>
     <row r="31" spans="1:37" ht="11.25" customHeight="1">
       <c r="A31" s="83"/>
-      <c r="B31" s="140" t="s">
+      <c r="B31" s="115" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="141"/>
-      <c r="D31" s="141"/>
-      <c r="E31" s="141"/>
+      <c r="C31" s="116"/>
+      <c r="D31" s="116"/>
+      <c r="E31" s="116"/>
       <c r="F31" s="114"/>
       <c r="G31" s="114"/>
       <c r="H31" s="114"/>
@@ -4852,12 +4852,12 @@
     </row>
     <row r="34" spans="1:37" ht="11.25" customHeight="1">
       <c r="A34" s="83"/>
-      <c r="B34" s="140" t="s">
+      <c r="B34" s="115" t="s">
         <v>11</v>
       </c>
-      <c r="C34" s="141"/>
-      <c r="D34" s="141"/>
-      <c r="E34" s="141"/>
+      <c r="C34" s="116"/>
+      <c r="D34" s="116"/>
+      <c r="E34" s="116"/>
       <c r="F34" s="114"/>
       <c r="G34" s="114"/>
       <c r="H34" s="114"/>
@@ -4869,7 +4869,7 @@
       <c r="N34" s="114"/>
       <c r="O34" s="114"/>
       <c r="P34" s="114"/>
-      <c r="Q34" s="143" t="s">
+      <c r="Q34" s="118" t="s">
         <v>6</v>
       </c>
       <c r="R34" s="40"/>
@@ -4910,7 +4910,7 @@
       <c r="N35" s="114"/>
       <c r="O35" s="114"/>
       <c r="P35" s="114"/>
-      <c r="Q35" s="143"/>
+      <c r="Q35" s="118"/>
       <c r="R35" s="40"/>
       <c r="S35" s="27"/>
       <c r="T35" s="27"/>
@@ -4975,12 +4975,12 @@
     </row>
     <row r="37" spans="1:37" ht="11.25" customHeight="1">
       <c r="A37" s="83"/>
-      <c r="B37" s="140" t="s">
+      <c r="B37" s="115" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="141"/>
-      <c r="D37" s="141"/>
-      <c r="E37" s="142"/>
+      <c r="C37" s="116"/>
+      <c r="D37" s="116"/>
+      <c r="E37" s="117"/>
       <c r="F37" s="114"/>
       <c r="G37" s="114"/>
       <c r="H37" s="114"/>
@@ -5254,6 +5254,22 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="F25:J26"/>
+    <mergeCell ref="AI1:AK1"/>
+    <mergeCell ref="T11:U12"/>
+    <mergeCell ref="V11:Z12"/>
+    <mergeCell ref="AA11:AE12"/>
+    <mergeCell ref="AF11:AJ12"/>
+    <mergeCell ref="AF2:AH2"/>
+    <mergeCell ref="AI2:AK2"/>
+    <mergeCell ref="L24:P24"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="T16:AJ16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="T17:T19"/>
+    <mergeCell ref="B6:AK8"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="Y19:AI19"/>
     <mergeCell ref="F36:Q38"/>
     <mergeCell ref="B37:E37"/>
     <mergeCell ref="F27:Q29"/>
@@ -5263,22 +5279,6 @@
     <mergeCell ref="B34:E34"/>
     <mergeCell ref="Q34:Q35"/>
     <mergeCell ref="B31:E31"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="T16:AJ16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="T17:T19"/>
-    <mergeCell ref="B6:AK8"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="Y19:AI19"/>
-    <mergeCell ref="F25:J26"/>
-    <mergeCell ref="AI1:AK1"/>
-    <mergeCell ref="T11:U12"/>
-    <mergeCell ref="V11:Z12"/>
-    <mergeCell ref="AA11:AE12"/>
-    <mergeCell ref="AF11:AJ12"/>
-    <mergeCell ref="AF2:AH2"/>
-    <mergeCell ref="AI2:AK2"/>
-    <mergeCell ref="L24:P24"/>
   </mergeCells>
   <phoneticPr fontId="15"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
hoa.nt2 : commit code 013
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/ローマ字氏名届_帳票テンプレート.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/ローマ字氏名届_帳票テンプレート.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE43FAE3-320C-4635-9FDA-D0A80CFBD005}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C2847C4-FA5E-4AE4-A787-2663A3FAD39A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1531,6 +1531,81 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="center" indent="1"/>
     </xf>
@@ -1541,81 +1616,6 @@
       <alignment horizontal="distributed" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1700,7 +1700,7 @@
             </a:lnSpc>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050">
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -1710,7 +1710,7 @@
             <a:t>【</a:t>
           </a:r>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1050">
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -1720,7 +1720,7 @@
             <a:t>記入上の注意</a:t>
           </a:r>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050">
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -1749,7 +1749,7 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1050">
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -1778,7 +1778,7 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1050">
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -1807,7 +1807,7 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1050">
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -1836,7 +1836,7 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1050">
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -1865,7 +1865,7 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1050">
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -1874,7 +1874,7 @@
             </a:rPr>
             <a:t>　　　氏名欄」に被保険者資格取得届等に記載したカナ氏名を記入のうえ、「理由記入欄」に その理由</a:t>
           </a:r>
-          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050">
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900">
             <a:solidFill>
               <a:sysClr val="windowText" lastClr="000000"/>
             </a:solidFill>
@@ -1901,7 +1901,7 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1050">
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -1930,7 +1930,7 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1050">
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -2000,7 +2000,7 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1050" baseline="0">
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -2012,7 +2012,7 @@
             <a:t>　</a:t>
           </a:r>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="1050" baseline="0">
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="900" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -2023,7 +2023,7 @@
             </a:rPr>
             <a:t>□短期在留者であるため</a:t>
           </a:r>
-          <a:endParaRPr lang="ja-JP" altLang="ja-JP" sz="1050">
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP" sz="900">
             <a:solidFill>
               <a:sysClr val="windowText" lastClr="000000"/>
             </a:solidFill>
@@ -2032,7 +2032,7 @@
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1050" baseline="0">
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -2043,7 +2043,7 @@
             </a:rPr>
             <a:t>　□海外に住所を有している者であるため</a:t>
           </a:r>
-          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" baseline="0">
             <a:solidFill>
               <a:sysClr val="windowText" lastClr="000000"/>
             </a:solidFill>
@@ -2055,7 +2055,7 @@
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1050" baseline="0">
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -2067,7 +2067,7 @@
             <a:t>　</a:t>
           </a:r>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="1050" baseline="0">
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="900" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -2079,7 +2079,7 @@
             <a:t>□在留カード</a:t>
           </a:r>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1050" baseline="0">
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -2091,7 +2091,7 @@
             <a:t>（または特別永住者証明書）</a:t>
           </a:r>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="1050" baseline="0">
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="900" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -2102,7 +2102,7 @@
             </a:rPr>
             <a:t>にローマ字氏名が記載されていないため</a:t>
           </a:r>
-          <a:endParaRPr lang="ja-JP" altLang="ja-JP" sz="1050">
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP" sz="900">
             <a:solidFill>
               <a:sysClr val="windowText" lastClr="000000"/>
             </a:solidFill>
@@ -2111,7 +2111,7 @@
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1050">
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -2123,7 +2123,7 @@
             <a:t>　</a:t>
           </a:r>
           <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="1050">
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="900">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -2134,7 +2134,7 @@
             </a:rPr>
             <a:t>□その他　理由（　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　          　）</a:t>
           </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1050">
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
             <a:solidFill>
               <a:sysClr val="windowText" lastClr="000000"/>
             </a:solidFill>
@@ -3482,8 +3482,8 @@
   </sheetPr>
   <dimension ref="A1:AL43"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="Y37" sqref="Y37"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="55" workbookViewId="0">
+      <selection activeCell="U32" sqref="U32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.140625" defaultRowHeight="15"/>
@@ -3526,11 +3526,11 @@
       <c r="AC1" s="27"/>
       <c r="AD1" s="27"/>
       <c r="AE1" s="27"/>
-      <c r="AI1" s="128">
+      <c r="AI1" s="115">
         <v>72073</v>
       </c>
-      <c r="AJ1" s="128"/>
-      <c r="AK1" s="128"/>
+      <c r="AJ1" s="115"/>
+      <c r="AK1" s="115"/>
       <c r="AL1" s="27"/>
     </row>
     <row r="2" spans="1:38" ht="26.25" customHeight="1">
@@ -3565,16 +3565,16 @@
       <c r="AC2" s="27"/>
       <c r="AD2" s="27"/>
       <c r="AE2" s="27"/>
-      <c r="AF2" s="139" t="s">
+      <c r="AF2" s="127" t="s">
         <v>23</v>
       </c>
-      <c r="AG2" s="140"/>
-      <c r="AH2" s="141"/>
-      <c r="AI2" s="142" t="s">
+      <c r="AG2" s="128"/>
+      <c r="AH2" s="129"/>
+      <c r="AI2" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="AJ2" s="140"/>
-      <c r="AK2" s="141"/>
+      <c r="AJ2" s="128"/>
+      <c r="AK2" s="129"/>
       <c r="AL2" s="27"/>
     </row>
     <row r="3" spans="1:38" ht="26.25" customHeight="1">
@@ -3698,122 +3698,122 @@
     </row>
     <row r="6" spans="1:38" ht="13.5" customHeight="1">
       <c r="A6" s="82"/>
-      <c r="B6" s="123" t="s">
+      <c r="B6" s="136" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="123"/>
-      <c r="D6" s="123"/>
-      <c r="E6" s="123"/>
-      <c r="F6" s="123"/>
-      <c r="G6" s="123"/>
-      <c r="H6" s="123"/>
-      <c r="I6" s="123"/>
-      <c r="J6" s="123"/>
-      <c r="K6" s="123"/>
-      <c r="L6" s="123"/>
-      <c r="M6" s="123"/>
-      <c r="N6" s="123"/>
-      <c r="O6" s="123"/>
-      <c r="P6" s="123"/>
-      <c r="Q6" s="123"/>
-      <c r="R6" s="123"/>
-      <c r="S6" s="123"/>
-      <c r="T6" s="123"/>
-      <c r="U6" s="123"/>
-      <c r="V6" s="123"/>
-      <c r="W6" s="123"/>
-      <c r="X6" s="123"/>
-      <c r="Y6" s="123"/>
-      <c r="Z6" s="123"/>
-      <c r="AA6" s="123"/>
-      <c r="AB6" s="123"/>
-      <c r="AC6" s="123"/>
-      <c r="AD6" s="123"/>
-      <c r="AE6" s="123"/>
-      <c r="AF6" s="123"/>
-      <c r="AG6" s="123"/>
-      <c r="AH6" s="123"/>
-      <c r="AI6" s="123"/>
-      <c r="AJ6" s="123"/>
-      <c r="AK6" s="124"/>
+      <c r="C6" s="136"/>
+      <c r="D6" s="136"/>
+      <c r="E6" s="136"/>
+      <c r="F6" s="136"/>
+      <c r="G6" s="136"/>
+      <c r="H6" s="136"/>
+      <c r="I6" s="136"/>
+      <c r="J6" s="136"/>
+      <c r="K6" s="136"/>
+      <c r="L6" s="136"/>
+      <c r="M6" s="136"/>
+      <c r="N6" s="136"/>
+      <c r="O6" s="136"/>
+      <c r="P6" s="136"/>
+      <c r="Q6" s="136"/>
+      <c r="R6" s="136"/>
+      <c r="S6" s="136"/>
+      <c r="T6" s="136"/>
+      <c r="U6" s="136"/>
+      <c r="V6" s="136"/>
+      <c r="W6" s="136"/>
+      <c r="X6" s="136"/>
+      <c r="Y6" s="136"/>
+      <c r="Z6" s="136"/>
+      <c r="AA6" s="136"/>
+      <c r="AB6" s="136"/>
+      <c r="AC6" s="136"/>
+      <c r="AD6" s="136"/>
+      <c r="AE6" s="136"/>
+      <c r="AF6" s="136"/>
+      <c r="AG6" s="136"/>
+      <c r="AH6" s="136"/>
+      <c r="AI6" s="136"/>
+      <c r="AJ6" s="136"/>
+      <c r="AK6" s="137"/>
     </row>
     <row r="7" spans="1:38" ht="13.5" customHeight="1">
       <c r="A7" s="83"/>
-      <c r="B7" s="125"/>
-      <c r="C7" s="125"/>
-      <c r="D7" s="125"/>
-      <c r="E7" s="125"/>
-      <c r="F7" s="125"/>
-      <c r="G7" s="125"/>
-      <c r="H7" s="125"/>
-      <c r="I7" s="125"/>
-      <c r="J7" s="125"/>
-      <c r="K7" s="125"/>
-      <c r="L7" s="125"/>
-      <c r="M7" s="125"/>
-      <c r="N7" s="125"/>
-      <c r="O7" s="125"/>
-      <c r="P7" s="125"/>
-      <c r="Q7" s="125"/>
-      <c r="R7" s="125"/>
-      <c r="S7" s="125"/>
-      <c r="T7" s="125"/>
-      <c r="U7" s="125"/>
-      <c r="V7" s="125"/>
-      <c r="W7" s="125"/>
-      <c r="X7" s="125"/>
-      <c r="Y7" s="125"/>
-      <c r="Z7" s="125"/>
-      <c r="AA7" s="125"/>
-      <c r="AB7" s="125"/>
-      <c r="AC7" s="125"/>
-      <c r="AD7" s="125"/>
-      <c r="AE7" s="125"/>
-      <c r="AF7" s="125"/>
-      <c r="AG7" s="125"/>
-      <c r="AH7" s="125"/>
-      <c r="AI7" s="125"/>
-      <c r="AJ7" s="125"/>
-      <c r="AK7" s="126"/>
+      <c r="B7" s="138"/>
+      <c r="C7" s="138"/>
+      <c r="D7" s="138"/>
+      <c r="E7" s="138"/>
+      <c r="F7" s="138"/>
+      <c r="G7" s="138"/>
+      <c r="H7" s="138"/>
+      <c r="I7" s="138"/>
+      <c r="J7" s="138"/>
+      <c r="K7" s="138"/>
+      <c r="L7" s="138"/>
+      <c r="M7" s="138"/>
+      <c r="N7" s="138"/>
+      <c r="O7" s="138"/>
+      <c r="P7" s="138"/>
+      <c r="Q7" s="138"/>
+      <c r="R7" s="138"/>
+      <c r="S7" s="138"/>
+      <c r="T7" s="138"/>
+      <c r="U7" s="138"/>
+      <c r="V7" s="138"/>
+      <c r="W7" s="138"/>
+      <c r="X7" s="138"/>
+      <c r="Y7" s="138"/>
+      <c r="Z7" s="138"/>
+      <c r="AA7" s="138"/>
+      <c r="AB7" s="138"/>
+      <c r="AC7" s="138"/>
+      <c r="AD7" s="138"/>
+      <c r="AE7" s="138"/>
+      <c r="AF7" s="138"/>
+      <c r="AG7" s="138"/>
+      <c r="AH7" s="138"/>
+      <c r="AI7" s="138"/>
+      <c r="AJ7" s="138"/>
+      <c r="AK7" s="139"/>
     </row>
     <row r="8" spans="1:38" ht="13.5" customHeight="1">
       <c r="A8" s="83"/>
-      <c r="B8" s="125"/>
-      <c r="C8" s="125"/>
-      <c r="D8" s="125"/>
-      <c r="E8" s="125"/>
-      <c r="F8" s="125"/>
-      <c r="G8" s="125"/>
-      <c r="H8" s="125"/>
-      <c r="I8" s="125"/>
-      <c r="J8" s="125"/>
-      <c r="K8" s="125"/>
-      <c r="L8" s="125"/>
-      <c r="M8" s="125"/>
-      <c r="N8" s="125"/>
-      <c r="O8" s="125"/>
-      <c r="P8" s="125"/>
-      <c r="Q8" s="125"/>
-      <c r="R8" s="125"/>
-      <c r="S8" s="125"/>
-      <c r="T8" s="125"/>
-      <c r="U8" s="125"/>
-      <c r="V8" s="125"/>
-      <c r="W8" s="125"/>
-      <c r="X8" s="125"/>
-      <c r="Y8" s="125"/>
-      <c r="Z8" s="125"/>
-      <c r="AA8" s="125"/>
-      <c r="AB8" s="125"/>
-      <c r="AC8" s="125"/>
-      <c r="AD8" s="125"/>
-      <c r="AE8" s="125"/>
-      <c r="AF8" s="125"/>
-      <c r="AG8" s="125"/>
-      <c r="AH8" s="125"/>
-      <c r="AI8" s="125"/>
-      <c r="AJ8" s="125"/>
-      <c r="AK8" s="126"/>
+      <c r="B8" s="138"/>
+      <c r="C8" s="138"/>
+      <c r="D8" s="138"/>
+      <c r="E8" s="138"/>
+      <c r="F8" s="138"/>
+      <c r="G8" s="138"/>
+      <c r="H8" s="138"/>
+      <c r="I8" s="138"/>
+      <c r="J8" s="138"/>
+      <c r="K8" s="138"/>
+      <c r="L8" s="138"/>
+      <c r="M8" s="138"/>
+      <c r="N8" s="138"/>
+      <c r="O8" s="138"/>
+      <c r="P8" s="138"/>
+      <c r="Q8" s="138"/>
+      <c r="R8" s="138"/>
+      <c r="S8" s="138"/>
+      <c r="T8" s="138"/>
+      <c r="U8" s="138"/>
+      <c r="V8" s="138"/>
+      <c r="W8" s="138"/>
+      <c r="X8" s="138"/>
+      <c r="Y8" s="138"/>
+      <c r="Z8" s="138"/>
+      <c r="AA8" s="138"/>
+      <c r="AB8" s="138"/>
+      <c r="AC8" s="138"/>
+      <c r="AD8" s="138"/>
+      <c r="AE8" s="138"/>
+      <c r="AF8" s="138"/>
+      <c r="AG8" s="138"/>
+      <c r="AH8" s="138"/>
+      <c r="AI8" s="138"/>
+      <c r="AJ8" s="138"/>
+      <c r="AK8" s="139"/>
     </row>
     <row r="9" spans="1:38" ht="18.75" customHeight="1">
       <c r="A9" s="83"/>
@@ -3929,27 +3929,27 @@
       <c r="S11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="T11" s="129" t="s">
+      <c r="T11" s="116" t="s">
         <v>27</v>
       </c>
-      <c r="U11" s="130"/>
-      <c r="V11" s="129" t="s">
+      <c r="U11" s="117"/>
+      <c r="V11" s="116" t="s">
         <v>18</v>
       </c>
-      <c r="W11" s="133"/>
-      <c r="X11" s="133"/>
-      <c r="Y11" s="133"/>
-      <c r="Z11" s="130"/>
-      <c r="AA11" s="134"/>
-      <c r="AB11" s="135"/>
-      <c r="AC11" s="135"/>
-      <c r="AD11" s="135"/>
-      <c r="AE11" s="135"/>
-      <c r="AF11" s="138"/>
-      <c r="AG11" s="135"/>
-      <c r="AH11" s="135"/>
-      <c r="AI11" s="135"/>
-      <c r="AJ11" s="135"/>
+      <c r="W11" s="120"/>
+      <c r="X11" s="120"/>
+      <c r="Y11" s="120"/>
+      <c r="Z11" s="117"/>
+      <c r="AA11" s="122"/>
+      <c r="AB11" s="123"/>
+      <c r="AC11" s="123"/>
+      <c r="AD11" s="123"/>
+      <c r="AE11" s="123"/>
+      <c r="AF11" s="126"/>
+      <c r="AG11" s="123"/>
+      <c r="AH11" s="123"/>
+      <c r="AI11" s="123"/>
+      <c r="AJ11" s="123"/>
       <c r="AK11" s="84"/>
     </row>
     <row r="12" spans="1:38" ht="40.5" customHeight="1" thickBot="1">
@@ -3972,23 +3972,23 @@
       <c r="Q12" s="57"/>
       <c r="R12" s="58"/>
       <c r="S12" s="50"/>
-      <c r="T12" s="131"/>
-      <c r="U12" s="132"/>
-      <c r="V12" s="131"/>
-      <c r="W12" s="127"/>
-      <c r="X12" s="127"/>
-      <c r="Y12" s="127"/>
-      <c r="Z12" s="132"/>
-      <c r="AA12" s="136"/>
-      <c r="AB12" s="137"/>
-      <c r="AC12" s="137"/>
-      <c r="AD12" s="137"/>
-      <c r="AE12" s="137"/>
-      <c r="AF12" s="137"/>
-      <c r="AG12" s="137"/>
-      <c r="AH12" s="137"/>
-      <c r="AI12" s="137"/>
-      <c r="AJ12" s="137"/>
+      <c r="T12" s="118"/>
+      <c r="U12" s="119"/>
+      <c r="V12" s="118"/>
+      <c r="W12" s="121"/>
+      <c r="X12" s="121"/>
+      <c r="Y12" s="121"/>
+      <c r="Z12" s="119"/>
+      <c r="AA12" s="124"/>
+      <c r="AB12" s="125"/>
+      <c r="AC12" s="125"/>
+      <c r="AD12" s="125"/>
+      <c r="AE12" s="125"/>
+      <c r="AF12" s="125"/>
+      <c r="AG12" s="125"/>
+      <c r="AH12" s="125"/>
+      <c r="AI12" s="125"/>
+      <c r="AJ12" s="125"/>
       <c r="AK12" s="84"/>
     </row>
     <row r="13" spans="1:38" ht="23.25" customHeight="1" thickBot="1">
@@ -4034,7 +4034,7 @@
     </row>
     <row r="14" spans="1:38" ht="25.5" customHeight="1">
       <c r="A14" s="83"/>
-      <c r="B14" s="119" t="s">
+      <c r="B14" s="132" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -4077,7 +4077,7 @@
     </row>
     <row r="15" spans="1:38" ht="60.75" customHeight="1" thickBot="1">
       <c r="A15" s="83"/>
-      <c r="B15" s="120"/>
+      <c r="B15" s="133"/>
       <c r="C15" s="6" t="s">
         <v>30</v>
       </c>
@@ -4138,30 +4138,30 @@
       <c r="Q16" s="64"/>
       <c r="R16" s="64"/>
       <c r="S16" s="64"/>
-      <c r="T16" s="121" t="s">
+      <c r="T16" s="134" t="s">
         <v>29</v>
       </c>
-      <c r="U16" s="121"/>
-      <c r="V16" s="121"/>
-      <c r="W16" s="121"/>
-      <c r="X16" s="121"/>
-      <c r="Y16" s="121"/>
-      <c r="Z16" s="121"/>
-      <c r="AA16" s="121"/>
-      <c r="AB16" s="121"/>
-      <c r="AC16" s="121"/>
-      <c r="AD16" s="121"/>
-      <c r="AE16" s="121"/>
-      <c r="AF16" s="121"/>
-      <c r="AG16" s="121"/>
-      <c r="AH16" s="121"/>
-      <c r="AI16" s="121"/>
-      <c r="AJ16" s="121"/>
+      <c r="U16" s="134"/>
+      <c r="V16" s="134"/>
+      <c r="W16" s="134"/>
+      <c r="X16" s="134"/>
+      <c r="Y16" s="134"/>
+      <c r="Z16" s="134"/>
+      <c r="AA16" s="134"/>
+      <c r="AB16" s="134"/>
+      <c r="AC16" s="134"/>
+      <c r="AD16" s="134"/>
+      <c r="AE16" s="134"/>
+      <c r="AF16" s="134"/>
+      <c r="AG16" s="134"/>
+      <c r="AH16" s="134"/>
+      <c r="AI16" s="134"/>
+      <c r="AJ16" s="134"/>
       <c r="AK16" s="84"/>
     </row>
     <row r="17" spans="1:37" ht="25.5" customHeight="1">
       <c r="A17" s="83"/>
-      <c r="B17" s="119" t="s">
+      <c r="B17" s="132" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -4183,7 +4183,7 @@
       <c r="Q17" s="101"/>
       <c r="R17" s="104"/>
       <c r="S17" s="27"/>
-      <c r="T17" s="119" t="s">
+      <c r="T17" s="132" t="s">
         <v>19</v>
       </c>
       <c r="U17" s="65"/>
@@ -4206,7 +4206,7 @@
     </row>
     <row r="18" spans="1:37" ht="37.5" customHeight="1" thickBot="1">
       <c r="A18" s="83"/>
-      <c r="B18" s="120"/>
+      <c r="B18" s="133"/>
       <c r="C18" s="6" t="s">
         <v>4</v>
       </c>
@@ -4228,7 +4228,7 @@
       <c r="Q18" s="100"/>
       <c r="R18" s="106"/>
       <c r="S18" s="27"/>
-      <c r="T18" s="122"/>
+      <c r="T18" s="135"/>
       <c r="U18" s="70"/>
       <c r="V18" s="27"/>
       <c r="W18" s="71"/>
@@ -4249,7 +4249,7 @@
     </row>
     <row r="19" spans="1:37" ht="25.5" customHeight="1" thickBot="1">
       <c r="A19" s="83"/>
-      <c r="B19" s="119" t="s">
+      <c r="B19" s="132" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="5" t="s">
@@ -4271,28 +4271,28 @@
       <c r="Q19" s="101"/>
       <c r="R19" s="104"/>
       <c r="S19" s="27"/>
-      <c r="T19" s="120"/>
+      <c r="T19" s="133"/>
       <c r="U19" s="43"/>
       <c r="V19" s="25"/>
       <c r="W19" s="25"/>
       <c r="X19" s="25"/>
-      <c r="Y19" s="127"/>
-      <c r="Z19" s="127"/>
-      <c r="AA19" s="127"/>
-      <c r="AB19" s="127"/>
-      <c r="AC19" s="127"/>
-      <c r="AD19" s="127"/>
-      <c r="AE19" s="127"/>
-      <c r="AF19" s="127"/>
-      <c r="AG19" s="127"/>
-      <c r="AH19" s="127"/>
-      <c r="AI19" s="127"/>
+      <c r="Y19" s="121"/>
+      <c r="Z19" s="121"/>
+      <c r="AA19" s="121"/>
+      <c r="AB19" s="121"/>
+      <c r="AC19" s="121"/>
+      <c r="AD19" s="121"/>
+      <c r="AE19" s="121"/>
+      <c r="AF19" s="121"/>
+      <c r="AG19" s="121"/>
+      <c r="AH19" s="121"/>
+      <c r="AI19" s="121"/>
       <c r="AJ19" s="24"/>
       <c r="AK19" s="84"/>
     </row>
     <row r="20" spans="1:37" ht="37.5" customHeight="1" thickBot="1">
       <c r="A20" s="83"/>
-      <c r="B20" s="120"/>
+      <c r="B20" s="133"/>
       <c r="C20" s="6" t="s">
         <v>4</v>
       </c>
@@ -4462,13 +4462,13 @@
       <c r="I24" s="28"/>
       <c r="J24" s="28"/>
       <c r="K24" s="28"/>
-      <c r="L24" s="143" t="s">
+      <c r="L24" s="131" t="s">
         <v>25</v>
       </c>
-      <c r="M24" s="143"/>
-      <c r="N24" s="143"/>
-      <c r="O24" s="143"/>
-      <c r="P24" s="143"/>
+      <c r="M24" s="131"/>
+      <c r="N24" s="131"/>
+      <c r="O24" s="131"/>
+      <c r="P24" s="131"/>
       <c r="Q24" s="29" t="s">
         <v>31</v>
       </c>
@@ -4614,12 +4614,12 @@
     </row>
     <row r="28" spans="1:37" ht="11.25" customHeight="1">
       <c r="A28" s="83"/>
-      <c r="B28" s="115" t="s">
+      <c r="B28" s="140" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="116"/>
-      <c r="D28" s="116"/>
-      <c r="E28" s="117"/>
+      <c r="C28" s="141"/>
+      <c r="D28" s="141"/>
+      <c r="E28" s="142"/>
       <c r="F28" s="114"/>
       <c r="G28" s="114"/>
       <c r="H28" s="114"/>
@@ -4733,12 +4733,12 @@
     </row>
     <row r="31" spans="1:37" ht="11.25" customHeight="1">
       <c r="A31" s="83"/>
-      <c r="B31" s="115" t="s">
+      <c r="B31" s="140" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="116"/>
-      <c r="D31" s="116"/>
-      <c r="E31" s="116"/>
+      <c r="C31" s="141"/>
+      <c r="D31" s="141"/>
+      <c r="E31" s="141"/>
       <c r="F31" s="114"/>
       <c r="G31" s="114"/>
       <c r="H31" s="114"/>
@@ -4852,12 +4852,12 @@
     </row>
     <row r="34" spans="1:37" ht="11.25" customHeight="1">
       <c r="A34" s="83"/>
-      <c r="B34" s="115" t="s">
+      <c r="B34" s="140" t="s">
         <v>11</v>
       </c>
-      <c r="C34" s="116"/>
-      <c r="D34" s="116"/>
-      <c r="E34" s="116"/>
+      <c r="C34" s="141"/>
+      <c r="D34" s="141"/>
+      <c r="E34" s="141"/>
       <c r="F34" s="114"/>
       <c r="G34" s="114"/>
       <c r="H34" s="114"/>
@@ -4869,7 +4869,7 @@
       <c r="N34" s="114"/>
       <c r="O34" s="114"/>
       <c r="P34" s="114"/>
-      <c r="Q34" s="118" t="s">
+      <c r="Q34" s="143" t="s">
         <v>6</v>
       </c>
       <c r="R34" s="40"/>
@@ -4910,7 +4910,7 @@
       <c r="N35" s="114"/>
       <c r="O35" s="114"/>
       <c r="P35" s="114"/>
-      <c r="Q35" s="118"/>
+      <c r="Q35" s="143"/>
       <c r="R35" s="40"/>
       <c r="S35" s="27"/>
       <c r="T35" s="27"/>
@@ -4975,12 +4975,12 @@
     </row>
     <row r="37" spans="1:37" ht="11.25" customHeight="1">
       <c r="A37" s="83"/>
-      <c r="B37" s="115" t="s">
+      <c r="B37" s="140" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="116"/>
-      <c r="D37" s="116"/>
-      <c r="E37" s="117"/>
+      <c r="C37" s="141"/>
+      <c r="D37" s="141"/>
+      <c r="E37" s="142"/>
       <c r="F37" s="114"/>
       <c r="G37" s="114"/>
       <c r="H37" s="114"/>
@@ -5254,6 +5254,22 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="F36:Q38"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="F27:Q29"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="F30:Q32"/>
+    <mergeCell ref="F33:P35"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="Q34:Q35"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="T16:AJ16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="T17:T19"/>
+    <mergeCell ref="B6:AK8"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="Y19:AI19"/>
     <mergeCell ref="F25:J26"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="T11:U12"/>
@@ -5263,22 +5279,6 @@
     <mergeCell ref="AF2:AH2"/>
     <mergeCell ref="AI2:AK2"/>
     <mergeCell ref="L24:P24"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="T16:AJ16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="T17:T19"/>
-    <mergeCell ref="B6:AK8"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="Y19:AI19"/>
-    <mergeCell ref="F36:Q38"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="F27:Q29"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="F30:Q32"/>
-    <mergeCell ref="F33:P35"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="Q34:Q35"/>
-    <mergeCell ref="B31:E31"/>
   </mergeCells>
   <phoneticPr fontId="15"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
hoant2 : comit code  fix kcp009
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/ローマ字氏名届_帳票テンプレート.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/ローマ字氏名届_帳票テンプレート.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA3BAFB8-A076-4AAF-9583-D6265B831A42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E3372E-FBFC-47BE-9750-6330D78BB96A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8BC8B0BF-E0AC-4C73-B25B-BE8089E69E19}"/>
   </bookViews>
   <sheets>
     <sheet name="2号" sheetId="14" r:id="rId1"/>
@@ -1563,9 +1563,54 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1584,9 +1629,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1616,48 +1658,6 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1706,8 +1706,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="8641292" y="8149167"/>
-          <a:ext cx="3563408" cy="463550"/>
+          <a:off x="8743950" y="8067675"/>
+          <a:ext cx="3609975" cy="447675"/>
           <a:chOff x="7124700" y="4981575"/>
           <a:chExt cx="2486025" cy="447675"/>
         </a:xfrm>
@@ -2189,8 +2189,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6521824" y="2588559"/>
-          <a:ext cx="257735" cy="190500"/>
+          <a:off x="6365565" y="2616574"/>
+          <a:ext cx="249018" cy="191744"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -2255,8 +2255,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6539753" y="2976283"/>
-          <a:ext cx="257735" cy="190500"/>
+          <a:off x="6383494" y="3005542"/>
+          <a:ext cx="249018" cy="190500"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -2321,8 +2321,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7734301" y="2602007"/>
-          <a:ext cx="257735" cy="190500"/>
+          <a:off x="7551894" y="2630022"/>
+          <a:ext cx="249019" cy="191744"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -2387,8 +2387,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7741025" y="2989730"/>
-          <a:ext cx="257735" cy="190500"/>
+          <a:off x="7558618" y="3018989"/>
+          <a:ext cx="249019" cy="190500"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -2430,369 +2430,309 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
+      <xdr:colOff>74085</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>168088</xdr:rowOff>
+      <xdr:rowOff>125754</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>34783</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>54355</xdr:rowOff>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>113243</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="23" name="A4_1">
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="6" name="Group 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C9977B7-AA7F-4696-999B-B5E8D06D9AEB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61AC5E13-898E-4E17-968B-E162CAC1C1B5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6970059" y="5076264"/>
-          <a:ext cx="191665" cy="211238"/>
+          <a:off x="6770160" y="5050179"/>
+          <a:ext cx="5525558" cy="1061696"/>
+          <a:chOff x="6688668" y="5078754"/>
+          <a:chExt cx="5457825" cy="1070163"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" cmpd="sng">
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="4" name="Group 3">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D2F1006-3A11-4E88-9E12-329095E9C098}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="6784537" y="5078754"/>
+            <a:ext cx="192912" cy="785103"/>
+            <a:chOff x="7027954" y="5089337"/>
+            <a:chExt cx="192912" cy="785103"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="23" name="A4_1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C9977B7-AA7F-4696-999B-B5E8D06D9AEB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7037916" y="5089337"/>
+              <a:ext cx="182950" cy="214350"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525" cmpd="sng">
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+                <a:t>✔</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="24" name="A4_2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E09B4BD-93B9-4795-878E-5C14966939AB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7034058" y="5277846"/>
+              <a:ext cx="182950" cy="211238"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525" cmpd="sng">
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+                <a:t>✔</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="25" name="A4_3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EBA8CF8-BD88-4077-91ED-EDBAF2DD8411}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7027954" y="5503331"/>
+              <a:ext cx="182950" cy="211238"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525" cmpd="sng">
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+                <a:t>✔</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="26" name="A4_4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34A15B02-F4A5-49CF-902E-ED0944041168}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7034680" y="5668805"/>
+              <a:ext cx="182950" cy="205635"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525" cmpd="sng">
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+                <a:t>✔</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="31" name="TextBox 30">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6734B847-95FE-49FA-AD58-A200A9A59A7B}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6688668" y="5101168"/>
+            <a:ext cx="5457825" cy="1047749"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
           <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-            <a:t>✔</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>197224</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>17929</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>41507</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>229167</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="24" name="A4_2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E09B4BD-93B9-4795-878E-5C14966939AB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6976783" y="5251076"/>
-          <a:ext cx="191665" cy="211238"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-            <a:t>✔</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>201706</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>45989</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>401738</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="25" name="A4_3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EBA8CF8-BD88-4077-91ED-EDBAF2DD8411}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6981265" y="5423647"/>
-          <a:ext cx="191665" cy="211238"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-            <a:t>✔</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>208430</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>387723</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>52713</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>117108</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="26" name="A4_4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34A15B02-F4A5-49CF-902E-ED0944041168}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6987989" y="5620870"/>
-          <a:ext cx="191665" cy="211238"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-            <a:t>✔</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>247650</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="184731" cy="264560"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0BA5F49-7D4B-4528-B273-CD18407A080B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6981825" y="5172075"/>
-          <a:ext cx="184731" cy="264560"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>102054</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>142874</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1713098" cy="275717"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="TextBox 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{482535D7-FE7B-4D73-A8A1-15C2D573BDE9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6749143" y="5055053"/>
-          <a:ext cx="1713098" cy="275717"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" baseline="0">
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>□ 短期在留者であるため</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -2800,333 +2740,175 @@
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>□ 短期在留者であるため</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>□ 海外に住所 を有している者であるため</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>□ 在留カード</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" sz="1100" b="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>（または特別永住者証明書） にローマ字氏名が記載されていないため</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>□ </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>その他　理由（          　</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>				</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>）</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
     <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>104776</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>2721</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="2629887" cy="275717"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="28" name="TextBox 27">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1ECE7316-ADD2-44B8-8574-246DB9D53F66}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6751865" y="5241471"/>
-          <a:ext cx="2629887" cy="275717"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>□ 海外に住所 を有している者であるため</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>107492</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>189141</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="5123710" cy="275717"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="29" name="TextBox 28">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B0F3E95-9E7D-4E97-9C0F-C01BB5076477}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6754581" y="5427891"/>
-          <a:ext cx="5123710" cy="275717"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>□ 在留カード</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" sz="1100" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>（または特別永住者証明書） にローマ字氏名が記載されていないため</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" b="0">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>103408</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>375559</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="5182968" cy="275717"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="30" name="TextBox 29">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94D65DAE-CD44-4365-AF3E-0D1A30380E5C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6750497" y="5614309"/>
-          <a:ext cx="5182968" cy="275717"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>□ </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>その他　理由（          　</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>				</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>）</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" b="0">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3456,8 +3238,8 @@
   </sheetPr>
   <dimension ref="A1:AL43"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A15" zoomScale="90" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="X20" sqref="X20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.140625" defaultRowHeight="15"/>
@@ -3500,11 +3282,11 @@
       <c r="AC1" s="27"/>
       <c r="AD1" s="27"/>
       <c r="AE1" s="27"/>
-      <c r="AI1" s="117">
+      <c r="AI1" s="132">
         <v>72073</v>
       </c>
-      <c r="AJ1" s="117"/>
-      <c r="AK1" s="117"/>
+      <c r="AJ1" s="132"/>
+      <c r="AK1" s="132"/>
       <c r="AL1" s="27"/>
     </row>
     <row r="2" spans="1:38" ht="26.25" customHeight="1">
@@ -3539,16 +3321,16 @@
       <c r="AC2" s="27"/>
       <c r="AD2" s="27"/>
       <c r="AE2" s="27"/>
-      <c r="AF2" s="129" t="s">
+      <c r="AF2" s="143" t="s">
         <v>23</v>
       </c>
-      <c r="AG2" s="130"/>
-      <c r="AH2" s="131"/>
-      <c r="AI2" s="132" t="s">
+      <c r="AG2" s="144"/>
+      <c r="AH2" s="145"/>
+      <c r="AI2" s="146" t="s">
         <v>24</v>
       </c>
-      <c r="AJ2" s="130"/>
-      <c r="AK2" s="131"/>
+      <c r="AJ2" s="144"/>
+      <c r="AK2" s="145"/>
       <c r="AL2" s="27"/>
     </row>
     <row r="3" spans="1:38" ht="26.25" customHeight="1">
@@ -3672,122 +3454,122 @@
     </row>
     <row r="6" spans="1:38" ht="13.5" customHeight="1">
       <c r="A6" s="82"/>
-      <c r="B6" s="138" t="s">
+      <c r="B6" s="127" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="138"/>
-      <c r="D6" s="138"/>
-      <c r="E6" s="138"/>
-      <c r="F6" s="138"/>
-      <c r="G6" s="138"/>
-      <c r="H6" s="138"/>
-      <c r="I6" s="138"/>
-      <c r="J6" s="138"/>
-      <c r="K6" s="138"/>
-      <c r="L6" s="138"/>
-      <c r="M6" s="138"/>
-      <c r="N6" s="138"/>
-      <c r="O6" s="138"/>
-      <c r="P6" s="138"/>
-      <c r="Q6" s="138"/>
-      <c r="R6" s="138"/>
-      <c r="S6" s="138"/>
-      <c r="T6" s="138"/>
-      <c r="U6" s="138"/>
-      <c r="V6" s="138"/>
-      <c r="W6" s="138"/>
-      <c r="X6" s="138"/>
-      <c r="Y6" s="138"/>
-      <c r="Z6" s="138"/>
-      <c r="AA6" s="138"/>
-      <c r="AB6" s="138"/>
-      <c r="AC6" s="138"/>
-      <c r="AD6" s="138"/>
-      <c r="AE6" s="138"/>
-      <c r="AF6" s="138"/>
-      <c r="AG6" s="138"/>
-      <c r="AH6" s="138"/>
-      <c r="AI6" s="138"/>
-      <c r="AJ6" s="138"/>
-      <c r="AK6" s="139"/>
+      <c r="C6" s="127"/>
+      <c r="D6" s="127"/>
+      <c r="E6" s="127"/>
+      <c r="F6" s="127"/>
+      <c r="G6" s="127"/>
+      <c r="H6" s="127"/>
+      <c r="I6" s="127"/>
+      <c r="J6" s="127"/>
+      <c r="K6" s="127"/>
+      <c r="L6" s="127"/>
+      <c r="M6" s="127"/>
+      <c r="N6" s="127"/>
+      <c r="O6" s="127"/>
+      <c r="P6" s="127"/>
+      <c r="Q6" s="127"/>
+      <c r="R6" s="127"/>
+      <c r="S6" s="127"/>
+      <c r="T6" s="127"/>
+      <c r="U6" s="127"/>
+      <c r="V6" s="127"/>
+      <c r="W6" s="127"/>
+      <c r="X6" s="127"/>
+      <c r="Y6" s="127"/>
+      <c r="Z6" s="127"/>
+      <c r="AA6" s="127"/>
+      <c r="AB6" s="127"/>
+      <c r="AC6" s="127"/>
+      <c r="AD6" s="127"/>
+      <c r="AE6" s="127"/>
+      <c r="AF6" s="127"/>
+      <c r="AG6" s="127"/>
+      <c r="AH6" s="127"/>
+      <c r="AI6" s="127"/>
+      <c r="AJ6" s="127"/>
+      <c r="AK6" s="128"/>
     </row>
     <row r="7" spans="1:38" ht="13.5" customHeight="1">
       <c r="A7" s="83"/>
-      <c r="B7" s="140"/>
-      <c r="C7" s="140"/>
-      <c r="D7" s="140"/>
-      <c r="E7" s="140"/>
-      <c r="F7" s="140"/>
-      <c r="G7" s="140"/>
-      <c r="H7" s="140"/>
-      <c r="I7" s="140"/>
-      <c r="J7" s="140"/>
-      <c r="K7" s="140"/>
-      <c r="L7" s="140"/>
-      <c r="M7" s="140"/>
-      <c r="N7" s="140"/>
-      <c r="O7" s="140"/>
-      <c r="P7" s="140"/>
-      <c r="Q7" s="140"/>
-      <c r="R7" s="140"/>
-      <c r="S7" s="140"/>
-      <c r="T7" s="140"/>
-      <c r="U7" s="140"/>
-      <c r="V7" s="140"/>
-      <c r="W7" s="140"/>
-      <c r="X7" s="140"/>
-      <c r="Y7" s="140"/>
-      <c r="Z7" s="140"/>
-      <c r="AA7" s="140"/>
-      <c r="AB7" s="140"/>
-      <c r="AC7" s="140"/>
-      <c r="AD7" s="140"/>
-      <c r="AE7" s="140"/>
-      <c r="AF7" s="140"/>
-      <c r="AG7" s="140"/>
-      <c r="AH7" s="140"/>
-      <c r="AI7" s="140"/>
-      <c r="AJ7" s="140"/>
-      <c r="AK7" s="141"/>
+      <c r="B7" s="129"/>
+      <c r="C7" s="129"/>
+      <c r="D7" s="129"/>
+      <c r="E7" s="129"/>
+      <c r="F7" s="129"/>
+      <c r="G7" s="129"/>
+      <c r="H7" s="129"/>
+      <c r="I7" s="129"/>
+      <c r="J7" s="129"/>
+      <c r="K7" s="129"/>
+      <c r="L7" s="129"/>
+      <c r="M7" s="129"/>
+      <c r="N7" s="129"/>
+      <c r="O7" s="129"/>
+      <c r="P7" s="129"/>
+      <c r="Q7" s="129"/>
+      <c r="R7" s="129"/>
+      <c r="S7" s="129"/>
+      <c r="T7" s="129"/>
+      <c r="U7" s="129"/>
+      <c r="V7" s="129"/>
+      <c r="W7" s="129"/>
+      <c r="X7" s="129"/>
+      <c r="Y7" s="129"/>
+      <c r="Z7" s="129"/>
+      <c r="AA7" s="129"/>
+      <c r="AB7" s="129"/>
+      <c r="AC7" s="129"/>
+      <c r="AD7" s="129"/>
+      <c r="AE7" s="129"/>
+      <c r="AF7" s="129"/>
+      <c r="AG7" s="129"/>
+      <c r="AH7" s="129"/>
+      <c r="AI7" s="129"/>
+      <c r="AJ7" s="129"/>
+      <c r="AK7" s="130"/>
     </row>
     <row r="8" spans="1:38" ht="13.5" customHeight="1">
       <c r="A8" s="83"/>
-      <c r="B8" s="140"/>
-      <c r="C8" s="140"/>
-      <c r="D8" s="140"/>
-      <c r="E8" s="140"/>
-      <c r="F8" s="140"/>
-      <c r="G8" s="140"/>
-      <c r="H8" s="140"/>
-      <c r="I8" s="140"/>
-      <c r="J8" s="140"/>
-      <c r="K8" s="140"/>
-      <c r="L8" s="140"/>
-      <c r="M8" s="140"/>
-      <c r="N8" s="140"/>
-      <c r="O8" s="140"/>
-      <c r="P8" s="140"/>
-      <c r="Q8" s="140"/>
-      <c r="R8" s="140"/>
-      <c r="S8" s="140"/>
-      <c r="T8" s="140"/>
-      <c r="U8" s="140"/>
-      <c r="V8" s="140"/>
-      <c r="W8" s="140"/>
-      <c r="X8" s="140"/>
-      <c r="Y8" s="140"/>
-      <c r="Z8" s="140"/>
-      <c r="AA8" s="140"/>
-      <c r="AB8" s="140"/>
-      <c r="AC8" s="140"/>
-      <c r="AD8" s="140"/>
-      <c r="AE8" s="140"/>
-      <c r="AF8" s="140"/>
-      <c r="AG8" s="140"/>
-      <c r="AH8" s="140"/>
-      <c r="AI8" s="140"/>
-      <c r="AJ8" s="140"/>
-      <c r="AK8" s="141"/>
+      <c r="B8" s="129"/>
+      <c r="C8" s="129"/>
+      <c r="D8" s="129"/>
+      <c r="E8" s="129"/>
+      <c r="F8" s="129"/>
+      <c r="G8" s="129"/>
+      <c r="H8" s="129"/>
+      <c r="I8" s="129"/>
+      <c r="J8" s="129"/>
+      <c r="K8" s="129"/>
+      <c r="L8" s="129"/>
+      <c r="M8" s="129"/>
+      <c r="N8" s="129"/>
+      <c r="O8" s="129"/>
+      <c r="P8" s="129"/>
+      <c r="Q8" s="129"/>
+      <c r="R8" s="129"/>
+      <c r="S8" s="129"/>
+      <c r="T8" s="129"/>
+      <c r="U8" s="129"/>
+      <c r="V8" s="129"/>
+      <c r="W8" s="129"/>
+      <c r="X8" s="129"/>
+      <c r="Y8" s="129"/>
+      <c r="Z8" s="129"/>
+      <c r="AA8" s="129"/>
+      <c r="AB8" s="129"/>
+      <c r="AC8" s="129"/>
+      <c r="AD8" s="129"/>
+      <c r="AE8" s="129"/>
+      <c r="AF8" s="129"/>
+      <c r="AG8" s="129"/>
+      <c r="AH8" s="129"/>
+      <c r="AI8" s="129"/>
+      <c r="AJ8" s="129"/>
+      <c r="AK8" s="130"/>
     </row>
     <row r="9" spans="1:38" ht="18.75" customHeight="1">
       <c r="A9" s="83"/>
@@ -3903,27 +3685,27 @@
       <c r="S11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="T11" s="118" t="s">
+      <c r="T11" s="133" t="s">
         <v>27</v>
       </c>
-      <c r="U11" s="119"/>
-      <c r="V11" s="118" t="s">
+      <c r="U11" s="134"/>
+      <c r="V11" s="133" t="s">
         <v>18</v>
       </c>
-      <c r="W11" s="122"/>
-      <c r="X11" s="122"/>
-      <c r="Y11" s="122"/>
-      <c r="Z11" s="119"/>
-      <c r="AA11" s="124"/>
-      <c r="AB11" s="125"/>
-      <c r="AC11" s="125"/>
-      <c r="AD11" s="125"/>
-      <c r="AE11" s="125"/>
-      <c r="AF11" s="128"/>
-      <c r="AG11" s="125"/>
-      <c r="AH11" s="125"/>
-      <c r="AI11" s="125"/>
-      <c r="AJ11" s="125"/>
+      <c r="W11" s="137"/>
+      <c r="X11" s="137"/>
+      <c r="Y11" s="137"/>
+      <c r="Z11" s="134"/>
+      <c r="AA11" s="138"/>
+      <c r="AB11" s="139"/>
+      <c r="AC11" s="139"/>
+      <c r="AD11" s="139"/>
+      <c r="AE11" s="139"/>
+      <c r="AF11" s="142"/>
+      <c r="AG11" s="139"/>
+      <c r="AH11" s="139"/>
+      <c r="AI11" s="139"/>
+      <c r="AJ11" s="139"/>
       <c r="AK11" s="84"/>
     </row>
     <row r="12" spans="1:38" ht="40.5" customHeight="1" thickBot="1">
@@ -3946,23 +3728,23 @@
       <c r="Q12" s="57"/>
       <c r="R12" s="58"/>
       <c r="S12" s="50"/>
-      <c r="T12" s="120"/>
-      <c r="U12" s="121"/>
-      <c r="V12" s="120"/>
-      <c r="W12" s="123"/>
-      <c r="X12" s="123"/>
-      <c r="Y12" s="123"/>
-      <c r="Z12" s="121"/>
-      <c r="AA12" s="126"/>
-      <c r="AB12" s="127"/>
-      <c r="AC12" s="127"/>
-      <c r="AD12" s="127"/>
-      <c r="AE12" s="127"/>
-      <c r="AF12" s="127"/>
-      <c r="AG12" s="127"/>
-      <c r="AH12" s="127"/>
-      <c r="AI12" s="127"/>
-      <c r="AJ12" s="127"/>
+      <c r="T12" s="135"/>
+      <c r="U12" s="136"/>
+      <c r="V12" s="135"/>
+      <c r="W12" s="131"/>
+      <c r="X12" s="131"/>
+      <c r="Y12" s="131"/>
+      <c r="Z12" s="136"/>
+      <c r="AA12" s="140"/>
+      <c r="AB12" s="141"/>
+      <c r="AC12" s="141"/>
+      <c r="AD12" s="141"/>
+      <c r="AE12" s="141"/>
+      <c r="AF12" s="141"/>
+      <c r="AG12" s="141"/>
+      <c r="AH12" s="141"/>
+      <c r="AI12" s="141"/>
+      <c r="AJ12" s="141"/>
       <c r="AK12" s="84"/>
     </row>
     <row r="13" spans="1:38" ht="23.25" customHeight="1" thickBot="1">
@@ -4008,7 +3790,7 @@
     </row>
     <row r="14" spans="1:38" ht="25.5" customHeight="1">
       <c r="A14" s="83"/>
-      <c r="B14" s="134" t="s">
+      <c r="B14" s="123" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -4051,7 +3833,7 @@
     </row>
     <row r="15" spans="1:38" ht="60.75" customHeight="1" thickBot="1">
       <c r="A15" s="83"/>
-      <c r="B15" s="135"/>
+      <c r="B15" s="124"/>
       <c r="C15" s="6" t="s">
         <v>30</v>
       </c>
@@ -4112,30 +3894,30 @@
       <c r="Q16" s="64"/>
       <c r="R16" s="64"/>
       <c r="S16" s="64"/>
-      <c r="T16" s="136" t="s">
+      <c r="T16" s="125" t="s">
         <v>29</v>
       </c>
-      <c r="U16" s="136"/>
-      <c r="V16" s="136"/>
-      <c r="W16" s="136"/>
-      <c r="X16" s="136"/>
-      <c r="Y16" s="136"/>
-      <c r="Z16" s="136"/>
-      <c r="AA16" s="136"/>
-      <c r="AB16" s="136"/>
-      <c r="AC16" s="136"/>
-      <c r="AD16" s="136"/>
-      <c r="AE16" s="136"/>
-      <c r="AF16" s="136"/>
-      <c r="AG16" s="136"/>
-      <c r="AH16" s="136"/>
-      <c r="AI16" s="136"/>
-      <c r="AJ16" s="136"/>
+      <c r="U16" s="125"/>
+      <c r="V16" s="125"/>
+      <c r="W16" s="125"/>
+      <c r="X16" s="125"/>
+      <c r="Y16" s="125"/>
+      <c r="Z16" s="125"/>
+      <c r="AA16" s="125"/>
+      <c r="AB16" s="125"/>
+      <c r="AC16" s="125"/>
+      <c r="AD16" s="125"/>
+      <c r="AE16" s="125"/>
+      <c r="AF16" s="125"/>
+      <c r="AG16" s="125"/>
+      <c r="AH16" s="125"/>
+      <c r="AI16" s="125"/>
+      <c r="AJ16" s="125"/>
       <c r="AK16" s="84"/>
     </row>
     <row r="17" spans="1:37" ht="25.5" customHeight="1">
       <c r="A17" s="83"/>
-      <c r="B17" s="134" t="s">
+      <c r="B17" s="123" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -4157,7 +3939,7 @@
       <c r="Q17" s="101"/>
       <c r="R17" s="104"/>
       <c r="S17" s="27"/>
-      <c r="T17" s="134" t="s">
+      <c r="T17" s="123" t="s">
         <v>19</v>
       </c>
       <c r="U17" s="65"/>
@@ -4180,7 +3962,7 @@
     </row>
     <row r="18" spans="1:37" ht="37.5" customHeight="1" thickBot="1">
       <c r="A18" s="83"/>
-      <c r="B18" s="135"/>
+      <c r="B18" s="124"/>
       <c r="C18" s="6" t="s">
         <v>4</v>
       </c>
@@ -4202,7 +3984,7 @@
       <c r="Q18" s="100"/>
       <c r="R18" s="106"/>
       <c r="S18" s="27"/>
-      <c r="T18" s="137"/>
+      <c r="T18" s="126"/>
       <c r="U18" s="70"/>
       <c r="V18" s="27"/>
       <c r="W18" s="71"/>
@@ -4223,7 +4005,7 @@
     </row>
     <row r="19" spans="1:37" ht="25.5" customHeight="1" thickBot="1">
       <c r="A19" s="83"/>
-      <c r="B19" s="134" t="s">
+      <c r="B19" s="123" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="5" t="s">
@@ -4245,28 +4027,28 @@
       <c r="Q19" s="101"/>
       <c r="R19" s="104"/>
       <c r="S19" s="27"/>
-      <c r="T19" s="135"/>
+      <c r="T19" s="124"/>
       <c r="U19" s="43"/>
       <c r="V19" s="25"/>
       <c r="W19" s="25"/>
       <c r="X19" s="25"/>
-      <c r="Y19" s="123"/>
-      <c r="Z19" s="123"/>
-      <c r="AA19" s="123"/>
-      <c r="AB19" s="123"/>
-      <c r="AC19" s="123"/>
-      <c r="AD19" s="123"/>
-      <c r="AE19" s="123"/>
-      <c r="AF19" s="123"/>
-      <c r="AG19" s="123"/>
-      <c r="AH19" s="123"/>
-      <c r="AI19" s="123"/>
+      <c r="Y19" s="131"/>
+      <c r="Z19" s="131"/>
+      <c r="AA19" s="131"/>
+      <c r="AB19" s="131"/>
+      <c r="AC19" s="131"/>
+      <c r="AD19" s="131"/>
+      <c r="AE19" s="131"/>
+      <c r="AF19" s="131"/>
+      <c r="AG19" s="131"/>
+      <c r="AH19" s="131"/>
+      <c r="AI19" s="131"/>
       <c r="AJ19" s="24"/>
       <c r="AK19" s="84"/>
     </row>
     <row r="20" spans="1:37" ht="37.5" customHeight="1" thickBot="1">
       <c r="A20" s="83"/>
-      <c r="B20" s="135"/>
+      <c r="B20" s="124"/>
       <c r="C20" s="6" t="s">
         <v>4</v>
       </c>
@@ -4327,7 +4109,7 @@
       <c r="Q21" s="27"/>
       <c r="R21" s="27"/>
       <c r="S21" s="114"/>
-      <c r="T21" s="146" t="s">
+      <c r="T21" s="116" t="s">
         <v>35</v>
       </c>
       <c r="U21" s="114"/>
@@ -4369,7 +4151,7 @@
       <c r="R22" s="27"/>
       <c r="S22" s="114"/>
       <c r="T22" s="114"/>
-      <c r="U22" s="147" t="s">
+      <c r="U22" s="117" t="s">
         <v>36</v>
       </c>
       <c r="V22" s="114"/>
@@ -4410,7 +4192,7 @@
       <c r="R23" s="38"/>
       <c r="S23" s="114"/>
       <c r="T23" s="114"/>
-      <c r="U23" s="147" t="s">
+      <c r="U23" s="117" t="s">
         <v>37</v>
       </c>
       <c r="V23" s="114"/>
@@ -4442,20 +4224,20 @@
       <c r="I24" s="28"/>
       <c r="J24" s="28"/>
       <c r="K24" s="28"/>
-      <c r="L24" s="133" t="s">
+      <c r="L24" s="147" t="s">
         <v>25</v>
       </c>
-      <c r="M24" s="133"/>
-      <c r="N24" s="133"/>
-      <c r="O24" s="133"/>
-      <c r="P24" s="133"/>
+      <c r="M24" s="147"/>
+      <c r="N24" s="147"/>
+      <c r="O24" s="147"/>
+      <c r="P24" s="147"/>
       <c r="Q24" s="29" t="s">
         <v>31</v>
       </c>
       <c r="R24" s="40"/>
       <c r="S24" s="114"/>
       <c r="T24" s="114"/>
-      <c r="U24" s="146" t="s">
+      <c r="U24" s="116" t="s">
         <v>38</v>
       </c>
       <c r="V24" s="114"/>
@@ -4481,13 +4263,13 @@
       <c r="C25" s="27"/>
       <c r="D25" s="27"/>
       <c r="E25" s="59"/>
-      <c r="F25" s="116" t="s">
+      <c r="F25" s="118" t="s">
         <v>28</v>
       </c>
-      <c r="G25" s="116"/>
-      <c r="H25" s="116"/>
-      <c r="I25" s="116"/>
-      <c r="J25" s="116"/>
+      <c r="G25" s="118"/>
+      <c r="H25" s="118"/>
+      <c r="I25" s="118"/>
+      <c r="J25" s="118"/>
       <c r="K25" s="28"/>
       <c r="L25" s="28"/>
       <c r="M25" s="28"/>
@@ -4498,7 +4280,7 @@
       <c r="R25" s="40"/>
       <c r="S25" s="114"/>
       <c r="T25" s="114"/>
-      <c r="U25" s="146" t="s">
+      <c r="U25" s="116" t="s">
         <v>39</v>
       </c>
       <c r="V25" s="114"/>
@@ -4524,11 +4306,11 @@
       <c r="C26" s="27"/>
       <c r="D26" s="27"/>
       <c r="E26" s="59"/>
-      <c r="F26" s="116"/>
-      <c r="G26" s="116"/>
-      <c r="H26" s="116"/>
-      <c r="I26" s="116"/>
-      <c r="J26" s="116"/>
+      <c r="F26" s="118"/>
+      <c r="G26" s="118"/>
+      <c r="H26" s="118"/>
+      <c r="I26" s="118"/>
+      <c r="J26" s="118"/>
       <c r="K26" s="28"/>
       <c r="L26" s="28"/>
       <c r="M26" s="28"/>
@@ -4539,7 +4321,7 @@
       <c r="R26" s="40"/>
       <c r="S26" s="114"/>
       <c r="T26" s="114"/>
-      <c r="U26" s="146" t="s">
+      <c r="U26" s="116" t="s">
         <v>40</v>
       </c>
       <c r="V26" s="114"/>
@@ -4565,22 +4347,22 @@
       <c r="C27" s="27"/>
       <c r="D27" s="27"/>
       <c r="E27" s="59"/>
-      <c r="F27" s="116"/>
-      <c r="G27" s="116"/>
-      <c r="H27" s="116"/>
-      <c r="I27" s="116"/>
-      <c r="J27" s="116"/>
-      <c r="K27" s="116"/>
-      <c r="L27" s="116"/>
-      <c r="M27" s="116"/>
-      <c r="N27" s="116"/>
-      <c r="O27" s="116"/>
-      <c r="P27" s="116"/>
-      <c r="Q27" s="116"/>
+      <c r="F27" s="118"/>
+      <c r="G27" s="118"/>
+      <c r="H27" s="118"/>
+      <c r="I27" s="118"/>
+      <c r="J27" s="118"/>
+      <c r="K27" s="118"/>
+      <c r="L27" s="118"/>
+      <c r="M27" s="118"/>
+      <c r="N27" s="118"/>
+      <c r="O27" s="118"/>
+      <c r="P27" s="118"/>
+      <c r="Q27" s="118"/>
       <c r="R27" s="40"/>
       <c r="S27" s="114"/>
       <c r="T27" s="114"/>
-      <c r="U27" s="146" t="s">
+      <c r="U27" s="116" t="s">
         <v>41</v>
       </c>
       <c r="V27" s="114"/>
@@ -4602,28 +4384,28 @@
     </row>
     <row r="28" spans="1:37" ht="11.25" customHeight="1">
       <c r="A28" s="83"/>
-      <c r="B28" s="142" t="s">
+      <c r="B28" s="119" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="143"/>
-      <c r="D28" s="143"/>
-      <c r="E28" s="144"/>
-      <c r="F28" s="116"/>
-      <c r="G28" s="116"/>
-      <c r="H28" s="116"/>
-      <c r="I28" s="116"/>
-      <c r="J28" s="116"/>
-      <c r="K28" s="116"/>
-      <c r="L28" s="116"/>
-      <c r="M28" s="116"/>
-      <c r="N28" s="116"/>
-      <c r="O28" s="116"/>
-      <c r="P28" s="116"/>
-      <c r="Q28" s="116"/>
+      <c r="C28" s="120"/>
+      <c r="D28" s="120"/>
+      <c r="E28" s="121"/>
+      <c r="F28" s="118"/>
+      <c r="G28" s="118"/>
+      <c r="H28" s="118"/>
+      <c r="I28" s="118"/>
+      <c r="J28" s="118"/>
+      <c r="K28" s="118"/>
+      <c r="L28" s="118"/>
+      <c r="M28" s="118"/>
+      <c r="N28" s="118"/>
+      <c r="O28" s="118"/>
+      <c r="P28" s="118"/>
+      <c r="Q28" s="118"/>
       <c r="R28" s="40"/>
       <c r="S28" s="114"/>
       <c r="T28" s="114"/>
-      <c r="U28" s="147" t="s">
+      <c r="U28" s="117" t="s">
         <v>42</v>
       </c>
       <c r="V28" s="114"/>
@@ -4649,18 +4431,18 @@
       <c r="C29" s="27"/>
       <c r="D29" s="27"/>
       <c r="E29" s="59"/>
-      <c r="F29" s="116"/>
-      <c r="G29" s="116"/>
-      <c r="H29" s="116"/>
-      <c r="I29" s="116"/>
-      <c r="J29" s="116"/>
-      <c r="K29" s="116"/>
-      <c r="L29" s="116"/>
-      <c r="M29" s="116"/>
-      <c r="N29" s="116"/>
-      <c r="O29" s="116"/>
-      <c r="P29" s="116"/>
-      <c r="Q29" s="116"/>
+      <c r="F29" s="118"/>
+      <c r="G29" s="118"/>
+      <c r="H29" s="118"/>
+      <c r="I29" s="118"/>
+      <c r="J29" s="118"/>
+      <c r="K29" s="118"/>
+      <c r="L29" s="118"/>
+      <c r="M29" s="118"/>
+      <c r="N29" s="118"/>
+      <c r="O29" s="118"/>
+      <c r="P29" s="118"/>
+      <c r="Q29" s="118"/>
       <c r="R29" s="40"/>
       <c r="S29" s="27"/>
       <c r="T29" s="27"/>
@@ -4688,18 +4470,18 @@
       <c r="C30" s="27"/>
       <c r="D30" s="27"/>
       <c r="E30" s="27"/>
-      <c r="F30" s="116"/>
-      <c r="G30" s="116"/>
-      <c r="H30" s="116"/>
-      <c r="I30" s="116"/>
-      <c r="J30" s="116"/>
-      <c r="K30" s="116"/>
-      <c r="L30" s="116"/>
-      <c r="M30" s="116"/>
-      <c r="N30" s="116"/>
-      <c r="O30" s="116"/>
-      <c r="P30" s="116"/>
-      <c r="Q30" s="116"/>
+      <c r="F30" s="118"/>
+      <c r="G30" s="118"/>
+      <c r="H30" s="118"/>
+      <c r="I30" s="118"/>
+      <c r="J30" s="118"/>
+      <c r="K30" s="118"/>
+      <c r="L30" s="118"/>
+      <c r="M30" s="118"/>
+      <c r="N30" s="118"/>
+      <c r="O30" s="118"/>
+      <c r="P30" s="118"/>
+      <c r="Q30" s="118"/>
       <c r="R30" s="40"/>
       <c r="S30" s="27"/>
       <c r="T30" s="27"/>
@@ -4723,24 +4505,24 @@
     </row>
     <row r="31" spans="1:37" ht="11.25" customHeight="1">
       <c r="A31" s="83"/>
-      <c r="B31" s="142" t="s">
+      <c r="B31" s="119" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="143"/>
-      <c r="D31" s="143"/>
-      <c r="E31" s="143"/>
-      <c r="F31" s="116"/>
-      <c r="G31" s="116"/>
-      <c r="H31" s="116"/>
-      <c r="I31" s="116"/>
-      <c r="J31" s="116"/>
-      <c r="K31" s="116"/>
-      <c r="L31" s="116"/>
-      <c r="M31" s="116"/>
-      <c r="N31" s="116"/>
-      <c r="O31" s="116"/>
-      <c r="P31" s="116"/>
-      <c r="Q31" s="116"/>
+      <c r="C31" s="120"/>
+      <c r="D31" s="120"/>
+      <c r="E31" s="120"/>
+      <c r="F31" s="118"/>
+      <c r="G31" s="118"/>
+      <c r="H31" s="118"/>
+      <c r="I31" s="118"/>
+      <c r="J31" s="118"/>
+      <c r="K31" s="118"/>
+      <c r="L31" s="118"/>
+      <c r="M31" s="118"/>
+      <c r="N31" s="118"/>
+      <c r="O31" s="118"/>
+      <c r="P31" s="118"/>
+      <c r="Q31" s="118"/>
       <c r="R31" s="40"/>
       <c r="S31" s="27"/>
       <c r="T31" s="27"/>
@@ -4768,18 +4550,18 @@
       <c r="C32" s="11"/>
       <c r="D32" s="11"/>
       <c r="E32" s="11"/>
-      <c r="F32" s="116"/>
-      <c r="G32" s="116"/>
-      <c r="H32" s="116"/>
-      <c r="I32" s="116"/>
-      <c r="J32" s="116"/>
-      <c r="K32" s="116"/>
-      <c r="L32" s="116"/>
-      <c r="M32" s="116"/>
-      <c r="N32" s="116"/>
-      <c r="O32" s="116"/>
-      <c r="P32" s="116"/>
-      <c r="Q32" s="116"/>
+      <c r="F32" s="118"/>
+      <c r="G32" s="118"/>
+      <c r="H32" s="118"/>
+      <c r="I32" s="118"/>
+      <c r="J32" s="118"/>
+      <c r="K32" s="118"/>
+      <c r="L32" s="118"/>
+      <c r="M32" s="118"/>
+      <c r="N32" s="118"/>
+      <c r="O32" s="118"/>
+      <c r="P32" s="118"/>
+      <c r="Q32" s="118"/>
       <c r="R32" s="40"/>
       <c r="S32" s="27"/>
       <c r="T32" s="27"/>
@@ -4807,17 +4589,17 @@
       <c r="C33" s="11"/>
       <c r="D33" s="11"/>
       <c r="E33" s="11"/>
-      <c r="F33" s="116"/>
-      <c r="G33" s="116"/>
-      <c r="H33" s="116"/>
-      <c r="I33" s="116"/>
-      <c r="J33" s="116"/>
-      <c r="K33" s="116"/>
-      <c r="L33" s="116"/>
-      <c r="M33" s="116"/>
-      <c r="N33" s="116"/>
-      <c r="O33" s="116"/>
-      <c r="P33" s="116"/>
+      <c r="F33" s="118"/>
+      <c r="G33" s="118"/>
+      <c r="H33" s="118"/>
+      <c r="I33" s="118"/>
+      <c r="J33" s="118"/>
+      <c r="K33" s="118"/>
+      <c r="L33" s="118"/>
+      <c r="M33" s="118"/>
+      <c r="N33" s="118"/>
+      <c r="O33" s="118"/>
+      <c r="P33" s="118"/>
       <c r="Q33" s="9"/>
       <c r="R33" s="40"/>
       <c r="S33" s="27"/>
@@ -4842,24 +4624,24 @@
     </row>
     <row r="34" spans="1:37" ht="11.25" customHeight="1">
       <c r="A34" s="83"/>
-      <c r="B34" s="142" t="s">
+      <c r="B34" s="119" t="s">
         <v>11</v>
       </c>
-      <c r="C34" s="143"/>
-      <c r="D34" s="143"/>
-      <c r="E34" s="143"/>
-      <c r="F34" s="116"/>
-      <c r="G34" s="116"/>
-      <c r="H34" s="116"/>
-      <c r="I34" s="116"/>
-      <c r="J34" s="116"/>
-      <c r="K34" s="116"/>
-      <c r="L34" s="116"/>
-      <c r="M34" s="116"/>
-      <c r="N34" s="116"/>
-      <c r="O34" s="116"/>
-      <c r="P34" s="116"/>
-      <c r="Q34" s="145" t="s">
+      <c r="C34" s="120"/>
+      <c r="D34" s="120"/>
+      <c r="E34" s="120"/>
+      <c r="F34" s="118"/>
+      <c r="G34" s="118"/>
+      <c r="H34" s="118"/>
+      <c r="I34" s="118"/>
+      <c r="J34" s="118"/>
+      <c r="K34" s="118"/>
+      <c r="L34" s="118"/>
+      <c r="M34" s="118"/>
+      <c r="N34" s="118"/>
+      <c r="O34" s="118"/>
+      <c r="P34" s="118"/>
+      <c r="Q34" s="122" t="s">
         <v>6</v>
       </c>
       <c r="R34" s="40"/>
@@ -4889,18 +4671,18 @@
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
       <c r="E35" s="10"/>
-      <c r="F35" s="116"/>
-      <c r="G35" s="116"/>
-      <c r="H35" s="116"/>
-      <c r="I35" s="116"/>
-      <c r="J35" s="116"/>
-      <c r="K35" s="116"/>
-      <c r="L35" s="116"/>
-      <c r="M35" s="116"/>
-      <c r="N35" s="116"/>
-      <c r="O35" s="116"/>
-      <c r="P35" s="116"/>
-      <c r="Q35" s="145"/>
+      <c r="F35" s="118"/>
+      <c r="G35" s="118"/>
+      <c r="H35" s="118"/>
+      <c r="I35" s="118"/>
+      <c r="J35" s="118"/>
+      <c r="K35" s="118"/>
+      <c r="L35" s="118"/>
+      <c r="M35" s="118"/>
+      <c r="N35" s="118"/>
+      <c r="O35" s="118"/>
+      <c r="P35" s="118"/>
+      <c r="Q35" s="122"/>
       <c r="R35" s="40"/>
       <c r="S35" s="27"/>
       <c r="T35" s="27"/>
@@ -4928,20 +4710,20 @@
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
       <c r="E36" s="61"/>
-      <c r="F36" s="116" t="s">
+      <c r="F36" s="118" t="s">
         <v>32</v>
       </c>
-      <c r="G36" s="116"/>
-      <c r="H36" s="116"/>
-      <c r="I36" s="116"/>
-      <c r="J36" s="116"/>
-      <c r="K36" s="116"/>
-      <c r="L36" s="116"/>
-      <c r="M36" s="116"/>
-      <c r="N36" s="116"/>
-      <c r="O36" s="116"/>
-      <c r="P36" s="116"/>
-      <c r="Q36" s="116"/>
+      <c r="G36" s="118"/>
+      <c r="H36" s="118"/>
+      <c r="I36" s="118"/>
+      <c r="J36" s="118"/>
+      <c r="K36" s="118"/>
+      <c r="L36" s="118"/>
+      <c r="M36" s="118"/>
+      <c r="N36" s="118"/>
+      <c r="O36" s="118"/>
+      <c r="P36" s="118"/>
+      <c r="Q36" s="118"/>
       <c r="R36" s="40"/>
       <c r="S36" s="27"/>
       <c r="T36" s="27"/>
@@ -4965,24 +4747,24 @@
     </row>
     <row r="37" spans="1:37" ht="11.25" customHeight="1">
       <c r="A37" s="83"/>
-      <c r="B37" s="142" t="s">
+      <c r="B37" s="119" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="143"/>
-      <c r="D37" s="143"/>
-      <c r="E37" s="144"/>
-      <c r="F37" s="116"/>
-      <c r="G37" s="116"/>
-      <c r="H37" s="116"/>
-      <c r="I37" s="116"/>
-      <c r="J37" s="116"/>
-      <c r="K37" s="116"/>
-      <c r="L37" s="116"/>
-      <c r="M37" s="116"/>
-      <c r="N37" s="116"/>
-      <c r="O37" s="116"/>
-      <c r="P37" s="116"/>
-      <c r="Q37" s="116"/>
+      <c r="C37" s="120"/>
+      <c r="D37" s="120"/>
+      <c r="E37" s="121"/>
+      <c r="F37" s="118"/>
+      <c r="G37" s="118"/>
+      <c r="H37" s="118"/>
+      <c r="I37" s="118"/>
+      <c r="J37" s="118"/>
+      <c r="K37" s="118"/>
+      <c r="L37" s="118"/>
+      <c r="M37" s="118"/>
+      <c r="N37" s="118"/>
+      <c r="O37" s="118"/>
+      <c r="P37" s="118"/>
+      <c r="Q37" s="118"/>
       <c r="R37" s="40"/>
       <c r="S37" s="27"/>
       <c r="T37" s="27"/>
@@ -5010,18 +4792,18 @@
       <c r="C38" s="27"/>
       <c r="D38" s="27"/>
       <c r="E38" s="59"/>
-      <c r="F38" s="116"/>
-      <c r="G38" s="116"/>
-      <c r="H38" s="116"/>
-      <c r="I38" s="116"/>
-      <c r="J38" s="116"/>
-      <c r="K38" s="116"/>
-      <c r="L38" s="116"/>
-      <c r="M38" s="116"/>
-      <c r="N38" s="116"/>
-      <c r="O38" s="116"/>
-      <c r="P38" s="116"/>
-      <c r="Q38" s="116"/>
+      <c r="F38" s="118"/>
+      <c r="G38" s="118"/>
+      <c r="H38" s="118"/>
+      <c r="I38" s="118"/>
+      <c r="J38" s="118"/>
+      <c r="K38" s="118"/>
+      <c r="L38" s="118"/>
+      <c r="M38" s="118"/>
+      <c r="N38" s="118"/>
+      <c r="O38" s="118"/>
+      <c r="P38" s="118"/>
+      <c r="Q38" s="118"/>
       <c r="R38" s="40"/>
       <c r="S38" s="27"/>
       <c r="T38" s="27"/>
@@ -5244,6 +5026,22 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="F25:J26"/>
+    <mergeCell ref="AI1:AK1"/>
+    <mergeCell ref="T11:U12"/>
+    <mergeCell ref="V11:Z12"/>
+    <mergeCell ref="AA11:AE12"/>
+    <mergeCell ref="AF11:AJ12"/>
+    <mergeCell ref="AF2:AH2"/>
+    <mergeCell ref="AI2:AK2"/>
+    <mergeCell ref="L24:P24"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="T16:AJ16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="T17:T19"/>
+    <mergeCell ref="B6:AK8"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="Y19:AI19"/>
     <mergeCell ref="F36:Q38"/>
     <mergeCell ref="B37:E37"/>
     <mergeCell ref="F27:Q29"/>
@@ -5253,22 +5051,6 @@
     <mergeCell ref="B34:E34"/>
     <mergeCell ref="Q34:Q35"/>
     <mergeCell ref="B31:E31"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="T16:AJ16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="T17:T19"/>
-    <mergeCell ref="B6:AK8"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="Y19:AI19"/>
-    <mergeCell ref="F25:J26"/>
-    <mergeCell ref="AI1:AK1"/>
-    <mergeCell ref="T11:U12"/>
-    <mergeCell ref="V11:Z12"/>
-    <mergeCell ref="AA11:AE12"/>
-    <mergeCell ref="AF11:AJ12"/>
-    <mergeCell ref="AF2:AH2"/>
-    <mergeCell ref="AI2:AK2"/>
-    <mergeCell ref="L24:P24"/>
   </mergeCells>
   <phoneticPr fontId="15"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
change template of QSI003
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/ローマ字氏名届_帳票テンプレート.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/ローマ字氏名届_帳票テンプレート.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF12FD03-D393-42FD-9DC9-4EC4388CF2E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504F31FB-1B36-4127-983D-56D6A5E6B7AE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8BC8B0BF-E0AC-4C73-B25B-BE8089E69E19}"/>
+    <workbookView xWindow="23415" yWindow="630" windowWidth="25965" windowHeight="14145" xr2:uid="{8BC8B0BF-E0AC-4C73-B25B-BE8089E69E19}"/>
   </bookViews>
   <sheets>
     <sheet name="2号" sheetId="14" r:id="rId1"/>
@@ -375,11 +375,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="35">
+  <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -485,7 +485,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -493,7 +493,7 @@
     <font>
       <sz val="8"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -501,7 +501,7 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -509,7 +509,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -524,7 +524,7 @@
     <font>
       <sz val="20"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -539,7 +539,7 @@
     <font>
       <sz val="9"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -547,7 +547,7 @@
     <font>
       <b/>
       <sz val="12"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -555,7 +555,7 @@
     <font>
       <b/>
       <sz val="26"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -564,7 +564,7 @@
       <b/>
       <sz val="26"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -573,7 +573,7 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -581,7 +581,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -589,7 +589,7 @@
     <font>
       <b/>
       <sz val="18"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -598,7 +598,7 @@
       <b/>
       <sz val="18"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -607,7 +607,7 @@
       <b/>
       <sz val="8"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -615,7 +615,7 @@
     <font>
       <b/>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -632,6 +632,8 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1541,7 +1543,7 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1627,8 +1629,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="8743950" y="8067675"/>
-          <a:ext cx="3609975" cy="447675"/>
+          <a:off x="9915525" y="8048625"/>
+          <a:ext cx="4133850" cy="447675"/>
           <a:chOff x="7124700" y="4981575"/>
           <a:chExt cx="2486025" cy="447675"/>
         </a:xfrm>
@@ -2413,14 +2415,26 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>□短期在留者であるため</a:t>
+            <a:t>□</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-ea"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>短期在留者であるため</a:t>
           </a:r>
           <a:endParaRPr kumimoji="0" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
             <a:solidFill>
               <a:sysClr val="windowText" lastClr="000000"/>
             </a:solidFill>
             <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
+            <a:latin typeface="+mn-ea"/>
             <a:ea typeface="+mn-ea"/>
             <a:cs typeface="+mn-cs"/>
           </a:endParaRPr>
@@ -2432,7 +2446,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="+mn-ea"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -2443,7 +2457,7 @@
               <a:sysClr val="windowText" lastClr="000000"/>
             </a:solidFill>
             <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
+            <a:latin typeface="+mn-ea"/>
             <a:ea typeface="+mn-ea"/>
             <a:cs typeface="+mn-cs"/>
           </a:endParaRPr>
@@ -2455,7 +2469,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="+mn-ea"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -2467,7 +2481,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="+mn-ea"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -2479,7 +2493,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="+mn-ea"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -2490,7 +2504,7 @@
               <a:sysClr val="windowText" lastClr="000000"/>
             </a:solidFill>
             <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
+            <a:latin typeface="+mn-ea"/>
             <a:ea typeface="+mn-ea"/>
             <a:cs typeface="+mn-cs"/>
           </a:endParaRPr>
@@ -2502,7 +2516,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="+mn-ea"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
@@ -2512,6 +2526,8 @@
             <a:solidFill>
               <a:sysClr val="windowText" lastClr="000000"/>
             </a:solidFill>
+            <a:latin typeface="+mn-ea"/>
+            <a:ea typeface="+mn-ea"/>
           </a:endParaRPr>
         </a:p>
       </xdr:txBody>
@@ -3107,19 +3123,17 @@
   </sheetPr>
   <dimension ref="A1:AL43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="X20" sqref="X20"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="5.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="15" customWidth="1"/>
-    <col min="2" max="36" width="5.140625" style="15"/>
+    <col min="1" max="1" width="2.75" style="15" customWidth="1"/>
+    <col min="2" max="36" width="5.125" style="15"/>
     <col min="37" max="37" width="4" style="15" customWidth="1"/>
-    <col min="38" max="16384" width="5.140625" style="15"/>
+    <col min="38" max="16384" width="5.125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="15.75">
+    <row r="1" spans="1:38" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A1" s="25"/>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
@@ -3158,7 +3172,7 @@
       <c r="AK1" s="102"/>
       <c r="AL1" s="25"/>
     </row>
-    <row r="2" spans="1:38" ht="26.25" customHeight="1">
+    <row r="2" spans="1:38" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="25"/>
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
@@ -3202,7 +3216,7 @@
       <c r="AK2" s="116"/>
       <c r="AL2" s="25"/>
     </row>
-    <row r="3" spans="1:38" ht="26.25" customHeight="1">
+    <row r="3" spans="1:38" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="25"/>
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
@@ -3242,7 +3256,7 @@
       <c r="AK3" s="74"/>
       <c r="AL3" s="25"/>
     </row>
-    <row r="4" spans="1:38" ht="26.25" customHeight="1">
+    <row r="4" spans="1:38" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="25"/>
       <c r="B4" s="25"/>
       <c r="C4" s="25"/>
@@ -3282,7 +3296,7 @@
       <c r="AK4" s="76"/>
       <c r="AL4" s="25"/>
     </row>
-    <row r="5" spans="1:38" ht="18.75" customHeight="1">
+    <row r="5" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="29"/>
       <c r="B5" s="69"/>
       <c r="C5" s="69"/>
@@ -3321,7 +3335,7 @@
       <c r="AJ5" s="71"/>
       <c r="AK5" s="71"/>
     </row>
-    <row r="6" spans="1:38" ht="13.5" customHeight="1">
+    <row r="6" spans="1:38" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="65"/>
       <c r="B6" s="132" t="s">
         <v>21</v>
@@ -3362,7 +3376,7 @@
       <c r="AJ6" s="132"/>
       <c r="AK6" s="133"/>
     </row>
-    <row r="7" spans="1:38" ht="13.5" customHeight="1">
+    <row r="7" spans="1:38" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="66"/>
       <c r="B7" s="134"/>
       <c r="C7" s="134"/>
@@ -3401,7 +3415,7 @@
       <c r="AJ7" s="134"/>
       <c r="AK7" s="135"/>
     </row>
-    <row r="8" spans="1:38" ht="13.5" customHeight="1">
+    <row r="8" spans="1:38" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="66"/>
       <c r="B8" s="134"/>
       <c r="C8" s="134"/>
@@ -3440,7 +3454,7 @@
       <c r="AJ8" s="134"/>
       <c r="AK8" s="135"/>
     </row>
-    <row r="9" spans="1:38" ht="18.75" customHeight="1">
+    <row r="9" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="66"/>
       <c r="B9" s="25"/>
       <c r="C9" s="25"/>
@@ -3479,7 +3493,7 @@
       <c r="AJ9" s="25"/>
       <c r="AK9" s="67"/>
     </row>
-    <row r="10" spans="1:38" ht="28.5" customHeight="1" thickBot="1">
+    <row r="10" spans="1:38" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A10" s="66"/>
       <c r="B10" s="12" t="s">
         <v>25</v>
@@ -3528,7 +3542,7 @@
       <c r="AJ10" s="77"/>
       <c r="AK10" s="67"/>
     </row>
-    <row r="11" spans="1:38" ht="13.5" customHeight="1">
+    <row r="11" spans="1:38" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="66"/>
       <c r="B11" s="19"/>
       <c r="C11" s="20"/>
@@ -3577,7 +3591,7 @@
       <c r="AJ11" s="110"/>
       <c r="AK11" s="67"/>
     </row>
-    <row r="12" spans="1:38" ht="40.5" customHeight="1" thickBot="1">
+    <row r="12" spans="1:38" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A12" s="66"/>
       <c r="B12" s="43"/>
       <c r="C12" s="44"/>
@@ -3616,7 +3630,7 @@
       <c r="AJ12" s="112"/>
       <c r="AK12" s="67"/>
     </row>
-    <row r="13" spans="1:38" ht="23.25" customHeight="1" thickBot="1">
+    <row r="13" spans="1:38" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A13" s="66"/>
       <c r="B13" s="136" t="s">
         <v>42</v>
@@ -3657,7 +3671,7 @@
       <c r="AJ13" s="138"/>
       <c r="AK13" s="67"/>
     </row>
-    <row r="14" spans="1:38" ht="25.5" customHeight="1">
+    <row r="14" spans="1:38" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="66"/>
       <c r="B14" s="128" t="s">
         <v>16</v>
@@ -3700,7 +3714,7 @@
       <c r="AJ14" s="94"/>
       <c r="AK14" s="67"/>
     </row>
-    <row r="15" spans="1:38" ht="60.75" customHeight="1" thickBot="1">
+    <row r="15" spans="1:38" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A15" s="66"/>
       <c r="B15" s="129"/>
       <c r="C15" s="6" t="s">
@@ -3741,7 +3755,7 @@
       <c r="AJ15" s="96"/>
       <c r="AK15" s="67"/>
     </row>
-    <row r="16" spans="1:38" ht="23.25" customHeight="1" thickBot="1">
+    <row r="16" spans="1:38" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A16" s="66"/>
       <c r="B16" s="60" t="s">
         <v>20</v>
@@ -3784,7 +3798,7 @@
       <c r="AJ16" s="130"/>
       <c r="AK16" s="67"/>
     </row>
-    <row r="17" spans="1:37" ht="25.5" customHeight="1">
+    <row r="17" spans="1:37" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="66"/>
       <c r="B17" s="128" t="s">
         <v>12</v>
@@ -3829,7 +3843,7 @@
       <c r="AJ17" s="121"/>
       <c r="AK17" s="67"/>
     </row>
-    <row r="18" spans="1:37" ht="37.5" customHeight="1" thickBot="1">
+    <row r="18" spans="1:37" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A18" s="66"/>
       <c r="B18" s="129"/>
       <c r="C18" s="6" t="s">
@@ -3872,7 +3886,7 @@
       <c r="AJ18" s="124"/>
       <c r="AK18" s="67"/>
     </row>
-    <row r="19" spans="1:37" ht="25.5" customHeight="1" thickBot="1">
+    <row r="19" spans="1:37" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A19" s="66"/>
       <c r="B19" s="128" t="s">
         <v>13</v>
@@ -3915,7 +3929,7 @@
       <c r="AJ19" s="127"/>
       <c r="AK19" s="67"/>
     </row>
-    <row r="20" spans="1:37" ht="37.5" customHeight="1" thickBot="1">
+    <row r="20" spans="1:37" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A20" s="66"/>
       <c r="B20" s="129"/>
       <c r="C20" s="6" t="s">
@@ -3958,7 +3972,7 @@
       <c r="AJ20" s="25"/>
       <c r="AK20" s="67"/>
     </row>
-    <row r="21" spans="1:37" ht="12.75" customHeight="1">
+    <row r="21" spans="1:37" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="66"/>
       <c r="B21" s="25"/>
       <c r="C21" s="25"/>
@@ -3999,7 +4013,7 @@
       <c r="AJ21" s="25"/>
       <c r="AK21" s="98"/>
     </row>
-    <row r="22" spans="1:37" ht="11.25" customHeight="1" thickBot="1">
+    <row r="22" spans="1:37" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A22" s="66"/>
       <c r="B22" s="25"/>
       <c r="C22" s="25"/>
@@ -4040,7 +4054,7 @@
       <c r="AJ22" s="25"/>
       <c r="AK22" s="98"/>
     </row>
-    <row r="23" spans="1:37" ht="11.25" customHeight="1">
+    <row r="23" spans="1:37" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="66"/>
       <c r="B23" s="19"/>
       <c r="C23" s="20"/>
@@ -4081,7 +4095,7 @@
       <c r="AJ23" s="25"/>
       <c r="AK23" s="98"/>
     </row>
-    <row r="24" spans="1:37" ht="11.25" customHeight="1">
+    <row r="24" spans="1:37" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="66"/>
       <c r="B24" s="36"/>
       <c r="C24" s="25"/>
@@ -4126,7 +4140,7 @@
       <c r="AJ24" s="25"/>
       <c r="AK24" s="98"/>
     </row>
-    <row r="25" spans="1:37" ht="11.25" customHeight="1">
+    <row r="25" spans="1:37" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="66"/>
       <c r="B25" s="36"/>
       <c r="C25" s="25"/>
@@ -4169,7 +4183,7 @@
       <c r="AJ25" s="25"/>
       <c r="AK25" s="98"/>
     </row>
-    <row r="26" spans="1:37" ht="11.25" customHeight="1">
+    <row r="26" spans="1:37" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="66"/>
       <c r="B26" s="36"/>
       <c r="C26" s="25"/>
@@ -4210,7 +4224,7 @@
       <c r="AJ26" s="25"/>
       <c r="AK26" s="98"/>
     </row>
-    <row r="27" spans="1:37" ht="11.25" customHeight="1">
+    <row r="27" spans="1:37" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="66"/>
       <c r="B27" s="36"/>
       <c r="C27" s="25"/>
@@ -4251,7 +4265,7 @@
       <c r="AJ27" s="25"/>
       <c r="AK27" s="98"/>
     </row>
-    <row r="28" spans="1:37" ht="11.25" customHeight="1">
+    <row r="28" spans="1:37" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="66"/>
       <c r="B28" s="139" t="s">
         <v>7</v>
@@ -4294,7 +4308,7 @@
       <c r="AJ28" s="25"/>
       <c r="AK28" s="98"/>
     </row>
-    <row r="29" spans="1:37" ht="11.25" customHeight="1">
+    <row r="29" spans="1:37" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="66"/>
       <c r="B29" s="36"/>
       <c r="C29" s="25"/>
@@ -4333,7 +4347,7 @@
       <c r="AJ29" s="25"/>
       <c r="AK29" s="67"/>
     </row>
-    <row r="30" spans="1:37" ht="11.25" customHeight="1">
+    <row r="30" spans="1:37" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="66"/>
       <c r="B30" s="36"/>
       <c r="C30" s="25"/>
@@ -4372,7 +4386,7 @@
       <c r="AJ30" s="25"/>
       <c r="AK30" s="67"/>
     </row>
-    <row r="31" spans="1:37" ht="11.25" customHeight="1">
+    <row r="31" spans="1:37" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="66"/>
       <c r="B31" s="139" t="s">
         <v>8</v>
@@ -4413,7 +4427,7 @@
       <c r="AJ31" s="25"/>
       <c r="AK31" s="67"/>
     </row>
-    <row r="32" spans="1:37" ht="11.25" customHeight="1">
+    <row r="32" spans="1:37" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="66"/>
       <c r="B32" s="38"/>
       <c r="C32" s="11"/>
@@ -4452,7 +4466,7 @@
       <c r="AJ32" s="25"/>
       <c r="AK32" s="67"/>
     </row>
-    <row r="33" spans="1:37" ht="11.25" customHeight="1">
+    <row r="33" spans="1:37" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="66"/>
       <c r="B33" s="38"/>
       <c r="C33" s="11"/>
@@ -4491,7 +4505,7 @@
       <c r="AJ33" s="25"/>
       <c r="AK33" s="67"/>
     </row>
-    <row r="34" spans="1:37" ht="11.25" customHeight="1">
+    <row r="34" spans="1:37" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="66"/>
       <c r="B34" s="139" t="s">
         <v>11</v>
@@ -4534,7 +4548,7 @@
       <c r="AJ34" s="25"/>
       <c r="AK34" s="67"/>
     </row>
-    <row r="35" spans="1:37" ht="11.25" customHeight="1">
+    <row r="35" spans="1:37" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="66"/>
       <c r="B35" s="39"/>
       <c r="C35" s="10"/>
@@ -4573,7 +4587,7 @@
       <c r="AJ35" s="25"/>
       <c r="AK35" s="67"/>
     </row>
-    <row r="36" spans="1:37" ht="11.25" customHeight="1">
+    <row r="36" spans="1:37" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="66"/>
       <c r="B36" s="39"/>
       <c r="C36" s="10"/>
@@ -4614,7 +4628,7 @@
       <c r="AJ36" s="25"/>
       <c r="AK36" s="67"/>
     </row>
-    <row r="37" spans="1:37" ht="11.25" customHeight="1">
+    <row r="37" spans="1:37" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="66"/>
       <c r="B37" s="139" t="s">
         <v>14</v>
@@ -4655,7 +4669,7 @@
       <c r="AJ37" s="25"/>
       <c r="AK37" s="67"/>
     </row>
-    <row r="38" spans="1:37" ht="11.25" customHeight="1">
+    <row r="38" spans="1:37" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="66"/>
       <c r="B38" s="36"/>
       <c r="C38" s="25"/>
@@ -4694,7 +4708,7 @@
       <c r="AJ38" s="25"/>
       <c r="AK38" s="67"/>
     </row>
-    <row r="39" spans="1:37" ht="11.25" customHeight="1" thickBot="1">
+    <row r="39" spans="1:37" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A39" s="66"/>
       <c r="B39" s="40"/>
       <c r="C39" s="23"/>
@@ -4733,7 +4747,7 @@
       <c r="AJ39" s="25"/>
       <c r="AK39" s="67"/>
     </row>
-    <row r="40" spans="1:37" ht="10.5" customHeight="1">
+    <row r="40" spans="1:37" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="66"/>
       <c r="B40" s="25"/>
       <c r="C40" s="25"/>
@@ -4772,7 +4786,7 @@
       <c r="AJ40" s="25"/>
       <c r="AK40" s="67"/>
     </row>
-    <row r="41" spans="1:37" ht="24" customHeight="1">
+    <row r="41" spans="1:37" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="66"/>
       <c r="B41" s="30" t="s">
         <v>19</v>
@@ -4813,7 +4827,7 @@
       <c r="AJ41" s="25"/>
       <c r="AK41" s="67"/>
     </row>
-    <row r="42" spans="1:37" ht="43.5" customHeight="1">
+    <row r="42" spans="1:37" ht="43.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="66"/>
       <c r="B42" s="28"/>
       <c r="C42" s="29"/>
@@ -4854,7 +4868,7 @@
       <c r="AJ42" s="25"/>
       <c r="AK42" s="67"/>
     </row>
-    <row r="43" spans="1:37" ht="5.25" customHeight="1">
+    <row r="43" spans="1:37" ht="5.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="28"/>
       <c r="B43" s="29"/>
       <c r="C43" s="29"/>

</xml_diff>

<commit_message>
commit code ccg001 , bug template 003
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/ローマ字氏名届_帳票テンプレート.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/ローマ字氏名届_帳票テンプレート.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C747861-6492-4C86-82EF-DD94960CD0A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9815FC00-D4D1-4720-8683-FC6DDE997234}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8BC8B0BF-E0AC-4C73-B25B-BE8089E69E19}"/>
   </bookViews>
@@ -1559,6 +1559,117 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="center" indent="1"/>
     </xf>
@@ -1570,117 +1681,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2584,14 +2584,14 @@
     <xdr:from>
       <xdr:col>20</xdr:col>
       <xdr:colOff>173631</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>36096</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>236121</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>15908</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>247334</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>447359</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2606,7 +2606,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6869706" y="5760621"/>
+          <a:off x="6869706" y="5484396"/>
           <a:ext cx="185177" cy="211238"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2649,14 +2649,14 @@
     <xdr:from>
       <xdr:col>20</xdr:col>
       <xdr:colOff>179854</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>237329</xdr:rowOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>37304</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>22131</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>442964</xdr:rowOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>242939</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2671,7 +2671,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6875929" y="5485604"/>
+          <a:off x="6875929" y="5761829"/>
           <a:ext cx="185177" cy="205635"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2705,190 +2705,6 @@
             <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
             <a:t>✔</a:t>
           </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>74696</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>30580</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="29" name="正方形/長方形 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78AE032C-F84D-480A-A50E-AE7202528B7F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3743325" y="3619500"/>
-          <a:ext cx="5427746" cy="1040230"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="12700">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>□</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-ea"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>短期在留者であるため</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="0" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
-            <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-ea"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-ea"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>□海外に住所を有している者であるため</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
-            <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-ea"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-ea"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>□在留カード</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-ea"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>（または特別永住者証明書）</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-ea"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>にローマ字氏名が記載されていないため</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="0" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
-            <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-ea"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="1100">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-ea"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>□その他　理由（　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　          　）</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
-            <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
-            </a:solidFill>
-            <a:latin typeface="+mn-ea"/>
-            <a:ea typeface="+mn-ea"/>
-          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -3350,8 +3166,8 @@
   </sheetPr>
   <dimension ref="A1:AL43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X20" sqref="X20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W20" sqref="W20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.140625" defaultRowHeight="15"/>
@@ -3394,11 +3210,11 @@
       <c r="AC1" s="25"/>
       <c r="AD1" s="25"/>
       <c r="AE1" s="25"/>
-      <c r="AI1" s="117">
+      <c r="AI1" s="102">
         <v>72073</v>
       </c>
-      <c r="AJ1" s="117"/>
-      <c r="AK1" s="117"/>
+      <c r="AJ1" s="102"/>
+      <c r="AK1" s="102"/>
       <c r="AL1" s="25"/>
     </row>
     <row r="2" spans="1:38" ht="26.25" customHeight="1">
@@ -3433,16 +3249,16 @@
       <c r="AC2" s="25"/>
       <c r="AD2" s="25"/>
       <c r="AE2" s="25"/>
-      <c r="AF2" s="129" t="s">
+      <c r="AF2" s="114" t="s">
         <v>22</v>
       </c>
-      <c r="AG2" s="130"/>
-      <c r="AH2" s="131"/>
-      <c r="AI2" s="132" t="s">
+      <c r="AG2" s="115"/>
+      <c r="AH2" s="116"/>
+      <c r="AI2" s="117" t="s">
         <v>23</v>
       </c>
-      <c r="AJ2" s="130"/>
-      <c r="AK2" s="131"/>
+      <c r="AJ2" s="115"/>
+      <c r="AK2" s="116"/>
       <c r="AL2" s="25"/>
     </row>
     <row r="3" spans="1:38" ht="26.25" customHeight="1">
@@ -3566,122 +3382,122 @@
     </row>
     <row r="6" spans="1:38" ht="13.5" customHeight="1">
       <c r="A6" s="65"/>
-      <c r="B6" s="110" t="s">
+      <c r="B6" s="132" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="110"/>
-      <c r="D6" s="110"/>
-      <c r="E6" s="110"/>
-      <c r="F6" s="110"/>
-      <c r="G6" s="110"/>
-      <c r="H6" s="110"/>
-      <c r="I6" s="110"/>
-      <c r="J6" s="110"/>
-      <c r="K6" s="110"/>
-      <c r="L6" s="110"/>
-      <c r="M6" s="110"/>
-      <c r="N6" s="110"/>
-      <c r="O6" s="110"/>
-      <c r="P6" s="110"/>
-      <c r="Q6" s="110"/>
-      <c r="R6" s="110"/>
-      <c r="S6" s="110"/>
-      <c r="T6" s="110"/>
-      <c r="U6" s="110"/>
-      <c r="V6" s="110"/>
-      <c r="W6" s="110"/>
-      <c r="X6" s="110"/>
-      <c r="Y6" s="110"/>
-      <c r="Z6" s="110"/>
-      <c r="AA6" s="110"/>
-      <c r="AB6" s="110"/>
-      <c r="AC6" s="110"/>
-      <c r="AD6" s="110"/>
-      <c r="AE6" s="110"/>
-      <c r="AF6" s="110"/>
-      <c r="AG6" s="110"/>
-      <c r="AH6" s="110"/>
-      <c r="AI6" s="110"/>
-      <c r="AJ6" s="110"/>
-      <c r="AK6" s="111"/>
+      <c r="C6" s="132"/>
+      <c r="D6" s="132"/>
+      <c r="E6" s="132"/>
+      <c r="F6" s="132"/>
+      <c r="G6" s="132"/>
+      <c r="H6" s="132"/>
+      <c r="I6" s="132"/>
+      <c r="J6" s="132"/>
+      <c r="K6" s="132"/>
+      <c r="L6" s="132"/>
+      <c r="M6" s="132"/>
+      <c r="N6" s="132"/>
+      <c r="O6" s="132"/>
+      <c r="P6" s="132"/>
+      <c r="Q6" s="132"/>
+      <c r="R6" s="132"/>
+      <c r="S6" s="132"/>
+      <c r="T6" s="132"/>
+      <c r="U6" s="132"/>
+      <c r="V6" s="132"/>
+      <c r="W6" s="132"/>
+      <c r="X6" s="132"/>
+      <c r="Y6" s="132"/>
+      <c r="Z6" s="132"/>
+      <c r="AA6" s="132"/>
+      <c r="AB6" s="132"/>
+      <c r="AC6" s="132"/>
+      <c r="AD6" s="132"/>
+      <c r="AE6" s="132"/>
+      <c r="AF6" s="132"/>
+      <c r="AG6" s="132"/>
+      <c r="AH6" s="132"/>
+      <c r="AI6" s="132"/>
+      <c r="AJ6" s="132"/>
+      <c r="AK6" s="133"/>
     </row>
     <row r="7" spans="1:38" ht="13.5" customHeight="1">
       <c r="A7" s="66"/>
-      <c r="B7" s="112"/>
-      <c r="C7" s="112"/>
-      <c r="D7" s="112"/>
-      <c r="E7" s="112"/>
-      <c r="F7" s="112"/>
-      <c r="G7" s="112"/>
-      <c r="H7" s="112"/>
-      <c r="I7" s="112"/>
-      <c r="J7" s="112"/>
-      <c r="K7" s="112"/>
-      <c r="L7" s="112"/>
-      <c r="M7" s="112"/>
-      <c r="N7" s="112"/>
-      <c r="O7" s="112"/>
-      <c r="P7" s="112"/>
-      <c r="Q7" s="112"/>
-      <c r="R7" s="112"/>
-      <c r="S7" s="112"/>
-      <c r="T7" s="112"/>
-      <c r="U7" s="112"/>
-      <c r="V7" s="112"/>
-      <c r="W7" s="112"/>
-      <c r="X7" s="112"/>
-      <c r="Y7" s="112"/>
-      <c r="Z7" s="112"/>
-      <c r="AA7" s="112"/>
-      <c r="AB7" s="112"/>
-      <c r="AC7" s="112"/>
-      <c r="AD7" s="112"/>
-      <c r="AE7" s="112"/>
-      <c r="AF7" s="112"/>
-      <c r="AG7" s="112"/>
-      <c r="AH7" s="112"/>
-      <c r="AI7" s="112"/>
-      <c r="AJ7" s="112"/>
-      <c r="AK7" s="113"/>
+      <c r="B7" s="134"/>
+      <c r="C7" s="134"/>
+      <c r="D7" s="134"/>
+      <c r="E7" s="134"/>
+      <c r="F7" s="134"/>
+      <c r="G7" s="134"/>
+      <c r="H7" s="134"/>
+      <c r="I7" s="134"/>
+      <c r="J7" s="134"/>
+      <c r="K7" s="134"/>
+      <c r="L7" s="134"/>
+      <c r="M7" s="134"/>
+      <c r="N7" s="134"/>
+      <c r="O7" s="134"/>
+      <c r="P7" s="134"/>
+      <c r="Q7" s="134"/>
+      <c r="R7" s="134"/>
+      <c r="S7" s="134"/>
+      <c r="T7" s="134"/>
+      <c r="U7" s="134"/>
+      <c r="V7" s="134"/>
+      <c r="W7" s="134"/>
+      <c r="X7" s="134"/>
+      <c r="Y7" s="134"/>
+      <c r="Z7" s="134"/>
+      <c r="AA7" s="134"/>
+      <c r="AB7" s="134"/>
+      <c r="AC7" s="134"/>
+      <c r="AD7" s="134"/>
+      <c r="AE7" s="134"/>
+      <c r="AF7" s="134"/>
+      <c r="AG7" s="134"/>
+      <c r="AH7" s="134"/>
+      <c r="AI7" s="134"/>
+      <c r="AJ7" s="134"/>
+      <c r="AK7" s="135"/>
     </row>
     <row r="8" spans="1:38" ht="13.5" customHeight="1">
       <c r="A8" s="66"/>
-      <c r="B8" s="112"/>
-      <c r="C8" s="112"/>
-      <c r="D8" s="112"/>
-      <c r="E8" s="112"/>
-      <c r="F8" s="112"/>
-      <c r="G8" s="112"/>
-      <c r="H8" s="112"/>
-      <c r="I8" s="112"/>
-      <c r="J8" s="112"/>
-      <c r="K8" s="112"/>
-      <c r="L8" s="112"/>
-      <c r="M8" s="112"/>
-      <c r="N8" s="112"/>
-      <c r="O8" s="112"/>
-      <c r="P8" s="112"/>
-      <c r="Q8" s="112"/>
-      <c r="R8" s="112"/>
-      <c r="S8" s="112"/>
-      <c r="T8" s="112"/>
-      <c r="U8" s="112"/>
-      <c r="V8" s="112"/>
-      <c r="W8" s="112"/>
-      <c r="X8" s="112"/>
-      <c r="Y8" s="112"/>
-      <c r="Z8" s="112"/>
-      <c r="AA8" s="112"/>
-      <c r="AB8" s="112"/>
-      <c r="AC8" s="112"/>
-      <c r="AD8" s="112"/>
-      <c r="AE8" s="112"/>
-      <c r="AF8" s="112"/>
-      <c r="AG8" s="112"/>
-      <c r="AH8" s="112"/>
-      <c r="AI8" s="112"/>
-      <c r="AJ8" s="112"/>
-      <c r="AK8" s="113"/>
+      <c r="B8" s="134"/>
+      <c r="C8" s="134"/>
+      <c r="D8" s="134"/>
+      <c r="E8" s="134"/>
+      <c r="F8" s="134"/>
+      <c r="G8" s="134"/>
+      <c r="H8" s="134"/>
+      <c r="I8" s="134"/>
+      <c r="J8" s="134"/>
+      <c r="K8" s="134"/>
+      <c r="L8" s="134"/>
+      <c r="M8" s="134"/>
+      <c r="N8" s="134"/>
+      <c r="O8" s="134"/>
+      <c r="P8" s="134"/>
+      <c r="Q8" s="134"/>
+      <c r="R8" s="134"/>
+      <c r="S8" s="134"/>
+      <c r="T8" s="134"/>
+      <c r="U8" s="134"/>
+      <c r="V8" s="134"/>
+      <c r="W8" s="134"/>
+      <c r="X8" s="134"/>
+      <c r="Y8" s="134"/>
+      <c r="Z8" s="134"/>
+      <c r="AA8" s="134"/>
+      <c r="AB8" s="134"/>
+      <c r="AC8" s="134"/>
+      <c r="AD8" s="134"/>
+      <c r="AE8" s="134"/>
+      <c r="AF8" s="134"/>
+      <c r="AG8" s="134"/>
+      <c r="AH8" s="134"/>
+      <c r="AI8" s="134"/>
+      <c r="AJ8" s="134"/>
+      <c r="AK8" s="135"/>
     </row>
     <row r="9" spans="1:38" ht="18.75" customHeight="1">
       <c r="A9" s="66"/>
@@ -3797,27 +3613,27 @@
       <c r="S11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="T11" s="118" t="s">
+      <c r="T11" s="103" t="s">
         <v>26</v>
       </c>
-      <c r="U11" s="119"/>
-      <c r="V11" s="118" t="s">
+      <c r="U11" s="104"/>
+      <c r="V11" s="103" t="s">
         <v>17</v>
       </c>
-      <c r="W11" s="122"/>
-      <c r="X11" s="122"/>
-      <c r="Y11" s="122"/>
-      <c r="Z11" s="119"/>
-      <c r="AA11" s="124"/>
-      <c r="AB11" s="125"/>
-      <c r="AC11" s="125"/>
-      <c r="AD11" s="125"/>
-      <c r="AE11" s="125"/>
-      <c r="AF11" s="128"/>
-      <c r="AG11" s="125"/>
-      <c r="AH11" s="125"/>
-      <c r="AI11" s="125"/>
-      <c r="AJ11" s="125"/>
+      <c r="W11" s="107"/>
+      <c r="X11" s="107"/>
+      <c r="Y11" s="107"/>
+      <c r="Z11" s="104"/>
+      <c r="AA11" s="109"/>
+      <c r="AB11" s="110"/>
+      <c r="AC11" s="110"/>
+      <c r="AD11" s="110"/>
+      <c r="AE11" s="110"/>
+      <c r="AF11" s="113"/>
+      <c r="AG11" s="110"/>
+      <c r="AH11" s="110"/>
+      <c r="AI11" s="110"/>
+      <c r="AJ11" s="110"/>
       <c r="AK11" s="67"/>
     </row>
     <row r="12" spans="1:38" ht="40.5" customHeight="1" thickBot="1">
@@ -3840,69 +3656,69 @@
       <c r="Q12" s="54"/>
       <c r="R12" s="55"/>
       <c r="S12" s="47"/>
-      <c r="T12" s="120"/>
-      <c r="U12" s="121"/>
-      <c r="V12" s="120"/>
-      <c r="W12" s="123"/>
-      <c r="X12" s="123"/>
-      <c r="Y12" s="123"/>
-      <c r="Z12" s="121"/>
-      <c r="AA12" s="126"/>
-      <c r="AB12" s="127"/>
-      <c r="AC12" s="127"/>
-      <c r="AD12" s="127"/>
-      <c r="AE12" s="127"/>
-      <c r="AF12" s="127"/>
-      <c r="AG12" s="127"/>
-      <c r="AH12" s="127"/>
-      <c r="AI12" s="127"/>
-      <c r="AJ12" s="127"/>
+      <c r="T12" s="105"/>
+      <c r="U12" s="106"/>
+      <c r="V12" s="105"/>
+      <c r="W12" s="108"/>
+      <c r="X12" s="108"/>
+      <c r="Y12" s="108"/>
+      <c r="Z12" s="106"/>
+      <c r="AA12" s="111"/>
+      <c r="AB12" s="112"/>
+      <c r="AC12" s="112"/>
+      <c r="AD12" s="112"/>
+      <c r="AE12" s="112"/>
+      <c r="AF12" s="112"/>
+      <c r="AG12" s="112"/>
+      <c r="AH12" s="112"/>
+      <c r="AI12" s="112"/>
+      <c r="AJ12" s="112"/>
       <c r="AK12" s="67"/>
     </row>
     <row r="13" spans="1:38" ht="23.25" customHeight="1" thickBot="1">
       <c r="A13" s="66"/>
-      <c r="B13" s="114" t="s">
+      <c r="B13" s="136" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="115"/>
-      <c r="D13" s="115"/>
-      <c r="E13" s="115"/>
-      <c r="F13" s="115"/>
-      <c r="G13" s="115"/>
-      <c r="H13" s="115"/>
-      <c r="I13" s="115"/>
-      <c r="J13" s="115"/>
-      <c r="K13" s="115"/>
-      <c r="L13" s="115"/>
-      <c r="M13" s="115"/>
-      <c r="N13" s="115"/>
-      <c r="O13" s="115"/>
-      <c r="P13" s="115"/>
-      <c r="Q13" s="115"/>
-      <c r="R13" s="115"/>
-      <c r="S13" s="115"/>
-      <c r="T13" s="115"/>
-      <c r="U13" s="115"/>
-      <c r="V13" s="115"/>
-      <c r="W13" s="115"/>
-      <c r="X13" s="115"/>
-      <c r="Y13" s="115"/>
-      <c r="Z13" s="115"/>
-      <c r="AA13" s="115"/>
-      <c r="AB13" s="115"/>
-      <c r="AC13" s="115"/>
-      <c r="AD13" s="115"/>
-      <c r="AE13" s="115"/>
-      <c r="AF13" s="115"/>
-      <c r="AG13" s="115"/>
-      <c r="AH13" s="115"/>
-      <c r="AI13" s="115"/>
-      <c r="AJ13" s="116"/>
+      <c r="C13" s="137"/>
+      <c r="D13" s="137"/>
+      <c r="E13" s="137"/>
+      <c r="F13" s="137"/>
+      <c r="G13" s="137"/>
+      <c r="H13" s="137"/>
+      <c r="I13" s="137"/>
+      <c r="J13" s="137"/>
+      <c r="K13" s="137"/>
+      <c r="L13" s="137"/>
+      <c r="M13" s="137"/>
+      <c r="N13" s="137"/>
+      <c r="O13" s="137"/>
+      <c r="P13" s="137"/>
+      <c r="Q13" s="137"/>
+      <c r="R13" s="137"/>
+      <c r="S13" s="137"/>
+      <c r="T13" s="137"/>
+      <c r="U13" s="137"/>
+      <c r="V13" s="137"/>
+      <c r="W13" s="137"/>
+      <c r="X13" s="137"/>
+      <c r="Y13" s="137"/>
+      <c r="Z13" s="137"/>
+      <c r="AA13" s="137"/>
+      <c r="AB13" s="137"/>
+      <c r="AC13" s="137"/>
+      <c r="AD13" s="137"/>
+      <c r="AE13" s="137"/>
+      <c r="AF13" s="137"/>
+      <c r="AG13" s="137"/>
+      <c r="AH13" s="137"/>
+      <c r="AI13" s="137"/>
+      <c r="AJ13" s="138"/>
       <c r="AK13" s="67"/>
     </row>
     <row r="14" spans="1:38" ht="25.5" customHeight="1">
       <c r="A14" s="66"/>
-      <c r="B14" s="106" t="s">
+      <c r="B14" s="128" t="s">
         <v>16</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -3945,7 +3761,7 @@
     </row>
     <row r="15" spans="1:38" ht="60.75" customHeight="1" thickBot="1">
       <c r="A15" s="66"/>
-      <c r="B15" s="107"/>
+      <c r="B15" s="129"/>
       <c r="C15" s="6" t="s">
         <v>29</v>
       </c>
@@ -4006,30 +3822,30 @@
       <c r="Q16" s="61"/>
       <c r="R16" s="61"/>
       <c r="S16" s="61"/>
-      <c r="T16" s="108" t="s">
+      <c r="T16" s="130" t="s">
         <v>28</v>
       </c>
-      <c r="U16" s="108"/>
-      <c r="V16" s="108"/>
-      <c r="W16" s="108"/>
-      <c r="X16" s="108"/>
-      <c r="Y16" s="108"/>
-      <c r="Z16" s="108"/>
-      <c r="AA16" s="108"/>
-      <c r="AB16" s="108"/>
-      <c r="AC16" s="108"/>
-      <c r="AD16" s="108"/>
-      <c r="AE16" s="108"/>
-      <c r="AF16" s="108"/>
-      <c r="AG16" s="108"/>
-      <c r="AH16" s="108"/>
-      <c r="AI16" s="108"/>
-      <c r="AJ16" s="108"/>
+      <c r="U16" s="130"/>
+      <c r="V16" s="130"/>
+      <c r="W16" s="130"/>
+      <c r="X16" s="130"/>
+      <c r="Y16" s="130"/>
+      <c r="Z16" s="130"/>
+      <c r="AA16" s="130"/>
+      <c r="AB16" s="130"/>
+      <c r="AC16" s="130"/>
+      <c r="AD16" s="130"/>
+      <c r="AE16" s="130"/>
+      <c r="AF16" s="130"/>
+      <c r="AG16" s="130"/>
+      <c r="AH16" s="130"/>
+      <c r="AI16" s="130"/>
+      <c r="AJ16" s="130"/>
       <c r="AK16" s="67"/>
     </row>
     <row r="17" spans="1:37" ht="25.5" customHeight="1">
       <c r="A17" s="66"/>
-      <c r="B17" s="106" t="s">
+      <c r="B17" s="128" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -4051,32 +3867,32 @@
       <c r="Q17" s="84"/>
       <c r="R17" s="87"/>
       <c r="S17" s="25"/>
-      <c r="T17" s="106" t="s">
+      <c r="T17" s="128" t="s">
         <v>18</v>
       </c>
-      <c r="U17" s="134" t="s">
+      <c r="U17" s="119" t="s">
         <v>43</v>
       </c>
-      <c r="V17" s="135"/>
-      <c r="W17" s="135"/>
-      <c r="X17" s="135"/>
-      <c r="Y17" s="135"/>
-      <c r="Z17" s="135"/>
-      <c r="AA17" s="135"/>
-      <c r="AB17" s="135"/>
-      <c r="AC17" s="135"/>
-      <c r="AD17" s="135"/>
-      <c r="AE17" s="135"/>
-      <c r="AF17" s="135"/>
-      <c r="AG17" s="135"/>
-      <c r="AH17" s="135"/>
-      <c r="AI17" s="135"/>
-      <c r="AJ17" s="136"/>
+      <c r="V17" s="120"/>
+      <c r="W17" s="120"/>
+      <c r="X17" s="120"/>
+      <c r="Y17" s="120"/>
+      <c r="Z17" s="120"/>
+      <c r="AA17" s="120"/>
+      <c r="AB17" s="120"/>
+      <c r="AC17" s="120"/>
+      <c r="AD17" s="120"/>
+      <c r="AE17" s="120"/>
+      <c r="AF17" s="120"/>
+      <c r="AG17" s="120"/>
+      <c r="AH17" s="120"/>
+      <c r="AI17" s="120"/>
+      <c r="AJ17" s="121"/>
       <c r="AK17" s="67"/>
     </row>
     <row r="18" spans="1:37" ht="37.5" customHeight="1" thickBot="1">
       <c r="A18" s="66"/>
-      <c r="B18" s="107"/>
+      <c r="B18" s="129"/>
       <c r="C18" s="6" t="s">
         <v>4</v>
       </c>
@@ -4098,28 +3914,28 @@
       <c r="Q18" s="83"/>
       <c r="R18" s="89"/>
       <c r="S18" s="25"/>
-      <c r="T18" s="109"/>
-      <c r="U18" s="137"/>
-      <c r="V18" s="138"/>
-      <c r="W18" s="138"/>
-      <c r="X18" s="138"/>
-      <c r="Y18" s="138"/>
-      <c r="Z18" s="138"/>
-      <c r="AA18" s="138"/>
-      <c r="AB18" s="138"/>
-      <c r="AC18" s="138"/>
-      <c r="AD18" s="138"/>
-      <c r="AE18" s="138"/>
-      <c r="AF18" s="138"/>
-      <c r="AG18" s="138"/>
-      <c r="AH18" s="138"/>
-      <c r="AI18" s="138"/>
-      <c r="AJ18" s="139"/>
+      <c r="T18" s="131"/>
+      <c r="U18" s="122"/>
+      <c r="V18" s="123"/>
+      <c r="W18" s="123"/>
+      <c r="X18" s="123"/>
+      <c r="Y18" s="123"/>
+      <c r="Z18" s="123"/>
+      <c r="AA18" s="123"/>
+      <c r="AB18" s="123"/>
+      <c r="AC18" s="123"/>
+      <c r="AD18" s="123"/>
+      <c r="AE18" s="123"/>
+      <c r="AF18" s="123"/>
+      <c r="AG18" s="123"/>
+      <c r="AH18" s="123"/>
+      <c r="AI18" s="123"/>
+      <c r="AJ18" s="124"/>
       <c r="AK18" s="67"/>
     </row>
     <row r="19" spans="1:37" ht="25.5" customHeight="1" thickBot="1">
       <c r="A19" s="66"/>
-      <c r="B19" s="106" t="s">
+      <c r="B19" s="128" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="5" t="s">
@@ -4141,28 +3957,28 @@
       <c r="Q19" s="84"/>
       <c r="R19" s="87"/>
       <c r="S19" s="25"/>
-      <c r="T19" s="107"/>
-      <c r="U19" s="140"/>
-      <c r="V19" s="141"/>
-      <c r="W19" s="141"/>
-      <c r="X19" s="141"/>
-      <c r="Y19" s="141"/>
-      <c r="Z19" s="141"/>
-      <c r="AA19" s="141"/>
-      <c r="AB19" s="141"/>
-      <c r="AC19" s="141"/>
-      <c r="AD19" s="141"/>
-      <c r="AE19" s="141"/>
-      <c r="AF19" s="141"/>
-      <c r="AG19" s="141"/>
-      <c r="AH19" s="141"/>
-      <c r="AI19" s="141"/>
-      <c r="AJ19" s="142"/>
+      <c r="T19" s="129"/>
+      <c r="U19" s="125"/>
+      <c r="V19" s="126"/>
+      <c r="W19" s="126"/>
+      <c r="X19" s="126"/>
+      <c r="Y19" s="126"/>
+      <c r="Z19" s="126"/>
+      <c r="AA19" s="126"/>
+      <c r="AB19" s="126"/>
+      <c r="AC19" s="126"/>
+      <c r="AD19" s="126"/>
+      <c r="AE19" s="126"/>
+      <c r="AF19" s="126"/>
+      <c r="AG19" s="126"/>
+      <c r="AH19" s="126"/>
+      <c r="AI19" s="126"/>
+      <c r="AJ19" s="127"/>
       <c r="AK19" s="67"/>
     </row>
     <row r="20" spans="1:37" ht="37.5" customHeight="1" thickBot="1">
       <c r="A20" s="66"/>
-      <c r="B20" s="107"/>
+      <c r="B20" s="129"/>
       <c r="C20" s="6" t="s">
         <v>4</v>
       </c>
@@ -4338,13 +4154,13 @@
       <c r="I24" s="26"/>
       <c r="J24" s="26"/>
       <c r="K24" s="26"/>
-      <c r="L24" s="133" t="s">
+      <c r="L24" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="M24" s="133"/>
-      <c r="N24" s="133"/>
-      <c r="O24" s="133"/>
-      <c r="P24" s="133"/>
+      <c r="M24" s="118"/>
+      <c r="N24" s="118"/>
+      <c r="O24" s="118"/>
+      <c r="P24" s="118"/>
       <c r="Q24" s="27" t="s">
         <v>30</v>
       </c>
@@ -4498,12 +4314,12 @@
     </row>
     <row r="28" spans="1:37" ht="11.25" customHeight="1">
       <c r="A28" s="66"/>
-      <c r="B28" s="102" t="s">
+      <c r="B28" s="139" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="103"/>
-      <c r="D28" s="103"/>
-      <c r="E28" s="104"/>
+      <c r="C28" s="140"/>
+      <c r="D28" s="140"/>
+      <c r="E28" s="141"/>
       <c r="F28" s="101"/>
       <c r="G28" s="101"/>
       <c r="H28" s="101"/>
@@ -4619,12 +4435,12 @@
     </row>
     <row r="31" spans="1:37" ht="11.25" customHeight="1">
       <c r="A31" s="66"/>
-      <c r="B31" s="102" t="s">
+      <c r="B31" s="139" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="103"/>
-      <c r="D31" s="103"/>
-      <c r="E31" s="103"/>
+      <c r="C31" s="140"/>
+      <c r="D31" s="140"/>
+      <c r="E31" s="140"/>
       <c r="F31" s="101"/>
       <c r="G31" s="101"/>
       <c r="H31" s="101"/>
@@ -4738,12 +4554,12 @@
     </row>
     <row r="34" spans="1:37" ht="11.25" customHeight="1">
       <c r="A34" s="66"/>
-      <c r="B34" s="102" t="s">
+      <c r="B34" s="139" t="s">
         <v>11</v>
       </c>
-      <c r="C34" s="103"/>
-      <c r="D34" s="103"/>
-      <c r="E34" s="103"/>
+      <c r="C34" s="140"/>
+      <c r="D34" s="140"/>
+      <c r="E34" s="140"/>
       <c r="F34" s="101"/>
       <c r="G34" s="101"/>
       <c r="H34" s="101"/>
@@ -4755,7 +4571,7 @@
       <c r="N34" s="101"/>
       <c r="O34" s="101"/>
       <c r="P34" s="101"/>
-      <c r="Q34" s="105" t="s">
+      <c r="Q34" s="142" t="s">
         <v>6</v>
       </c>
       <c r="R34" s="37"/>
@@ -4796,7 +4612,7 @@
       <c r="N35" s="101"/>
       <c r="O35" s="101"/>
       <c r="P35" s="101"/>
-      <c r="Q35" s="105"/>
+      <c r="Q35" s="142"/>
       <c r="R35" s="37"/>
       <c r="S35" s="25"/>
       <c r="T35" s="25"/>
@@ -4861,12 +4677,12 @@
     </row>
     <row r="37" spans="1:37" ht="11.25" customHeight="1">
       <c r="A37" s="66"/>
-      <c r="B37" s="102" t="s">
+      <c r="B37" s="139" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="103"/>
-      <c r="D37" s="103"/>
-      <c r="E37" s="104"/>
+      <c r="C37" s="140"/>
+      <c r="D37" s="140"/>
+      <c r="E37" s="141"/>
       <c r="F37" s="101"/>
       <c r="G37" s="101"/>
       <c r="H37" s="101"/>
@@ -5140,6 +4956,22 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="F36:Q38"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="F27:Q29"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="F30:Q32"/>
+    <mergeCell ref="F33:P35"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="Q34:Q35"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="T16:AJ16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="T17:T19"/>
+    <mergeCell ref="B6:AK8"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B13:AJ13"/>
     <mergeCell ref="F25:J26"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="T11:U12"/>
@@ -5150,22 +4982,6 @@
     <mergeCell ref="AI2:AK2"/>
     <mergeCell ref="L24:P24"/>
     <mergeCell ref="U17:AJ19"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="T16:AJ16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="T17:T19"/>
-    <mergeCell ref="B6:AK8"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B13:AJ13"/>
-    <mergeCell ref="F36:Q38"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="F27:Q29"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="F30:Q32"/>
-    <mergeCell ref="F33:P35"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="Q34:Q35"/>
-    <mergeCell ref="B31:E31"/>
   </mergeCells>
   <phoneticPr fontId="15"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
HoaNT2 : fix template #11617
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/ローマ字氏名届_帳票テンプレート.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/ローマ字氏名届_帳票テンプレート.xlsx
@@ -399,14 +399,14 @@
         <family val="3"/>
         <charset val="128"/>
       </rPr>
-      <t>その他　理由（                                                                                                                                                   ）</t>
+      <t xml:space="preserve">その他　理由                                                                                   </t>
     </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="29">
     <font>
       <sz val="11"/>
@@ -1141,9 +1141,336 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1156,35 +1483,47 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1192,120 +1531,12 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1315,257 +1546,26 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1604,7 +1604,7 @@
         <xdr:cNvPr id="19768" name="グループ化 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-0000384D0000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000384D0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1625,7 +1625,7 @@
           <xdr:cNvPr id="19769" name="グループ化 17">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-0000394D0000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000394D0000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1646,7 +1646,7 @@
             <xdr:cNvPr id="27" name="Text Box 13">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001B000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001B000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1720,7 +1720,7 @@
             <xdr:cNvPr id="19776" name="Group 15">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-0000404D0000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000404D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1741,7 +1741,7 @@
               <xdr:cNvPr id="19777" name="Line 10">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-0000414D0000}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000414D0000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -1780,7 +1780,7 @@
               <xdr:cNvPr id="19778" name="Line 11">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-0000424D0000}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000424D0000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -1819,7 +1819,7 @@
               <xdr:cNvPr id="19779" name="Line 12">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-0000434D0000}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000434D0000}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -1860,7 +1860,7 @@
           <xdr:cNvPr id="21" name="Text Box 13">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000015000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1934,7 +1934,7 @@
           <xdr:cNvPr id="19771" name="Group 15">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003B4D0000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003B4D0000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1955,7 +1955,7 @@
             <xdr:cNvPr id="19772" name="Line 10">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003C4D0000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003C4D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1994,7 +1994,7 @@
             <xdr:cNvPr id="19773" name="Line 11">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003D4D0000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003D4D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2033,7 +2033,7 @@
             <xdr:cNvPr id="19774" name="Line 12">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00003E4D0000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003E4D0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2089,7 +2089,7 @@
         <xdr:cNvPr id="5" name="A1_3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9F27A5BA-FC88-423C-8EC5-3992C20BB050}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F27A5BA-FC88-423C-8EC5-3992C20BB050}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2155,7 +2155,7 @@
         <xdr:cNvPr id="19" name="A1_4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{398ECDA3-7C25-4682-847B-CEDFF80DF526}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{398ECDA3-7C25-4682-847B-CEDFF80DF526}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2221,7 +2221,7 @@
         <xdr:cNvPr id="20" name="A1_5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C9FF28E8-8FE8-407B-B415-209FAF6ED4F8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9FF28E8-8FE8-407B-B415-209FAF6ED4F8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2287,7 +2287,7 @@
         <xdr:cNvPr id="22" name="A1_6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0A8DDCC9-04FA-4994-92F2-789B01B7EBD6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A8DDCC9-04FA-4994-92F2-789B01B7EBD6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2353,7 +2353,7 @@
         <xdr:cNvPr id="24" name="A4_1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F0C2BFF4-3A46-455F-B24D-225727E21669}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0C2BFF4-3A46-455F-B24D-225727E21669}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2418,7 +2418,7 @@
         <xdr:cNvPr id="25" name="A4_2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BA76FBB9-1F09-48C5-9A8C-FF34E5CAA19B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA76FBB9-1F09-48C5-9A8C-FF34E5CAA19B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2483,7 +2483,7 @@
         <xdr:cNvPr id="26" name="A4_3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{26870D4B-17DE-46D7-8C98-692A53DB1515}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26870D4B-17DE-46D7-8C98-692A53DB1515}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2548,7 +2548,7 @@
         <xdr:cNvPr id="28" name="A4_4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BB0C932C-3D2F-4F9C-A973-9CD9ADC7673A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB0C932C-3D2F-4F9C-A973-9CD9ADC7673A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2597,23 +2597,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>276224</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>4080</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>458561</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>323849</xdr:colOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>51705</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>247650</xdr:rowOff>
+      <xdr:rowOff>220436</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="4" name="A4_5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A8226EA9-DDD1-4CF2-AA93-DFB1552F716E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8226EA9-DDD1-4CF2-AA93-DFB1552F716E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2621,8 +2621,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8334374" y="5991225"/>
-          <a:ext cx="2447925" cy="238125"/>
+          <a:off x="8345259" y="6023882"/>
+          <a:ext cx="2428875" cy="238125"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2954,7 +2954,9 @@
   </sheetPr>
   <dimension ref="A1:AL43"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="106" zoomScaleSheetLayoutView="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="106" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection activeCell="Z20" sqref="Z20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.140625" defaultRowHeight="13.5"/>
   <cols>
@@ -2998,11 +3000,11 @@
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
       <c r="AE1" s="1"/>
-      <c r="AI1" s="3">
+      <c r="AI1" s="101">
         <v>72073</v>
       </c>
-      <c r="AJ1" s="3"/>
-      <c r="AK1" s="3"/>
+      <c r="AJ1" s="101"/>
+      <c r="AK1" s="101"/>
       <c r="AL1" s="1"/>
     </row>
     <row r="2" spans="1:38" ht="26.25" customHeight="1">
@@ -3037,16 +3039,16 @@
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
       <c r="AE2" s="1"/>
-      <c r="AF2" s="4" t="s">
+      <c r="AF2" s="113" t="s">
         <v>17</v>
       </c>
-      <c r="AG2" s="5"/>
-      <c r="AH2" s="6"/>
-      <c r="AI2" s="7" t="s">
+      <c r="AG2" s="114"/>
+      <c r="AH2" s="115"/>
+      <c r="AI2" s="116" t="s">
         <v>18</v>
       </c>
-      <c r="AJ2" s="5"/>
-      <c r="AK2" s="6"/>
+      <c r="AJ2" s="114"/>
+      <c r="AK2" s="115"/>
       <c r="AL2" s="1"/>
     </row>
     <row r="3" spans="1:38" ht="26.25" customHeight="1">
@@ -3081,12 +3083,12 @@
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
       <c r="AE3" s="1"/>
-      <c r="AF3" s="8"/>
-      <c r="AG3" s="9"/>
-      <c r="AH3" s="10"/>
-      <c r="AI3" s="8"/>
-      <c r="AJ3" s="9"/>
-      <c r="AK3" s="10"/>
+      <c r="AF3" s="3"/>
+      <c r="AG3" s="4"/>
+      <c r="AH3" s="5"/>
+      <c r="AI3" s="3"/>
+      <c r="AJ3" s="4"/>
+      <c r="AK3" s="5"/>
       <c r="AL3" s="1"/>
     </row>
     <row r="4" spans="1:38" ht="26.25" customHeight="1">
@@ -3121,174 +3123,174 @@
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
       <c r="AE4" s="1"/>
-      <c r="AF4" s="11"/>
-      <c r="AG4" s="12"/>
-      <c r="AH4" s="13"/>
-      <c r="AI4" s="11"/>
-      <c r="AJ4" s="12"/>
-      <c r="AK4" s="13"/>
+      <c r="AF4" s="6"/>
+      <c r="AG4" s="7"/>
+      <c r="AH4" s="8"/>
+      <c r="AI4" s="6"/>
+      <c r="AJ4" s="7"/>
+      <c r="AK4" s="8"/>
       <c r="AL4" s="1"/>
     </row>
     <row r="5" spans="1:38" ht="18.75" customHeight="1">
-      <c r="A5" s="14"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="14"/>
-      <c r="S5" s="14"/>
-      <c r="T5" s="14"/>
-      <c r="U5" s="14"/>
-      <c r="V5" s="14"/>
-      <c r="W5" s="14"/>
-      <c r="X5" s="14"/>
-      <c r="Y5" s="12"/>
-      <c r="Z5" s="12"/>
-      <c r="AA5" s="12"/>
-      <c r="AB5" s="12"/>
-      <c r="AC5" s="12"/>
-      <c r="AD5" s="12"/>
-      <c r="AE5" s="12"/>
-      <c r="AF5" s="12"/>
-      <c r="AG5" s="12"/>
-      <c r="AH5" s="12"/>
-      <c r="AI5" s="12"/>
-      <c r="AJ5" s="12"/>
-      <c r="AK5" s="12"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="9"/>
+      <c r="V5" s="9"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="9"/>
+      <c r="Y5" s="7"/>
+      <c r="Z5" s="7"/>
+      <c r="AA5" s="7"/>
+      <c r="AB5" s="7"/>
+      <c r="AC5" s="7"/>
+      <c r="AD5" s="7"/>
+      <c r="AE5" s="7"/>
+      <c r="AF5" s="7"/>
+      <c r="AG5" s="7"/>
+      <c r="AH5" s="7"/>
+      <c r="AI5" s="7"/>
+      <c r="AJ5" s="7"/>
+      <c r="AK5" s="7"/>
     </row>
     <row r="6" spans="1:38" ht="13.5" customHeight="1">
-      <c r="A6" s="17"/>
-      <c r="B6" s="18" t="s">
+      <c r="A6" s="12"/>
+      <c r="B6" s="131" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18"/>
-      <c r="O6" s="18"/>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="18"/>
-      <c r="S6" s="18"/>
-      <c r="T6" s="18"/>
-      <c r="U6" s="18"/>
-      <c r="V6" s="18"/>
-      <c r="W6" s="18"/>
-      <c r="X6" s="18"/>
-      <c r="Y6" s="18"/>
-      <c r="Z6" s="18"/>
-      <c r="AA6" s="18"/>
-      <c r="AB6" s="18"/>
-      <c r="AC6" s="18"/>
-      <c r="AD6" s="18"/>
-      <c r="AE6" s="18"/>
-      <c r="AF6" s="18"/>
-      <c r="AG6" s="18"/>
-      <c r="AH6" s="18"/>
-      <c r="AI6" s="18"/>
-      <c r="AJ6" s="18"/>
-      <c r="AK6" s="19"/>
+      <c r="C6" s="131"/>
+      <c r="D6" s="131"/>
+      <c r="E6" s="131"/>
+      <c r="F6" s="131"/>
+      <c r="G6" s="131"/>
+      <c r="H6" s="131"/>
+      <c r="I6" s="131"/>
+      <c r="J6" s="131"/>
+      <c r="K6" s="131"/>
+      <c r="L6" s="131"/>
+      <c r="M6" s="131"/>
+      <c r="N6" s="131"/>
+      <c r="O6" s="131"/>
+      <c r="P6" s="131"/>
+      <c r="Q6" s="131"/>
+      <c r="R6" s="131"/>
+      <c r="S6" s="131"/>
+      <c r="T6" s="131"/>
+      <c r="U6" s="131"/>
+      <c r="V6" s="131"/>
+      <c r="W6" s="131"/>
+      <c r="X6" s="131"/>
+      <c r="Y6" s="131"/>
+      <c r="Z6" s="131"/>
+      <c r="AA6" s="131"/>
+      <c r="AB6" s="131"/>
+      <c r="AC6" s="131"/>
+      <c r="AD6" s="131"/>
+      <c r="AE6" s="131"/>
+      <c r="AF6" s="131"/>
+      <c r="AG6" s="131"/>
+      <c r="AH6" s="131"/>
+      <c r="AI6" s="131"/>
+      <c r="AJ6" s="131"/>
+      <c r="AK6" s="132"/>
     </row>
     <row r="7" spans="1:38" ht="13.5" customHeight="1">
-      <c r="A7" s="20"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21"/>
-      <c r="O7" s="21"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="21"/>
-      <c r="R7" s="21"/>
-      <c r="S7" s="21"/>
-      <c r="T7" s="21"/>
-      <c r="U7" s="21"/>
-      <c r="V7" s="21"/>
-      <c r="W7" s="21"/>
-      <c r="X7" s="21"/>
-      <c r="Y7" s="21"/>
-      <c r="Z7" s="21"/>
-      <c r="AA7" s="21"/>
-      <c r="AB7" s="21"/>
-      <c r="AC7" s="21"/>
-      <c r="AD7" s="21"/>
-      <c r="AE7" s="21"/>
-      <c r="AF7" s="21"/>
-      <c r="AG7" s="21"/>
-      <c r="AH7" s="21"/>
-      <c r="AI7" s="21"/>
-      <c r="AJ7" s="21"/>
-      <c r="AK7" s="22"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="133"/>
+      <c r="C7" s="133"/>
+      <c r="D7" s="133"/>
+      <c r="E7" s="133"/>
+      <c r="F7" s="133"/>
+      <c r="G7" s="133"/>
+      <c r="H7" s="133"/>
+      <c r="I7" s="133"/>
+      <c r="J7" s="133"/>
+      <c r="K7" s="133"/>
+      <c r="L7" s="133"/>
+      <c r="M7" s="133"/>
+      <c r="N7" s="133"/>
+      <c r="O7" s="133"/>
+      <c r="P7" s="133"/>
+      <c r="Q7" s="133"/>
+      <c r="R7" s="133"/>
+      <c r="S7" s="133"/>
+      <c r="T7" s="133"/>
+      <c r="U7" s="133"/>
+      <c r="V7" s="133"/>
+      <c r="W7" s="133"/>
+      <c r="X7" s="133"/>
+      <c r="Y7" s="133"/>
+      <c r="Z7" s="133"/>
+      <c r="AA7" s="133"/>
+      <c r="AB7" s="133"/>
+      <c r="AC7" s="133"/>
+      <c r="AD7" s="133"/>
+      <c r="AE7" s="133"/>
+      <c r="AF7" s="133"/>
+      <c r="AG7" s="133"/>
+      <c r="AH7" s="133"/>
+      <c r="AI7" s="133"/>
+      <c r="AJ7" s="133"/>
+      <c r="AK7" s="134"/>
     </row>
     <row r="8" spans="1:38" ht="13.5" customHeight="1">
-      <c r="A8" s="20"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="21"/>
-      <c r="O8" s="21"/>
-      <c r="P8" s="21"/>
-      <c r="Q8" s="21"/>
-      <c r="R8" s="21"/>
-      <c r="S8" s="21"/>
-      <c r="T8" s="21"/>
-      <c r="U8" s="21"/>
-      <c r="V8" s="21"/>
-      <c r="W8" s="21"/>
-      <c r="X8" s="21"/>
-      <c r="Y8" s="21"/>
-      <c r="Z8" s="21"/>
-      <c r="AA8" s="21"/>
-      <c r="AB8" s="21"/>
-      <c r="AC8" s="21"/>
-      <c r="AD8" s="21"/>
-      <c r="AE8" s="21"/>
-      <c r="AF8" s="21"/>
-      <c r="AG8" s="21"/>
-      <c r="AH8" s="21"/>
-      <c r="AI8" s="21"/>
-      <c r="AJ8" s="21"/>
-      <c r="AK8" s="22"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="133"/>
+      <c r="C8" s="133"/>
+      <c r="D8" s="133"/>
+      <c r="E8" s="133"/>
+      <c r="F8" s="133"/>
+      <c r="G8" s="133"/>
+      <c r="H8" s="133"/>
+      <c r="I8" s="133"/>
+      <c r="J8" s="133"/>
+      <c r="K8" s="133"/>
+      <c r="L8" s="133"/>
+      <c r="M8" s="133"/>
+      <c r="N8" s="133"/>
+      <c r="O8" s="133"/>
+      <c r="P8" s="133"/>
+      <c r="Q8" s="133"/>
+      <c r="R8" s="133"/>
+      <c r="S8" s="133"/>
+      <c r="T8" s="133"/>
+      <c r="U8" s="133"/>
+      <c r="V8" s="133"/>
+      <c r="W8" s="133"/>
+      <c r="X8" s="133"/>
+      <c r="Y8" s="133"/>
+      <c r="Z8" s="133"/>
+      <c r="AA8" s="133"/>
+      <c r="AB8" s="133"/>
+      <c r="AC8" s="133"/>
+      <c r="AD8" s="133"/>
+      <c r="AE8" s="133"/>
+      <c r="AF8" s="133"/>
+      <c r="AG8" s="133"/>
+      <c r="AH8" s="133"/>
+      <c r="AI8" s="133"/>
+      <c r="AJ8" s="133"/>
+      <c r="AK8" s="134"/>
     </row>
     <row r="9" spans="1:38" ht="18.75" customHeight="1">
-      <c r="A9" s="20"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -3324,469 +3326,469 @@
       <c r="AH9" s="1"/>
       <c r="AI9" s="1"/>
       <c r="AJ9" s="1"/>
-      <c r="AK9" s="23"/>
+      <c r="AK9" s="14"/>
     </row>
     <row r="10" spans="1:38" ht="28.5" customHeight="1" thickBot="1">
-      <c r="A10" s="20"/>
-      <c r="B10" s="24" t="s">
+      <c r="A10" s="13"/>
+      <c r="B10" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="24" t="s">
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
-      <c r="O10" s="25"/>
-      <c r="P10" s="25"/>
-      <c r="Q10" s="25"/>
-      <c r="R10" s="25"/>
-      <c r="S10" s="26"/>
-      <c r="T10" s="24" t="s">
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="16"/>
+      <c r="S10" s="17"/>
+      <c r="T10" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="U10" s="26"/>
-      <c r="V10" s="27" t="s">
+      <c r="U10" s="17"/>
+      <c r="V10" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="W10" s="28"/>
-      <c r="X10" s="28"/>
-      <c r="Y10" s="28"/>
-      <c r="Z10" s="29"/>
-      <c r="AA10" s="30" t="s">
+      <c r="W10" s="19"/>
+      <c r="X10" s="19"/>
+      <c r="Y10" s="19"/>
+      <c r="Z10" s="20"/>
+      <c r="AA10" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="AB10" s="30"/>
-      <c r="AC10" s="30"/>
-      <c r="AD10" s="30"/>
-      <c r="AE10" s="30"/>
-      <c r="AF10" s="30"/>
-      <c r="AG10" s="30"/>
-      <c r="AH10" s="30"/>
-      <c r="AI10" s="30"/>
-      <c r="AJ10" s="30"/>
-      <c r="AK10" s="23"/>
+      <c r="AB10" s="21"/>
+      <c r="AC10" s="21"/>
+      <c r="AD10" s="21"/>
+      <c r="AE10" s="21"/>
+      <c r="AF10" s="21"/>
+      <c r="AG10" s="21"/>
+      <c r="AH10" s="21"/>
+      <c r="AI10" s="21"/>
+      <c r="AJ10" s="21"/>
+      <c r="AK10" s="14"/>
     </row>
     <row r="11" spans="1:38" ht="13.5" customHeight="1">
-      <c r="A11" s="20"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="34"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="36"/>
-      <c r="N11" s="36"/>
-      <c r="O11" s="37" t="s">
+      <c r="A11" s="13"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="27"/>
+      <c r="N11" s="27"/>
+      <c r="O11" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="P11" s="38"/>
-      <c r="Q11" s="37" t="s">
+      <c r="P11" s="29"/>
+      <c r="Q11" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="R11" s="38"/>
-      <c r="S11" s="39" t="s">
+      <c r="R11" s="29"/>
+      <c r="S11" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="T11" s="40" t="s">
+      <c r="T11" s="102" t="s">
         <v>20</v>
       </c>
-      <c r="U11" s="41"/>
-      <c r="V11" s="40" t="s">
+      <c r="U11" s="103"/>
+      <c r="V11" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="W11" s="42"/>
-      <c r="X11" s="42"/>
-      <c r="Y11" s="42"/>
-      <c r="Z11" s="41"/>
-      <c r="AA11" s="43"/>
-      <c r="AB11" s="44"/>
-      <c r="AC11" s="44"/>
-      <c r="AD11" s="44"/>
-      <c r="AE11" s="44"/>
-      <c r="AF11" s="45"/>
-      <c r="AG11" s="44"/>
-      <c r="AH11" s="44"/>
-      <c r="AI11" s="44"/>
-      <c r="AJ11" s="44"/>
-      <c r="AK11" s="23"/>
+      <c r="W11" s="106"/>
+      <c r="X11" s="106"/>
+      <c r="Y11" s="106"/>
+      <c r="Z11" s="103"/>
+      <c r="AA11" s="108"/>
+      <c r="AB11" s="109"/>
+      <c r="AC11" s="109"/>
+      <c r="AD11" s="109"/>
+      <c r="AE11" s="109"/>
+      <c r="AF11" s="112"/>
+      <c r="AG11" s="109"/>
+      <c r="AH11" s="109"/>
+      <c r="AI11" s="109"/>
+      <c r="AJ11" s="109"/>
+      <c r="AK11" s="14"/>
     </row>
     <row r="12" spans="1:38" ht="40.5" customHeight="1" thickBot="1">
-      <c r="A12" s="20"/>
-      <c r="B12" s="46"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="47"/>
-      <c r="I12" s="47"/>
-      <c r="J12" s="47"/>
-      <c r="K12" s="50"/>
-      <c r="L12" s="46"/>
-      <c r="M12" s="47"/>
-      <c r="N12" s="47"/>
-      <c r="O12" s="51"/>
-      <c r="P12" s="52"/>
-      <c r="Q12" s="51"/>
-      <c r="R12" s="52"/>
-      <c r="S12" s="50"/>
-      <c r="T12" s="53"/>
-      <c r="U12" s="54"/>
-      <c r="V12" s="53"/>
-      <c r="W12" s="55"/>
-      <c r="X12" s="55"/>
-      <c r="Y12" s="55"/>
-      <c r="Z12" s="54"/>
-      <c r="AA12" s="56"/>
-      <c r="AB12" s="57"/>
-      <c r="AC12" s="57"/>
-      <c r="AD12" s="57"/>
-      <c r="AE12" s="57"/>
-      <c r="AF12" s="57"/>
-      <c r="AG12" s="57"/>
-      <c r="AH12" s="57"/>
-      <c r="AI12" s="57"/>
-      <c r="AJ12" s="57"/>
-      <c r="AK12" s="23"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="35"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="32"/>
+      <c r="N12" s="32"/>
+      <c r="O12" s="36"/>
+      <c r="P12" s="37"/>
+      <c r="Q12" s="36"/>
+      <c r="R12" s="37"/>
+      <c r="S12" s="35"/>
+      <c r="T12" s="104"/>
+      <c r="U12" s="105"/>
+      <c r="V12" s="104"/>
+      <c r="W12" s="107"/>
+      <c r="X12" s="107"/>
+      <c r="Y12" s="107"/>
+      <c r="Z12" s="105"/>
+      <c r="AA12" s="110"/>
+      <c r="AB12" s="111"/>
+      <c r="AC12" s="111"/>
+      <c r="AD12" s="111"/>
+      <c r="AE12" s="111"/>
+      <c r="AF12" s="111"/>
+      <c r="AG12" s="111"/>
+      <c r="AH12" s="111"/>
+      <c r="AI12" s="111"/>
+      <c r="AJ12" s="111"/>
+      <c r="AK12" s="14"/>
     </row>
     <row r="13" spans="1:38" ht="23.25" customHeight="1" thickBot="1">
-      <c r="A13" s="20"/>
-      <c r="B13" s="58" t="s">
+      <c r="A13" s="13"/>
+      <c r="B13" s="135" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="59"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="59"/>
-      <c r="G13" s="59"/>
-      <c r="H13" s="59"/>
-      <c r="I13" s="59"/>
-      <c r="J13" s="59"/>
-      <c r="K13" s="59"/>
-      <c r="L13" s="59"/>
-      <c r="M13" s="59"/>
-      <c r="N13" s="59"/>
-      <c r="O13" s="59"/>
-      <c r="P13" s="59"/>
-      <c r="Q13" s="59"/>
-      <c r="R13" s="59"/>
-      <c r="S13" s="59"/>
-      <c r="T13" s="59"/>
-      <c r="U13" s="59"/>
-      <c r="V13" s="59"/>
-      <c r="W13" s="59"/>
-      <c r="X13" s="59"/>
-      <c r="Y13" s="59"/>
-      <c r="Z13" s="59"/>
-      <c r="AA13" s="59"/>
-      <c r="AB13" s="59"/>
-      <c r="AC13" s="59"/>
-      <c r="AD13" s="59"/>
-      <c r="AE13" s="59"/>
-      <c r="AF13" s="59"/>
-      <c r="AG13" s="59"/>
-      <c r="AH13" s="59"/>
-      <c r="AI13" s="59"/>
-      <c r="AJ13" s="60"/>
-      <c r="AK13" s="23"/>
+      <c r="C13" s="136"/>
+      <c r="D13" s="136"/>
+      <c r="E13" s="136"/>
+      <c r="F13" s="136"/>
+      <c r="G13" s="136"/>
+      <c r="H13" s="136"/>
+      <c r="I13" s="136"/>
+      <c r="J13" s="136"/>
+      <c r="K13" s="136"/>
+      <c r="L13" s="136"/>
+      <c r="M13" s="136"/>
+      <c r="N13" s="136"/>
+      <c r="O13" s="136"/>
+      <c r="P13" s="136"/>
+      <c r="Q13" s="136"/>
+      <c r="R13" s="136"/>
+      <c r="S13" s="136"/>
+      <c r="T13" s="136"/>
+      <c r="U13" s="136"/>
+      <c r="V13" s="136"/>
+      <c r="W13" s="136"/>
+      <c r="X13" s="136"/>
+      <c r="Y13" s="136"/>
+      <c r="Z13" s="136"/>
+      <c r="AA13" s="136"/>
+      <c r="AB13" s="136"/>
+      <c r="AC13" s="136"/>
+      <c r="AD13" s="136"/>
+      <c r="AE13" s="136"/>
+      <c r="AF13" s="136"/>
+      <c r="AG13" s="136"/>
+      <c r="AH13" s="136"/>
+      <c r="AI13" s="136"/>
+      <c r="AJ13" s="137"/>
+      <c r="AK13" s="14"/>
     </row>
     <row r="14" spans="1:38" ht="25.5" customHeight="1">
-      <c r="A14" s="20"/>
-      <c r="B14" s="61" t="s">
+      <c r="A14" s="13"/>
+      <c r="B14" s="127" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="62" t="s">
+      <c r="C14" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="63"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="65"/>
-      <c r="G14" s="65"/>
-      <c r="H14" s="65"/>
-      <c r="I14" s="65"/>
-      <c r="J14" s="65"/>
-      <c r="K14" s="65"/>
-      <c r="L14" s="65"/>
-      <c r="M14" s="65"/>
-      <c r="N14" s="65"/>
-      <c r="O14" s="65"/>
-      <c r="P14" s="65"/>
-      <c r="Q14" s="65"/>
-      <c r="R14" s="65"/>
-      <c r="S14" s="65"/>
-      <c r="T14" s="65"/>
-      <c r="U14" s="65"/>
-      <c r="V14" s="65"/>
-      <c r="W14" s="65"/>
-      <c r="X14" s="65"/>
-      <c r="Y14" s="65"/>
-      <c r="Z14" s="65"/>
-      <c r="AA14" s="65"/>
-      <c r="AB14" s="65"/>
-      <c r="AC14" s="65"/>
-      <c r="AD14" s="65"/>
-      <c r="AE14" s="65"/>
-      <c r="AF14" s="65"/>
-      <c r="AG14" s="65"/>
-      <c r="AH14" s="65"/>
-      <c r="AI14" s="65"/>
-      <c r="AJ14" s="66"/>
-      <c r="AK14" s="23"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="41"/>
+      <c r="K14" s="41"/>
+      <c r="L14" s="41"/>
+      <c r="M14" s="41"/>
+      <c r="N14" s="41"/>
+      <c r="O14" s="41"/>
+      <c r="P14" s="41"/>
+      <c r="Q14" s="41"/>
+      <c r="R14" s="41"/>
+      <c r="S14" s="41"/>
+      <c r="T14" s="41"/>
+      <c r="U14" s="41"/>
+      <c r="V14" s="41"/>
+      <c r="W14" s="41"/>
+      <c r="X14" s="41"/>
+      <c r="Y14" s="41"/>
+      <c r="Z14" s="41"/>
+      <c r="AA14" s="41"/>
+      <c r="AB14" s="41"/>
+      <c r="AC14" s="41"/>
+      <c r="AD14" s="41"/>
+      <c r="AE14" s="41"/>
+      <c r="AF14" s="41"/>
+      <c r="AG14" s="41"/>
+      <c r="AH14" s="41"/>
+      <c r="AI14" s="41"/>
+      <c r="AJ14" s="42"/>
+      <c r="AK14" s="14"/>
     </row>
     <row r="15" spans="1:38" ht="60.75" customHeight="1" thickBot="1">
-      <c r="A15" s="20"/>
-      <c r="B15" s="67"/>
-      <c r="C15" s="68" t="s">
+      <c r="A15" s="13"/>
+      <c r="B15" s="128"/>
+      <c r="C15" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="69"/>
-      <c r="E15" s="70"/>
-      <c r="F15" s="71"/>
-      <c r="G15" s="71"/>
-      <c r="H15" s="71"/>
-      <c r="I15" s="71"/>
-      <c r="J15" s="71"/>
-      <c r="K15" s="71"/>
-      <c r="L15" s="71"/>
-      <c r="M15" s="71"/>
-      <c r="N15" s="71"/>
-      <c r="O15" s="71"/>
-      <c r="P15" s="71"/>
-      <c r="Q15" s="71"/>
-      <c r="R15" s="71"/>
-      <c r="S15" s="71"/>
-      <c r="T15" s="71"/>
-      <c r="U15" s="71"/>
-      <c r="V15" s="71"/>
-      <c r="W15" s="71"/>
-      <c r="X15" s="71"/>
-      <c r="Y15" s="71"/>
-      <c r="Z15" s="71"/>
-      <c r="AA15" s="71"/>
-      <c r="AB15" s="71"/>
-      <c r="AC15" s="71"/>
-      <c r="AD15" s="71"/>
-      <c r="AE15" s="71"/>
-      <c r="AF15" s="71"/>
-      <c r="AG15" s="71"/>
-      <c r="AH15" s="71"/>
-      <c r="AI15" s="71"/>
-      <c r="AJ15" s="72"/>
-      <c r="AK15" s="23"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="46"/>
+      <c r="I15" s="46"/>
+      <c r="J15" s="46"/>
+      <c r="K15" s="46"/>
+      <c r="L15" s="46"/>
+      <c r="M15" s="46"/>
+      <c r="N15" s="46"/>
+      <c r="O15" s="46"/>
+      <c r="P15" s="46"/>
+      <c r="Q15" s="46"/>
+      <c r="R15" s="46"/>
+      <c r="S15" s="46"/>
+      <c r="T15" s="46"/>
+      <c r="U15" s="46"/>
+      <c r="V15" s="46"/>
+      <c r="W15" s="46"/>
+      <c r="X15" s="46"/>
+      <c r="Y15" s="46"/>
+      <c r="Z15" s="46"/>
+      <c r="AA15" s="46"/>
+      <c r="AB15" s="46"/>
+      <c r="AC15" s="46"/>
+      <c r="AD15" s="46"/>
+      <c r="AE15" s="46"/>
+      <c r="AF15" s="46"/>
+      <c r="AG15" s="46"/>
+      <c r="AH15" s="46"/>
+      <c r="AI15" s="46"/>
+      <c r="AJ15" s="47"/>
+      <c r="AK15" s="14"/>
     </row>
     <row r="16" spans="1:38" ht="43.5" customHeight="1" thickBot="1">
-      <c r="A16" s="20"/>
-      <c r="B16" s="73" t="s">
+      <c r="A16" s="13"/>
+      <c r="B16" s="138" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="73"/>
-      <c r="D16" s="73"/>
-      <c r="E16" s="73"/>
-      <c r="F16" s="73"/>
-      <c r="G16" s="73"/>
-      <c r="H16" s="73"/>
-      <c r="I16" s="73"/>
-      <c r="J16" s="73"/>
-      <c r="K16" s="73"/>
-      <c r="L16" s="73"/>
-      <c r="M16" s="73"/>
-      <c r="N16" s="73"/>
-      <c r="O16" s="73"/>
-      <c r="P16" s="73"/>
-      <c r="Q16" s="73"/>
-      <c r="R16" s="73"/>
-      <c r="S16" s="73"/>
-      <c r="T16" s="74" t="s">
+      <c r="C16" s="138"/>
+      <c r="D16" s="138"/>
+      <c r="E16" s="138"/>
+      <c r="F16" s="138"/>
+      <c r="G16" s="138"/>
+      <c r="H16" s="138"/>
+      <c r="I16" s="138"/>
+      <c r="J16" s="138"/>
+      <c r="K16" s="138"/>
+      <c r="L16" s="138"/>
+      <c r="M16" s="138"/>
+      <c r="N16" s="138"/>
+      <c r="O16" s="138"/>
+      <c r="P16" s="138"/>
+      <c r="Q16" s="138"/>
+      <c r="R16" s="138"/>
+      <c r="S16" s="138"/>
+      <c r="T16" s="129" t="s">
         <v>22</v>
       </c>
-      <c r="U16" s="74"/>
-      <c r="V16" s="74"/>
-      <c r="W16" s="74"/>
-      <c r="X16" s="74"/>
-      <c r="Y16" s="74"/>
-      <c r="Z16" s="74"/>
-      <c r="AA16" s="74"/>
-      <c r="AB16" s="74"/>
-      <c r="AC16" s="74"/>
-      <c r="AD16" s="74"/>
-      <c r="AE16" s="74"/>
-      <c r="AF16" s="74"/>
-      <c r="AG16" s="74"/>
-      <c r="AH16" s="74"/>
-      <c r="AI16" s="74"/>
-      <c r="AJ16" s="74"/>
-      <c r="AK16" s="23"/>
+      <c r="U16" s="129"/>
+      <c r="V16" s="129"/>
+      <c r="W16" s="129"/>
+      <c r="X16" s="129"/>
+      <c r="Y16" s="129"/>
+      <c r="Z16" s="129"/>
+      <c r="AA16" s="129"/>
+      <c r="AB16" s="129"/>
+      <c r="AC16" s="129"/>
+      <c r="AD16" s="129"/>
+      <c r="AE16" s="129"/>
+      <c r="AF16" s="129"/>
+      <c r="AG16" s="129"/>
+      <c r="AH16" s="129"/>
+      <c r="AI16" s="129"/>
+      <c r="AJ16" s="129"/>
+      <c r="AK16" s="14"/>
     </row>
     <row r="17" spans="1:37" ht="25.5" customHeight="1">
-      <c r="A17" s="20"/>
-      <c r="B17" s="61" t="s">
+      <c r="A17" s="13"/>
+      <c r="B17" s="127" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="62" t="s">
+      <c r="C17" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="63"/>
-      <c r="E17" s="75"/>
-      <c r="F17" s="75"/>
-      <c r="G17" s="75"/>
-      <c r="H17" s="75"/>
-      <c r="I17" s="75"/>
-      <c r="J17" s="76"/>
-      <c r="K17" s="77"/>
-      <c r="L17" s="78"/>
-      <c r="M17" s="75"/>
-      <c r="N17" s="79"/>
-      <c r="O17" s="80"/>
-      <c r="P17" s="81"/>
-      <c r="Q17" s="78"/>
-      <c r="R17" s="82"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="49"/>
+      <c r="K17" s="50"/>
+      <c r="L17" s="51"/>
+      <c r="M17" s="48"/>
+      <c r="N17" s="52"/>
+      <c r="O17" s="53"/>
+      <c r="P17" s="54"/>
+      <c r="Q17" s="51"/>
+      <c r="R17" s="55"/>
       <c r="S17" s="1"/>
-      <c r="T17" s="61" t="s">
+      <c r="T17" s="127" t="s">
         <v>14</v>
       </c>
-      <c r="U17" s="83" t="s">
+      <c r="U17" s="118" t="s">
         <v>43</v>
       </c>
-      <c r="V17" s="84"/>
-      <c r="W17" s="84"/>
-      <c r="X17" s="84"/>
-      <c r="Y17" s="84"/>
-      <c r="Z17" s="84"/>
-      <c r="AA17" s="84"/>
-      <c r="AB17" s="84"/>
-      <c r="AC17" s="84"/>
-      <c r="AD17" s="84"/>
-      <c r="AE17" s="84"/>
-      <c r="AF17" s="84"/>
-      <c r="AG17" s="84"/>
-      <c r="AH17" s="84"/>
-      <c r="AI17" s="84"/>
-      <c r="AJ17" s="85"/>
-      <c r="AK17" s="23"/>
+      <c r="V17" s="119"/>
+      <c r="W17" s="119"/>
+      <c r="X17" s="119"/>
+      <c r="Y17" s="119"/>
+      <c r="Z17" s="119"/>
+      <c r="AA17" s="119"/>
+      <c r="AB17" s="119"/>
+      <c r="AC17" s="119"/>
+      <c r="AD17" s="119"/>
+      <c r="AE17" s="119"/>
+      <c r="AF17" s="119"/>
+      <c r="AG17" s="119"/>
+      <c r="AH17" s="119"/>
+      <c r="AI17" s="119"/>
+      <c r="AJ17" s="120"/>
+      <c r="AK17" s="14"/>
     </row>
     <row r="18" spans="1:37" ht="37.5" customHeight="1" thickBot="1">
-      <c r="A18" s="20"/>
-      <c r="B18" s="67"/>
-      <c r="C18" s="68" t="s">
+      <c r="A18" s="13"/>
+      <c r="B18" s="128"/>
+      <c r="C18" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="86"/>
-      <c r="E18" s="87"/>
-      <c r="F18" s="88"/>
-      <c r="G18" s="88"/>
-      <c r="H18" s="88"/>
-      <c r="I18" s="88"/>
-      <c r="J18" s="89"/>
-      <c r="K18" s="90" t="s">
+      <c r="D18" s="56"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="58"/>
+      <c r="G18" s="58"/>
+      <c r="H18" s="58"/>
+      <c r="I18" s="58"/>
+      <c r="J18" s="59"/>
+      <c r="K18" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="L18" s="91"/>
-      <c r="M18" s="87"/>
-      <c r="N18" s="88"/>
-      <c r="O18" s="88"/>
-      <c r="P18" s="89"/>
-      <c r="Q18" s="89"/>
-      <c r="R18" s="92"/>
+      <c r="L18" s="61"/>
+      <c r="M18" s="57"/>
+      <c r="N18" s="58"/>
+      <c r="O18" s="58"/>
+      <c r="P18" s="59"/>
+      <c r="Q18" s="59"/>
+      <c r="R18" s="62"/>
       <c r="S18" s="1"/>
-      <c r="T18" s="93"/>
-      <c r="U18" s="94"/>
-      <c r="V18" s="95"/>
-      <c r="W18" s="95"/>
-      <c r="X18" s="95"/>
-      <c r="Y18" s="95"/>
-      <c r="Z18" s="95"/>
-      <c r="AA18" s="95"/>
-      <c r="AB18" s="95"/>
-      <c r="AC18" s="95"/>
-      <c r="AD18" s="95"/>
-      <c r="AE18" s="95"/>
-      <c r="AF18" s="95"/>
-      <c r="AG18" s="95"/>
-      <c r="AH18" s="95"/>
-      <c r="AI18" s="95"/>
-      <c r="AJ18" s="96"/>
-      <c r="AK18" s="23"/>
+      <c r="T18" s="130"/>
+      <c r="U18" s="121"/>
+      <c r="V18" s="122"/>
+      <c r="W18" s="122"/>
+      <c r="X18" s="122"/>
+      <c r="Y18" s="122"/>
+      <c r="Z18" s="122"/>
+      <c r="AA18" s="122"/>
+      <c r="AB18" s="122"/>
+      <c r="AC18" s="122"/>
+      <c r="AD18" s="122"/>
+      <c r="AE18" s="122"/>
+      <c r="AF18" s="122"/>
+      <c r="AG18" s="122"/>
+      <c r="AH18" s="122"/>
+      <c r="AI18" s="122"/>
+      <c r="AJ18" s="123"/>
+      <c r="AK18" s="14"/>
     </row>
     <row r="19" spans="1:37" ht="25.5" customHeight="1" thickBot="1">
-      <c r="A19" s="20"/>
-      <c r="B19" s="61" t="s">
+      <c r="A19" s="13"/>
+      <c r="B19" s="127" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="62" t="s">
+      <c r="C19" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="63"/>
-      <c r="E19" s="75"/>
-      <c r="F19" s="75"/>
-      <c r="G19" s="75"/>
-      <c r="H19" s="75"/>
-      <c r="I19" s="75"/>
-      <c r="J19" s="76"/>
-      <c r="K19" s="77"/>
-      <c r="L19" s="78"/>
-      <c r="M19" s="75"/>
-      <c r="N19" s="79"/>
-      <c r="O19" s="80"/>
-      <c r="P19" s="81"/>
-      <c r="Q19" s="78"/>
-      <c r="R19" s="82"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="49"/>
+      <c r="K19" s="50"/>
+      <c r="L19" s="51"/>
+      <c r="M19" s="48"/>
+      <c r="N19" s="52"/>
+      <c r="O19" s="53"/>
+      <c r="P19" s="54"/>
+      <c r="Q19" s="51"/>
+      <c r="R19" s="55"/>
       <c r="S19" s="1"/>
-      <c r="T19" s="67"/>
-      <c r="U19" s="97"/>
-      <c r="V19" s="98"/>
-      <c r="W19" s="98"/>
-      <c r="X19" s="98"/>
-      <c r="Y19" s="98"/>
-      <c r="Z19" s="98"/>
-      <c r="AA19" s="98"/>
-      <c r="AB19" s="98"/>
-      <c r="AC19" s="98"/>
-      <c r="AD19" s="98"/>
-      <c r="AE19" s="98"/>
-      <c r="AF19" s="98"/>
-      <c r="AG19" s="98"/>
-      <c r="AH19" s="98"/>
-      <c r="AI19" s="98"/>
-      <c r="AJ19" s="99"/>
-      <c r="AK19" s="23"/>
+      <c r="T19" s="128"/>
+      <c r="U19" s="124"/>
+      <c r="V19" s="125"/>
+      <c r="W19" s="125"/>
+      <c r="X19" s="125"/>
+      <c r="Y19" s="125"/>
+      <c r="Z19" s="125"/>
+      <c r="AA19" s="125"/>
+      <c r="AB19" s="125"/>
+      <c r="AC19" s="125"/>
+      <c r="AD19" s="125"/>
+      <c r="AE19" s="125"/>
+      <c r="AF19" s="125"/>
+      <c r="AG19" s="125"/>
+      <c r="AH19" s="125"/>
+      <c r="AI19" s="125"/>
+      <c r="AJ19" s="126"/>
+      <c r="AK19" s="14"/>
     </row>
     <row r="20" spans="1:37" ht="37.5" customHeight="1" thickBot="1">
-      <c r="A20" s="20"/>
-      <c r="B20" s="67"/>
-      <c r="C20" s="68" t="s">
+      <c r="A20" s="13"/>
+      <c r="B20" s="128"/>
+      <c r="C20" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="86"/>
-      <c r="E20" s="87"/>
-      <c r="F20" s="100"/>
-      <c r="G20" s="100"/>
-      <c r="H20" s="100"/>
-      <c r="I20" s="100"/>
-      <c r="J20" s="91"/>
-      <c r="K20" s="90" t="s">
+      <c r="D20" s="56"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="63"/>
+      <c r="G20" s="63"/>
+      <c r="H20" s="63"/>
+      <c r="I20" s="63"/>
+      <c r="J20" s="61"/>
+      <c r="K20" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="L20" s="91"/>
-      <c r="M20" s="87"/>
-      <c r="N20" s="100"/>
-      <c r="O20" s="100"/>
-      <c r="P20" s="91"/>
-      <c r="Q20" s="91"/>
-      <c r="R20" s="101"/>
+      <c r="L20" s="61"/>
+      <c r="M20" s="57"/>
+      <c r="N20" s="63"/>
+      <c r="O20" s="63"/>
+      <c r="P20" s="61"/>
+      <c r="Q20" s="61"/>
+      <c r="R20" s="64"/>
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
@@ -3805,10 +3807,10 @@
       <c r="AH20" s="1"/>
       <c r="AI20" s="1"/>
       <c r="AJ20" s="1"/>
-      <c r="AK20" s="23"/>
+      <c r="AK20" s="14"/>
     </row>
     <row r="21" spans="1:37" ht="12.75" customHeight="1">
-      <c r="A21" s="20"/>
+      <c r="A21" s="13"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -3826,8 +3828,8 @@
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
-      <c r="S21" s="102"/>
-      <c r="T21" s="103" t="s">
+      <c r="S21" s="65"/>
+      <c r="T21" s="66" t="s">
         <v>39</v>
       </c>
       <c r="U21" s="1"/>
@@ -3846,10 +3848,10 @@
       <c r="AH21" s="1"/>
       <c r="AI21" s="1"/>
       <c r="AJ21" s="1"/>
-      <c r="AK21" s="104"/>
+      <c r="AK21" s="67"/>
     </row>
     <row r="22" spans="1:37" ht="11.25" customHeight="1" thickBot="1">
-      <c r="A22" s="20"/>
+      <c r="A22" s="13"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -3867,301 +3869,301 @@
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
-      <c r="S22" s="102"/>
+      <c r="S22" s="65"/>
       <c r="T22" s="1"/>
-      <c r="U22" s="103" t="s">
+      <c r="U22" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="V22" s="105"/>
-      <c r="W22" s="105"/>
-      <c r="X22" s="105"/>
-      <c r="Y22" s="105"/>
-      <c r="Z22" s="105"/>
-      <c r="AA22" s="105"/>
-      <c r="AB22" s="105"/>
-      <c r="AC22" s="105"/>
-      <c r="AD22" s="105"/>
-      <c r="AE22" s="105"/>
-      <c r="AF22" s="105"/>
-      <c r="AG22" s="105"/>
-      <c r="AH22" s="105"/>
-      <c r="AI22" s="105"/>
+      <c r="V22" s="68"/>
+      <c r="W22" s="68"/>
+      <c r="X22" s="68"/>
+      <c r="Y22" s="68"/>
+      <c r="Z22" s="68"/>
+      <c r="AA22" s="68"/>
+      <c r="AB22" s="68"/>
+      <c r="AC22" s="68"/>
+      <c r="AD22" s="68"/>
+      <c r="AE22" s="68"/>
+      <c r="AF22" s="68"/>
+      <c r="AG22" s="68"/>
+      <c r="AH22" s="68"/>
+      <c r="AI22" s="68"/>
       <c r="AJ22" s="1"/>
-      <c r="AK22" s="104"/>
+      <c r="AK22" s="67"/>
     </row>
     <row r="23" spans="1:37" ht="11.25" customHeight="1">
-      <c r="A23" s="20"/>
-      <c r="B23" s="106"/>
-      <c r="C23" s="107"/>
-      <c r="D23" s="107"/>
-      <c r="E23" s="108"/>
-      <c r="F23" s="109"/>
-      <c r="G23" s="109"/>
-      <c r="H23" s="109"/>
-      <c r="I23" s="109"/>
-      <c r="J23" s="109"/>
-      <c r="K23" s="109"/>
-      <c r="L23" s="109"/>
-      <c r="M23" s="109"/>
-      <c r="N23" s="109"/>
-      <c r="O23" s="109"/>
-      <c r="P23" s="109"/>
-      <c r="Q23" s="109"/>
-      <c r="R23" s="110"/>
-      <c r="S23" s="102"/>
+      <c r="A23" s="13"/>
+      <c r="B23" s="69"/>
+      <c r="C23" s="70"/>
+      <c r="D23" s="70"/>
+      <c r="E23" s="71"/>
+      <c r="F23" s="72"/>
+      <c r="G23" s="72"/>
+      <c r="H23" s="72"/>
+      <c r="I23" s="72"/>
+      <c r="J23" s="72"/>
+      <c r="K23" s="72"/>
+      <c r="L23" s="72"/>
+      <c r="M23" s="72"/>
+      <c r="N23" s="72"/>
+      <c r="O23" s="72"/>
+      <c r="P23" s="72"/>
+      <c r="Q23" s="72"/>
+      <c r="R23" s="73"/>
+      <c r="S23" s="65"/>
       <c r="T23" s="1"/>
-      <c r="U23" s="103" t="s">
+      <c r="U23" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="V23" s="105"/>
-      <c r="W23" s="105"/>
-      <c r="X23" s="105"/>
-      <c r="Y23" s="105"/>
-      <c r="Z23" s="105"/>
-      <c r="AA23" s="105"/>
-      <c r="AB23" s="105"/>
-      <c r="AC23" s="105"/>
-      <c r="AD23" s="105"/>
-      <c r="AE23" s="105"/>
-      <c r="AF23" s="105"/>
-      <c r="AG23" s="105"/>
-      <c r="AH23" s="105"/>
-      <c r="AI23" s="105"/>
+      <c r="V23" s="68"/>
+      <c r="W23" s="68"/>
+      <c r="X23" s="68"/>
+      <c r="Y23" s="68"/>
+      <c r="Z23" s="68"/>
+      <c r="AA23" s="68"/>
+      <c r="AB23" s="68"/>
+      <c r="AC23" s="68"/>
+      <c r="AD23" s="68"/>
+      <c r="AE23" s="68"/>
+      <c r="AF23" s="68"/>
+      <c r="AG23" s="68"/>
+      <c r="AH23" s="68"/>
+      <c r="AI23" s="68"/>
       <c r="AJ23" s="1"/>
-      <c r="AK23" s="104"/>
+      <c r="AK23" s="67"/>
     </row>
     <row r="24" spans="1:37" ht="11.25" customHeight="1">
-      <c r="A24" s="20"/>
-      <c r="B24" s="111"/>
-      <c r="C24" s="112"/>
-      <c r="D24" s="112"/>
-      <c r="E24" s="113"/>
-      <c r="F24" s="114"/>
-      <c r="G24" s="114"/>
-      <c r="H24" s="114"/>
-      <c r="I24" s="114"/>
-      <c r="J24" s="114"/>
-      <c r="K24" s="114"/>
-      <c r="L24" s="115" t="s">
+      <c r="A24" s="13"/>
+      <c r="B24" s="74"/>
+      <c r="C24" s="75"/>
+      <c r="D24" s="75"/>
+      <c r="E24" s="76"/>
+      <c r="F24" s="77"/>
+      <c r="G24" s="77"/>
+      <c r="H24" s="77"/>
+      <c r="I24" s="77"/>
+      <c r="J24" s="77"/>
+      <c r="K24" s="77"/>
+      <c r="L24" s="117" t="s">
         <v>42</v>
       </c>
-      <c r="M24" s="115"/>
-      <c r="N24" s="115"/>
-      <c r="O24" s="115"/>
-      <c r="P24" s="115"/>
-      <c r="Q24" s="116" t="s">
+      <c r="M24" s="117"/>
+      <c r="N24" s="117"/>
+      <c r="O24" s="117"/>
+      <c r="P24" s="117"/>
+      <c r="Q24" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="R24" s="117"/>
-      <c r="S24" s="102"/>
+      <c r="R24" s="79"/>
+      <c r="S24" s="65"/>
       <c r="T24" s="1"/>
-      <c r="U24" s="103" t="s">
+      <c r="U24" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="V24" s="105"/>
-      <c r="W24" s="105"/>
-      <c r="X24" s="105"/>
-      <c r="Y24" s="105"/>
-      <c r="Z24" s="105"/>
-      <c r="AA24" s="105"/>
-      <c r="AB24" s="105"/>
-      <c r="AC24" s="105"/>
-      <c r="AD24" s="105"/>
-      <c r="AE24" s="105"/>
-      <c r="AF24" s="105"/>
-      <c r="AG24" s="105"/>
-      <c r="AH24" s="105"/>
-      <c r="AI24" s="105"/>
+      <c r="V24" s="68"/>
+      <c r="W24" s="68"/>
+      <c r="X24" s="68"/>
+      <c r="Y24" s="68"/>
+      <c r="Z24" s="68"/>
+      <c r="AA24" s="68"/>
+      <c r="AB24" s="68"/>
+      <c r="AC24" s="68"/>
+      <c r="AD24" s="68"/>
+      <c r="AE24" s="68"/>
+      <c r="AF24" s="68"/>
+      <c r="AG24" s="68"/>
+      <c r="AH24" s="68"/>
+      <c r="AI24" s="68"/>
       <c r="AJ24" s="1"/>
-      <c r="AK24" s="104"/>
+      <c r="AK24" s="67"/>
     </row>
     <row r="25" spans="1:37" ht="11.25" customHeight="1">
-      <c r="A25" s="20"/>
-      <c r="B25" s="111"/>
-      <c r="C25" s="112"/>
-      <c r="D25" s="112"/>
-      <c r="E25" s="113"/>
-      <c r="F25" s="118" t="s">
+      <c r="A25" s="13"/>
+      <c r="B25" s="74"/>
+      <c r="C25" s="75"/>
+      <c r="D25" s="75"/>
+      <c r="E25" s="76"/>
+      <c r="F25" s="100" t="s">
         <v>21</v>
       </c>
-      <c r="G25" s="118"/>
-      <c r="H25" s="118"/>
-      <c r="I25" s="118"/>
-      <c r="J25" s="118"/>
-      <c r="K25" s="114"/>
-      <c r="L25" s="114"/>
-      <c r="M25" s="114"/>
-      <c r="N25" s="114"/>
-      <c r="O25" s="114"/>
-      <c r="P25" s="114"/>
-      <c r="Q25" s="116"/>
-      <c r="R25" s="117"/>
-      <c r="S25" s="102"/>
+      <c r="G25" s="100"/>
+      <c r="H25" s="100"/>
+      <c r="I25" s="100"/>
+      <c r="J25" s="100"/>
+      <c r="K25" s="77"/>
+      <c r="L25" s="77"/>
+      <c r="M25" s="77"/>
+      <c r="N25" s="77"/>
+      <c r="O25" s="77"/>
+      <c r="P25" s="77"/>
+      <c r="Q25" s="78"/>
+      <c r="R25" s="79"/>
+      <c r="S25" s="65"/>
       <c r="T25" s="1"/>
-      <c r="U25" s="103" t="s">
+      <c r="U25" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="V25" s="105"/>
-      <c r="W25" s="105"/>
-      <c r="X25" s="105"/>
-      <c r="Y25" s="105"/>
-      <c r="Z25" s="105"/>
-      <c r="AA25" s="105"/>
-      <c r="AB25" s="105"/>
-      <c r="AC25" s="105"/>
-      <c r="AD25" s="105"/>
-      <c r="AE25" s="105"/>
-      <c r="AF25" s="105"/>
-      <c r="AG25" s="105"/>
-      <c r="AH25" s="105"/>
-      <c r="AI25" s="105"/>
+      <c r="V25" s="68"/>
+      <c r="W25" s="68"/>
+      <c r="X25" s="68"/>
+      <c r="Y25" s="68"/>
+      <c r="Z25" s="68"/>
+      <c r="AA25" s="68"/>
+      <c r="AB25" s="68"/>
+      <c r="AC25" s="68"/>
+      <c r="AD25" s="68"/>
+      <c r="AE25" s="68"/>
+      <c r="AF25" s="68"/>
+      <c r="AG25" s="68"/>
+      <c r="AH25" s="68"/>
+      <c r="AI25" s="68"/>
       <c r="AJ25" s="1"/>
-      <c r="AK25" s="104"/>
+      <c r="AK25" s="67"/>
     </row>
     <row r="26" spans="1:37" ht="11.25" customHeight="1">
-      <c r="A26" s="20"/>
-      <c r="B26" s="111"/>
-      <c r="C26" s="112"/>
-      <c r="D26" s="112"/>
-      <c r="E26" s="113"/>
-      <c r="F26" s="118"/>
-      <c r="G26" s="118"/>
-      <c r="H26" s="118"/>
-      <c r="I26" s="118"/>
-      <c r="J26" s="118"/>
-      <c r="K26" s="114"/>
-      <c r="L26" s="114"/>
-      <c r="M26" s="114"/>
-      <c r="N26" s="114"/>
-      <c r="O26" s="114"/>
-      <c r="P26" s="114"/>
-      <c r="Q26" s="114"/>
-      <c r="R26" s="117"/>
-      <c r="S26" s="102"/>
+      <c r="A26" s="13"/>
+      <c r="B26" s="74"/>
+      <c r="C26" s="75"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="76"/>
+      <c r="F26" s="100"/>
+      <c r="G26" s="100"/>
+      <c r="H26" s="100"/>
+      <c r="I26" s="100"/>
+      <c r="J26" s="100"/>
+      <c r="K26" s="77"/>
+      <c r="L26" s="77"/>
+      <c r="M26" s="77"/>
+      <c r="N26" s="77"/>
+      <c r="O26" s="77"/>
+      <c r="P26" s="77"/>
+      <c r="Q26" s="77"/>
+      <c r="R26" s="79"/>
+      <c r="S26" s="65"/>
       <c r="T26" s="1"/>
-      <c r="U26" s="103" t="s">
+      <c r="U26" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="V26" s="105"/>
-      <c r="W26" s="105"/>
-      <c r="X26" s="105"/>
-      <c r="Y26" s="105"/>
-      <c r="Z26" s="105"/>
-      <c r="AA26" s="105"/>
-      <c r="AB26" s="105"/>
-      <c r="AC26" s="105"/>
-      <c r="AD26" s="105"/>
-      <c r="AE26" s="105"/>
-      <c r="AF26" s="105"/>
-      <c r="AG26" s="105"/>
-      <c r="AH26" s="105"/>
-      <c r="AI26" s="105"/>
+      <c r="V26" s="68"/>
+      <c r="W26" s="68"/>
+      <c r="X26" s="68"/>
+      <c r="Y26" s="68"/>
+      <c r="Z26" s="68"/>
+      <c r="AA26" s="68"/>
+      <c r="AB26" s="68"/>
+      <c r="AC26" s="68"/>
+      <c r="AD26" s="68"/>
+      <c r="AE26" s="68"/>
+      <c r="AF26" s="68"/>
+      <c r="AG26" s="68"/>
+      <c r="AH26" s="68"/>
+      <c r="AI26" s="68"/>
       <c r="AJ26" s="1"/>
-      <c r="AK26" s="104"/>
+      <c r="AK26" s="67"/>
     </row>
     <row r="27" spans="1:37" ht="11.25" customHeight="1">
-      <c r="A27" s="20"/>
-      <c r="B27" s="111"/>
-      <c r="C27" s="112"/>
-      <c r="D27" s="112"/>
-      <c r="E27" s="113"/>
-      <c r="F27" s="118"/>
-      <c r="G27" s="118"/>
-      <c r="H27" s="118"/>
-      <c r="I27" s="118"/>
-      <c r="J27" s="118"/>
-      <c r="K27" s="118"/>
-      <c r="L27" s="118"/>
-      <c r="M27" s="118"/>
-      <c r="N27" s="118"/>
-      <c r="O27" s="118"/>
-      <c r="P27" s="118"/>
-      <c r="Q27" s="118"/>
-      <c r="R27" s="117"/>
-      <c r="S27" s="102"/>
+      <c r="A27" s="13"/>
+      <c r="B27" s="74"/>
+      <c r="C27" s="75"/>
+      <c r="D27" s="75"/>
+      <c r="E27" s="76"/>
+      <c r="F27" s="100"/>
+      <c r="G27" s="100"/>
+      <c r="H27" s="100"/>
+      <c r="I27" s="100"/>
+      <c r="J27" s="100"/>
+      <c r="K27" s="100"/>
+      <c r="L27" s="100"/>
+      <c r="M27" s="100"/>
+      <c r="N27" s="100"/>
+      <c r="O27" s="100"/>
+      <c r="P27" s="100"/>
+      <c r="Q27" s="100"/>
+      <c r="R27" s="79"/>
+      <c r="S27" s="65"/>
       <c r="T27" s="1"/>
-      <c r="U27" s="103" t="s">
+      <c r="U27" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="V27" s="105"/>
-      <c r="W27" s="105"/>
-      <c r="X27" s="105"/>
-      <c r="Y27" s="105"/>
-      <c r="Z27" s="105"/>
-      <c r="AA27" s="105"/>
-      <c r="AB27" s="105"/>
-      <c r="AC27" s="105"/>
-      <c r="AD27" s="105"/>
-      <c r="AE27" s="105"/>
-      <c r="AF27" s="105"/>
-      <c r="AG27" s="105"/>
-      <c r="AH27" s="105"/>
-      <c r="AI27" s="105"/>
+      <c r="V27" s="68"/>
+      <c r="W27" s="68"/>
+      <c r="X27" s="68"/>
+      <c r="Y27" s="68"/>
+      <c r="Z27" s="68"/>
+      <c r="AA27" s="68"/>
+      <c r="AB27" s="68"/>
+      <c r="AC27" s="68"/>
+      <c r="AD27" s="68"/>
+      <c r="AE27" s="68"/>
+      <c r="AF27" s="68"/>
+      <c r="AG27" s="68"/>
+      <c r="AH27" s="68"/>
+      <c r="AI27" s="68"/>
       <c r="AJ27" s="1"/>
-      <c r="AK27" s="104"/>
+      <c r="AK27" s="67"/>
     </row>
     <row r="28" spans="1:37" ht="11.25" customHeight="1">
-      <c r="A28" s="20"/>
-      <c r="B28" s="119" t="s">
+      <c r="A28" s="13"/>
+      <c r="B28" s="139" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="120"/>
-      <c r="D28" s="120"/>
-      <c r="E28" s="121"/>
-      <c r="F28" s="118"/>
-      <c r="G28" s="118"/>
-      <c r="H28" s="118"/>
-      <c r="I28" s="118"/>
-      <c r="J28" s="118"/>
-      <c r="K28" s="118"/>
-      <c r="L28" s="118"/>
-      <c r="M28" s="118"/>
-      <c r="N28" s="118"/>
-      <c r="O28" s="118"/>
-      <c r="P28" s="118"/>
-      <c r="Q28" s="118"/>
-      <c r="R28" s="117"/>
-      <c r="S28" s="102"/>
+      <c r="C28" s="142"/>
+      <c r="D28" s="142"/>
+      <c r="E28" s="143"/>
+      <c r="F28" s="100"/>
+      <c r="G28" s="100"/>
+      <c r="H28" s="100"/>
+      <c r="I28" s="100"/>
+      <c r="J28" s="100"/>
+      <c r="K28" s="100"/>
+      <c r="L28" s="100"/>
+      <c r="M28" s="100"/>
+      <c r="N28" s="100"/>
+      <c r="O28" s="100"/>
+      <c r="P28" s="100"/>
+      <c r="Q28" s="100"/>
+      <c r="R28" s="79"/>
+      <c r="S28" s="65"/>
       <c r="T28" s="1"/>
-      <c r="U28" s="103" t="s">
+      <c r="U28" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="V28" s="105"/>
-      <c r="W28" s="105"/>
-      <c r="X28" s="105"/>
-      <c r="Y28" s="105"/>
-      <c r="Z28" s="105"/>
-      <c r="AA28" s="105"/>
-      <c r="AB28" s="105"/>
-      <c r="AC28" s="105"/>
-      <c r="AD28" s="105"/>
-      <c r="AE28" s="105"/>
-      <c r="AF28" s="105"/>
-      <c r="AG28" s="105"/>
-      <c r="AH28" s="105"/>
-      <c r="AI28" s="105"/>
+      <c r="V28" s="68"/>
+      <c r="W28" s="68"/>
+      <c r="X28" s="68"/>
+      <c r="Y28" s="68"/>
+      <c r="Z28" s="68"/>
+      <c r="AA28" s="68"/>
+      <c r="AB28" s="68"/>
+      <c r="AC28" s="68"/>
+      <c r="AD28" s="68"/>
+      <c r="AE28" s="68"/>
+      <c r="AF28" s="68"/>
+      <c r="AG28" s="68"/>
+      <c r="AH28" s="68"/>
+      <c r="AI28" s="68"/>
       <c r="AJ28" s="1"/>
-      <c r="AK28" s="104"/>
+      <c r="AK28" s="67"/>
     </row>
     <row r="29" spans="1:37" ht="11.25" customHeight="1">
-      <c r="A29" s="20"/>
-      <c r="B29" s="122"/>
-      <c r="C29" s="123"/>
-      <c r="D29" s="123"/>
-      <c r="E29" s="124"/>
-      <c r="F29" s="118"/>
-      <c r="G29" s="118"/>
-      <c r="H29" s="118"/>
-      <c r="I29" s="118"/>
-      <c r="J29" s="118"/>
-      <c r="K29" s="118"/>
-      <c r="L29" s="118"/>
-      <c r="M29" s="118"/>
-      <c r="N29" s="118"/>
-      <c r="O29" s="118"/>
-      <c r="P29" s="118"/>
-      <c r="Q29" s="118"/>
-      <c r="R29" s="117"/>
+      <c r="A29" s="13"/>
+      <c r="B29" s="80"/>
+      <c r="C29" s="81"/>
+      <c r="D29" s="81"/>
+      <c r="E29" s="82"/>
+      <c r="F29" s="100"/>
+      <c r="G29" s="100"/>
+      <c r="H29" s="100"/>
+      <c r="I29" s="100"/>
+      <c r="J29" s="100"/>
+      <c r="K29" s="100"/>
+      <c r="L29" s="100"/>
+      <c r="M29" s="100"/>
+      <c r="N29" s="100"/>
+      <c r="O29" s="100"/>
+      <c r="P29" s="100"/>
+      <c r="Q29" s="100"/>
+      <c r="R29" s="79"/>
       <c r="S29" s="1"/>
       <c r="T29" s="1"/>
       <c r="U29" s="1"/>
@@ -4180,27 +4182,27 @@
       <c r="AH29" s="1"/>
       <c r="AI29" s="1"/>
       <c r="AJ29" s="1"/>
-      <c r="AK29" s="23"/>
+      <c r="AK29" s="14"/>
     </row>
     <row r="30" spans="1:37" ht="11.25" customHeight="1">
-      <c r="A30" s="20"/>
-      <c r="B30" s="122"/>
-      <c r="C30" s="123"/>
-      <c r="D30" s="123"/>
-      <c r="E30" s="124"/>
-      <c r="F30" s="118"/>
-      <c r="G30" s="118"/>
-      <c r="H30" s="118"/>
-      <c r="I30" s="118"/>
-      <c r="J30" s="118"/>
-      <c r="K30" s="118"/>
-      <c r="L30" s="118"/>
-      <c r="M30" s="118"/>
-      <c r="N30" s="118"/>
-      <c r="O30" s="118"/>
-      <c r="P30" s="118"/>
-      <c r="Q30" s="118"/>
-      <c r="R30" s="117"/>
+      <c r="A30" s="13"/>
+      <c r="B30" s="80"/>
+      <c r="C30" s="81"/>
+      <c r="D30" s="81"/>
+      <c r="E30" s="82"/>
+      <c r="F30" s="100"/>
+      <c r="G30" s="100"/>
+      <c r="H30" s="100"/>
+      <c r="I30" s="100"/>
+      <c r="J30" s="100"/>
+      <c r="K30" s="100"/>
+      <c r="L30" s="100"/>
+      <c r="M30" s="100"/>
+      <c r="N30" s="100"/>
+      <c r="O30" s="100"/>
+      <c r="P30" s="100"/>
+      <c r="Q30" s="100"/>
+      <c r="R30" s="79"/>
       <c r="S30" s="1"/>
       <c r="T30" s="1"/>
       <c r="U30" s="1"/>
@@ -4219,29 +4221,29 @@
       <c r="AH30" s="1"/>
       <c r="AI30" s="1"/>
       <c r="AJ30" s="1"/>
-      <c r="AK30" s="23"/>
+      <c r="AK30" s="14"/>
     </row>
     <row r="31" spans="1:37" ht="11.25" customHeight="1">
-      <c r="A31" s="20"/>
-      <c r="B31" s="119" t="s">
+      <c r="A31" s="13"/>
+      <c r="B31" s="139" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="120"/>
-      <c r="D31" s="120"/>
-      <c r="E31" s="121"/>
-      <c r="F31" s="118"/>
-      <c r="G31" s="118"/>
-      <c r="H31" s="118"/>
-      <c r="I31" s="118"/>
-      <c r="J31" s="118"/>
-      <c r="K31" s="118"/>
-      <c r="L31" s="118"/>
-      <c r="M31" s="118"/>
-      <c r="N31" s="118"/>
-      <c r="O31" s="118"/>
-      <c r="P31" s="118"/>
-      <c r="Q31" s="118"/>
-      <c r="R31" s="117"/>
+      <c r="C31" s="142"/>
+      <c r="D31" s="142"/>
+      <c r="E31" s="143"/>
+      <c r="F31" s="100"/>
+      <c r="G31" s="100"/>
+      <c r="H31" s="100"/>
+      <c r="I31" s="100"/>
+      <c r="J31" s="100"/>
+      <c r="K31" s="100"/>
+      <c r="L31" s="100"/>
+      <c r="M31" s="100"/>
+      <c r="N31" s="100"/>
+      <c r="O31" s="100"/>
+      <c r="P31" s="100"/>
+      <c r="Q31" s="100"/>
+      <c r="R31" s="79"/>
       <c r="S31" s="1"/>
       <c r="T31" s="1"/>
       <c r="U31" s="1"/>
@@ -4260,27 +4262,27 @@
       <c r="AH31" s="1"/>
       <c r="AI31" s="1"/>
       <c r="AJ31" s="1"/>
-      <c r="AK31" s="23"/>
+      <c r="AK31" s="14"/>
     </row>
     <row r="32" spans="1:37" ht="11.25" customHeight="1">
-      <c r="A32" s="20"/>
-      <c r="B32" s="125"/>
-      <c r="C32" s="126"/>
-      <c r="D32" s="126"/>
-      <c r="E32" s="127"/>
-      <c r="F32" s="118"/>
-      <c r="G32" s="118"/>
-      <c r="H32" s="118"/>
-      <c r="I32" s="118"/>
-      <c r="J32" s="118"/>
-      <c r="K32" s="118"/>
-      <c r="L32" s="118"/>
-      <c r="M32" s="118"/>
-      <c r="N32" s="118"/>
-      <c r="O32" s="118"/>
-      <c r="P32" s="118"/>
-      <c r="Q32" s="118"/>
-      <c r="R32" s="117"/>
+      <c r="A32" s="13"/>
+      <c r="B32" s="83"/>
+      <c r="C32" s="84"/>
+      <c r="D32" s="84"/>
+      <c r="E32" s="85"/>
+      <c r="F32" s="100"/>
+      <c r="G32" s="100"/>
+      <c r="H32" s="100"/>
+      <c r="I32" s="100"/>
+      <c r="J32" s="100"/>
+      <c r="K32" s="100"/>
+      <c r="L32" s="100"/>
+      <c r="M32" s="100"/>
+      <c r="N32" s="100"/>
+      <c r="O32" s="100"/>
+      <c r="P32" s="100"/>
+      <c r="Q32" s="100"/>
+      <c r="R32" s="79"/>
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
       <c r="U32" s="1"/>
@@ -4299,27 +4301,27 @@
       <c r="AH32" s="1"/>
       <c r="AI32" s="1"/>
       <c r="AJ32" s="1"/>
-      <c r="AK32" s="23"/>
+      <c r="AK32" s="14"/>
     </row>
     <row r="33" spans="1:37" ht="11.25" customHeight="1">
-      <c r="A33" s="20"/>
-      <c r="B33" s="125"/>
-      <c r="C33" s="126"/>
-      <c r="D33" s="126"/>
-      <c r="E33" s="127"/>
-      <c r="F33" s="118"/>
-      <c r="G33" s="118"/>
-      <c r="H33" s="118"/>
-      <c r="I33" s="118"/>
-      <c r="J33" s="118"/>
-      <c r="K33" s="118"/>
-      <c r="L33" s="118"/>
-      <c r="M33" s="118"/>
-      <c r="N33" s="118"/>
-      <c r="O33" s="118"/>
-      <c r="P33" s="118"/>
-      <c r="Q33" s="128"/>
-      <c r="R33" s="117"/>
+      <c r="A33" s="13"/>
+      <c r="B33" s="83"/>
+      <c r="C33" s="84"/>
+      <c r="D33" s="84"/>
+      <c r="E33" s="85"/>
+      <c r="F33" s="100"/>
+      <c r="G33" s="100"/>
+      <c r="H33" s="100"/>
+      <c r="I33" s="100"/>
+      <c r="J33" s="100"/>
+      <c r="K33" s="100"/>
+      <c r="L33" s="100"/>
+      <c r="M33" s="100"/>
+      <c r="N33" s="100"/>
+      <c r="O33" s="100"/>
+      <c r="P33" s="100"/>
+      <c r="Q33" s="86"/>
+      <c r="R33" s="79"/>
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
       <c r="U33" s="1"/>
@@ -4338,31 +4340,31 @@
       <c r="AH33" s="1"/>
       <c r="AI33" s="1"/>
       <c r="AJ33" s="1"/>
-      <c r="AK33" s="23"/>
+      <c r="AK33" s="14"/>
     </row>
     <row r="34" spans="1:37" ht="11.25" customHeight="1">
-      <c r="A34" s="20"/>
-      <c r="B34" s="119" t="s">
+      <c r="A34" s="13"/>
+      <c r="B34" s="139" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="129"/>
-      <c r="D34" s="129"/>
-      <c r="E34" s="130"/>
-      <c r="F34" s="118"/>
-      <c r="G34" s="118"/>
-      <c r="H34" s="118"/>
-      <c r="I34" s="118"/>
-      <c r="J34" s="118"/>
-      <c r="K34" s="118"/>
-      <c r="L34" s="118"/>
-      <c r="M34" s="118"/>
-      <c r="N34" s="118"/>
-      <c r="O34" s="118"/>
-      <c r="P34" s="118"/>
-      <c r="Q34" s="131" t="s">
+      <c r="C34" s="140"/>
+      <c r="D34" s="140"/>
+      <c r="E34" s="141"/>
+      <c r="F34" s="100"/>
+      <c r="G34" s="100"/>
+      <c r="H34" s="100"/>
+      <c r="I34" s="100"/>
+      <c r="J34" s="100"/>
+      <c r="K34" s="100"/>
+      <c r="L34" s="100"/>
+      <c r="M34" s="100"/>
+      <c r="N34" s="100"/>
+      <c r="O34" s="100"/>
+      <c r="P34" s="100"/>
+      <c r="Q34" s="144" t="s">
         <v>6</v>
       </c>
-      <c r="R34" s="117"/>
+      <c r="R34" s="79"/>
       <c r="S34" s="1"/>
       <c r="T34" s="1"/>
       <c r="U34" s="1"/>
@@ -4381,27 +4383,27 @@
       <c r="AH34" s="1"/>
       <c r="AI34" s="1"/>
       <c r="AJ34" s="1"/>
-      <c r="AK34" s="23"/>
+      <c r="AK34" s="14"/>
     </row>
     <row r="35" spans="1:37" ht="11.25" customHeight="1">
-      <c r="A35" s="20"/>
-      <c r="B35" s="125"/>
-      <c r="C35" s="126"/>
-      <c r="D35" s="126"/>
-      <c r="E35" s="127"/>
-      <c r="F35" s="118"/>
-      <c r="G35" s="118"/>
-      <c r="H35" s="118"/>
-      <c r="I35" s="118"/>
-      <c r="J35" s="118"/>
-      <c r="K35" s="118"/>
-      <c r="L35" s="118"/>
-      <c r="M35" s="118"/>
-      <c r="N35" s="118"/>
-      <c r="O35" s="118"/>
-      <c r="P35" s="118"/>
-      <c r="Q35" s="131"/>
-      <c r="R35" s="117"/>
+      <c r="A35" s="13"/>
+      <c r="B35" s="83"/>
+      <c r="C35" s="84"/>
+      <c r="D35" s="84"/>
+      <c r="E35" s="85"/>
+      <c r="F35" s="100"/>
+      <c r="G35" s="100"/>
+      <c r="H35" s="100"/>
+      <c r="I35" s="100"/>
+      <c r="J35" s="100"/>
+      <c r="K35" s="100"/>
+      <c r="L35" s="100"/>
+      <c r="M35" s="100"/>
+      <c r="N35" s="100"/>
+      <c r="O35" s="100"/>
+      <c r="P35" s="100"/>
+      <c r="Q35" s="144"/>
+      <c r="R35" s="79"/>
       <c r="S35" s="1"/>
       <c r="T35" s="1"/>
       <c r="U35" s="1"/>
@@ -4420,29 +4422,29 @@
       <c r="AH35" s="1"/>
       <c r="AI35" s="1"/>
       <c r="AJ35" s="1"/>
-      <c r="AK35" s="23"/>
+      <c r="AK35" s="14"/>
     </row>
     <row r="36" spans="1:37" ht="11.25" customHeight="1">
-      <c r="A36" s="20"/>
-      <c r="B36" s="125"/>
-      <c r="C36" s="126"/>
-      <c r="D36" s="126"/>
-      <c r="E36" s="127"/>
-      <c r="F36" s="118" t="s">
+      <c r="A36" s="13"/>
+      <c r="B36" s="83"/>
+      <c r="C36" s="84"/>
+      <c r="D36" s="84"/>
+      <c r="E36" s="85"/>
+      <c r="F36" s="100" t="s">
         <v>25</v>
       </c>
-      <c r="G36" s="118"/>
-      <c r="H36" s="118"/>
-      <c r="I36" s="118"/>
-      <c r="J36" s="118"/>
-      <c r="K36" s="118"/>
-      <c r="L36" s="118"/>
-      <c r="M36" s="118"/>
-      <c r="N36" s="118"/>
-      <c r="O36" s="118"/>
-      <c r="P36" s="118"/>
-      <c r="Q36" s="118"/>
-      <c r="R36" s="117"/>
+      <c r="G36" s="100"/>
+      <c r="H36" s="100"/>
+      <c r="I36" s="100"/>
+      <c r="J36" s="100"/>
+      <c r="K36" s="100"/>
+      <c r="L36" s="100"/>
+      <c r="M36" s="100"/>
+      <c r="N36" s="100"/>
+      <c r="O36" s="100"/>
+      <c r="P36" s="100"/>
+      <c r="Q36" s="100"/>
+      <c r="R36" s="79"/>
       <c r="S36" s="1"/>
       <c r="T36" s="1"/>
       <c r="U36" s="1"/>
@@ -4461,29 +4463,29 @@
       <c r="AH36" s="1"/>
       <c r="AI36" s="1"/>
       <c r="AJ36" s="1"/>
-      <c r="AK36" s="23"/>
+      <c r="AK36" s="14"/>
     </row>
     <row r="37" spans="1:37" ht="11.25" customHeight="1">
-      <c r="A37" s="20"/>
-      <c r="B37" s="119" t="s">
+      <c r="A37" s="13"/>
+      <c r="B37" s="139" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="129"/>
-      <c r="D37" s="129"/>
-      <c r="E37" s="130"/>
-      <c r="F37" s="118"/>
-      <c r="G37" s="118"/>
-      <c r="H37" s="118"/>
-      <c r="I37" s="118"/>
-      <c r="J37" s="118"/>
-      <c r="K37" s="118"/>
-      <c r="L37" s="118"/>
-      <c r="M37" s="118"/>
-      <c r="N37" s="118"/>
-      <c r="O37" s="118"/>
-      <c r="P37" s="118"/>
-      <c r="Q37" s="118"/>
-      <c r="R37" s="117"/>
+      <c r="C37" s="140"/>
+      <c r="D37" s="140"/>
+      <c r="E37" s="141"/>
+      <c r="F37" s="100"/>
+      <c r="G37" s="100"/>
+      <c r="H37" s="100"/>
+      <c r="I37" s="100"/>
+      <c r="J37" s="100"/>
+      <c r="K37" s="100"/>
+      <c r="L37" s="100"/>
+      <c r="M37" s="100"/>
+      <c r="N37" s="100"/>
+      <c r="O37" s="100"/>
+      <c r="P37" s="100"/>
+      <c r="Q37" s="100"/>
+      <c r="R37" s="79"/>
       <c r="S37" s="1"/>
       <c r="T37" s="1"/>
       <c r="U37" s="1"/>
@@ -4502,27 +4504,27 @@
       <c r="AH37" s="1"/>
       <c r="AI37" s="1"/>
       <c r="AJ37" s="1"/>
-      <c r="AK37" s="23"/>
+      <c r="AK37" s="14"/>
     </row>
     <row r="38" spans="1:37" ht="11.25" customHeight="1">
-      <c r="A38" s="20"/>
-      <c r="B38" s="122"/>
-      <c r="C38" s="123"/>
-      <c r="D38" s="123"/>
-      <c r="E38" s="124"/>
-      <c r="F38" s="118"/>
-      <c r="G38" s="118"/>
-      <c r="H38" s="118"/>
-      <c r="I38" s="118"/>
-      <c r="J38" s="118"/>
-      <c r="K38" s="118"/>
-      <c r="L38" s="118"/>
-      <c r="M38" s="118"/>
-      <c r="N38" s="118"/>
-      <c r="O38" s="118"/>
-      <c r="P38" s="118"/>
-      <c r="Q38" s="118"/>
-      <c r="R38" s="117"/>
+      <c r="A38" s="13"/>
+      <c r="B38" s="80"/>
+      <c r="C38" s="81"/>
+      <c r="D38" s="81"/>
+      <c r="E38" s="82"/>
+      <c r="F38" s="100"/>
+      <c r="G38" s="100"/>
+      <c r="H38" s="100"/>
+      <c r="I38" s="100"/>
+      <c r="J38" s="100"/>
+      <c r="K38" s="100"/>
+      <c r="L38" s="100"/>
+      <c r="M38" s="100"/>
+      <c r="N38" s="100"/>
+      <c r="O38" s="100"/>
+      <c r="P38" s="100"/>
+      <c r="Q38" s="100"/>
+      <c r="R38" s="79"/>
       <c r="S38" s="1"/>
       <c r="T38" s="1"/>
       <c r="U38" s="1"/>
@@ -4541,27 +4543,27 @@
       <c r="AH38" s="1"/>
       <c r="AI38" s="1"/>
       <c r="AJ38" s="1"/>
-      <c r="AK38" s="23"/>
+      <c r="AK38" s="14"/>
     </row>
     <row r="39" spans="1:37" ht="11.25" customHeight="1" thickBot="1">
-      <c r="A39" s="20"/>
-      <c r="B39" s="132"/>
-      <c r="C39" s="133"/>
-      <c r="D39" s="133"/>
-      <c r="E39" s="134"/>
-      <c r="F39" s="135"/>
-      <c r="G39" s="135"/>
-      <c r="H39" s="135"/>
-      <c r="I39" s="135"/>
-      <c r="J39" s="135"/>
-      <c r="K39" s="135"/>
-      <c r="L39" s="135"/>
-      <c r="M39" s="135"/>
-      <c r="N39" s="135"/>
-      <c r="O39" s="135"/>
-      <c r="P39" s="135"/>
-      <c r="Q39" s="135"/>
-      <c r="R39" s="136"/>
+      <c r="A39" s="13"/>
+      <c r="B39" s="87"/>
+      <c r="C39" s="88"/>
+      <c r="D39" s="88"/>
+      <c r="E39" s="89"/>
+      <c r="F39" s="90"/>
+      <c r="G39" s="90"/>
+      <c r="H39" s="90"/>
+      <c r="I39" s="90"/>
+      <c r="J39" s="90"/>
+      <c r="K39" s="90"/>
+      <c r="L39" s="90"/>
+      <c r="M39" s="90"/>
+      <c r="N39" s="90"/>
+      <c r="O39" s="90"/>
+      <c r="P39" s="90"/>
+      <c r="Q39" s="90"/>
+      <c r="R39" s="91"/>
       <c r="S39" s="1"/>
       <c r="T39" s="1"/>
       <c r="U39" s="1"/>
@@ -4580,10 +4582,10 @@
       <c r="AH39" s="1"/>
       <c r="AI39" s="1"/>
       <c r="AJ39" s="1"/>
-      <c r="AK39" s="23"/>
+      <c r="AK39" s="14"/>
     </row>
     <row r="40" spans="1:37" ht="10.5" customHeight="1">
-      <c r="A40" s="20"/>
+      <c r="A40" s="13"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -4619,29 +4621,29 @@
       <c r="AH40" s="1"/>
       <c r="AI40" s="1"/>
       <c r="AJ40" s="1"/>
-      <c r="AK40" s="23"/>
+      <c r="AK40" s="14"/>
     </row>
     <row r="41" spans="1:37" ht="24" customHeight="1">
-      <c r="A41" s="20"/>
-      <c r="B41" s="137" t="s">
+      <c r="A41" s="13"/>
+      <c r="B41" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="C41" s="138"/>
-      <c r="D41" s="138"/>
-      <c r="E41" s="138"/>
-      <c r="F41" s="138"/>
-      <c r="G41" s="138"/>
-      <c r="H41" s="138"/>
-      <c r="I41" s="138"/>
-      <c r="J41" s="138"/>
-      <c r="K41" s="138"/>
-      <c r="L41" s="138"/>
-      <c r="M41" s="138"/>
-      <c r="N41" s="138"/>
-      <c r="O41" s="138"/>
-      <c r="P41" s="138"/>
-      <c r="Q41" s="138"/>
-      <c r="R41" s="139"/>
+      <c r="C41" s="93"/>
+      <c r="D41" s="93"/>
+      <c r="E41" s="93"/>
+      <c r="F41" s="93"/>
+      <c r="G41" s="93"/>
+      <c r="H41" s="93"/>
+      <c r="I41" s="93"/>
+      <c r="J41" s="93"/>
+      <c r="K41" s="93"/>
+      <c r="L41" s="93"/>
+      <c r="M41" s="93"/>
+      <c r="N41" s="93"/>
+      <c r="O41" s="93"/>
+      <c r="P41" s="93"/>
+      <c r="Q41" s="93"/>
+      <c r="R41" s="94"/>
       <c r="S41" s="1"/>
       <c r="T41" s="1"/>
       <c r="U41" s="1"/>
@@ -4660,29 +4662,29 @@
       <c r="AH41" s="1"/>
       <c r="AI41" s="1"/>
       <c r="AJ41" s="1"/>
-      <c r="AK41" s="23"/>
+      <c r="AK41" s="14"/>
     </row>
     <row r="42" spans="1:37" ht="43.5" customHeight="1">
-      <c r="A42" s="20"/>
-      <c r="B42" s="140"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="14"/>
-      <c r="K42" s="14"/>
-      <c r="L42" s="14"/>
-      <c r="M42" s="14"/>
-      <c r="N42" s="14"/>
-      <c r="O42" s="14"/>
-      <c r="P42" s="141"/>
-      <c r="Q42" s="142" t="s">
+      <c r="A42" s="13"/>
+      <c r="B42" s="95"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="9"/>
+      <c r="K42" s="9"/>
+      <c r="L42" s="9"/>
+      <c r="M42" s="9"/>
+      <c r="N42" s="9"/>
+      <c r="O42" s="9"/>
+      <c r="P42" s="96"/>
+      <c r="Q42" s="97" t="s">
         <v>8</v>
       </c>
-      <c r="R42" s="143"/>
+      <c r="R42" s="98"/>
       <c r="S42" s="1"/>
       <c r="T42" s="1"/>
       <c r="U42" s="1"/>
@@ -4701,49 +4703,66 @@
       <c r="AH42" s="1"/>
       <c r="AI42" s="1"/>
       <c r="AJ42" s="1"/>
-      <c r="AK42" s="23"/>
+      <c r="AK42" s="14"/>
     </row>
     <row r="43" spans="1:37" ht="5.25" customHeight="1">
-      <c r="A43" s="140"/>
-      <c r="B43" s="14"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="14"/>
-      <c r="K43" s="14"/>
-      <c r="L43" s="14"/>
-      <c r="M43" s="14"/>
-      <c r="N43" s="14"/>
-      <c r="O43" s="14"/>
-      <c r="P43" s="14"/>
-      <c r="Q43" s="14"/>
-      <c r="R43" s="14"/>
-      <c r="S43" s="14"/>
-      <c r="T43" s="14"/>
-      <c r="U43" s="14"/>
-      <c r="V43" s="14"/>
-      <c r="W43" s="14"/>
-      <c r="X43" s="14"/>
-      <c r="Y43" s="14"/>
-      <c r="Z43" s="14"/>
-      <c r="AA43" s="14"/>
-      <c r="AB43" s="14"/>
-      <c r="AC43" s="14"/>
-      <c r="AD43" s="14"/>
-      <c r="AE43" s="14"/>
-      <c r="AF43" s="14"/>
-      <c r="AG43" s="14"/>
-      <c r="AH43" s="14"/>
-      <c r="AI43" s="14"/>
-      <c r="AJ43" s="14"/>
-      <c r="AK43" s="144"/>
+      <c r="A43" s="95"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="9"/>
+      <c r="J43" s="9"/>
+      <c r="K43" s="9"/>
+      <c r="L43" s="9"/>
+      <c r="M43" s="9"/>
+      <c r="N43" s="9"/>
+      <c r="O43" s="9"/>
+      <c r="P43" s="9"/>
+      <c r="Q43" s="9"/>
+      <c r="R43" s="9"/>
+      <c r="S43" s="9"/>
+      <c r="T43" s="9"/>
+      <c r="U43" s="9"/>
+      <c r="V43" s="9"/>
+      <c r="W43" s="9"/>
+      <c r="X43" s="9"/>
+      <c r="Y43" s="9"/>
+      <c r="Z43" s="9"/>
+      <c r="AA43" s="9"/>
+      <c r="AB43" s="9"/>
+      <c r="AC43" s="9"/>
+      <c r="AD43" s="9"/>
+      <c r="AE43" s="9"/>
+      <c r="AF43" s="9"/>
+      <c r="AG43" s="9"/>
+      <c r="AH43" s="9"/>
+      <c r="AI43" s="9"/>
+      <c r="AJ43" s="9"/>
+      <c r="AK43" s="99"/>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="F36:Q38"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="F27:Q29"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="F30:Q32"/>
+    <mergeCell ref="F33:P35"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="Q34:Q35"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="T16:AJ16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="T17:T19"/>
+    <mergeCell ref="B6:AK8"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B13:AJ13"/>
+    <mergeCell ref="B16:S16"/>
     <mergeCell ref="F25:J26"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="T11:U12"/>
@@ -4754,23 +4773,6 @@
     <mergeCell ref="AI2:AK2"/>
     <mergeCell ref="L24:P24"/>
     <mergeCell ref="U17:AJ19"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="T16:AJ16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="T17:T19"/>
-    <mergeCell ref="B6:AK8"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B13:AJ13"/>
-    <mergeCell ref="B16:S16"/>
-    <mergeCell ref="F36:Q38"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="F27:Q29"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="F30:Q32"/>
-    <mergeCell ref="F33:P35"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="Q34:Q35"/>
-    <mergeCell ref="B31:E31"/>
   </mergeCells>
   <phoneticPr fontId="5"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
HoaNT2 : fix bug 12396
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/ローマ字氏名届_帳票テンプレート.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/ローマ字氏名届_帳票テンプレート.xlsx
@@ -1435,6 +1435,60 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1512,60 +1566,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2074,15 +2074,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>127671</xdr:colOff>
+      <xdr:colOff>73243</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>51729</xdr:rowOff>
+      <xdr:rowOff>78943</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>38023</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>323773</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>74140</xdr:rowOff>
+      <xdr:rowOff>101354</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2097,8 +2097,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6775118" y="2598413"/>
-          <a:ext cx="251247" cy="192859"/>
+          <a:off x="6713529" y="2664300"/>
+          <a:ext cx="250530" cy="199304"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -2140,13 +2140,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>107577</xdr:colOff>
+      <xdr:colOff>66756</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>273445</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>17929</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>317286</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>463945</xdr:rowOff>
     </xdr:to>
@@ -2163,8 +2163,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6766091" y="2996157"/>
-          <a:ext cx="251814" cy="190500"/>
+          <a:off x="6707042" y="3035695"/>
+          <a:ext cx="250530" cy="190500"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -2206,15 +2206,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>317729</xdr:colOff>
+      <xdr:colOff>236087</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>60812</xdr:rowOff>
+      <xdr:rowOff>74419</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>228082</xdr:colOff>
+      <xdr:colOff>146440</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>83223</xdr:rowOff>
+      <xdr:rowOff>96830</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2229,7 +2229,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7978550" y="2673383"/>
+          <a:off x="7896908" y="2659776"/>
           <a:ext cx="250532" cy="199304"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -2272,13 +2272,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>307522</xdr:colOff>
+      <xdr:colOff>239487</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>264299</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>217875</xdr:colOff>
+      <xdr:colOff>149840</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>454799</xdr:rowOff>
     </xdr:to>
@@ -2295,7 +2295,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7968343" y="3053763"/>
+          <a:off x="7900308" y="3026549"/>
           <a:ext cx="250532" cy="190500"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -2954,8 +2954,8 @@
   </sheetPr>
   <dimension ref="A1:AL43"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="106" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="Z20" sqref="Z20"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScale="70" zoomScaleNormal="106" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection activeCell="Y15" sqref="Y15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.140625" defaultRowHeight="13.5"/>
@@ -3000,11 +3000,11 @@
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
       <c r="AE1" s="1"/>
-      <c r="AI1" s="101">
+      <c r="AI1" s="119">
         <v>72073</v>
       </c>
-      <c r="AJ1" s="101"/>
-      <c r="AK1" s="101"/>
+      <c r="AJ1" s="119"/>
+      <c r="AK1" s="119"/>
       <c r="AL1" s="1"/>
     </row>
     <row r="2" spans="1:38" ht="26.25" customHeight="1">
@@ -3039,16 +3039,16 @@
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
       <c r="AE2" s="1"/>
-      <c r="AF2" s="113" t="s">
+      <c r="AF2" s="131" t="s">
         <v>17</v>
       </c>
-      <c r="AG2" s="114"/>
-      <c r="AH2" s="115"/>
-      <c r="AI2" s="116" t="s">
+      <c r="AG2" s="132"/>
+      <c r="AH2" s="133"/>
+      <c r="AI2" s="134" t="s">
         <v>18</v>
       </c>
-      <c r="AJ2" s="114"/>
-      <c r="AK2" s="115"/>
+      <c r="AJ2" s="132"/>
+      <c r="AK2" s="133"/>
       <c r="AL2" s="1"/>
     </row>
     <row r="3" spans="1:38" ht="26.25" customHeight="1">
@@ -3172,122 +3172,122 @@
     </row>
     <row r="6" spans="1:38" ht="13.5" customHeight="1">
       <c r="A6" s="12"/>
-      <c r="B6" s="131" t="s">
+      <c r="B6" s="111" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="131"/>
-      <c r="D6" s="131"/>
-      <c r="E6" s="131"/>
-      <c r="F6" s="131"/>
-      <c r="G6" s="131"/>
-      <c r="H6" s="131"/>
-      <c r="I6" s="131"/>
-      <c r="J6" s="131"/>
-      <c r="K6" s="131"/>
-      <c r="L6" s="131"/>
-      <c r="M6" s="131"/>
-      <c r="N6" s="131"/>
-      <c r="O6" s="131"/>
-      <c r="P6" s="131"/>
-      <c r="Q6" s="131"/>
-      <c r="R6" s="131"/>
-      <c r="S6" s="131"/>
-      <c r="T6" s="131"/>
-      <c r="U6" s="131"/>
-      <c r="V6" s="131"/>
-      <c r="W6" s="131"/>
-      <c r="X6" s="131"/>
-      <c r="Y6" s="131"/>
-      <c r="Z6" s="131"/>
-      <c r="AA6" s="131"/>
-      <c r="AB6" s="131"/>
-      <c r="AC6" s="131"/>
-      <c r="AD6" s="131"/>
-      <c r="AE6" s="131"/>
-      <c r="AF6" s="131"/>
-      <c r="AG6" s="131"/>
-      <c r="AH6" s="131"/>
-      <c r="AI6" s="131"/>
-      <c r="AJ6" s="131"/>
-      <c r="AK6" s="132"/>
+      <c r="C6" s="111"/>
+      <c r="D6" s="111"/>
+      <c r="E6" s="111"/>
+      <c r="F6" s="111"/>
+      <c r="G6" s="111"/>
+      <c r="H6" s="111"/>
+      <c r="I6" s="111"/>
+      <c r="J6" s="111"/>
+      <c r="K6" s="111"/>
+      <c r="L6" s="111"/>
+      <c r="M6" s="111"/>
+      <c r="N6" s="111"/>
+      <c r="O6" s="111"/>
+      <c r="P6" s="111"/>
+      <c r="Q6" s="111"/>
+      <c r="R6" s="111"/>
+      <c r="S6" s="111"/>
+      <c r="T6" s="111"/>
+      <c r="U6" s="111"/>
+      <c r="V6" s="111"/>
+      <c r="W6" s="111"/>
+      <c r="X6" s="111"/>
+      <c r="Y6" s="111"/>
+      <c r="Z6" s="111"/>
+      <c r="AA6" s="111"/>
+      <c r="AB6" s="111"/>
+      <c r="AC6" s="111"/>
+      <c r="AD6" s="111"/>
+      <c r="AE6" s="111"/>
+      <c r="AF6" s="111"/>
+      <c r="AG6" s="111"/>
+      <c r="AH6" s="111"/>
+      <c r="AI6" s="111"/>
+      <c r="AJ6" s="111"/>
+      <c r="AK6" s="112"/>
     </row>
     <row r="7" spans="1:38" ht="13.5" customHeight="1">
       <c r="A7" s="13"/>
-      <c r="B7" s="133"/>
-      <c r="C7" s="133"/>
-      <c r="D7" s="133"/>
-      <c r="E7" s="133"/>
-      <c r="F7" s="133"/>
-      <c r="G7" s="133"/>
-      <c r="H7" s="133"/>
-      <c r="I7" s="133"/>
-      <c r="J7" s="133"/>
-      <c r="K7" s="133"/>
-      <c r="L7" s="133"/>
-      <c r="M7" s="133"/>
-      <c r="N7" s="133"/>
-      <c r="O7" s="133"/>
-      <c r="P7" s="133"/>
-      <c r="Q7" s="133"/>
-      <c r="R7" s="133"/>
-      <c r="S7" s="133"/>
-      <c r="T7" s="133"/>
-      <c r="U7" s="133"/>
-      <c r="V7" s="133"/>
-      <c r="W7" s="133"/>
-      <c r="X7" s="133"/>
-      <c r="Y7" s="133"/>
-      <c r="Z7" s="133"/>
-      <c r="AA7" s="133"/>
-      <c r="AB7" s="133"/>
-      <c r="AC7" s="133"/>
-      <c r="AD7" s="133"/>
-      <c r="AE7" s="133"/>
-      <c r="AF7" s="133"/>
-      <c r="AG7" s="133"/>
-      <c r="AH7" s="133"/>
-      <c r="AI7" s="133"/>
-      <c r="AJ7" s="133"/>
-      <c r="AK7" s="134"/>
+      <c r="B7" s="113"/>
+      <c r="C7" s="113"/>
+      <c r="D7" s="113"/>
+      <c r="E7" s="113"/>
+      <c r="F7" s="113"/>
+      <c r="G7" s="113"/>
+      <c r="H7" s="113"/>
+      <c r="I7" s="113"/>
+      <c r="J7" s="113"/>
+      <c r="K7" s="113"/>
+      <c r="L7" s="113"/>
+      <c r="M7" s="113"/>
+      <c r="N7" s="113"/>
+      <c r="O7" s="113"/>
+      <c r="P7" s="113"/>
+      <c r="Q7" s="113"/>
+      <c r="R7" s="113"/>
+      <c r="S7" s="113"/>
+      <c r="T7" s="113"/>
+      <c r="U7" s="113"/>
+      <c r="V7" s="113"/>
+      <c r="W7" s="113"/>
+      <c r="X7" s="113"/>
+      <c r="Y7" s="113"/>
+      <c r="Z7" s="113"/>
+      <c r="AA7" s="113"/>
+      <c r="AB7" s="113"/>
+      <c r="AC7" s="113"/>
+      <c r="AD7" s="113"/>
+      <c r="AE7" s="113"/>
+      <c r="AF7" s="113"/>
+      <c r="AG7" s="113"/>
+      <c r="AH7" s="113"/>
+      <c r="AI7" s="113"/>
+      <c r="AJ7" s="113"/>
+      <c r="AK7" s="114"/>
     </row>
     <row r="8" spans="1:38" ht="13.5" customHeight="1">
       <c r="A8" s="13"/>
-      <c r="B8" s="133"/>
-      <c r="C8" s="133"/>
-      <c r="D8" s="133"/>
-      <c r="E8" s="133"/>
-      <c r="F8" s="133"/>
-      <c r="G8" s="133"/>
-      <c r="H8" s="133"/>
-      <c r="I8" s="133"/>
-      <c r="J8" s="133"/>
-      <c r="K8" s="133"/>
-      <c r="L8" s="133"/>
-      <c r="M8" s="133"/>
-      <c r="N8" s="133"/>
-      <c r="O8" s="133"/>
-      <c r="P8" s="133"/>
-      <c r="Q8" s="133"/>
-      <c r="R8" s="133"/>
-      <c r="S8" s="133"/>
-      <c r="T8" s="133"/>
-      <c r="U8" s="133"/>
-      <c r="V8" s="133"/>
-      <c r="W8" s="133"/>
-      <c r="X8" s="133"/>
-      <c r="Y8" s="133"/>
-      <c r="Z8" s="133"/>
-      <c r="AA8" s="133"/>
-      <c r="AB8" s="133"/>
-      <c r="AC8" s="133"/>
-      <c r="AD8" s="133"/>
-      <c r="AE8" s="133"/>
-      <c r="AF8" s="133"/>
-      <c r="AG8" s="133"/>
-      <c r="AH8" s="133"/>
-      <c r="AI8" s="133"/>
-      <c r="AJ8" s="133"/>
-      <c r="AK8" s="134"/>
+      <c r="B8" s="113"/>
+      <c r="C8" s="113"/>
+      <c r="D8" s="113"/>
+      <c r="E8" s="113"/>
+      <c r="F8" s="113"/>
+      <c r="G8" s="113"/>
+      <c r="H8" s="113"/>
+      <c r="I8" s="113"/>
+      <c r="J8" s="113"/>
+      <c r="K8" s="113"/>
+      <c r="L8" s="113"/>
+      <c r="M8" s="113"/>
+      <c r="N8" s="113"/>
+      <c r="O8" s="113"/>
+      <c r="P8" s="113"/>
+      <c r="Q8" s="113"/>
+      <c r="R8" s="113"/>
+      <c r="S8" s="113"/>
+      <c r="T8" s="113"/>
+      <c r="U8" s="113"/>
+      <c r="V8" s="113"/>
+      <c r="W8" s="113"/>
+      <c r="X8" s="113"/>
+      <c r="Y8" s="113"/>
+      <c r="Z8" s="113"/>
+      <c r="AA8" s="113"/>
+      <c r="AB8" s="113"/>
+      <c r="AC8" s="113"/>
+      <c r="AD8" s="113"/>
+      <c r="AE8" s="113"/>
+      <c r="AF8" s="113"/>
+      <c r="AG8" s="113"/>
+      <c r="AH8" s="113"/>
+      <c r="AI8" s="113"/>
+      <c r="AJ8" s="113"/>
+      <c r="AK8" s="114"/>
     </row>
     <row r="9" spans="1:38" ht="18.75" customHeight="1">
       <c r="A9" s="13"/>
@@ -3403,27 +3403,27 @@
       <c r="S11" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="T11" s="102" t="s">
+      <c r="T11" s="120" t="s">
         <v>20</v>
       </c>
-      <c r="U11" s="103"/>
-      <c r="V11" s="102" t="s">
+      <c r="U11" s="121"/>
+      <c r="V11" s="120" t="s">
         <v>13</v>
       </c>
-      <c r="W11" s="106"/>
-      <c r="X11" s="106"/>
-      <c r="Y11" s="106"/>
-      <c r="Z11" s="103"/>
-      <c r="AA11" s="108"/>
-      <c r="AB11" s="109"/>
-      <c r="AC11" s="109"/>
-      <c r="AD11" s="109"/>
-      <c r="AE11" s="109"/>
-      <c r="AF11" s="112"/>
-      <c r="AG11" s="109"/>
-      <c r="AH11" s="109"/>
-      <c r="AI11" s="109"/>
-      <c r="AJ11" s="109"/>
+      <c r="W11" s="124"/>
+      <c r="X11" s="124"/>
+      <c r="Y11" s="124"/>
+      <c r="Z11" s="121"/>
+      <c r="AA11" s="126"/>
+      <c r="AB11" s="127"/>
+      <c r="AC11" s="127"/>
+      <c r="AD11" s="127"/>
+      <c r="AE11" s="127"/>
+      <c r="AF11" s="130"/>
+      <c r="AG11" s="127"/>
+      <c r="AH11" s="127"/>
+      <c r="AI11" s="127"/>
+      <c r="AJ11" s="127"/>
       <c r="AK11" s="14"/>
     </row>
     <row r="12" spans="1:38" ht="40.5" customHeight="1" thickBot="1">
@@ -3446,69 +3446,69 @@
       <c r="Q12" s="36"/>
       <c r="R12" s="37"/>
       <c r="S12" s="35"/>
-      <c r="T12" s="104"/>
-      <c r="U12" s="105"/>
-      <c r="V12" s="104"/>
-      <c r="W12" s="107"/>
-      <c r="X12" s="107"/>
-      <c r="Y12" s="107"/>
-      <c r="Z12" s="105"/>
-      <c r="AA12" s="110"/>
-      <c r="AB12" s="111"/>
-      <c r="AC12" s="111"/>
-      <c r="AD12" s="111"/>
-      <c r="AE12" s="111"/>
-      <c r="AF12" s="111"/>
-      <c r="AG12" s="111"/>
-      <c r="AH12" s="111"/>
-      <c r="AI12" s="111"/>
-      <c r="AJ12" s="111"/>
+      <c r="T12" s="122"/>
+      <c r="U12" s="123"/>
+      <c r="V12" s="122"/>
+      <c r="W12" s="125"/>
+      <c r="X12" s="125"/>
+      <c r="Y12" s="125"/>
+      <c r="Z12" s="123"/>
+      <c r="AA12" s="128"/>
+      <c r="AB12" s="129"/>
+      <c r="AC12" s="129"/>
+      <c r="AD12" s="129"/>
+      <c r="AE12" s="129"/>
+      <c r="AF12" s="129"/>
+      <c r="AG12" s="129"/>
+      <c r="AH12" s="129"/>
+      <c r="AI12" s="129"/>
+      <c r="AJ12" s="129"/>
       <c r="AK12" s="14"/>
     </row>
     <row r="13" spans="1:38" ht="23.25" customHeight="1" thickBot="1">
       <c r="A13" s="13"/>
-      <c r="B13" s="135" t="s">
+      <c r="B13" s="115" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="136"/>
-      <c r="D13" s="136"/>
-      <c r="E13" s="136"/>
-      <c r="F13" s="136"/>
-      <c r="G13" s="136"/>
-      <c r="H13" s="136"/>
-      <c r="I13" s="136"/>
-      <c r="J13" s="136"/>
-      <c r="K13" s="136"/>
-      <c r="L13" s="136"/>
-      <c r="M13" s="136"/>
-      <c r="N13" s="136"/>
-      <c r="O13" s="136"/>
-      <c r="P13" s="136"/>
-      <c r="Q13" s="136"/>
-      <c r="R13" s="136"/>
-      <c r="S13" s="136"/>
-      <c r="T13" s="136"/>
-      <c r="U13" s="136"/>
-      <c r="V13" s="136"/>
-      <c r="W13" s="136"/>
-      <c r="X13" s="136"/>
-      <c r="Y13" s="136"/>
-      <c r="Z13" s="136"/>
-      <c r="AA13" s="136"/>
-      <c r="AB13" s="136"/>
-      <c r="AC13" s="136"/>
-      <c r="AD13" s="136"/>
-      <c r="AE13" s="136"/>
-      <c r="AF13" s="136"/>
-      <c r="AG13" s="136"/>
-      <c r="AH13" s="136"/>
-      <c r="AI13" s="136"/>
-      <c r="AJ13" s="137"/>
+      <c r="C13" s="116"/>
+      <c r="D13" s="116"/>
+      <c r="E13" s="116"/>
+      <c r="F13" s="116"/>
+      <c r="G13" s="116"/>
+      <c r="H13" s="116"/>
+      <c r="I13" s="116"/>
+      <c r="J13" s="116"/>
+      <c r="K13" s="116"/>
+      <c r="L13" s="116"/>
+      <c r="M13" s="116"/>
+      <c r="N13" s="116"/>
+      <c r="O13" s="116"/>
+      <c r="P13" s="116"/>
+      <c r="Q13" s="116"/>
+      <c r="R13" s="116"/>
+      <c r="S13" s="116"/>
+      <c r="T13" s="116"/>
+      <c r="U13" s="116"/>
+      <c r="V13" s="116"/>
+      <c r="W13" s="116"/>
+      <c r="X13" s="116"/>
+      <c r="Y13" s="116"/>
+      <c r="Z13" s="116"/>
+      <c r="AA13" s="116"/>
+      <c r="AB13" s="116"/>
+      <c r="AC13" s="116"/>
+      <c r="AD13" s="116"/>
+      <c r="AE13" s="116"/>
+      <c r="AF13" s="116"/>
+      <c r="AG13" s="116"/>
+      <c r="AH13" s="116"/>
+      <c r="AI13" s="116"/>
+      <c r="AJ13" s="117"/>
       <c r="AK13" s="14"/>
     </row>
     <row r="14" spans="1:38" ht="25.5" customHeight="1">
       <c r="A14" s="13"/>
-      <c r="B14" s="127" t="s">
+      <c r="B14" s="107" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="38" t="s">
@@ -3551,7 +3551,7 @@
     </row>
     <row r="15" spans="1:38" ht="60.75" customHeight="1" thickBot="1">
       <c r="A15" s="13"/>
-      <c r="B15" s="128"/>
+      <c r="B15" s="108"/>
       <c r="C15" s="43" t="s">
         <v>23</v>
       </c>
@@ -3592,50 +3592,50 @@
     </row>
     <row r="16" spans="1:38" ht="43.5" customHeight="1" thickBot="1">
       <c r="A16" s="13"/>
-      <c r="B16" s="138" t="s">
+      <c r="B16" s="118" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="138"/>
-      <c r="D16" s="138"/>
-      <c r="E16" s="138"/>
-      <c r="F16" s="138"/>
-      <c r="G16" s="138"/>
-      <c r="H16" s="138"/>
-      <c r="I16" s="138"/>
-      <c r="J16" s="138"/>
-      <c r="K16" s="138"/>
-      <c r="L16" s="138"/>
-      <c r="M16" s="138"/>
-      <c r="N16" s="138"/>
-      <c r="O16" s="138"/>
-      <c r="P16" s="138"/>
-      <c r="Q16" s="138"/>
-      <c r="R16" s="138"/>
-      <c r="S16" s="138"/>
-      <c r="T16" s="129" t="s">
+      <c r="C16" s="118"/>
+      <c r="D16" s="118"/>
+      <c r="E16" s="118"/>
+      <c r="F16" s="118"/>
+      <c r="G16" s="118"/>
+      <c r="H16" s="118"/>
+      <c r="I16" s="118"/>
+      <c r="J16" s="118"/>
+      <c r="K16" s="118"/>
+      <c r="L16" s="118"/>
+      <c r="M16" s="118"/>
+      <c r="N16" s="118"/>
+      <c r="O16" s="118"/>
+      <c r="P16" s="118"/>
+      <c r="Q16" s="118"/>
+      <c r="R16" s="118"/>
+      <c r="S16" s="118"/>
+      <c r="T16" s="109" t="s">
         <v>22</v>
       </c>
-      <c r="U16" s="129"/>
-      <c r="V16" s="129"/>
-      <c r="W16" s="129"/>
-      <c r="X16" s="129"/>
-      <c r="Y16" s="129"/>
-      <c r="Z16" s="129"/>
-      <c r="AA16" s="129"/>
-      <c r="AB16" s="129"/>
-      <c r="AC16" s="129"/>
-      <c r="AD16" s="129"/>
-      <c r="AE16" s="129"/>
-      <c r="AF16" s="129"/>
-      <c r="AG16" s="129"/>
-      <c r="AH16" s="129"/>
-      <c r="AI16" s="129"/>
-      <c r="AJ16" s="129"/>
+      <c r="U16" s="109"/>
+      <c r="V16" s="109"/>
+      <c r="W16" s="109"/>
+      <c r="X16" s="109"/>
+      <c r="Y16" s="109"/>
+      <c r="Z16" s="109"/>
+      <c r="AA16" s="109"/>
+      <c r="AB16" s="109"/>
+      <c r="AC16" s="109"/>
+      <c r="AD16" s="109"/>
+      <c r="AE16" s="109"/>
+      <c r="AF16" s="109"/>
+      <c r="AG16" s="109"/>
+      <c r="AH16" s="109"/>
+      <c r="AI16" s="109"/>
+      <c r="AJ16" s="109"/>
       <c r="AK16" s="14"/>
     </row>
     <row r="17" spans="1:37" ht="25.5" customHeight="1">
       <c r="A17" s="13"/>
-      <c r="B17" s="127" t="s">
+      <c r="B17" s="107" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="38" t="s">
@@ -3657,32 +3657,32 @@
       <c r="Q17" s="51"/>
       <c r="R17" s="55"/>
       <c r="S17" s="1"/>
-      <c r="T17" s="127" t="s">
+      <c r="T17" s="107" t="s">
         <v>14</v>
       </c>
-      <c r="U17" s="118" t="s">
+      <c r="U17" s="136" t="s">
         <v>43</v>
       </c>
-      <c r="V17" s="119"/>
-      <c r="W17" s="119"/>
-      <c r="X17" s="119"/>
-      <c r="Y17" s="119"/>
-      <c r="Z17" s="119"/>
-      <c r="AA17" s="119"/>
-      <c r="AB17" s="119"/>
-      <c r="AC17" s="119"/>
-      <c r="AD17" s="119"/>
-      <c r="AE17" s="119"/>
-      <c r="AF17" s="119"/>
-      <c r="AG17" s="119"/>
-      <c r="AH17" s="119"/>
-      <c r="AI17" s="119"/>
-      <c r="AJ17" s="120"/>
+      <c r="V17" s="137"/>
+      <c r="W17" s="137"/>
+      <c r="X17" s="137"/>
+      <c r="Y17" s="137"/>
+      <c r="Z17" s="137"/>
+      <c r="AA17" s="137"/>
+      <c r="AB17" s="137"/>
+      <c r="AC17" s="137"/>
+      <c r="AD17" s="137"/>
+      <c r="AE17" s="137"/>
+      <c r="AF17" s="137"/>
+      <c r="AG17" s="137"/>
+      <c r="AH17" s="137"/>
+      <c r="AI17" s="137"/>
+      <c r="AJ17" s="138"/>
       <c r="AK17" s="14"/>
     </row>
     <row r="18" spans="1:37" ht="37.5" customHeight="1" thickBot="1">
       <c r="A18" s="13"/>
-      <c r="B18" s="128"/>
+      <c r="B18" s="108"/>
       <c r="C18" s="43" t="s">
         <v>4</v>
       </c>
@@ -3704,28 +3704,28 @@
       <c r="Q18" s="59"/>
       <c r="R18" s="62"/>
       <c r="S18" s="1"/>
-      <c r="T18" s="130"/>
-      <c r="U18" s="121"/>
-      <c r="V18" s="122"/>
-      <c r="W18" s="122"/>
-      <c r="X18" s="122"/>
-      <c r="Y18" s="122"/>
-      <c r="Z18" s="122"/>
-      <c r="AA18" s="122"/>
-      <c r="AB18" s="122"/>
-      <c r="AC18" s="122"/>
-      <c r="AD18" s="122"/>
-      <c r="AE18" s="122"/>
-      <c r="AF18" s="122"/>
-      <c r="AG18" s="122"/>
-      <c r="AH18" s="122"/>
-      <c r="AI18" s="122"/>
-      <c r="AJ18" s="123"/>
+      <c r="T18" s="110"/>
+      <c r="U18" s="139"/>
+      <c r="V18" s="140"/>
+      <c r="W18" s="140"/>
+      <c r="X18" s="140"/>
+      <c r="Y18" s="140"/>
+      <c r="Z18" s="140"/>
+      <c r="AA18" s="140"/>
+      <c r="AB18" s="140"/>
+      <c r="AC18" s="140"/>
+      <c r="AD18" s="140"/>
+      <c r="AE18" s="140"/>
+      <c r="AF18" s="140"/>
+      <c r="AG18" s="140"/>
+      <c r="AH18" s="140"/>
+      <c r="AI18" s="140"/>
+      <c r="AJ18" s="141"/>
       <c r="AK18" s="14"/>
     </row>
     <row r="19" spans="1:37" ht="25.5" customHeight="1" thickBot="1">
       <c r="A19" s="13"/>
-      <c r="B19" s="127" t="s">
+      <c r="B19" s="107" t="s">
         <v>10</v>
       </c>
       <c r="C19" s="38" t="s">
@@ -3747,28 +3747,28 @@
       <c r="Q19" s="51"/>
       <c r="R19" s="55"/>
       <c r="S19" s="1"/>
-      <c r="T19" s="128"/>
-      <c r="U19" s="124"/>
-      <c r="V19" s="125"/>
-      <c r="W19" s="125"/>
-      <c r="X19" s="125"/>
-      <c r="Y19" s="125"/>
-      <c r="Z19" s="125"/>
-      <c r="AA19" s="125"/>
-      <c r="AB19" s="125"/>
-      <c r="AC19" s="125"/>
-      <c r="AD19" s="125"/>
-      <c r="AE19" s="125"/>
-      <c r="AF19" s="125"/>
-      <c r="AG19" s="125"/>
-      <c r="AH19" s="125"/>
-      <c r="AI19" s="125"/>
-      <c r="AJ19" s="126"/>
+      <c r="T19" s="108"/>
+      <c r="U19" s="142"/>
+      <c r="V19" s="143"/>
+      <c r="W19" s="143"/>
+      <c r="X19" s="143"/>
+      <c r="Y19" s="143"/>
+      <c r="Z19" s="143"/>
+      <c r="AA19" s="143"/>
+      <c r="AB19" s="143"/>
+      <c r="AC19" s="143"/>
+      <c r="AD19" s="143"/>
+      <c r="AE19" s="143"/>
+      <c r="AF19" s="143"/>
+      <c r="AG19" s="143"/>
+      <c r="AH19" s="143"/>
+      <c r="AI19" s="143"/>
+      <c r="AJ19" s="144"/>
       <c r="AK19" s="14"/>
     </row>
     <row r="20" spans="1:37" ht="37.5" customHeight="1" thickBot="1">
       <c r="A20" s="13"/>
-      <c r="B20" s="128"/>
+      <c r="B20" s="108"/>
       <c r="C20" s="43" t="s">
         <v>4</v>
       </c>
@@ -3944,13 +3944,13 @@
       <c r="I24" s="77"/>
       <c r="J24" s="77"/>
       <c r="K24" s="77"/>
-      <c r="L24" s="117" t="s">
+      <c r="L24" s="135" t="s">
         <v>42</v>
       </c>
-      <c r="M24" s="117"/>
-      <c r="N24" s="117"/>
-      <c r="O24" s="117"/>
-      <c r="P24" s="117"/>
+      <c r="M24" s="135"/>
+      <c r="N24" s="135"/>
+      <c r="O24" s="135"/>
+      <c r="P24" s="135"/>
       <c r="Q24" s="78" t="s">
         <v>24</v>
       </c>
@@ -4104,12 +4104,12 @@
     </row>
     <row r="28" spans="1:37" ht="11.25" customHeight="1">
       <c r="A28" s="13"/>
-      <c r="B28" s="139" t="s">
+      <c r="B28" s="101" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="142"/>
-      <c r="D28" s="142"/>
-      <c r="E28" s="143"/>
+      <c r="C28" s="104"/>
+      <c r="D28" s="104"/>
+      <c r="E28" s="105"/>
       <c r="F28" s="100"/>
       <c r="G28" s="100"/>
       <c r="H28" s="100"/>
@@ -4225,12 +4225,12 @@
     </row>
     <row r="31" spans="1:37" ht="11.25" customHeight="1">
       <c r="A31" s="13"/>
-      <c r="B31" s="139" t="s">
+      <c r="B31" s="101" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="142"/>
-      <c r="D31" s="142"/>
-      <c r="E31" s="143"/>
+      <c r="C31" s="104"/>
+      <c r="D31" s="104"/>
+      <c r="E31" s="105"/>
       <c r="F31" s="100"/>
       <c r="G31" s="100"/>
       <c r="H31" s="100"/>
@@ -4344,12 +4344,12 @@
     </row>
     <row r="34" spans="1:37" ht="11.25" customHeight="1">
       <c r="A34" s="13"/>
-      <c r="B34" s="139" t="s">
+      <c r="B34" s="101" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="140"/>
-      <c r="D34" s="140"/>
-      <c r="E34" s="141"/>
+      <c r="C34" s="102"/>
+      <c r="D34" s="102"/>
+      <c r="E34" s="103"/>
       <c r="F34" s="100"/>
       <c r="G34" s="100"/>
       <c r="H34" s="100"/>
@@ -4361,7 +4361,7 @@
       <c r="N34" s="100"/>
       <c r="O34" s="100"/>
       <c r="P34" s="100"/>
-      <c r="Q34" s="144" t="s">
+      <c r="Q34" s="106" t="s">
         <v>6</v>
       </c>
       <c r="R34" s="79"/>
@@ -4402,7 +4402,7 @@
       <c r="N35" s="100"/>
       <c r="O35" s="100"/>
       <c r="P35" s="100"/>
-      <c r="Q35" s="144"/>
+      <c r="Q35" s="106"/>
       <c r="R35" s="79"/>
       <c r="S35" s="1"/>
       <c r="T35" s="1"/>
@@ -4467,12 +4467,12 @@
     </row>
     <row r="37" spans="1:37" ht="11.25" customHeight="1">
       <c r="A37" s="13"/>
-      <c r="B37" s="139" t="s">
+      <c r="B37" s="101" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="140"/>
-      <c r="D37" s="140"/>
-      <c r="E37" s="141"/>
+      <c r="C37" s="102"/>
+      <c r="D37" s="102"/>
+      <c r="E37" s="103"/>
       <c r="F37" s="100"/>
       <c r="G37" s="100"/>
       <c r="H37" s="100"/>
@@ -4746,23 +4746,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="F36:Q38"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="F27:Q29"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="F30:Q32"/>
-    <mergeCell ref="F33:P35"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="Q34:Q35"/>
-    <mergeCell ref="B31:E31"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="T16:AJ16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="T17:T19"/>
-    <mergeCell ref="B6:AK8"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B13:AJ13"/>
-    <mergeCell ref="B16:S16"/>
     <mergeCell ref="F25:J26"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="T11:U12"/>
@@ -4773,6 +4756,23 @@
     <mergeCell ref="AI2:AK2"/>
     <mergeCell ref="L24:P24"/>
     <mergeCell ref="U17:AJ19"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="T16:AJ16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="T17:T19"/>
+    <mergeCell ref="B6:AK8"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B13:AJ13"/>
+    <mergeCell ref="B16:S16"/>
+    <mergeCell ref="F36:Q38"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="F27:Q29"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="F30:Q32"/>
+    <mergeCell ref="F33:P35"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="Q34:Q35"/>
+    <mergeCell ref="B31:E31"/>
   </mergeCells>
   <phoneticPr fontId="5"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>